<commit_message>
Boat Enabled - Al Jazeera E
Boat Enabled - Al Jazeera E
</commit_message>
<xml_diff>
--- a/System_2.1.8.xlsx
+++ b/System_2.1.8.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Work_For_\Work\Running AppS\System_Work_RW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ACA4959-2DCF-43B9-A633-2760651FFEFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C4029E6-810F-477A-A8CF-BE0545B2F283}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1129" uniqueCount="633">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1129" uniqueCount="634">
   <si>
     <t>Zone</t>
   </si>
@@ -1938,6 +1938,9 @@
   </si>
   <si>
     <t xml:space="preserve"> WL F Police</t>
+  </si>
+  <si>
+    <t>France 24 ES</t>
   </si>
 </sst>
 </file>
@@ -4946,6 +4949,18 @@
     <xf numFmtId="0" fontId="4" fillId="53" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4994,6 +5009,288 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
     <xf numFmtId="0" fontId="32" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -5033,269 +5330,71 @@
     <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="43" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="43" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="43" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="40" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="40" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="40" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="52" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="52" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="14" fontId="5" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="14" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="14" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -5309,130 +5408,25 @@
     <xf numFmtId="0" fontId="3" fillId="35" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="43" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="43" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="43" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="40" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="40" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="40" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="52" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="52" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="14" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="14" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5510,38 +5504,47 @@
     <xf numFmtId="0" fontId="3" fillId="21" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5892,10 +5895,10 @@
       <c r="I2" s="412" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="588" t="s">
+      <c r="J2" s="592" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="589"/>
+      <c r="K2" s="593"/>
       <c r="L2" s="1" t="s">
         <v>8</v>
       </c>
@@ -5905,14 +5908,14 @@
       <c r="N2" s="358" t="s">
         <v>10</v>
       </c>
-      <c r="O2" s="590" t="s">
+      <c r="O2" s="594" t="s">
         <v>382</v>
       </c>
-      <c r="P2" s="591"/>
-      <c r="Q2" s="592"/>
-      <c r="R2" s="592"/>
-      <c r="S2" s="592"/>
-      <c r="T2" s="593" t="s">
+      <c r="P2" s="595"/>
+      <c r="Q2" s="596"/>
+      <c r="R2" s="596"/>
+      <c r="S2" s="596"/>
+      <c r="T2" s="597" t="s">
         <v>383</v>
       </c>
       <c r="V2" s="2" t="s">
@@ -5926,7 +5929,7 @@
       <c r="C3" s="168" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="585"/>
+      <c r="D3" s="589"/>
       <c r="E3" s="346"/>
       <c r="F3" s="270" t="s">
         <v>69</v>
@@ -5962,7 +5965,7 @@
       <c r="S3" s="24">
         <v>1</v>
       </c>
-      <c r="T3" s="594"/>
+      <c r="T3" s="598"/>
       <c r="U3" s="19" t="s">
         <v>577</v>
       </c>
@@ -5978,7 +5981,7 @@
       <c r="C4" s="168" t="s">
         <v>360</v>
       </c>
-      <c r="D4" s="586"/>
+      <c r="D4" s="590"/>
       <c r="E4" s="61"/>
       <c r="F4" s="368" t="s">
         <v>42</v>
@@ -5995,7 +5998,7 @@
       </c>
       <c r="O4" s="6"/>
       <c r="P4" s="319"/>
-      <c r="T4" s="594"/>
+      <c r="T4" s="598"/>
     </row>
     <row r="5" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
@@ -6004,7 +6007,7 @@
       <c r="C5" s="168" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="587"/>
+      <c r="D5" s="591"/>
       <c r="F5" s="372" t="s">
         <v>42</v>
       </c>
@@ -6023,7 +6026,7 @@
         <v>512</v>
       </c>
       <c r="P5" s="319"/>
-      <c r="T5" s="594"/>
+      <c r="T5" s="598"/>
       <c r="U5" s="208" t="s">
         <v>227</v>
       </c>
@@ -6062,7 +6065,7 @@
       <c r="P6" s="319"/>
       <c r="Q6" s="16"/>
       <c r="R6" s="6"/>
-      <c r="T6" s="594"/>
+      <c r="T6" s="598"/>
     </row>
     <row r="7" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="213" t="s">
@@ -6100,7 +6103,7 @@
       <c r="S7" s="24">
         <v>1</v>
       </c>
-      <c r="T7" s="594"/>
+      <c r="T7" s="598"/>
     </row>
     <row r="8" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
@@ -6129,7 +6132,7 @@
       <c r="P8" s="319"/>
       <c r="Q8" s="16"/>
       <c r="R8" s="6"/>
-      <c r="T8" s="594"/>
+      <c r="T8" s="598"/>
     </row>
     <row r="9" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
@@ -6174,7 +6177,7 @@
       <c r="S9" s="24">
         <v>1</v>
       </c>
-      <c r="T9" s="594"/>
+      <c r="T9" s="598"/>
     </row>
     <row r="10" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
@@ -6206,7 +6209,7 @@
         <v>512</v>
       </c>
       <c r="P10" s="319"/>
-      <c r="T10" s="594"/>
+      <c r="T10" s="598"/>
     </row>
     <row r="11" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
@@ -6248,7 +6251,7 @@
       <c r="S11" s="24">
         <v>1</v>
       </c>
-      <c r="T11" s="594"/>
+      <c r="T11" s="598"/>
       <c r="U11" s="208" t="s">
         <v>226</v>
       </c>
@@ -6281,7 +6284,7 @@
       <c r="P12" s="319"/>
       <c r="Q12" s="16"/>
       <c r="R12" s="142"/>
-      <c r="T12" s="594"/>
+      <c r="T12" s="598"/>
     </row>
     <row r="13" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="260" t="s">
@@ -6313,7 +6316,7 @@
       </c>
       <c r="P13" s="319"/>
       <c r="R13" s="142"/>
-      <c r="T13" s="594"/>
+      <c r="T13" s="598"/>
       <c r="U13" s="2" t="s">
         <v>601</v>
       </c>
@@ -6323,7 +6326,7 @@
     </row>
     <row r="14" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="P14" s="319"/>
-      <c r="T14" s="594"/>
+      <c r="T14" s="598"/>
     </row>
     <row r="15" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
@@ -6349,10 +6352,10 @@
       <c r="L15" s="137" t="s">
         <v>15</v>
       </c>
-      <c r="M15" s="582">
+      <c r="M15" s="586">
         <v>45275</v>
       </c>
-      <c r="N15" s="585" t="s">
+      <c r="N15" s="589" t="s">
         <v>22</v>
       </c>
       <c r="O15" s="496" t="s">
@@ -6370,7 +6373,7 @@
       <c r="S15" s="24">
         <v>1</v>
       </c>
-      <c r="T15" s="594"/>
+      <c r="T15" s="598"/>
     </row>
     <row r="16" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="483" t="s">
@@ -6396,8 +6399,8 @@
       <c r="L16" s="198" t="s">
         <v>15</v>
       </c>
-      <c r="M16" s="583"/>
-      <c r="N16" s="586"/>
+      <c r="M16" s="587"/>
+      <c r="N16" s="590"/>
       <c r="P16" s="319">
         <v>1</v>
       </c>
@@ -6410,7 +6413,7 @@
       <c r="S16" s="112">
         <v>1</v>
       </c>
-      <c r="T16" s="594"/>
+      <c r="T16" s="598"/>
     </row>
     <row r="17" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="2"/>
@@ -6436,8 +6439,8 @@
       <c r="L17" s="135" t="s">
         <v>15</v>
       </c>
-      <c r="M17" s="584"/>
-      <c r="N17" s="587"/>
+      <c r="M17" s="588"/>
+      <c r="N17" s="591"/>
       <c r="O17" s="496" t="s">
         <v>44</v>
       </c>
@@ -6453,11 +6456,11 @@
       <c r="S17" s="24">
         <v>1</v>
       </c>
-      <c r="T17" s="594"/>
+      <c r="T17" s="598"/>
     </row>
     <row r="18" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="P18" s="319"/>
-      <c r="T18" s="594"/>
+      <c r="T18" s="598"/>
     </row>
     <row r="19" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
@@ -6483,14 +6486,14 @@
       <c r="L19" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="M19" s="582">
+      <c r="M19" s="586">
         <v>45275</v>
       </c>
       <c r="N19" s="411" t="s">
         <v>512</v>
       </c>
       <c r="P19" s="319"/>
-      <c r="T19" s="594"/>
+      <c r="T19" s="598"/>
     </row>
     <row r="20" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="245" t="s">
@@ -6516,7 +6519,7 @@
       <c r="L20" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="M20" s="583"/>
+      <c r="M20" s="587"/>
       <c r="N20" s="401" t="s">
         <v>26</v>
       </c>
@@ -6532,7 +6535,7 @@
       <c r="S20" s="24">
         <v>1</v>
       </c>
-      <c r="T20" s="594"/>
+      <c r="T20" s="598"/>
     </row>
     <row r="21" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="245" t="s">
@@ -6558,7 +6561,7 @@
       <c r="L21" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="M21" s="583"/>
+      <c r="M21" s="587"/>
       <c r="N21" s="401" t="s">
         <v>18</v>
       </c>
@@ -6574,11 +6577,11 @@
       <c r="S21" s="24">
         <v>1</v>
       </c>
-      <c r="T21" s="594"/>
-      <c r="U21" s="580" t="s">
+      <c r="T21" s="598"/>
+      <c r="U21" s="584" t="s">
         <v>225</v>
       </c>
-      <c r="V21" s="581"/>
+      <c r="V21" s="585"/>
     </row>
     <row r="22" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="275" t="s">
@@ -6602,12 +6605,12 @@
       <c r="L22" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="M22" s="583"/>
+      <c r="M22" s="587"/>
       <c r="N22" s="381" t="s">
         <v>26</v>
       </c>
       <c r="P22" s="319"/>
-      <c r="T22" s="594"/>
+      <c r="T22" s="598"/>
       <c r="X22" s="19" t="s">
         <v>620</v>
       </c>
@@ -6634,12 +6637,12 @@
       <c r="L23" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="M23" s="583"/>
+      <c r="M23" s="587"/>
       <c r="N23" s="61" t="s">
         <v>513</v>
       </c>
       <c r="P23" s="319"/>
-      <c r="T23" s="594"/>
+      <c r="T23" s="598"/>
       <c r="U23" s="2" t="s">
         <v>610</v>
       </c>
@@ -6672,7 +6675,7 @@
       <c r="L24" s="135" t="s">
         <v>32</v>
       </c>
-      <c r="M24" s="583"/>
+      <c r="M24" s="587"/>
       <c r="N24" s="61" t="s">
         <v>26</v>
       </c>
@@ -6681,7 +6684,7 @@
       </c>
       <c r="P24" s="541"/>
       <c r="S24" s="80"/>
-      <c r="T24" s="594"/>
+      <c r="T24" s="598"/>
     </row>
     <row r="25" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="3" t="s">
@@ -6707,7 +6710,7 @@
       <c r="L25" s="135" t="s">
         <v>35</v>
       </c>
-      <c r="M25" s="583"/>
+      <c r="M25" s="587"/>
       <c r="N25" s="61" t="s">
         <v>26</v>
       </c>
@@ -6723,7 +6726,7 @@
       <c r="S25" s="21">
         <v>1</v>
       </c>
-      <c r="T25" s="594"/>
+      <c r="T25" s="598"/>
       <c r="V25" s="19"/>
     </row>
     <row r="26" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6750,12 +6753,12 @@
       <c r="L26" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="M26" s="583"/>
+      <c r="M26" s="587"/>
       <c r="N26" s="61" t="s">
         <v>514</v>
       </c>
       <c r="P26" s="319"/>
-      <c r="T26" s="594"/>
+      <c r="T26" s="598"/>
       <c r="V26" s="542" t="s">
         <v>619</v>
       </c>
@@ -6780,7 +6783,7 @@
       <c r="J27" s="408"/>
       <c r="K27" s="409"/>
       <c r="L27" s="410"/>
-      <c r="M27" s="583"/>
+      <c r="M27" s="587"/>
       <c r="N27" s="61"/>
       <c r="P27" s="319">
         <v>1</v>
@@ -6794,7 +6797,7 @@
       <c r="S27" s="24">
         <v>1</v>
       </c>
-      <c r="T27" s="594"/>
+      <c r="T27" s="598"/>
       <c r="W27" s="2" t="s">
         <v>593</v>
       </c>
@@ -6823,7 +6826,7 @@
       <c r="L28" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="M28" s="584"/>
+      <c r="M28" s="588"/>
       <c r="N28" s="61" t="s">
         <v>514</v>
       </c>
@@ -6839,7 +6842,7 @@
       <c r="S28" s="21">
         <v>1</v>
       </c>
-      <c r="T28" s="595"/>
+      <c r="T28" s="599"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -6927,7 +6930,7 @@
       <c r="H1" s="97" t="s">
         <v>349</v>
       </c>
-      <c r="I1" s="611" t="s">
+      <c r="I1" s="604" t="s">
         <v>375</v>
       </c>
       <c r="J1" s="2" t="s">
@@ -6963,7 +6966,7 @@
       <c r="X1" s="451" t="s">
         <v>156</v>
       </c>
-      <c r="Y1" s="670" t="s">
+      <c r="Y1" s="648" t="s">
         <v>539</v>
       </c>
       <c r="Z1" s="427">
@@ -6988,7 +6991,7 @@
         <v>507</v>
       </c>
       <c r="AM1" s="423"/>
-      <c r="AN1" s="652"/>
+      <c r="AN1" s="631"/>
       <c r="AO1" s="347" t="s">
         <v>478</v>
       </c>
@@ -6997,23 +7000,23 @@
       </c>
     </row>
     <row r="2" spans="1:43" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="634">
+      <c r="A2" s="657">
         <f ca="1">TODAY()</f>
         <v>45282</v>
       </c>
-      <c r="B2" s="636" t="s">
+      <c r="B2" s="659" t="s">
         <v>376</v>
       </c>
-      <c r="C2" s="613" t="s">
+      <c r="C2" s="636" t="s">
         <v>363</v>
       </c>
-      <c r="D2" s="638" t="s">
+      <c r="D2" s="661" t="s">
         <v>361</v>
       </c>
-      <c r="E2" s="682" t="s">
+      <c r="E2" s="600" t="s">
         <v>65</v>
       </c>
-      <c r="F2" s="657" t="s">
+      <c r="F2" s="610" t="s">
         <v>103</v>
       </c>
       <c r="G2" s="414" t="s">
@@ -7022,31 +7025,31 @@
       <c r="H2" s="80" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="612"/>
+      <c r="I2" s="605"/>
       <c r="J2" s="81" t="s">
         <v>77</v>
       </c>
-      <c r="K2" s="684" t="s">
+      <c r="K2" s="602" t="s">
         <v>348</v>
       </c>
-      <c r="L2" s="685"/>
-      <c r="M2" s="657" t="s">
+      <c r="L2" s="603"/>
+      <c r="M2" s="610" t="s">
         <v>103</v>
       </c>
       <c r="N2" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="O2" s="661" t="s">
+      <c r="O2" s="640" t="s">
         <v>103</v>
       </c>
       <c r="P2" s="85" t="s">
         <v>148</v>
       </c>
-      <c r="Q2" s="613" t="s">
+      <c r="Q2" s="636" t="s">
         <v>144</v>
       </c>
-      <c r="R2" s="585"/>
-      <c r="S2" s="674" t="s">
+      <c r="R2" s="589"/>
+      <c r="S2" s="625" t="s">
         <v>149</v>
       </c>
       <c r="T2" s="89"/>
@@ -7056,7 +7059,7 @@
       <c r="X2" s="452" t="s">
         <v>157</v>
       </c>
-      <c r="Y2" s="671"/>
+      <c r="Y2" s="649"/>
       <c r="Z2" s="428">
         <v>1</v>
       </c>
@@ -7079,15 +7082,15 @@
         <v>472</v>
       </c>
       <c r="AM2" s="449"/>
-      <c r="AN2" s="653"/>
+      <c r="AN2" s="632"/>
     </row>
     <row r="3" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="635"/>
-      <c r="B3" s="637"/>
-      <c r="C3" s="614"/>
-      <c r="D3" s="639"/>
-      <c r="E3" s="683"/>
-      <c r="F3" s="658"/>
+      <c r="A3" s="658"/>
+      <c r="B3" s="660"/>
+      <c r="C3" s="637"/>
+      <c r="D3" s="662"/>
+      <c r="E3" s="601"/>
+      <c r="F3" s="611"/>
       <c r="G3" s="415" t="s">
         <v>28</v>
       </c>
@@ -7106,17 +7109,17 @@
       <c r="L3" s="205" t="s">
         <v>108</v>
       </c>
-      <c r="M3" s="658"/>
+      <c r="M3" s="611"/>
       <c r="N3" s="69" t="s">
         <v>147</v>
       </c>
-      <c r="O3" s="662"/>
+      <c r="O3" s="641"/>
       <c r="P3" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="Q3" s="614"/>
-      <c r="R3" s="587"/>
-      <c r="S3" s="675"/>
+      <c r="Q3" s="637"/>
+      <c r="R3" s="591"/>
+      <c r="S3" s="627"/>
       <c r="T3" s="89"/>
       <c r="U3" s="124"/>
       <c r="V3" s="120"/>
@@ -7124,7 +7127,7 @@
       <c r="X3" s="452" t="s">
         <v>158</v>
       </c>
-      <c r="Y3" s="671"/>
+      <c r="Y3" s="649"/>
       <c r="Z3" s="429">
         <v>1</v>
       </c>
@@ -7133,7 +7136,7 @@
       <c r="AC3" s="100" t="s">
         <v>489</v>
       </c>
-      <c r="AD3" s="673" t="s">
+      <c r="AD3" s="622" t="s">
         <v>464</v>
       </c>
       <c r="AE3" s="261"/>
@@ -7145,16 +7148,16 @@
       <c r="AK3" s="261"/>
       <c r="AL3" s="16"/>
       <c r="AM3" s="449"/>
-      <c r="AN3" s="653"/>
+      <c r="AN3" s="632"/>
     </row>
     <row r="4" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="242" t="s">
         <v>184</v>
       </c>
-      <c r="B4" s="650" t="s">
+      <c r="B4" s="673" t="s">
         <v>379</v>
       </c>
-      <c r="C4" s="613" t="s">
+      <c r="C4" s="636" t="s">
         <v>155</v>
       </c>
       <c r="D4" s="356" t="s">
@@ -7163,7 +7166,7 @@
       <c r="E4" s="393">
         <v>2</v>
       </c>
-      <c r="F4" s="658"/>
+      <c r="F4" s="611"/>
       <c r="G4" s="397" t="s">
         <v>203</v>
       </c>
@@ -7180,11 +7183,11 @@
         <v>151</v>
       </c>
       <c r="L4" s="208"/>
-      <c r="M4" s="658"/>
+      <c r="M4" s="611"/>
       <c r="N4" s="178" t="s">
         <v>70</v>
       </c>
-      <c r="O4" s="662"/>
+      <c r="O4" s="641"/>
       <c r="P4" s="2" t="s">
         <v>192</v>
       </c>
@@ -7206,12 +7209,12 @@
       <c r="X4" s="452" t="s">
         <v>159</v>
       </c>
-      <c r="Y4" s="671"/>
+      <c r="Y4" s="649"/>
       <c r="Z4" s="430"/>
       <c r="AA4" s="312"/>
       <c r="AB4" s="213"/>
       <c r="AC4" s="16"/>
-      <c r="AD4" s="673"/>
+      <c r="AD4" s="622"/>
       <c r="AE4" s="261"/>
       <c r="AF4" s="261"/>
       <c r="AG4" s="16"/>
@@ -7221,37 +7224,37 @@
       <c r="AK4" s="261"/>
       <c r="AL4" s="16"/>
       <c r="AM4" s="449"/>
-      <c r="AN4" s="653"/>
+      <c r="AN4" s="632"/>
       <c r="AO4" s="347" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="611" t="s">
+      <c r="A5" s="604" t="s">
         <v>427</v>
       </c>
-      <c r="B5" s="651"/>
-      <c r="C5" s="614"/>
+      <c r="B5" s="674"/>
+      <c r="C5" s="637"/>
       <c r="D5" s="61" t="s">
         <v>154</v>
       </c>
       <c r="E5" s="394">
         <v>1</v>
       </c>
-      <c r="F5" s="658"/>
-      <c r="G5" s="642" t="s">
+      <c r="F5" s="611"/>
+      <c r="G5" s="665" t="s">
         <v>193</v>
       </c>
-      <c r="H5" s="642"/>
-      <c r="I5" s="642"/>
-      <c r="J5" s="642"/>
-      <c r="K5" s="642"/>
-      <c r="L5" s="643"/>
-      <c r="M5" s="658"/>
+      <c r="H5" s="665"/>
+      <c r="I5" s="665"/>
+      <c r="J5" s="665"/>
+      <c r="K5" s="665"/>
+      <c r="L5" s="666"/>
+      <c r="M5" s="611"/>
       <c r="N5" s="21">
         <v>8</v>
       </c>
-      <c r="O5" s="662"/>
+      <c r="O5" s="641"/>
       <c r="T5" s="89"/>
       <c r="U5" s="124"/>
       <c r="V5" s="120"/>
@@ -7259,7 +7262,7 @@
       <c r="X5" s="452" t="s">
         <v>160</v>
       </c>
-      <c r="Y5" s="671"/>
+      <c r="Y5" s="649"/>
       <c r="Z5" s="430">
         <v>1</v>
       </c>
@@ -7282,24 +7285,24 @@
       <c r="AK5" s="261"/>
       <c r="AL5" s="80"/>
       <c r="AM5" s="449"/>
-      <c r="AN5" s="653"/>
+      <c r="AN5" s="632"/>
     </row>
     <row r="6" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="612"/>
-      <c r="B6" s="648" t="s">
+      <c r="A6" s="605"/>
+      <c r="B6" s="671" t="s">
         <v>178</v>
       </c>
-      <c r="C6" s="609"/>
-      <c r="D6" s="610"/>
-      <c r="F6" s="658"/>
-      <c r="G6" s="644"/>
-      <c r="H6" s="644"/>
-      <c r="I6" s="644"/>
-      <c r="J6" s="644"/>
-      <c r="K6" s="644"/>
-      <c r="L6" s="645"/>
-      <c r="M6" s="658"/>
-      <c r="O6" s="662"/>
+      <c r="C6" s="619"/>
+      <c r="D6" s="620"/>
+      <c r="F6" s="611"/>
+      <c r="G6" s="667"/>
+      <c r="H6" s="667"/>
+      <c r="I6" s="667"/>
+      <c r="J6" s="667"/>
+      <c r="K6" s="667"/>
+      <c r="L6" s="668"/>
+      <c r="M6" s="611"/>
+      <c r="O6" s="641"/>
       <c r="T6" s="89"/>
       <c r="U6" s="124"/>
       <c r="V6" s="98" t="s">
@@ -7309,7 +7312,7 @@
       <c r="X6" s="452" t="s">
         <v>161</v>
       </c>
-      <c r="Y6" s="671"/>
+      <c r="Y6" s="649"/>
       <c r="Z6" s="428">
         <v>1</v>
       </c>
@@ -7323,16 +7326,16 @@
       <c r="AF6" s="261"/>
       <c r="AG6" s="261"/>
       <c r="AH6" s="261"/>
-      <c r="AI6" s="667"/>
+      <c r="AI6" s="621"/>
       <c r="AJ6" s="462" t="s">
         <v>467</v>
       </c>
-      <c r="AK6" s="667" t="s">
+      <c r="AK6" s="621" t="s">
         <v>255</v>
       </c>
       <c r="AL6" s="261"/>
       <c r="AM6" s="449"/>
-      <c r="AN6" s="653"/>
+      <c r="AN6" s="632"/>
       <c r="AO6" s="347" t="s">
         <v>479</v>
       </c>
@@ -7341,7 +7344,7 @@
       <c r="A7" s="236" t="s">
         <v>584</v>
       </c>
-      <c r="B7" s="649"/>
+      <c r="B7" s="672"/>
       <c r="C7" s="206" t="s">
         <v>380</v>
       </c>
@@ -7351,7 +7354,7 @@
       <c r="E7" s="270">
         <v>3</v>
       </c>
-      <c r="F7" s="658"/>
+      <c r="F7" s="611"/>
       <c r="G7" s="416">
         <v>0</v>
       </c>
@@ -7364,14 +7367,14 @@
       <c r="J7" s="30">
         <v>0</v>
       </c>
-      <c r="K7" s="585">
+      <c r="K7" s="589">
         <v>0</v>
       </c>
       <c r="L7" s="216">
         <v>0</v>
       </c>
-      <c r="M7" s="658"/>
-      <c r="O7" s="662"/>
+      <c r="M7" s="611"/>
+      <c r="O7" s="641"/>
       <c r="R7" s="99" t="s">
         <v>44</v>
       </c>
@@ -7385,7 +7388,7 @@
       <c r="X7" s="452" t="s">
         <v>162</v>
       </c>
-      <c r="Y7" s="671"/>
+      <c r="Y7" s="649"/>
       <c r="Z7" s="428">
         <v>1</v>
       </c>
@@ -7395,18 +7398,18 @@
       <c r="AD7" s="16"/>
       <c r="AE7" s="261"/>
       <c r="AF7" s="261"/>
-      <c r="AG7" s="673" t="s">
+      <c r="AG7" s="622" t="s">
         <v>463</v>
       </c>
       <c r="AH7" s="261"/>
-      <c r="AI7" s="667"/>
+      <c r="AI7" s="621"/>
       <c r="AJ7" s="261"/>
-      <c r="AK7" s="667"/>
+      <c r="AK7" s="621"/>
       <c r="AL7" s="80" t="s">
         <v>505</v>
       </c>
       <c r="AM7" s="449"/>
-      <c r="AN7" s="653"/>
+      <c r="AN7" s="632"/>
       <c r="AP7" s="76" t="s">
         <v>480</v>
       </c>
@@ -7423,27 +7426,27 @@
         <f>SUM(G7:N9)</f>
         <v>15</v>
       </c>
-      <c r="F8" s="658"/>
-      <c r="G8" s="643">
-        <v>0</v>
-      </c>
-      <c r="H8" s="640" t="s">
+      <c r="F8" s="611"/>
+      <c r="G8" s="666">
+        <v>0</v>
+      </c>
+      <c r="H8" s="663" t="s">
         <v>105</v>
       </c>
-      <c r="I8" s="585">
-        <v>0</v>
-      </c>
-      <c r="J8" s="640" t="s">
+      <c r="I8" s="589">
+        <v>0</v>
+      </c>
+      <c r="J8" s="663" t="s">
         <v>105</v>
       </c>
-      <c r="K8" s="646"/>
-      <c r="L8" s="676"/>
-      <c r="M8" s="659"/>
-      <c r="N8" s="679">
+      <c r="K8" s="669"/>
+      <c r="L8" s="623"/>
+      <c r="M8" s="638"/>
+      <c r="N8" s="628">
         <f>N5+N11</f>
         <v>15</v>
       </c>
-      <c r="O8" s="662"/>
+      <c r="O8" s="641"/>
       <c r="T8" s="103" t="s">
         <v>44</v>
       </c>
@@ -7453,7 +7456,7 @@
       <c r="X8" s="452" t="s">
         <v>163</v>
       </c>
-      <c r="Y8" s="671"/>
+      <c r="Y8" s="649"/>
       <c r="Z8" s="430"/>
       <c r="AA8" s="312"/>
       <c r="AB8" s="213"/>
@@ -7461,14 +7464,14 @@
       <c r="AD8" s="16"/>
       <c r="AE8" s="261"/>
       <c r="AF8" s="261"/>
-      <c r="AG8" s="673"/>
+      <c r="AG8" s="622"/>
       <c r="AH8" s="261"/>
-      <c r="AI8" s="667"/>
+      <c r="AI8" s="621"/>
       <c r="AJ8" s="261"/>
       <c r="AK8" s="261"/>
       <c r="AL8" s="261"/>
       <c r="AM8" s="449"/>
-      <c r="AN8" s="653"/>
+      <c r="AN8" s="632"/>
     </row>
     <row r="9" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="236" t="s">
@@ -7483,17 +7486,17 @@
       <c r="D9" s="357" t="s">
         <v>285</v>
       </c>
-      <c r="F9" s="658"/>
-      <c r="G9" s="645"/>
-      <c r="H9" s="641"/>
-      <c r="I9" s="587"/>
-      <c r="J9" s="641"/>
-      <c r="K9" s="647"/>
-      <c r="L9" s="677"/>
-      <c r="M9" s="660"/>
-      <c r="N9" s="680"/>
-      <c r="O9" s="663"/>
-      <c r="S9" s="674" t="s">
+      <c r="F9" s="611"/>
+      <c r="G9" s="668"/>
+      <c r="H9" s="664"/>
+      <c r="I9" s="591"/>
+      <c r="J9" s="664"/>
+      <c r="K9" s="670"/>
+      <c r="L9" s="624"/>
+      <c r="M9" s="639"/>
+      <c r="N9" s="629"/>
+      <c r="O9" s="642"/>
+      <c r="S9" s="625" t="s">
         <v>62</v>
       </c>
       <c r="T9" s="89"/>
@@ -7505,7 +7508,7 @@
       <c r="X9" s="452" t="s">
         <v>164</v>
       </c>
-      <c r="Y9" s="671"/>
+      <c r="Y9" s="649"/>
       <c r="Z9" s="431"/>
       <c r="AA9" s="312"/>
       <c r="AB9" s="213"/>
@@ -7515,16 +7518,16 @@
       </c>
       <c r="AE9" s="261"/>
       <c r="AF9" s="261"/>
-      <c r="AG9" s="673"/>
+      <c r="AG9" s="622"/>
       <c r="AH9" s="261"/>
-      <c r="AI9" s="667"/>
+      <c r="AI9" s="621"/>
       <c r="AJ9" s="80"/>
-      <c r="AK9" s="667" t="s">
+      <c r="AK9" s="621" t="s">
         <v>255</v>
       </c>
       <c r="AL9" s="261"/>
       <c r="AM9" s="449"/>
-      <c r="AN9" s="653"/>
+      <c r="AN9" s="632"/>
       <c r="AP9" s="2" t="s">
         <v>517</v>
       </c>
@@ -7541,20 +7544,20 @@
         <f>Boat!W8</f>
         <v>37</v>
       </c>
-      <c r="F10" s="658"/>
+      <c r="F10" s="611"/>
       <c r="N10" s="439" t="s">
         <v>403</v>
       </c>
-      <c r="O10" s="691" t="s">
+      <c r="O10" s="613" t="s">
         <v>103</v>
       </c>
-      <c r="P10" s="664" t="s">
+      <c r="P10" s="643" t="s">
         <v>407</v>
       </c>
       <c r="R10" s="74" t="s">
         <v>44</v>
       </c>
-      <c r="S10" s="678"/>
+      <c r="S10" s="626"/>
       <c r="T10" s="89"/>
       <c r="U10" s="123" t="s">
         <v>177</v>
@@ -7566,7 +7569,7 @@
       <c r="X10" s="452" t="s">
         <v>165</v>
       </c>
-      <c r="Y10" s="671"/>
+      <c r="Y10" s="649"/>
       <c r="Z10" s="430">
         <v>0</v>
       </c>
@@ -7584,16 +7587,16 @@
       <c r="AF10" s="242" t="s">
         <v>317</v>
       </c>
-      <c r="AG10" s="673"/>
+      <c r="AG10" s="622"/>
       <c r="AH10" s="80"/>
-      <c r="AI10" s="667"/>
+      <c r="AI10" s="621"/>
       <c r="AJ10" s="261"/>
-      <c r="AK10" s="667"/>
+      <c r="AK10" s="621"/>
       <c r="AL10" s="261"/>
       <c r="AM10" s="463" t="s">
         <v>324</v>
       </c>
-      <c r="AN10" s="653"/>
+      <c r="AN10" s="632"/>
       <c r="AO10" s="208" t="s">
         <v>95</v>
       </c>
@@ -7602,7 +7605,7 @@
       <c r="A11" s="227" t="s">
         <v>289</v>
       </c>
-      <c r="B11" s="585" t="s">
+      <c r="B11" s="589" t="s">
         <v>287</v>
       </c>
       <c r="C11" s="478" t="s">
@@ -7611,18 +7614,18 @@
       <c r="D11" s="174" t="s">
         <v>361</v>
       </c>
-      <c r="F11" s="658"/>
+      <c r="F11" s="611"/>
       <c r="M11" s="6"/>
       <c r="N11" s="117">
         <v>7</v>
       </c>
-      <c r="O11" s="692"/>
-      <c r="P11" s="665"/>
+      <c r="O11" s="614"/>
+      <c r="P11" s="644"/>
       <c r="Q11" s="65"/>
       <c r="R11" s="120" t="s">
         <v>222</v>
       </c>
-      <c r="S11" s="678"/>
+      <c r="S11" s="626"/>
       <c r="T11" s="102" t="s">
         <v>44</v>
       </c>
@@ -7632,7 +7635,7 @@
       <c r="X11" s="452" t="s">
         <v>166</v>
       </c>
-      <c r="Y11" s="671"/>
+      <c r="Y11" s="649"/>
       <c r="Z11" s="430"/>
       <c r="AA11" s="312">
         <v>1</v>
@@ -7646,14 +7649,14 @@
       <c r="AF11" s="261" t="s">
         <v>485</v>
       </c>
-      <c r="AG11" s="673"/>
+      <c r="AG11" s="622"/>
       <c r="AH11" s="261"/>
       <c r="AI11" s="70"/>
       <c r="AJ11" s="261"/>
       <c r="AK11" s="261"/>
       <c r="AL11" s="261"/>
       <c r="AM11" s="449"/>
-      <c r="AN11" s="653"/>
+      <c r="AN11" s="632"/>
       <c r="AP11" s="76" t="s">
         <v>493</v>
       </c>
@@ -7662,7 +7665,7 @@
       <c r="A12" s="231" t="s">
         <v>390</v>
       </c>
-      <c r="B12" s="587"/>
+      <c r="B12" s="591"/>
       <c r="C12" s="479" t="s">
         <v>391</v>
       </c>
@@ -7672,25 +7675,25 @@
       <c r="E12" s="228">
         <v>3</v>
       </c>
-      <c r="F12" s="658"/>
+      <c r="F12" s="611"/>
       <c r="G12" s="346" t="s">
         <v>407</v>
       </c>
-      <c r="H12" s="590" t="s">
+      <c r="H12" s="594" t="s">
         <v>438</v>
       </c>
-      <c r="I12" s="592"/>
-      <c r="J12" s="592"/>
-      <c r="K12" s="696"/>
+      <c r="I12" s="596"/>
+      <c r="J12" s="596"/>
+      <c r="K12" s="618"/>
       <c r="L12" s="207"/>
       <c r="M12" s="207"/>
       <c r="N12" s="207"/>
-      <c r="O12" s="692"/>
-      <c r="P12" s="665"/>
+      <c r="O12" s="614"/>
+      <c r="P12" s="644"/>
       <c r="R12" s="122" t="s">
         <v>181</v>
       </c>
-      <c r="S12" s="675"/>
+      <c r="S12" s="627"/>
       <c r="T12" s="101" t="s">
         <v>44</v>
       </c>
@@ -7700,7 +7703,7 @@
       <c r="X12" s="452" t="s">
         <v>167</v>
       </c>
-      <c r="Y12" s="671"/>
+      <c r="Y12" s="649"/>
       <c r="Z12" s="428">
         <v>1</v>
       </c>
@@ -7711,16 +7714,16 @@
       <c r="AC12" s="100" t="s">
         <v>490</v>
       </c>
-      <c r="AD12" s="681" t="s">
+      <c r="AD12" s="630" t="s">
         <v>244</v>
       </c>
       <c r="AE12" s="462" t="s">
         <v>243</v>
       </c>
-      <c r="AF12" s="673" t="s">
+      <c r="AF12" s="622" t="s">
         <v>230</v>
       </c>
-      <c r="AG12" s="673"/>
+      <c r="AG12" s="622"/>
       <c r="AH12" s="242" t="s">
         <v>263</v>
       </c>
@@ -7730,10 +7733,10 @@
       <c r="AJ12" s="261"/>
       <c r="AK12" s="261"/>
       <c r="AL12" s="261"/>
-      <c r="AM12" s="668" t="s">
+      <c r="AM12" s="646" t="s">
         <v>253</v>
       </c>
-      <c r="AN12" s="653"/>
+      <c r="AN12" s="632"/>
       <c r="AO12" s="347" t="s">
         <v>97</v>
       </c>
@@ -7745,17 +7748,17 @@
       <c r="E13" s="469">
         <v>-3</v>
       </c>
-      <c r="F13" s="658"/>
-      <c r="G13" s="592" t="s">
+      <c r="F13" s="611"/>
+      <c r="G13" s="596" t="s">
         <v>439</v>
       </c>
-      <c r="H13" s="592"/>
-      <c r="I13" s="592"/>
-      <c r="J13" s="696"/>
+      <c r="H13" s="596"/>
+      <c r="I13" s="596"/>
+      <c r="J13" s="618"/>
       <c r="M13" s="6"/>
       <c r="N13" s="6"/>
-      <c r="O13" s="692"/>
-      <c r="P13" s="666"/>
+      <c r="O13" s="614"/>
+      <c r="P13" s="645"/>
       <c r="T13" s="105" t="s">
         <v>44</v>
       </c>
@@ -7765,7 +7768,7 @@
       <c r="X13" s="452" t="s">
         <v>168</v>
       </c>
-      <c r="Y13" s="671"/>
+      <c r="Y13" s="649"/>
       <c r="Z13" s="428">
         <v>1</v>
       </c>
@@ -7776,8 +7779,8 @@
         <v>509</v>
       </c>
       <c r="AC13" s="16"/>
-      <c r="AD13" s="681"/>
-      <c r="AF13" s="673"/>
+      <c r="AD13" s="630"/>
+      <c r="AF13" s="622"/>
       <c r="AG13" s="80"/>
       <c r="AH13" s="242" t="s">
         <v>313</v>
@@ -7788,8 +7791,8 @@
       <c r="AJ13" s="80"/>
       <c r="AK13" s="261"/>
       <c r="AL13" s="261"/>
-      <c r="AM13" s="668"/>
-      <c r="AN13" s="653"/>
+      <c r="AM13" s="646"/>
+      <c r="AN13" s="632"/>
     </row>
     <row r="14" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="471"/>
@@ -7797,18 +7800,18 @@
       <c r="C14" s="480"/>
       <c r="D14" s="473"/>
       <c r="E14" s="474"/>
-      <c r="F14" s="658"/>
-      <c r="G14" s="592" t="s">
+      <c r="F14" s="611"/>
+      <c r="G14" s="596" t="s">
         <v>438</v>
       </c>
-      <c r="H14" s="592"/>
-      <c r="I14" s="592"/>
-      <c r="J14" s="696"/>
+      <c r="H14" s="596"/>
+      <c r="I14" s="596"/>
+      <c r="J14" s="618"/>
       <c r="K14" s="2">
         <v>12</v>
       </c>
       <c r="N14" s="6"/>
-      <c r="O14" s="692"/>
+      <c r="O14" s="614"/>
       <c r="Q14" s="61" t="s">
         <v>543</v>
       </c>
@@ -7822,34 +7825,34 @@
       <c r="X14" s="452" t="s">
         <v>169</v>
       </c>
-      <c r="Y14" s="671"/>
+      <c r="Y14" s="649"/>
       <c r="Z14" s="428">
         <v>1</v>
       </c>
       <c r="AA14" s="312"/>
       <c r="AB14" s="213"/>
       <c r="AC14" s="16"/>
-      <c r="AD14" s="681"/>
+      <c r="AD14" s="630"/>
       <c r="AE14" s="261"/>
-      <c r="AF14" s="673"/>
+      <c r="AF14" s="622"/>
       <c r="AG14" s="261"/>
       <c r="AH14" s="261"/>
       <c r="AI14" s="70"/>
       <c r="AJ14" s="261"/>
       <c r="AK14" s="261"/>
       <c r="AL14" s="261"/>
-      <c r="AM14" s="668"/>
-      <c r="AN14" s="653"/>
+      <c r="AM14" s="646"/>
+      <c r="AN14" s="632"/>
     </row>
     <row r="15" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="470" t="s">
         <v>515</v>
       </c>
-      <c r="C15" s="585" t="s">
+      <c r="C15" s="589" t="s">
         <v>379</v>
       </c>
-      <c r="F15" s="658"/>
-      <c r="O15" s="692"/>
+      <c r="F15" s="611"/>
+      <c r="O15" s="614"/>
       <c r="R15" s="99" t="s">
         <v>44</v>
       </c>
@@ -7862,7 +7865,7 @@
       <c r="X15" s="452" t="s">
         <v>170</v>
       </c>
-      <c r="Y15" s="671"/>
+      <c r="Y15" s="649"/>
       <c r="Z15" s="430">
         <v>1</v>
       </c>
@@ -7871,8 +7874,8 @@
       <c r="AC15" s="76" t="s">
         <v>488</v>
       </c>
-      <c r="AD15" s="681"/>
-      <c r="AF15" s="673"/>
+      <c r="AD15" s="630"/>
+      <c r="AF15" s="622"/>
       <c r="AG15" s="80"/>
       <c r="AH15" s="242" t="s">
         <v>457</v>
@@ -7885,8 +7888,8 @@
       </c>
       <c r="AK15" s="261"/>
       <c r="AL15" s="261"/>
-      <c r="AM15" s="668"/>
-      <c r="AN15" s="653"/>
+      <c r="AM15" s="646"/>
+      <c r="AN15" s="632"/>
       <c r="AP15" s="76" t="s">
         <v>74</v>
       </c>
@@ -7901,20 +7904,20 @@
       <c r="B16" s="21" t="s">
         <v>413</v>
       </c>
-      <c r="C16" s="587"/>
+      <c r="C16" s="591"/>
       <c r="D16" s="61" t="s">
         <v>502</v>
       </c>
       <c r="E16" s="228">
         <v>1</v>
       </c>
-      <c r="F16" s="658"/>
+      <c r="F16" s="611"/>
       <c r="G16" s="346" t="s">
         <v>497</v>
       </c>
       <c r="I16" s="491"/>
       <c r="J16" s="20"/>
-      <c r="O16" s="692"/>
+      <c r="O16" s="614"/>
       <c r="R16" s="456" t="s">
         <v>185</v>
       </c>
@@ -7925,7 +7928,7 @@
       <c r="X16" s="452" t="s">
         <v>171</v>
       </c>
-      <c r="Y16" s="671"/>
+      <c r="Y16" s="649"/>
       <c r="Z16" s="428">
         <v>1</v>
       </c>
@@ -7946,18 +7949,18 @@
       <c r="AM16" s="449" t="s">
         <v>323</v>
       </c>
-      <c r="AN16" s="653"/>
+      <c r="AN16" s="632"/>
       <c r="AP16" s="76" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="17" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="80"/>
-      <c r="F17" s="658"/>
+      <c r="F17" s="611"/>
       <c r="I17" s="492"/>
       <c r="J17" s="20"/>
       <c r="N17" s="6"/>
-      <c r="O17" s="692"/>
+      <c r="O17" s="614"/>
       <c r="Q17" s="21" t="s">
         <v>541</v>
       </c>
@@ -7977,7 +7980,7 @@
       <c r="X17" s="452" t="s">
         <v>172</v>
       </c>
-      <c r="Y17" s="671"/>
+      <c r="Y17" s="649"/>
       <c r="Z17" s="430"/>
       <c r="AA17" s="312"/>
       <c r="AB17" s="213"/>
@@ -8002,7 +8005,7 @@
       <c r="AK17" s="261"/>
       <c r="AL17" s="80"/>
       <c r="AM17" s="449"/>
-      <c r="AN17" s="653"/>
+      <c r="AN17" s="632"/>
       <c r="AO17" s="208" t="s">
         <v>506</v>
       </c>
@@ -8026,21 +8029,21 @@
       <c r="E18" s="99" t="s">
         <v>44</v>
       </c>
-      <c r="F18" s="658"/>
+      <c r="F18" s="611"/>
       <c r="G18" s="346" t="s">
         <v>538</v>
       </c>
       <c r="I18" s="24"/>
       <c r="J18" s="20"/>
-      <c r="O18" s="692"/>
+      <c r="O18" s="614"/>
       <c r="Q18" s="112"/>
-      <c r="R18" s="686" t="s">
+      <c r="R18" s="606" t="s">
         <v>546</v>
       </c>
       <c r="T18" s="100" t="s">
         <v>44</v>
       </c>
-      <c r="U18" s="631" t="s">
+      <c r="U18" s="654" t="s">
         <v>44</v>
       </c>
       <c r="V18" s="120"/>
@@ -8050,7 +8053,7 @@
       <c r="X18" s="452" t="s">
         <v>173</v>
       </c>
-      <c r="Y18" s="671"/>
+      <c r="Y18" s="649"/>
       <c r="Z18" s="430">
         <v>1</v>
       </c>
@@ -8061,38 +8064,38 @@
       <c r="AC18" s="16"/>
       <c r="AD18" s="16"/>
       <c r="AE18" s="261"/>
-      <c r="AF18" s="667" t="s">
+      <c r="AF18" s="621" t="s">
         <v>484</v>
       </c>
       <c r="AG18" s="261"/>
       <c r="AH18" s="70"/>
       <c r="AI18" s="70"/>
-      <c r="AJ18" s="669" t="s">
+      <c r="AJ18" s="647" t="s">
         <v>321</v>
       </c>
       <c r="AK18" s="261"/>
       <c r="AL18" s="80"/>
       <c r="AM18" s="449"/>
-      <c r="AN18" s="653"/>
+      <c r="AN18" s="632"/>
       <c r="AP18" s="76" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F19" s="658"/>
+      <c r="F19" s="611"/>
       <c r="I19" s="223"/>
-      <c r="O19" s="692"/>
-      <c r="R19" s="687"/>
+      <c r="O19" s="614"/>
+      <c r="R19" s="607"/>
       <c r="S19" s="30" t="s">
         <v>544</v>
       </c>
-      <c r="U19" s="632"/>
+      <c r="U19" s="655"/>
       <c r="V19" s="146"/>
       <c r="W19" s="146"/>
       <c r="X19" s="452" t="s">
         <v>174</v>
       </c>
-      <c r="Y19" s="671"/>
+      <c r="Y19" s="649"/>
       <c r="Z19" s="428">
         <v>1</v>
       </c>
@@ -8101,17 +8104,17 @@
       <c r="AC19" s="16"/>
       <c r="AD19" s="16"/>
       <c r="AE19" s="261"/>
-      <c r="AF19" s="667"/>
+      <c r="AF19" s="621"/>
       <c r="AG19" s="261"/>
       <c r="AH19" s="261"/>
       <c r="AI19" s="70"/>
-      <c r="AJ19" s="669"/>
+      <c r="AJ19" s="647"/>
       <c r="AK19" s="481" t="s">
         <v>255</v>
       </c>
       <c r="AL19" s="80"/>
       <c r="AM19" s="449"/>
-      <c r="AN19" s="653"/>
+      <c r="AN19" s="632"/>
       <c r="AP19" s="76" t="s">
         <v>477</v>
       </c>
@@ -8132,24 +8135,24 @@
       <c r="E20" s="458">
         <v>-1</v>
       </c>
-      <c r="F20" s="658"/>
+      <c r="F20" s="611"/>
       <c r="G20" s="346" t="s">
         <v>500</v>
       </c>
       <c r="I20" s="223"/>
-      <c r="O20" s="692"/>
-      <c r="Q20" s="694" t="s">
+      <c r="O20" s="614"/>
+      <c r="Q20" s="616" t="s">
         <v>48</v>
       </c>
       <c r="T20" s="425" t="s">
         <v>44</v>
       </c>
-      <c r="U20" s="633"/>
+      <c r="U20" s="656"/>
       <c r="W20" s="426"/>
       <c r="X20" s="453" t="s">
         <v>175</v>
       </c>
-      <c r="Y20" s="671"/>
+      <c r="Y20" s="649"/>
       <c r="Z20" s="432">
         <v>1</v>
       </c>
@@ -8174,7 +8177,7 @@
       <c r="AM20" s="397" t="s">
         <v>253</v>
       </c>
-      <c r="AN20" s="653"/>
+      <c r="AN20" s="632"/>
       <c r="AO20" s="347" t="s">
         <v>469</v>
       </c>
@@ -8195,20 +8198,20 @@
       <c r="E21" s="270">
         <v>0</v>
       </c>
-      <c r="F21" s="658"/>
+      <c r="F21" s="611"/>
       <c r="I21" s="223"/>
-      <c r="O21" s="692"/>
-      <c r="Q21" s="695"/>
+      <c r="O21" s="614"/>
+      <c r="Q21" s="617"/>
       <c r="T21" s="443"/>
       <c r="U21" s="14"/>
-      <c r="V21" s="628"/>
+      <c r="V21" s="651"/>
       <c r="W21" s="447" t="s">
         <v>176</v>
       </c>
       <c r="X21" s="450" t="s">
         <v>187</v>
       </c>
-      <c r="Y21" s="671"/>
+      <c r="Y21" s="649"/>
       <c r="Z21" s="466">
         <v>3</v>
       </c>
@@ -8239,15 +8242,15 @@
       <c r="AM21" s="449" t="s">
         <v>555</v>
       </c>
-      <c r="AN21" s="653"/>
+      <c r="AN21" s="632"/>
     </row>
     <row r="22" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F22" s="658"/>
+      <c r="F22" s="611"/>
       <c r="G22" s="346" t="s">
         <v>498</v>
       </c>
       <c r="I22" s="223"/>
-      <c r="O22" s="692"/>
+      <c r="O22" s="614"/>
       <c r="R22" s="455" t="s">
         <v>44</v>
       </c>
@@ -8255,14 +8258,14 @@
         <v>44</v>
       </c>
       <c r="U22" s="15"/>
-      <c r="V22" s="629"/>
+      <c r="V22" s="652"/>
       <c r="W22" s="447" t="s">
         <v>176</v>
       </c>
       <c r="X22" s="450" t="s">
         <v>188</v>
       </c>
-      <c r="Y22" s="671"/>
+      <c r="Y22" s="649"/>
       <c r="Z22" s="436"/>
       <c r="AA22" s="10"/>
       <c r="AB22" s="436"/>
@@ -8273,7 +8276,7 @@
       <c r="AG22" s="6"/>
       <c r="AH22" s="6"/>
       <c r="AI22" s="6"/>
-      <c r="AJ22" s="667" t="s">
+      <c r="AJ22" s="621" t="s">
         <v>481</v>
       </c>
       <c r="AK22" s="261"/>
@@ -8281,7 +8284,7 @@
         <v>487</v>
       </c>
       <c r="AM22" s="305"/>
-      <c r="AN22" s="653"/>
+      <c r="AN22" s="632"/>
     </row>
     <row r="23" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="235" t="s">
@@ -8299,22 +8302,22 @@
       <c r="E23" s="229">
         <v>1</v>
       </c>
-      <c r="F23" s="658"/>
+      <c r="F23" s="611"/>
       <c r="I23" s="223"/>
-      <c r="O23" s="692"/>
-      <c r="Q23" s="694" t="s">
+      <c r="O23" s="614"/>
+      <c r="Q23" s="616" t="s">
         <v>145</v>
       </c>
       <c r="T23" s="17"/>
       <c r="U23" s="441" t="s">
         <v>44</v>
       </c>
-      <c r="V23" s="629"/>
+      <c r="V23" s="652"/>
       <c r="W23" s="148"/>
       <c r="X23" s="450" t="s">
         <v>189</v>
       </c>
-      <c r="Y23" s="671"/>
+      <c r="Y23" s="649"/>
       <c r="Z23" s="17"/>
       <c r="AA23" s="10"/>
       <c r="AB23" s="436"/>
@@ -8325,13 +8328,13 @@
       <c r="AG23" s="6"/>
       <c r="AH23" s="6"/>
       <c r="AI23" s="6"/>
-      <c r="AJ23" s="667"/>
+      <c r="AJ23" s="621"/>
       <c r="AK23" s="261"/>
       <c r="AL23" s="80" t="s">
         <v>516</v>
       </c>
       <c r="AM23" s="305"/>
-      <c r="AN23" s="653"/>
+      <c r="AN23" s="632"/>
     </row>
     <row r="24" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="461" t="s">
@@ -8349,23 +8352,23 @@
       <c r="E24" s="457">
         <v>1</v>
       </c>
-      <c r="F24" s="658"/>
+      <c r="F24" s="611"/>
       <c r="G24" s="61" t="s">
         <v>499</v>
       </c>
       <c r="I24" s="223"/>
-      <c r="O24" s="692"/>
-      <c r="Q24" s="695"/>
+      <c r="O24" s="614"/>
+      <c r="Q24" s="617"/>
       <c r="T24" s="17"/>
       <c r="U24" s="231" t="s">
         <v>44</v>
       </c>
-      <c r="V24" s="629"/>
+      <c r="V24" s="652"/>
       <c r="W24" s="148"/>
       <c r="X24" s="450" t="s">
         <v>186</v>
       </c>
-      <c r="Y24" s="671"/>
+      <c r="Y24" s="649"/>
       <c r="Z24" s="17"/>
       <c r="AA24" s="10"/>
       <c r="AB24" s="436"/>
@@ -8384,12 +8387,12 @@
         <v>472</v>
       </c>
       <c r="AM24" s="305"/>
-      <c r="AN24" s="653"/>
+      <c r="AN24" s="632"/>
     </row>
     <row r="25" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F25" s="658"/>
+      <c r="F25" s="611"/>
       <c r="I25" s="223"/>
-      <c r="O25" s="692"/>
+      <c r="O25" s="614"/>
       <c r="P25" s="208" t="s">
         <v>284</v>
       </c>
@@ -8402,12 +8405,12 @@
       <c r="U25" s="421" t="s">
         <v>44</v>
       </c>
-      <c r="V25" s="630"/>
+      <c r="V25" s="653"/>
       <c r="W25" s="148"/>
       <c r="X25" s="450" t="s">
         <v>190</v>
       </c>
-      <c r="Y25" s="671"/>
+      <c r="Y25" s="649"/>
       <c r="Z25" s="17"/>
       <c r="AA25" s="10"/>
       <c r="AB25" s="436"/>
@@ -8424,7 +8427,7 @@
       <c r="AK25" s="142"/>
       <c r="AL25" s="6"/>
       <c r="AM25" s="305"/>
-      <c r="AN25" s="653"/>
+      <c r="AN25" s="632"/>
     </row>
     <row r="26" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="235" t="s">
@@ -8442,17 +8445,17 @@
       <c r="E26" s="395">
         <v>1</v>
       </c>
-      <c r="F26" s="658"/>
+      <c r="F26" s="611"/>
       <c r="G26" s="346" t="s">
         <v>496</v>
       </c>
       <c r="I26" s="223"/>
-      <c r="O26" s="692"/>
-      <c r="P26" s="655" t="s">
+      <c r="O26" s="614"/>
+      <c r="P26" s="634" t="s">
         <v>536</v>
       </c>
-      <c r="Q26" s="656"/>
-      <c r="R26" s="688" t="s">
+      <c r="Q26" s="635"/>
+      <c r="R26" s="608" t="s">
         <v>545</v>
       </c>
       <c r="T26" s="182"/>
@@ -8464,7 +8467,7 @@
       <c r="X26" s="450" t="s">
         <v>182</v>
       </c>
-      <c r="Y26" s="671"/>
+      <c r="Y26" s="649"/>
       <c r="Z26" s="17"/>
       <c r="AA26" s="10"/>
       <c r="AB26" s="436"/>
@@ -8491,7 +8494,7 @@
       <c r="AM26" s="463" t="s">
         <v>465</v>
       </c>
-      <c r="AN26" s="653"/>
+      <c r="AN26" s="632"/>
     </row>
     <row r="27" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="21" t="s">
@@ -8503,13 +8506,13 @@
       <c r="E27" s="270" t="s">
         <v>44</v>
       </c>
-      <c r="F27" s="690"/>
+      <c r="F27" s="612"/>
       <c r="G27" s="61" t="s">
         <v>554</v>
       </c>
       <c r="I27" s="224"/>
-      <c r="O27" s="693"/>
-      <c r="R27" s="689"/>
+      <c r="O27" s="615"/>
+      <c r="R27" s="609"/>
       <c r="S27" s="442" t="s">
         <v>54</v>
       </c>
@@ -8522,7 +8525,7 @@
       <c r="X27" s="450" t="s">
         <v>540</v>
       </c>
-      <c r="Y27" s="672"/>
+      <c r="Y27" s="650"/>
       <c r="Z27" s="163"/>
       <c r="AA27" s="13"/>
       <c r="AB27" s="437"/>
@@ -8539,32 +8542,26 @@
       <c r="AM27" s="397" t="s">
         <v>325</v>
       </c>
-      <c r="AN27" s="654"/>
+      <c r="AN27" s="633"/>
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="R18:R19"/>
-    <mergeCell ref="R26:R27"/>
-    <mergeCell ref="F2:F27"/>
-    <mergeCell ref="O10:O27"/>
-    <mergeCell ref="Q20:Q21"/>
-    <mergeCell ref="Q23:Q24"/>
-    <mergeCell ref="G14:J14"/>
-    <mergeCell ref="G13:J13"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="AI6:AI10"/>
-    <mergeCell ref="AF12:AF15"/>
-    <mergeCell ref="AG7:AG12"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="S9:S12"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="AD12:AD15"/>
-    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="V21:V25"/>
+    <mergeCell ref="U18:U20"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="G5:L6"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="K7:K9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B4:B5"/>
     <mergeCell ref="AN1:AN27"/>
     <mergeCell ref="P26:Q26"/>
     <mergeCell ref="Q2:Q3"/>
@@ -8581,22 +8578,28 @@
     <mergeCell ref="AD3:AD4"/>
     <mergeCell ref="S2:S3"/>
     <mergeCell ref="R2:R3"/>
-    <mergeCell ref="V21:V25"/>
-    <mergeCell ref="U18:U20"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="G5:L6"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="K7:K9"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="AI6:AI10"/>
+    <mergeCell ref="AF12:AF15"/>
+    <mergeCell ref="AG7:AG12"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="S9:S12"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="AD12:AD15"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="R18:R19"/>
+    <mergeCell ref="R26:R27"/>
+    <mergeCell ref="F2:F27"/>
+    <mergeCell ref="O10:O27"/>
+    <mergeCell ref="Q20:Q21"/>
+    <mergeCell ref="Q23:Q24"/>
+    <mergeCell ref="G14:J14"/>
+    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="H12:K12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8630,15 +8633,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="590" t="s">
+      <c r="B1" s="594" t="s">
         <v>316</v>
       </c>
-      <c r="C1" s="696"/>
+      <c r="C1" s="618"/>
       <c r="D1" s="208"/>
-      <c r="J1" s="590" t="s">
+      <c r="J1" s="594" t="s">
         <v>70</v>
       </c>
-      <c r="K1" s="696"/>
+      <c r="K1" s="618"/>
       <c r="L1" s="199" t="s">
         <v>336</v>
       </c>
@@ -8676,13 +8679,13 @@
         <v>34</v>
       </c>
       <c r="L2" s="200"/>
-      <c r="M2" s="723"/>
+      <c r="M2" s="675"/>
       <c r="N2" s="154">
         <v>2</v>
       </c>
       <c r="O2" s="155"/>
       <c r="P2" s="5"/>
-      <c r="Q2" s="726" t="s">
+      <c r="Q2" s="678" t="s">
         <v>44</v>
       </c>
       <c r="R2" s="19">
@@ -8705,13 +8708,13 @@
       <c r="K3" s="6" t="s">
         <v>333</v>
       </c>
-      <c r="M3" s="724"/>
+      <c r="M3" s="676"/>
       <c r="N3" s="17">
         <v>1</v>
       </c>
       <c r="O3" s="15"/>
       <c r="P3" s="10"/>
-      <c r="Q3" s="727"/>
+      <c r="Q3" s="679"/>
       <c r="R3" s="223"/>
     </row>
     <row r="4" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8730,13 +8733,13 @@
       <c r="K4" s="6" t="s">
         <v>334</v>
       </c>
-      <c r="M4" s="724"/>
+      <c r="M4" s="676"/>
       <c r="N4" s="17"/>
       <c r="O4" s="15">
         <v>1</v>
       </c>
       <c r="P4" s="10"/>
-      <c r="Q4" s="727"/>
+      <c r="Q4" s="679"/>
       <c r="R4" s="223"/>
     </row>
     <row r="5" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8756,13 +8759,13 @@
         <v>13</v>
       </c>
       <c r="L5" s="200"/>
-      <c r="M5" s="724"/>
+      <c r="M5" s="676"/>
       <c r="N5" s="17">
         <v>1</v>
       </c>
       <c r="O5" s="15"/>
       <c r="P5" s="10"/>
-      <c r="Q5" s="727"/>
+      <c r="Q5" s="679"/>
       <c r="R5" s="19">
         <v>-1</v>
       </c>
@@ -8783,13 +8786,13 @@
       <c r="K6" s="6" t="s">
         <v>332</v>
       </c>
-      <c r="M6" s="724"/>
+      <c r="M6" s="676"/>
       <c r="N6" s="17">
         <v>1</v>
       </c>
       <c r="O6" s="15"/>
       <c r="P6" s="10"/>
-      <c r="Q6" s="727"/>
+      <c r="Q6" s="679"/>
       <c r="R6" s="223"/>
     </row>
     <row r="7" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8809,13 +8812,13 @@
         <v>333</v>
       </c>
       <c r="L7" s="202"/>
-      <c r="M7" s="724"/>
+      <c r="M7" s="676"/>
       <c r="N7" s="17">
         <v>1</v>
       </c>
       <c r="O7" s="15"/>
       <c r="P7" s="10"/>
-      <c r="Q7" s="727"/>
+      <c r="Q7" s="679"/>
       <c r="R7" s="19">
         <v>-1</v>
       </c>
@@ -8836,13 +8839,13 @@
       <c r="K8" s="6" t="s">
         <v>331</v>
       </c>
-      <c r="M8" s="724"/>
+      <c r="M8" s="676"/>
       <c r="N8" s="17">
         <v>1</v>
       </c>
       <c r="O8" s="15"/>
       <c r="P8" s="10"/>
-      <c r="Q8" s="727"/>
+      <c r="Q8" s="679"/>
       <c r="R8" s="223"/>
     </row>
     <row r="9" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8862,13 +8865,13 @@
         <v>335</v>
       </c>
       <c r="L9" s="185"/>
-      <c r="M9" s="725"/>
+      <c r="M9" s="677"/>
       <c r="N9" s="163"/>
       <c r="O9" s="18"/>
       <c r="P9" s="13">
         <v>1</v>
       </c>
-      <c r="Q9" s="728"/>
+      <c r="Q9" s="680"/>
       <c r="R9" s="224"/>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.25">
@@ -8973,7 +8976,7 @@
   <dimension ref="A1:AK31"/>
   <sheetViews>
     <sheetView topLeftCell="N12" workbookViewId="0">
-      <selection activeCell="AA26" sqref="AA26"/>
+      <selection activeCell="X28" sqref="X28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9040,7 +9043,7 @@
       <c r="P1" s="419" t="s">
         <v>404</v>
       </c>
-      <c r="Q1" s="618" t="s">
+      <c r="Q1" s="684" t="s">
         <v>181</v>
       </c>
       <c r="R1" s="100" t="s">
@@ -9064,7 +9067,7 @@
       <c r="AA1" s="546" t="s">
         <v>446</v>
       </c>
-      <c r="AB1" s="625" t="s">
+      <c r="AB1" s="691" t="s">
         <v>608</v>
       </c>
       <c r="AC1" s="99" t="s">
@@ -9085,32 +9088,32 @@
       </c>
     </row>
     <row r="2" spans="1:37" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="599">
+      <c r="A2" s="697">
         <f ca="1">TODAY()</f>
         <v>45282</v>
       </c>
-      <c r="B2" s="601" t="s">
+      <c r="B2" s="699" t="s">
         <v>386</v>
       </c>
-      <c r="C2" s="613" t="s">
+      <c r="C2" s="636" t="s">
         <v>363</v>
       </c>
-      <c r="D2" s="603" t="s">
+      <c r="D2" s="701" t="s">
         <v>103</v>
       </c>
-      <c r="E2" s="605" t="s">
+      <c r="E2" s="703" t="s">
         <v>65</v>
       </c>
       <c r="F2" s="195" t="s">
         <v>220</v>
       </c>
-      <c r="G2" s="611" t="s">
+      <c r="G2" s="604" t="s">
         <v>378</v>
       </c>
       <c r="H2" s="210" t="s">
         <v>220</v>
       </c>
-      <c r="I2" s="622" t="s">
+      <c r="I2" s="688" t="s">
         <v>103</v>
       </c>
       <c r="J2" s="417" t="s">
@@ -9134,7 +9137,7 @@
       <c r="P2" s="420">
         <v>40</v>
       </c>
-      <c r="Q2" s="619"/>
+      <c r="Q2" s="685"/>
       <c r="R2" s="21">
         <f>R7+R20</f>
         <v>1</v>
@@ -9159,7 +9162,7 @@
         <f>IF((Z2+T2)&gt;0,0,-1)</f>
         <v>0</v>
       </c>
-      <c r="AB2" s="626"/>
+      <c r="AB2" s="692"/>
       <c r="AC2" s="35"/>
       <c r="AH2" s="6" t="s">
         <v>617</v>
@@ -9175,14 +9178,14 @@
       </c>
     </row>
     <row r="3" spans="1:37" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="600"/>
-      <c r="B3" s="602"/>
-      <c r="C3" s="614"/>
-      <c r="D3" s="604"/>
-      <c r="E3" s="606"/>
-      <c r="G3" s="612"/>
+      <c r="A3" s="698"/>
+      <c r="B3" s="700"/>
+      <c r="C3" s="637"/>
+      <c r="D3" s="702"/>
+      <c r="E3" s="704"/>
+      <c r="G3" s="605"/>
       <c r="H3" s="6"/>
-      <c r="I3" s="623"/>
+      <c r="I3" s="689"/>
       <c r="K3" s="24">
         <v>2</v>
       </c>
@@ -9197,7 +9200,7 @@
       <c r="V3" s="492"/>
       <c r="W3" s="6"/>
       <c r="X3" s="492"/>
-      <c r="AB3" s="626"/>
+      <c r="AB3" s="692"/>
       <c r="AC3" s="35"/>
       <c r="AE3" s="100" t="s">
         <v>603</v>
@@ -9225,10 +9228,10 @@
         <v>387</v>
       </c>
       <c r="B4" s="247"/>
-      <c r="C4" s="607" t="s">
+      <c r="C4" s="705" t="s">
         <v>178</v>
       </c>
-      <c r="I4" s="623"/>
+      <c r="I4" s="689"/>
       <c r="R4" s="493" t="s">
         <v>603</v>
       </c>
@@ -9240,7 +9243,7 @@
       <c r="V4" s="492"/>
       <c r="W4" s="6"/>
       <c r="X4" s="492"/>
-      <c r="AB4" s="626"/>
+      <c r="AB4" s="692"/>
       <c r="AC4" s="35"/>
       <c r="AE4" s="20"/>
       <c r="AF4" s="100" t="s">
@@ -9270,7 +9273,7 @@
       <c r="B5" s="100" t="s">
         <v>363</v>
       </c>
-      <c r="C5" s="608"/>
+      <c r="C5" s="706"/>
       <c r="D5" s="226" t="s">
         <v>103</v>
       </c>
@@ -9280,13 +9283,13 @@
       <c r="F5" s="210" t="s">
         <v>220</v>
       </c>
-      <c r="G5" s="585" t="s">
+      <c r="G5" s="589" t="s">
         <v>275</v>
       </c>
       <c r="H5" s="210" t="s">
         <v>220</v>
       </c>
-      <c r="I5" s="623"/>
+      <c r="I5" s="689"/>
       <c r="J5" s="418" t="s">
         <v>272</v>
       </c>
@@ -9313,7 +9316,7 @@
       <c r="V5" s="490"/>
       <c r="W5" s="6"/>
       <c r="X5" s="490"/>
-      <c r="AB5" s="626"/>
+      <c r="AB5" s="692"/>
       <c r="AC5" s="2" t="s">
         <v>606</v>
       </c>
@@ -9326,19 +9329,19 @@
       <c r="AK5" s="490"/>
     </row>
     <row r="6" spans="1:37" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="596" t="s">
+      <c r="A6" s="694" t="s">
         <v>289</v>
       </c>
       <c r="B6" s="105" t="s">
         <v>199</v>
       </c>
-      <c r="C6" s="609"/>
-      <c r="D6" s="610"/>
+      <c r="C6" s="619"/>
+      <c r="D6" s="620"/>
       <c r="E6" s="96">
         <v>1</v>
       </c>
-      <c r="G6" s="586"/>
-      <c r="I6" s="623"/>
+      <c r="G6" s="590"/>
+      <c r="I6" s="689"/>
       <c r="P6" s="61" t="s">
         <v>606</v>
       </c>
@@ -9350,7 +9353,7 @@
         <f>S7-S12-SUM(V2:V10)</f>
         <v>0</v>
       </c>
-      <c r="AB6" s="626"/>
+      <c r="AB6" s="692"/>
       <c r="AC6" s="35"/>
       <c r="AE6" s="64">
         <f>AE7-SUM(AI1:AI10)+AE11</f>
@@ -9365,7 +9368,7 @@
       <c r="AK6" s="554"/>
     </row>
     <row r="7" spans="1:37" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="597"/>
+      <c r="A7" s="695"/>
       <c r="B7" s="100" t="s">
         <v>155</v>
       </c>
@@ -9375,8 +9378,8 @@
       <c r="D7" s="30" t="s">
         <v>136</v>
       </c>
-      <c r="G7" s="586"/>
-      <c r="I7" s="623"/>
+      <c r="G7" s="590"/>
+      <c r="I7" s="689"/>
       <c r="M7" s="16" t="s">
         <v>353</v>
       </c>
@@ -9408,7 +9411,7 @@
       <c r="X7" s="491">
         <v>1</v>
       </c>
-      <c r="AB7" s="626"/>
+      <c r="AB7" s="692"/>
       <c r="AC7" s="99" t="s">
         <v>607</v>
       </c>
@@ -9433,7 +9436,7 @@
       <c r="AK7" s="491"/>
     </row>
     <row r="8" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="598"/>
+      <c r="A8" s="696"/>
       <c r="B8" s="216" t="s">
         <v>28</v>
       </c>
@@ -9441,14 +9444,14 @@
       <c r="E8" s="30">
         <v>3</v>
       </c>
-      <c r="G8" s="586"/>
-      <c r="I8" s="623"/>
+      <c r="G8" s="590"/>
+      <c r="I8" s="689"/>
       <c r="N8" s="80"/>
       <c r="U8" s="6"/>
       <c r="V8" s="24"/>
       <c r="W8" s="6"/>
       <c r="X8" s="489"/>
-      <c r="AB8" s="626"/>
+      <c r="AB8" s="692"/>
       <c r="AC8" s="544"/>
       <c r="AH8" s="6"/>
       <c r="AI8" s="578"/>
@@ -9472,9 +9475,9 @@
       <c r="D9" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="G9" s="586"/>
+      <c r="G9" s="590"/>
       <c r="H9" s="6"/>
-      <c r="I9" s="623"/>
+      <c r="I9" s="689"/>
       <c r="M9" s="19" t="s">
         <v>535</v>
       </c>
@@ -9482,7 +9485,7 @@
       <c r="U9" s="6"/>
       <c r="V9" s="24"/>
       <c r="X9" s="489"/>
-      <c r="AB9" s="626"/>
+      <c r="AB9" s="692"/>
       <c r="AC9" s="544"/>
       <c r="AE9" s="20"/>
       <c r="AF9" s="20"/>
@@ -9512,8 +9515,8 @@
         <f>Boat!W8</f>
         <v>37</v>
       </c>
-      <c r="G10" s="586"/>
-      <c r="I10" s="623"/>
+      <c r="G10" s="590"/>
+      <c r="I10" s="689"/>
       <c r="J10" s="24" t="s">
         <v>378</v>
       </c>
@@ -9528,7 +9531,7 @@
       <c r="V10" s="492"/>
       <c r="W10" s="6"/>
       <c r="X10" s="489"/>
-      <c r="AB10" s="626"/>
+      <c r="AB10" s="692"/>
       <c r="AC10" s="544"/>
       <c r="AE10" s="20"/>
       <c r="AF10" s="20"/>
@@ -9549,7 +9552,7 @@
       <c r="A11" s="99" t="s">
         <v>184</v>
       </c>
-      <c r="B11" s="585" t="s">
+      <c r="B11" s="589" t="s">
         <v>389</v>
       </c>
       <c r="C11" s="175" t="s">
@@ -9558,8 +9561,8 @@
       <c r="D11" s="221" t="s">
         <v>269</v>
       </c>
-      <c r="G11" s="586"/>
-      <c r="I11" s="623"/>
+      <c r="G11" s="590"/>
+      <c r="I11" s="689"/>
       <c r="J11" s="24" t="s">
         <v>195</v>
       </c>
@@ -9585,13 +9588,13 @@
       <c r="S11" s="24">
         <v>3</v>
       </c>
-      <c r="U11" s="615" t="s">
+      <c r="U11" s="681" t="s">
         <v>569</v>
       </c>
-      <c r="V11" s="616"/>
-      <c r="W11" s="616"/>
-      <c r="X11" s="617"/>
-      <c r="AB11" s="627"/>
+      <c r="V11" s="682"/>
+      <c r="W11" s="682"/>
+      <c r="X11" s="683"/>
+      <c r="AB11" s="693"/>
       <c r="AC11" s="99" t="s">
         <v>609</v>
       </c>
@@ -9605,23 +9608,23 @@
         <v>2</v>
       </c>
       <c r="AG11" s="435"/>
-      <c r="AH11" s="615" t="s">
+      <c r="AH11" s="681" t="s">
         <v>628</v>
       </c>
-      <c r="AI11" s="616"/>
-      <c r="AJ11" s="616"/>
-      <c r="AK11" s="617"/>
+      <c r="AI11" s="682"/>
+      <c r="AJ11" s="682"/>
+      <c r="AK11" s="683"/>
     </row>
     <row r="12" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="231" t="s">
         <v>390</v>
       </c>
-      <c r="B12" s="587"/>
+      <c r="B12" s="591"/>
       <c r="E12" s="233">
         <v>3</v>
       </c>
-      <c r="G12" s="586"/>
-      <c r="I12" s="623"/>
+      <c r="G12" s="590"/>
+      <c r="I12" s="689"/>
       <c r="J12" s="24" t="s">
         <v>526</v>
       </c>
@@ -9649,12 +9652,12 @@
       <c r="B13" s="220" t="s">
         <v>329</v>
       </c>
-      <c r="C13" s="585" t="s">
+      <c r="C13" s="589" t="s">
         <v>195</v>
       </c>
       <c r="D13" s="20"/>
-      <c r="G13" s="586"/>
-      <c r="I13" s="623"/>
+      <c r="G13" s="590"/>
+      <c r="I13" s="689"/>
       <c r="J13" s="108" t="s">
         <v>559</v>
       </c>
@@ -9684,7 +9687,7 @@
       <c r="B14" s="177" t="s">
         <v>150</v>
       </c>
-      <c r="C14" s="587"/>
+      <c r="C14" s="591"/>
       <c r="D14" s="208" t="s">
         <v>154</v>
       </c>
@@ -9694,11 +9697,11 @@
       <c r="F14" s="210" t="s">
         <v>220</v>
       </c>
-      <c r="G14" s="587"/>
+      <c r="G14" s="591"/>
       <c r="H14" s="210" t="s">
         <v>220</v>
       </c>
-      <c r="I14" s="623"/>
+      <c r="I14" s="689"/>
       <c r="U14" s="67" t="s">
         <v>81</v>
       </c>
@@ -9725,7 +9728,7 @@
       <c r="H15" s="276">
         <v>0</v>
       </c>
-      <c r="I15" s="623"/>
+      <c r="I15" s="689"/>
       <c r="J15" s="108" t="s">
         <v>154</v>
       </c>
@@ -9756,7 +9759,7 @@
       <c r="D16" s="2" t="s">
         <v>501</v>
       </c>
-      <c r="I16" s="623"/>
+      <c r="I16" s="689"/>
       <c r="K16" s="100" t="s">
         <v>44</v>
       </c>
@@ -9800,7 +9803,7 @@
       <c r="G17" s="2" t="s">
         <v>432</v>
       </c>
-      <c r="I17" s="623"/>
+      <c r="I17" s="689"/>
       <c r="L17" s="2" t="s">
         <v>435</v>
       </c>
@@ -9818,13 +9821,13 @@
     </row>
     <row r="18" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G18" s="16"/>
-      <c r="I18" s="623"/>
+      <c r="I18" s="689"/>
       <c r="L18" s="16"/>
       <c r="M18" s="21"/>
-      <c r="O18" s="620" t="s">
+      <c r="O18" s="686" t="s">
         <v>527</v>
       </c>
-      <c r="P18" s="621"/>
+      <c r="P18" s="687"/>
       <c r="Q18" s="127" t="s">
         <v>44</v>
       </c>
@@ -9850,7 +9853,7 @@
       </c>
     </row>
     <row r="19" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I19" s="623"/>
+      <c r="I19" s="689"/>
       <c r="M19" s="21" t="s">
         <v>434</v>
       </c>
@@ -9886,7 +9889,7 @@
       <c r="G20" s="2" t="s">
         <v>432</v>
       </c>
-      <c r="I20" s="623"/>
+      <c r="I20" s="689"/>
       <c r="K20" s="19" t="s">
         <v>431</v>
       </c>
@@ -9921,7 +9924,7 @@
       </c>
     </row>
     <row r="21" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I21" s="623"/>
+      <c r="I21" s="689"/>
       <c r="M21" s="220" t="s">
         <v>418</v>
       </c>
@@ -9955,7 +9958,7 @@
       <c r="G22" s="2" t="s">
         <v>432</v>
       </c>
-      <c r="I22" s="623"/>
+      <c r="I22" s="689"/>
       <c r="P22" s="99" t="s">
         <v>605</v>
       </c>
@@ -9970,7 +9973,7 @@
       <c r="E23" s="288" t="s">
         <v>44</v>
       </c>
-      <c r="I23" s="623"/>
+      <c r="I23" s="689"/>
       <c r="Q23" s="24">
         <f>SUM(V23:V31)</f>
         <v>5</v>
@@ -9987,7 +9990,7 @@
       </c>
     </row>
     <row r="24" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I24" s="623"/>
+      <c r="I24" s="689"/>
       <c r="U24" s="35"/>
       <c r="V24" s="533">
         <v>0</v>
@@ -10015,7 +10018,7 @@
       <c r="H25" s="195" t="s">
         <v>270</v>
       </c>
-      <c r="I25" s="623"/>
+      <c r="I25" s="689"/>
       <c r="J25" s="418" t="s">
         <v>273</v>
       </c>
@@ -10060,7 +10063,7 @@
       <c r="H26" s="19" t="s">
         <v>220</v>
       </c>
-      <c r="I26" s="623"/>
+      <c r="I26" s="689"/>
       <c r="K26" s="24">
         <v>15</v>
       </c>
@@ -10095,7 +10098,7 @@
       </c>
     </row>
     <row r="27" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I27" s="623"/>
+      <c r="I27" s="689"/>
       <c r="O27" s="2" t="s">
         <v>99</v>
       </c>
@@ -10122,7 +10125,7 @@
       <c r="E28" s="219">
         <v>2</v>
       </c>
-      <c r="I28" s="623"/>
+      <c r="I28" s="689"/>
       <c r="Q28" s="6"/>
       <c r="R28" s="112"/>
       <c r="T28" s="142"/>
@@ -10144,7 +10147,7 @@
       <c r="H29" s="195" t="s">
         <v>271</v>
       </c>
-      <c r="I29" s="624"/>
+      <c r="I29" s="690"/>
       <c r="J29" s="330"/>
       <c r="L29" s="96" t="s">
         <v>277</v>
@@ -10202,12 +10205,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="AH11:AK11"/>
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="U11:X11"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="I2:I29"/>
-    <mergeCell ref="AB1:AB11"/>
     <mergeCell ref="C13:C14"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="G5:G14"/>
@@ -10220,6 +10217,12 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="C2:C3"/>
+    <mergeCell ref="AH11:AK11"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="U11:X11"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="I2:I29"/>
+    <mergeCell ref="AB1:AB11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10229,8 +10232,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2029A93E-B53C-4201-9F17-439C144F3CF1}">
   <dimension ref="A1:AP37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="X13" sqref="X13"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="AP11" sqref="AP11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10326,14 +10329,14 @@
         <f ca="1">TODAY()</f>
         <v>45282</v>
       </c>
-      <c r="T1" s="720"/>
+      <c r="T1" s="726"/>
       <c r="U1" s="142"/>
       <c r="V1" s="142"/>
       <c r="W1" s="6"/>
-      <c r="X1" s="704" t="s">
+      <c r="X1" s="710" t="s">
         <v>450</v>
       </c>
-      <c r="Y1" s="705"/>
+      <c r="Y1" s="711"/>
       <c r="Z1" s="311">
         <f>68-(W8+Y3+X3+U3)</f>
         <v>0</v>
@@ -10349,21 +10352,21 @@
       <c r="AD1" s="307" t="s">
         <v>44</v>
       </c>
-      <c r="AE1" s="706" t="s">
+      <c r="AE1" s="712" t="s">
         <v>191</v>
       </c>
-      <c r="AF1" s="707"/>
-      <c r="AG1" s="708"/>
-      <c r="AH1" s="709" t="s">
+      <c r="AF1" s="713"/>
+      <c r="AG1" s="714"/>
+      <c r="AH1" s="715" t="s">
         <v>297</v>
       </c>
-      <c r="AI1" s="710"/>
-      <c r="AJ1" s="711"/>
-      <c r="AK1" s="701" t="s">
+      <c r="AI1" s="716"/>
+      <c r="AJ1" s="717"/>
+      <c r="AK1" s="707" t="s">
         <v>453</v>
       </c>
-      <c r="AL1" s="702"/>
-      <c r="AM1" s="703"/>
+      <c r="AL1" s="708"/>
+      <c r="AM1" s="709"/>
       <c r="AP1" s="142"/>
     </row>
     <row r="2" spans="1:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10384,19 +10387,19 @@
       <c r="L2" s="324">
         <v>-3</v>
       </c>
-      <c r="M2" s="712">
+      <c r="M2" s="718">
         <f>SUM(M5:M30)</f>
         <v>1</v>
       </c>
-      <c r="N2" s="714">
+      <c r="N2" s="720">
         <f>SUM(N4:N29)</f>
         <v>10</v>
       </c>
-      <c r="O2" s="716">
+      <c r="O2" s="722">
         <f>SUM(O4:O29)</f>
-        <v>8</v>
-      </c>
-      <c r="P2" s="679">
+        <v>9</v>
+      </c>
+      <c r="P2" s="628">
         <f>SUM(N30:N37)* (-1)</f>
         <v>-3</v>
       </c>
@@ -10409,14 +10412,14 @@
       <c r="S2" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="T2" s="721"/>
+      <c r="T2" s="727"/>
       <c r="U2" s="566" t="s">
         <v>266</v>
       </c>
       <c r="V2" s="505" t="s">
         <v>221</v>
       </c>
-      <c r="W2" s="718" t="s">
+      <c r="W2" s="724" t="s">
         <v>238</v>
       </c>
       <c r="X2" s="506" t="s">
@@ -10485,10 +10488,10 @@
         <f>V3+X3+Y3+U3</f>
         <v>68</v>
       </c>
-      <c r="M3" s="713"/>
-      <c r="N3" s="715"/>
-      <c r="O3" s="717"/>
-      <c r="P3" s="680"/>
+      <c r="M3" s="719"/>
+      <c r="N3" s="721"/>
+      <c r="O3" s="723"/>
+      <c r="P3" s="629"/>
       <c r="Q3" s="176">
         <f>(M2+N2)-Y3</f>
         <v>0</v>
@@ -10496,7 +10499,7 @@
       <c r="S3" s="161" t="s">
         <v>248</v>
       </c>
-      <c r="T3" s="722"/>
+      <c r="T3" s="728"/>
       <c r="U3" s="567">
         <f>SUM(U4:U29)</f>
         <v>12</v>
@@ -10505,7 +10508,7 @@
         <f>SUM(V4:V29)</f>
         <v>37</v>
       </c>
-      <c r="W3" s="719"/>
+      <c r="W3" s="725"/>
       <c r="X3" s="508">
         <f t="shared" ref="X3:AC3" si="0">SUM(X4:X29)</f>
         <v>8</v>
@@ -10520,15 +10523,15 @@
       </c>
       <c r="AA3" s="66">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="AB3" s="66">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="AC3" s="66">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="AD3" s="66">
         <f t="shared" ref="AD3:AM3" si="1">SUM(AD4:AD29)</f>
@@ -10536,7 +10539,7 @@
       </c>
       <c r="AE3" s="66">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="AF3" s="66">
         <f t="shared" si="1"/>
@@ -10548,7 +10551,7 @@
       </c>
       <c r="AH3" s="66">
         <f>SUM(AH4:AH29)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="AI3" s="383">
         <f t="shared" si="1"/>
@@ -10560,15 +10563,15 @@
       </c>
       <c r="AK3" s="100">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="AL3" s="316">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="AM3" s="317">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="AP3" s="142"/>
     </row>
@@ -10605,7 +10608,7 @@
         <f>AC4</f>
         <v>0</v>
       </c>
-      <c r="P4" s="698" t="s">
+      <c r="P4" s="730" t="s">
         <v>200</v>
       </c>
       <c r="Q4" s="20"/>
@@ -10687,7 +10690,7 @@
         <f>AC5</f>
         <v>0</v>
       </c>
-      <c r="P5" s="699"/>
+      <c r="P5" s="731"/>
       <c r="Q5" s="20"/>
       <c r="R5" s="2" t="s">
         <v>346</v>
@@ -10777,7 +10780,7 @@
         <f>AC6</f>
         <v>0</v>
       </c>
-      <c r="P6" s="699"/>
+      <c r="P6" s="731"/>
       <c r="Q6" s="19" t="s">
         <v>341</v>
       </c>
@@ -10857,7 +10860,7 @@
         <v>0</v>
       </c>
       <c r="H7" s="273"/>
-      <c r="I7" s="776"/>
+      <c r="I7" s="581"/>
       <c r="J7" s="117"/>
       <c r="K7" s="111" t="s">
         <v>425</v>
@@ -10875,7 +10878,7 @@
         <f t="shared" ref="O7:O37" si="10">AC7</f>
         <v>0</v>
       </c>
-      <c r="P7" s="699"/>
+      <c r="P7" s="731"/>
       <c r="Q7" s="20"/>
       <c r="R7" s="2" t="s">
         <v>341</v>
@@ -10987,7 +10990,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P8" s="699"/>
+      <c r="P8" s="731"/>
       <c r="Q8" s="21" t="s">
         <v>237</v>
       </c>
@@ -11074,7 +11077,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P9" s="699"/>
+      <c r="P9" s="731"/>
       <c r="Q9" s="21" t="s">
         <v>341</v>
       </c>
@@ -11176,7 +11179,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P10" s="699"/>
+      <c r="P10" s="731"/>
       <c r="Q10" s="20"/>
       <c r="R10" s="2" t="s">
         <v>346</v>
@@ -11262,7 +11265,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P11" s="699"/>
+      <c r="P11" s="731"/>
       <c r="Q11" s="21" t="s">
         <v>341</v>
       </c>
@@ -11325,7 +11328,7 @@
       <c r="AP11" s="142"/>
     </row>
     <row r="12" spans="1:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="643" t="s">
+      <c r="A12" s="666" t="s">
         <v>55</v>
       </c>
       <c r="B12" s="30">
@@ -11334,7 +11337,7 @@
       <c r="C12" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E12" s="694" t="s">
+      <c r="E12" s="616" t="s">
         <v>57</v>
       </c>
       <c r="G12" s="266"/>
@@ -11356,7 +11359,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P12" s="699"/>
+      <c r="P12" s="731"/>
       <c r="Q12" s="21" t="s">
         <v>341</v>
       </c>
@@ -11431,14 +11434,14 @@
       </c>
     </row>
     <row r="13" spans="1:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="645"/>
+      <c r="A13" s="668"/>
       <c r="B13" s="153">
         <v>12</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E13" s="695"/>
+      <c r="E13" s="617"/>
       <c r="F13" s="176">
         <v>0</v>
       </c>
@@ -11462,7 +11465,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P13" s="699"/>
+      <c r="P13" s="731"/>
       <c r="Q13" s="21" t="s">
         <v>341</v>
       </c>
@@ -11531,7 +11534,7 @@
       <c r="H14" s="42">
         <v>-1</v>
       </c>
-      <c r="I14" s="777"/>
+      <c r="I14" s="582"/>
       <c r="K14" s="267"/>
       <c r="L14" s="400"/>
       <c r="M14" s="335"/>
@@ -11540,9 +11543,9 @@
       </c>
       <c r="O14" s="298">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="P14" s="699"/>
+        <v>1</v>
+      </c>
+      <c r="P14" s="731"/>
       <c r="Q14" s="20"/>
       <c r="R14" s="204" t="s">
         <v>345</v>
@@ -11562,47 +11565,47 @@
       </c>
       <c r="X14" s="519"/>
       <c r="Y14" s="513">
-        <f t="shared" si="2"/>
+        <f>SUM(M14:N14)</f>
         <v>0</v>
       </c>
       <c r="Z14" s="301"/>
       <c r="AA14" s="117">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB14" s="295">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC14" s="295">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD14" s="295">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AE14" s="299">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF14" s="305"/>
       <c r="AG14" s="301"/>
       <c r="AH14" s="301">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI14" s="345"/>
       <c r="AJ14" s="158"/>
       <c r="AK14" s="313">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL14" s="314">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM14" s="315">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN14" s="6" t="s">
         <v>570</v>
@@ -11611,7 +11614,7 @@
         <v>573</v>
       </c>
       <c r="AP14" s="142" t="s">
-        <v>479</v>
+        <v>633</v>
       </c>
     </row>
     <row r="15" spans="1:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11641,7 +11644,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P15" s="699"/>
+      <c r="P15" s="731"/>
       <c r="Q15" s="20"/>
       <c r="R15" s="204" t="s">
         <v>345</v>
@@ -11731,7 +11734,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P16" s="699"/>
+      <c r="P16" s="731"/>
       <c r="Q16" s="21" t="s">
         <v>341</v>
       </c>
@@ -11820,7 +11823,7 @@
       <c r="H17" s="273">
         <v>-1</v>
       </c>
-      <c r="I17" s="778"/>
+      <c r="I17" s="583"/>
       <c r="J17" s="6"/>
       <c r="L17" s="402" t="s">
         <v>315</v>
@@ -11833,7 +11836,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P17" s="699"/>
+      <c r="P17" s="731"/>
       <c r="Q17" s="20"/>
       <c r="R17" s="2" t="s">
         <v>347</v>
@@ -11932,7 +11935,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P18" s="699"/>
+      <c r="P18" s="731"/>
       <c r="Q18" s="21" t="s">
         <v>341</v>
       </c>
@@ -12005,7 +12008,7 @@
       <c r="H19" s="273">
         <v>-2</v>
       </c>
-      <c r="I19" s="778"/>
+      <c r="I19" s="583"/>
       <c r="L19" s="402" t="s">
         <v>308</v>
       </c>
@@ -12019,7 +12022,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P19" s="699"/>
+      <c r="P19" s="731"/>
       <c r="Q19" s="20"/>
       <c r="R19" s="2" t="s">
         <v>340</v>
@@ -12107,7 +12110,7 @@
       <c r="H20" s="42">
         <v>-2</v>
       </c>
-      <c r="I20" s="777"/>
+      <c r="I20" s="582"/>
       <c r="J20" s="80"/>
       <c r="K20" s="112" t="s">
         <v>354</v>
@@ -12123,11 +12126,11 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P20" s="700"/>
-      <c r="Q20" s="590" t="s">
+      <c r="P20" s="732"/>
+      <c r="Q20" s="594" t="s">
         <v>341</v>
       </c>
-      <c r="R20" s="696"/>
+      <c r="R20" s="618"/>
       <c r="S20" s="563" t="s">
         <v>86</v>
       </c>
@@ -12373,7 +12376,7 @@
     </row>
     <row r="23" spans="1:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="24"/>
-      <c r="E23" s="650" t="s">
+      <c r="E23" s="673" t="s">
         <v>293</v>
       </c>
       <c r="F23" s="184"/>
@@ -12475,12 +12478,12 @@
       <c r="C24" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="E24" s="651"/>
+      <c r="E24" s="674"/>
       <c r="F24" s="176"/>
       <c r="H24" s="42">
         <v>-1</v>
       </c>
-      <c r="I24" s="777"/>
+      <c r="I24" s="582"/>
       <c r="L24" s="400" t="s">
         <v>300</v>
       </c>
@@ -12494,10 +12497,10 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="Q24" s="590" t="s">
+      <c r="Q24" s="594" t="s">
         <v>341</v>
       </c>
-      <c r="R24" s="696"/>
+      <c r="R24" s="618"/>
       <c r="S24" s="563" t="s">
         <v>253</v>
       </c>
@@ -12607,7 +12610,7 @@
       <c r="W25" s="555">
         <v>-2</v>
       </c>
-      <c r="X25" s="775">
+      <c r="X25" s="580">
         <v>1</v>
       </c>
       <c r="Y25" s="557">
@@ -13124,10 +13127,10 @@
         <v>-1</v>
       </c>
       <c r="I32"/>
-      <c r="J32" s="646" t="s">
+      <c r="J32" s="669" t="s">
         <v>599</v>
       </c>
-      <c r="K32" s="697"/>
+      <c r="K32" s="729"/>
       <c r="L32" s="403"/>
       <c r="M32" s="537">
         <v>0</v>
@@ -13291,7 +13294,7 @@
       <c r="H34" s="42">
         <v>-2</v>
       </c>
-      <c r="I34" s="777"/>
+      <c r="I34" s="582"/>
       <c r="L34" s="400" t="s">
         <v>304</v>
       </c>
@@ -13638,6 +13641,13 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="J32:K32"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="Q20:R20"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="Q24:R24"/>
+    <mergeCell ref="P4:P20"/>
     <mergeCell ref="AK1:AM1"/>
     <mergeCell ref="X1:Y1"/>
     <mergeCell ref="AE1:AG1"/>
@@ -13648,13 +13658,6 @@
     <mergeCell ref="P2:P3"/>
     <mergeCell ref="W2:W3"/>
     <mergeCell ref="T1:T3"/>
-    <mergeCell ref="J32:K32"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="Q20:R20"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="Q24:R24"/>
-    <mergeCell ref="P4:P20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -13719,10 +13722,10 @@
         <f ca="1">TODAY()</f>
         <v>45282</v>
       </c>
-      <c r="V1" s="590" t="s">
+      <c r="V1" s="594" t="s">
         <v>71</v>
       </c>
-      <c r="W1" s="696"/>
+      <c r="W1" s="618"/>
       <c r="X1" s="62" t="s">
         <v>102</v>
       </c>
@@ -13741,7 +13744,7 @@
       <c r="AC1" s="116" t="s">
         <v>191</v>
       </c>
-      <c r="AD1" s="743" t="s">
+      <c r="AD1" s="740" t="s">
         <v>213</v>
       </c>
       <c r="AE1" s="116" t="s">
@@ -13758,10 +13761,10 @@
       <c r="E2" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="F2" s="774" t="s">
+      <c r="F2" s="739" t="s">
         <v>75</v>
       </c>
-      <c r="G2" s="731" t="s">
+      <c r="G2" s="767" t="s">
         <v>44</v>
       </c>
       <c r="H2" s="40" t="s">
@@ -13789,10 +13792,10 @@
       <c r="U2" s="60" t="s">
         <v>106</v>
       </c>
-      <c r="V2" s="704" t="s">
+      <c r="V2" s="710" t="s">
         <v>121</v>
       </c>
-      <c r="W2" s="705"/>
+      <c r="W2" s="711"/>
       <c r="X2" s="64" t="s">
         <v>110</v>
       </c>
@@ -13811,7 +13814,7 @@
       <c r="AC2" s="117" t="s">
         <v>99</v>
       </c>
-      <c r="AD2" s="744"/>
+      <c r="AD2" s="741"/>
       <c r="AE2" s="64" t="s">
         <v>99</v>
       </c>
@@ -13830,8 +13833,8 @@
       <c r="E3" s="39" t="s">
         <v>80</v>
       </c>
-      <c r="F3" s="647"/>
-      <c r="G3" s="732"/>
+      <c r="F3" s="670"/>
+      <c r="G3" s="768"/>
       <c r="H3" s="40" t="s">
         <v>81</v>
       </c>
@@ -13842,13 +13845,13 @@
         <v>82</v>
       </c>
       <c r="N3" s="44"/>
-      <c r="O3" s="741" t="s">
+      <c r="O3" s="777" t="s">
         <v>44</v>
       </c>
-      <c r="P3" s="762" t="s">
+      <c r="P3" s="759" t="s">
         <v>219</v>
       </c>
-      <c r="Q3" s="763"/>
+      <c r="Q3" s="760"/>
       <c r="S3" s="57" t="s">
         <v>220</v>
       </c>
@@ -13858,15 +13861,15 @@
       <c r="W3" s="59" t="s">
         <v>105</v>
       </c>
-      <c r="AD3" s="744"/>
+      <c r="AD3" s="741"/>
     </row>
     <row r="4" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G4" s="732"/>
+      <c r="G4" s="768"/>
       <c r="H4" s="6"/>
-      <c r="L4" s="726" t="s">
+      <c r="L4" s="678" t="s">
         <v>83</v>
       </c>
-      <c r="O4" s="742"/>
+      <c r="O4" s="778"/>
       <c r="T4" s="55" t="s">
         <v>98</v>
       </c>
@@ -13876,12 +13879,12 @@
       <c r="X4" s="67" t="s">
         <v>223</v>
       </c>
-      <c r="Y4" s="590" t="s">
+      <c r="Y4" s="594" t="s">
         <v>195</v>
       </c>
-      <c r="Z4" s="592"/>
-      <c r="AA4" s="696"/>
-      <c r="AD4" s="744"/>
+      <c r="Z4" s="596"/>
+      <c r="AA4" s="618"/>
+      <c r="AD4" s="741"/>
     </row>
     <row r="5" spans="1:31" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="52" t="s">
@@ -13896,21 +13899,21 @@
       <c r="F5" s="66" t="s">
         <v>85</v>
       </c>
-      <c r="G5" s="732"/>
+      <c r="G5" s="768"/>
       <c r="H5" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="K5" s="749" t="s">
+      <c r="K5" s="746" t="s">
         <v>217</v>
       </c>
-      <c r="L5" s="764"/>
+      <c r="L5" s="761"/>
       <c r="M5" s="2" t="s">
         <v>215</v>
       </c>
       <c r="N5" s="61" t="s">
         <v>214</v>
       </c>
-      <c r="O5" s="742"/>
+      <c r="O5" s="778"/>
       <c r="P5" s="108" t="s">
         <v>216</v>
       </c>
@@ -13926,11 +13929,11 @@
       <c r="U5" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="Y5" s="752" t="s">
+      <c r="Y5" s="749" t="s">
         <v>286</v>
       </c>
-      <c r="Z5" s="753"/>
-      <c r="AD5" s="744"/>
+      <c r="Z5" s="750"/>
+      <c r="AD5" s="741"/>
     </row>
     <row r="6" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="109"/>
@@ -13940,16 +13943,16 @@
       <c r="E6" s="45" t="s">
         <v>86</v>
       </c>
-      <c r="G6" s="732"/>
+      <c r="G6" s="768"/>
       <c r="H6" s="46" t="s">
         <v>81</v>
       </c>
       <c r="I6" s="23">
         <v>15</v>
       </c>
-      <c r="K6" s="750"/>
-      <c r="L6" s="764"/>
-      <c r="O6" s="742"/>
+      <c r="K6" s="747"/>
+      <c r="L6" s="761"/>
+      <c r="O6" s="778"/>
       <c r="T6" s="2" t="s">
         <v>101</v>
       </c>
@@ -13959,23 +13962,23 @@
       <c r="V6" s="21">
         <v>-1</v>
       </c>
-      <c r="AD6" s="744"/>
+      <c r="AD6" s="741"/>
     </row>
     <row r="7" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="110"/>
-      <c r="G7" s="732"/>
+      <c r="G7" s="768"/>
       <c r="H7" s="6"/>
-      <c r="K7" s="750"/>
-      <c r="L7" s="764"/>
+      <c r="K7" s="747"/>
+      <c r="L7" s="761"/>
       <c r="N7" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="O7" s="742"/>
+      <c r="O7" s="778"/>
       <c r="P7" s="73"/>
       <c r="U7" s="104" t="s">
         <v>20</v>
       </c>
-      <c r="AD7" s="744"/>
+      <c r="AD7" s="741"/>
     </row>
     <row r="8" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="130"/>
@@ -13988,7 +13991,7 @@
       <c r="F8" s="66" t="s">
         <v>87</v>
       </c>
-      <c r="G8" s="732"/>
+      <c r="G8" s="768"/>
       <c r="H8" s="50" t="s">
         <v>76</v>
       </c>
@@ -13998,41 +14001,41 @@
       <c r="J8" s="111">
         <v>115</v>
       </c>
-      <c r="K8" s="750"/>
-      <c r="L8" s="764"/>
-      <c r="O8" s="742"/>
+      <c r="K8" s="747"/>
+      <c r="L8" s="761"/>
+      <c r="O8" s="778"/>
       <c r="P8" s="49"/>
-      <c r="S8" s="746" t="s">
+      <c r="S8" s="743" t="s">
         <v>212</v>
       </c>
-      <c r="T8" s="747"/>
-      <c r="U8" s="747"/>
-      <c r="V8" s="747"/>
-      <c r="W8" s="747"/>
-      <c r="X8" s="747"/>
-      <c r="Y8" s="747"/>
-      <c r="Z8" s="747"/>
-      <c r="AA8" s="747"/>
-      <c r="AB8" s="747"/>
-      <c r="AC8" s="748"/>
-      <c r="AD8" s="744"/>
+      <c r="T8" s="744"/>
+      <c r="U8" s="744"/>
+      <c r="V8" s="744"/>
+      <c r="W8" s="744"/>
+      <c r="X8" s="744"/>
+      <c r="Y8" s="744"/>
+      <c r="Z8" s="744"/>
+      <c r="AA8" s="744"/>
+      <c r="AB8" s="744"/>
+      <c r="AC8" s="745"/>
+      <c r="AD8" s="741"/>
     </row>
     <row r="9" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="768"/>
-      <c r="G9" s="732"/>
+      <c r="C9" s="733"/>
+      <c r="G9" s="768"/>
       <c r="H9" s="6"/>
-      <c r="K9" s="750"/>
-      <c r="L9" s="735" t="s">
+      <c r="K9" s="747"/>
+      <c r="L9" s="771" t="s">
         <v>218</v>
       </c>
-      <c r="M9" s="736"/>
-      <c r="N9" s="737"/>
-      <c r="O9" s="742"/>
+      <c r="M9" s="772"/>
+      <c r="N9" s="773"/>
+      <c r="O9" s="778"/>
       <c r="P9" s="75"/>
-      <c r="AD9" s="744"/>
+      <c r="AD9" s="741"/>
     </row>
     <row r="10" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="769"/>
+      <c r="C10" s="734"/>
       <c r="D10" s="23"/>
       <c r="E10" s="45" t="s">
         <v>88</v>
@@ -14040,7 +14043,7 @@
       <c r="F10" s="66" t="s">
         <v>89</v>
       </c>
-      <c r="G10" s="732"/>
+      <c r="G10" s="768"/>
       <c r="H10" s="51"/>
       <c r="I10" s="21" t="s">
         <v>81</v>
@@ -14048,33 +14051,33 @@
       <c r="J10" s="3">
         <v>15</v>
       </c>
-      <c r="K10" s="750"/>
-      <c r="M10" s="771" t="s">
+      <c r="K10" s="747"/>
+      <c r="M10" s="736" t="s">
         <v>90</v>
       </c>
-      <c r="N10" s="772"/>
-      <c r="O10" s="772"/>
-      <c r="P10" s="772"/>
-      <c r="Q10" s="772"/>
-      <c r="R10" s="772"/>
-      <c r="S10" s="772"/>
-      <c r="T10" s="772"/>
-      <c r="U10" s="772"/>
-      <c r="V10" s="772"/>
-      <c r="W10" s="772"/>
-      <c r="X10" s="772"/>
-      <c r="Y10" s="772"/>
-      <c r="Z10" s="772"/>
-      <c r="AA10" s="772"/>
-      <c r="AB10" s="772"/>
-      <c r="AC10" s="773"/>
-      <c r="AD10" s="744"/>
+      <c r="N10" s="737"/>
+      <c r="O10" s="737"/>
+      <c r="P10" s="737"/>
+      <c r="Q10" s="737"/>
+      <c r="R10" s="737"/>
+      <c r="S10" s="737"/>
+      <c r="T10" s="737"/>
+      <c r="U10" s="737"/>
+      <c r="V10" s="737"/>
+      <c r="W10" s="737"/>
+      <c r="X10" s="737"/>
+      <c r="Y10" s="737"/>
+      <c r="Z10" s="737"/>
+      <c r="AA10" s="737"/>
+      <c r="AB10" s="737"/>
+      <c r="AC10" s="738"/>
+      <c r="AD10" s="741"/>
     </row>
     <row r="11" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="770"/>
-      <c r="G11" s="732"/>
+      <c r="C11" s="735"/>
+      <c r="G11" s="768"/>
       <c r="H11" s="6"/>
-      <c r="K11" s="750"/>
+      <c r="K11" s="747"/>
       <c r="R11" s="52" t="s">
         <v>44</v>
       </c>
@@ -14082,17 +14085,17 @@
       <c r="Y11" s="68" t="s">
         <v>121</v>
       </c>
-      <c r="Z11" s="760" t="s">
+      <c r="Z11" s="757" t="s">
         <v>121</v>
       </c>
-      <c r="AA11" s="761"/>
+      <c r="AA11" s="758"/>
       <c r="AB11" s="52" t="s">
         <v>44</v>
       </c>
       <c r="AC11" s="118" t="s">
         <v>121</v>
       </c>
-      <c r="AD11" s="744"/>
+      <c r="AD11" s="741"/>
     </row>
     <row r="12" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="129"/>
@@ -14105,7 +14108,7 @@
       <c r="F12" s="66" t="s">
         <v>92</v>
       </c>
-      <c r="G12" s="732"/>
+      <c r="G12" s="768"/>
       <c r="H12" s="128"/>
       <c r="I12" s="19" t="s">
         <v>81</v>
@@ -14113,8 +14116,8 @@
       <c r="J12" s="3">
         <v>15</v>
       </c>
-      <c r="K12" s="750"/>
-      <c r="L12" s="765" t="s">
+      <c r="K12" s="747"/>
+      <c r="L12" s="762" t="s">
         <v>93</v>
       </c>
       <c r="M12" s="21" t="s">
@@ -14129,7 +14132,7 @@
       <c r="Q12" s="113" t="s">
         <v>44</v>
       </c>
-      <c r="S12" s="585" t="s">
+      <c r="S12" s="589" t="s">
         <v>107</v>
       </c>
       <c r="T12" s="2" t="s">
@@ -14145,26 +14148,26 @@
         <v>116</v>
       </c>
       <c r="Y12" s="6"/>
-      <c r="AA12" s="754" t="s">
+      <c r="AA12" s="751" t="s">
         <v>126</v>
       </c>
-      <c r="AB12" s="755"/>
+      <c r="AB12" s="752"/>
       <c r="AC12" s="21" t="s">
         <v>232</v>
       </c>
-      <c r="AD12" s="744"/>
+      <c r="AD12" s="741"/>
     </row>
     <row r="13" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="768"/>
-      <c r="G13" s="732"/>
-      <c r="K13" s="750"/>
-      <c r="L13" s="766"/>
+      <c r="C13" s="733"/>
+      <c r="G13" s="768"/>
+      <c r="K13" s="747"/>
+      <c r="L13" s="763"/>
       <c r="M13" s="47"/>
-      <c r="Q13" s="734" t="s">
+      <c r="Q13" s="770" t="s">
         <v>210</v>
       </c>
-      <c r="R13" s="656"/>
-      <c r="S13" s="586"/>
+      <c r="R13" s="635"/>
+      <c r="S13" s="590"/>
       <c r="T13" s="6"/>
       <c r="U13" s="96" t="s">
         <v>132</v>
@@ -14172,17 +14175,17 @@
       <c r="X13" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="AA13" s="756"/>
-      <c r="AB13" s="757"/>
-      <c r="AD13" s="744"/>
+      <c r="AA13" s="753"/>
+      <c r="AB13" s="754"/>
+      <c r="AD13" s="741"/>
     </row>
     <row r="14" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="C14" s="770"/>
+      <c r="C14" s="735"/>
       <c r="D14" s="23"/>
-      <c r="G14" s="732"/>
+      <c r="G14" s="768"/>
       <c r="H14" s="125"/>
       <c r="I14" s="99" t="s">
         <v>44</v>
@@ -14190,8 +14193,8 @@
       <c r="J14" s="111">
         <v>115</v>
       </c>
-      <c r="K14" s="750"/>
-      <c r="L14" s="766"/>
+      <c r="K14" s="747"/>
+      <c r="L14" s="763"/>
       <c r="M14" s="21" t="s">
         <v>111</v>
       </c>
@@ -14201,7 +14204,7 @@
       <c r="R14" s="115" t="s">
         <v>44</v>
       </c>
-      <c r="S14" s="586"/>
+      <c r="S14" s="590"/>
       <c r="T14" s="77" t="s">
         <v>130</v>
       </c>
@@ -14212,9 +14215,9 @@
       <c r="Y14" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="AA14" s="756"/>
-      <c r="AB14" s="757"/>
-      <c r="AD14" s="744"/>
+      <c r="AA14" s="753"/>
+      <c r="AB14" s="754"/>
+      <c r="AD14" s="741"/>
     </row>
     <row r="15" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="130" t="s">
@@ -14229,20 +14232,20 @@
       <c r="F15" s="66" t="s">
         <v>94</v>
       </c>
-      <c r="G15" s="732"/>
+      <c r="G15" s="768"/>
       <c r="H15" s="2" t="s">
         <v>81</v>
       </c>
       <c r="I15" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="K15" s="750"/>
-      <c r="L15" s="767"/>
-      <c r="Q15" s="734" t="s">
+      <c r="K15" s="747"/>
+      <c r="L15" s="764"/>
+      <c r="Q15" s="770" t="s">
         <v>211</v>
       </c>
-      <c r="R15" s="656"/>
-      <c r="S15" s="586"/>
+      <c r="R15" s="635"/>
+      <c r="S15" s="590"/>
       <c r="T15" s="6"/>
       <c r="V15" s="68" t="s">
         <v>44</v>
@@ -14250,14 +14253,14 @@
       <c r="X15" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="AA15" s="756"/>
-      <c r="AB15" s="757"/>
-      <c r="AD15" s="744"/>
+      <c r="AA15" s="753"/>
+      <c r="AB15" s="754"/>
+      <c r="AD15" s="741"/>
     </row>
     <row r="16" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C16" s="132"/>
-      <c r="G16" s="732"/>
-      <c r="K16" s="750"/>
+      <c r="G16" s="768"/>
+      <c r="K16" s="747"/>
       <c r="N16" s="47"/>
       <c r="O16" s="61" t="s">
         <v>109</v>
@@ -14265,7 +14268,7 @@
       <c r="R16" s="114" t="s">
         <v>44</v>
       </c>
-      <c r="S16" s="586"/>
+      <c r="S16" s="590"/>
       <c r="T16" s="76" t="s">
         <v>129</v>
       </c>
@@ -14276,34 +14279,34 @@
       <c r="Z16" s="76" t="s">
         <v>127</v>
       </c>
-      <c r="AA16" s="756"/>
-      <c r="AB16" s="757"/>
-      <c r="AD16" s="744"/>
+      <c r="AA16" s="753"/>
+      <c r="AB16" s="754"/>
+      <c r="AD16" s="741"/>
     </row>
     <row r="17" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C17" s="109"/>
       <c r="E17" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F17" s="729" t="s">
+      <c r="F17" s="765" t="s">
         <v>96</v>
       </c>
-      <c r="G17" s="732"/>
+      <c r="G17" s="768"/>
       <c r="H17" s="54"/>
       <c r="I17" s="133" t="s">
         <v>81</v>
       </c>
-      <c r="K17" s="750"/>
-      <c r="S17" s="586"/>
+      <c r="K17" s="747"/>
+      <c r="S17" s="590"/>
       <c r="V17" s="68" t="s">
         <v>44</v>
       </c>
       <c r="X17" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="AA17" s="756"/>
-      <c r="AB17" s="757"/>
-      <c r="AD17" s="744"/>
+      <c r="AA17" s="753"/>
+      <c r="AB17" s="754"/>
+      <c r="AD17" s="741"/>
     </row>
     <row r="18" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C18" s="130"/>
@@ -14313,58 +14316,61 @@
       <c r="E18" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="F18" s="730"/>
-      <c r="G18" s="732"/>
+      <c r="F18" s="766"/>
+      <c r="G18" s="768"/>
       <c r="H18" s="108" t="s">
         <v>76</v>
       </c>
       <c r="I18" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="K18" s="750"/>
+      <c r="K18" s="747"/>
       <c r="O18" s="64" t="s">
         <v>115</v>
       </c>
-      <c r="S18" s="586"/>
+      <c r="S18" s="590"/>
       <c r="U18" s="76" t="s">
         <v>133</v>
       </c>
       <c r="X18" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="AA18" s="758"/>
-      <c r="AB18" s="759"/>
-      <c r="AD18" s="744"/>
+      <c r="AA18" s="755"/>
+      <c r="AB18" s="756"/>
+      <c r="AD18" s="741"/>
     </row>
     <row r="19" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F19" s="64" t="s">
         <v>209</v>
       </c>
-      <c r="G19" s="733"/>
-      <c r="K19" s="751"/>
+      <c r="G19" s="769"/>
+      <c r="K19" s="748"/>
       <c r="Q19" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="R19" s="738" t="s">
+      <c r="R19" s="774" t="s">
         <v>124</v>
       </c>
-      <c r="S19" s="739"/>
-      <c r="T19" s="740"/>
+      <c r="S19" s="775"/>
+      <c r="T19" s="776"/>
       <c r="V19" s="77" t="s">
         <v>115</v>
       </c>
       <c r="Y19" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="AD19" s="745"/>
+      <c r="AD19" s="742"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="M10:AC10"/>
-    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G2:G19"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="Q15:R15"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="R19:T19"/>
+    <mergeCell ref="S12:S18"/>
+    <mergeCell ref="O3:O9"/>
     <mergeCell ref="AD1:AD19"/>
     <mergeCell ref="S8:AC8"/>
     <mergeCell ref="K5:K19"/>
@@ -14376,14 +14382,11 @@
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="L4:L8"/>
     <mergeCell ref="L12:L15"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="G2:G19"/>
-    <mergeCell ref="Q13:R13"/>
-    <mergeCell ref="Q15:R15"/>
-    <mergeCell ref="L9:N9"/>
-    <mergeCell ref="R19:T19"/>
-    <mergeCell ref="S12:S18"/>
-    <mergeCell ref="O3:O9"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="M10:AC10"/>
+    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Rw - Updates - ABP Majha
ShieldW Enabled - ABP Majha
</commit_message>
<xml_diff>
--- a/System_2.1.8.xlsx
+++ b/System_2.1.8.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Work_For_\Work\Running AppS\System_Work_RW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C4029E6-810F-477A-A8CF-BE0545B2F283}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A729B76F-4DA0-4770-B79C-1D79F36E2C0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BoardRW" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1129" uniqueCount="634">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1131" uniqueCount="634">
   <si>
     <t>Zone</t>
   </si>
@@ -5009,6 +5009,186 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5021,12 +5201,6 @@
     <xf numFmtId="0" fontId="17" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5038,12 +5212,6 @@
     </xf>
     <xf numFmtId="0" fontId="38" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
@@ -5066,190 +5234,61 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="13" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5291,44 +5330,17 @@
     <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="43" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -5396,37 +5408,46 @@
     <xf numFmtId="14" fontId="5" fillId="14" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5504,46 +5525,25 @@
     <xf numFmtId="0" fontId="3" fillId="21" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -6930,7 +6930,7 @@
       <c r="H1" s="97" t="s">
         <v>349</v>
       </c>
-      <c r="I1" s="604" t="s">
+      <c r="I1" s="650" t="s">
         <v>375</v>
       </c>
       <c r="J1" s="2" t="s">
@@ -6966,7 +6966,7 @@
       <c r="X1" s="451" t="s">
         <v>156</v>
       </c>
-      <c r="Y1" s="648" t="s">
+      <c r="Y1" s="644" t="s">
         <v>539</v>
       </c>
       <c r="Z1" s="427">
@@ -6991,7 +6991,7 @@
         <v>507</v>
       </c>
       <c r="AM1" s="423"/>
-      <c r="AN1" s="631"/>
+      <c r="AN1" s="626"/>
       <c r="AO1" s="347" t="s">
         <v>478</v>
       </c>
@@ -7000,23 +7000,23 @@
       </c>
     </row>
     <row r="2" spans="1:43" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="657">
+      <c r="A2" s="608">
         <f ca="1">TODAY()</f>
         <v>45282</v>
       </c>
-      <c r="B2" s="659" t="s">
+      <c r="B2" s="610" t="s">
         <v>376</v>
       </c>
-      <c r="C2" s="636" t="s">
+      <c r="C2" s="606" t="s">
         <v>363</v>
       </c>
-      <c r="D2" s="661" t="s">
+      <c r="D2" s="612" t="s">
         <v>361</v>
       </c>
-      <c r="E2" s="600" t="s">
+      <c r="E2" s="660" t="s">
         <v>65</v>
       </c>
-      <c r="F2" s="610" t="s">
+      <c r="F2" s="631" t="s">
         <v>103</v>
       </c>
       <c r="G2" s="414" t="s">
@@ -7025,31 +7025,31 @@
       <c r="H2" s="80" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="605"/>
+      <c r="I2" s="651"/>
       <c r="J2" s="81" t="s">
         <v>77</v>
       </c>
-      <c r="K2" s="602" t="s">
+      <c r="K2" s="662" t="s">
         <v>348</v>
       </c>
-      <c r="L2" s="603"/>
-      <c r="M2" s="610" t="s">
+      <c r="L2" s="663"/>
+      <c r="M2" s="631" t="s">
         <v>103</v>
       </c>
       <c r="N2" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="O2" s="640" t="s">
+      <c r="O2" s="635" t="s">
         <v>103</v>
       </c>
       <c r="P2" s="85" t="s">
         <v>148</v>
       </c>
-      <c r="Q2" s="636" t="s">
+      <c r="Q2" s="606" t="s">
         <v>144</v>
       </c>
       <c r="R2" s="589"/>
-      <c r="S2" s="625" t="s">
+      <c r="S2" s="648" t="s">
         <v>149</v>
       </c>
       <c r="T2" s="89"/>
@@ -7059,7 +7059,7 @@
       <c r="X2" s="452" t="s">
         <v>157</v>
       </c>
-      <c r="Y2" s="649"/>
+      <c r="Y2" s="645"/>
       <c r="Z2" s="428">
         <v>1</v>
       </c>
@@ -7082,15 +7082,15 @@
         <v>472</v>
       </c>
       <c r="AM2" s="449"/>
-      <c r="AN2" s="632"/>
+      <c r="AN2" s="627"/>
     </row>
     <row r="3" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="658"/>
-      <c r="B3" s="660"/>
-      <c r="C3" s="637"/>
-      <c r="D3" s="662"/>
-      <c r="E3" s="601"/>
-      <c r="F3" s="611"/>
+      <c r="A3" s="609"/>
+      <c r="B3" s="611"/>
+      <c r="C3" s="607"/>
+      <c r="D3" s="613"/>
+      <c r="E3" s="661"/>
+      <c r="F3" s="632"/>
       <c r="G3" s="415" t="s">
         <v>28</v>
       </c>
@@ -7109,17 +7109,17 @@
       <c r="L3" s="205" t="s">
         <v>108</v>
       </c>
-      <c r="M3" s="611"/>
+      <c r="M3" s="632"/>
       <c r="N3" s="69" t="s">
         <v>147</v>
       </c>
-      <c r="O3" s="641"/>
+      <c r="O3" s="636"/>
       <c r="P3" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="Q3" s="637"/>
+      <c r="Q3" s="607"/>
       <c r="R3" s="591"/>
-      <c r="S3" s="627"/>
+      <c r="S3" s="649"/>
       <c r="T3" s="89"/>
       <c r="U3" s="124"/>
       <c r="V3" s="120"/>
@@ -7127,7 +7127,7 @@
       <c r="X3" s="452" t="s">
         <v>158</v>
       </c>
-      <c r="Y3" s="649"/>
+      <c r="Y3" s="645"/>
       <c r="Z3" s="429">
         <v>1</v>
       </c>
@@ -7136,7 +7136,7 @@
       <c r="AC3" s="100" t="s">
         <v>489</v>
       </c>
-      <c r="AD3" s="622" t="s">
+      <c r="AD3" s="647" t="s">
         <v>464</v>
       </c>
       <c r="AE3" s="261"/>
@@ -7148,16 +7148,16 @@
       <c r="AK3" s="261"/>
       <c r="AL3" s="16"/>
       <c r="AM3" s="449"/>
-      <c r="AN3" s="632"/>
+      <c r="AN3" s="627"/>
     </row>
     <row r="4" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="242" t="s">
         <v>184</v>
       </c>
-      <c r="B4" s="673" t="s">
+      <c r="B4" s="624" t="s">
         <v>379</v>
       </c>
-      <c r="C4" s="636" t="s">
+      <c r="C4" s="606" t="s">
         <v>155</v>
       </c>
       <c r="D4" s="356" t="s">
@@ -7166,7 +7166,7 @@
       <c r="E4" s="393">
         <v>2</v>
       </c>
-      <c r="F4" s="611"/>
+      <c r="F4" s="632"/>
       <c r="G4" s="397" t="s">
         <v>203</v>
       </c>
@@ -7183,11 +7183,11 @@
         <v>151</v>
       </c>
       <c r="L4" s="208"/>
-      <c r="M4" s="611"/>
+      <c r="M4" s="632"/>
       <c r="N4" s="178" t="s">
         <v>70</v>
       </c>
-      <c r="O4" s="641"/>
+      <c r="O4" s="636"/>
       <c r="P4" s="2" t="s">
         <v>192</v>
       </c>
@@ -7209,12 +7209,12 @@
       <c r="X4" s="452" t="s">
         <v>159</v>
       </c>
-      <c r="Y4" s="649"/>
+      <c r="Y4" s="645"/>
       <c r="Z4" s="430"/>
       <c r="AA4" s="312"/>
       <c r="AB4" s="213"/>
       <c r="AC4" s="16"/>
-      <c r="AD4" s="622"/>
+      <c r="AD4" s="647"/>
       <c r="AE4" s="261"/>
       <c r="AF4" s="261"/>
       <c r="AG4" s="16"/>
@@ -7224,37 +7224,37 @@
       <c r="AK4" s="261"/>
       <c r="AL4" s="16"/>
       <c r="AM4" s="449"/>
-      <c r="AN4" s="632"/>
+      <c r="AN4" s="627"/>
       <c r="AO4" s="347" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="604" t="s">
+      <c r="A5" s="650" t="s">
         <v>427</v>
       </c>
-      <c r="B5" s="674"/>
-      <c r="C5" s="637"/>
+      <c r="B5" s="625"/>
+      <c r="C5" s="607"/>
       <c r="D5" s="61" t="s">
         <v>154</v>
       </c>
       <c r="E5" s="394">
         <v>1</v>
       </c>
-      <c r="F5" s="611"/>
-      <c r="G5" s="665" t="s">
+      <c r="F5" s="632"/>
+      <c r="G5" s="616" t="s">
         <v>193</v>
       </c>
-      <c r="H5" s="665"/>
-      <c r="I5" s="665"/>
-      <c r="J5" s="665"/>
-      <c r="K5" s="665"/>
-      <c r="L5" s="666"/>
-      <c r="M5" s="611"/>
+      <c r="H5" s="616"/>
+      <c r="I5" s="616"/>
+      <c r="J5" s="616"/>
+      <c r="K5" s="616"/>
+      <c r="L5" s="617"/>
+      <c r="M5" s="632"/>
       <c r="N5" s="21">
         <v>8</v>
       </c>
-      <c r="O5" s="641"/>
+      <c r="O5" s="636"/>
       <c r="T5" s="89"/>
       <c r="U5" s="124"/>
       <c r="V5" s="120"/>
@@ -7262,7 +7262,7 @@
       <c r="X5" s="452" t="s">
         <v>160</v>
       </c>
-      <c r="Y5" s="649"/>
+      <c r="Y5" s="645"/>
       <c r="Z5" s="430">
         <v>1</v>
       </c>
@@ -7285,24 +7285,24 @@
       <c r="AK5" s="261"/>
       <c r="AL5" s="80"/>
       <c r="AM5" s="449"/>
-      <c r="AN5" s="632"/>
+      <c r="AN5" s="627"/>
     </row>
     <row r="6" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="605"/>
-      <c r="B6" s="671" t="s">
+      <c r="A6" s="651"/>
+      <c r="B6" s="622" t="s">
         <v>178</v>
       </c>
-      <c r="C6" s="619"/>
-      <c r="D6" s="620"/>
-      <c r="F6" s="611"/>
-      <c r="G6" s="667"/>
-      <c r="H6" s="667"/>
-      <c r="I6" s="667"/>
-      <c r="J6" s="667"/>
-      <c r="K6" s="667"/>
-      <c r="L6" s="668"/>
-      <c r="M6" s="611"/>
-      <c r="O6" s="641"/>
+      <c r="C6" s="652"/>
+      <c r="D6" s="653"/>
+      <c r="F6" s="632"/>
+      <c r="G6" s="618"/>
+      <c r="H6" s="618"/>
+      <c r="I6" s="618"/>
+      <c r="J6" s="618"/>
+      <c r="K6" s="618"/>
+      <c r="L6" s="619"/>
+      <c r="M6" s="632"/>
+      <c r="O6" s="636"/>
       <c r="T6" s="89"/>
       <c r="U6" s="124"/>
       <c r="V6" s="98" t="s">
@@ -7312,7 +7312,7 @@
       <c r="X6" s="452" t="s">
         <v>161</v>
       </c>
-      <c r="Y6" s="649"/>
+      <c r="Y6" s="645"/>
       <c r="Z6" s="428">
         <v>1</v>
       </c>
@@ -7326,16 +7326,16 @@
       <c r="AF6" s="261"/>
       <c r="AG6" s="261"/>
       <c r="AH6" s="261"/>
-      <c r="AI6" s="621"/>
+      <c r="AI6" s="641"/>
       <c r="AJ6" s="462" t="s">
         <v>467</v>
       </c>
-      <c r="AK6" s="621" t="s">
+      <c r="AK6" s="641" t="s">
         <v>255</v>
       </c>
       <c r="AL6" s="261"/>
       <c r="AM6" s="449"/>
-      <c r="AN6" s="632"/>
+      <c r="AN6" s="627"/>
       <c r="AO6" s="347" t="s">
         <v>479</v>
       </c>
@@ -7344,7 +7344,7 @@
       <c r="A7" s="236" t="s">
         <v>584</v>
       </c>
-      <c r="B7" s="672"/>
+      <c r="B7" s="623"/>
       <c r="C7" s="206" t="s">
         <v>380</v>
       </c>
@@ -7354,7 +7354,7 @@
       <c r="E7" s="270">
         <v>3</v>
       </c>
-      <c r="F7" s="611"/>
+      <c r="F7" s="632"/>
       <c r="G7" s="416">
         <v>0</v>
       </c>
@@ -7373,8 +7373,8 @@
       <c r="L7" s="216">
         <v>0</v>
       </c>
-      <c r="M7" s="611"/>
-      <c r="O7" s="641"/>
+      <c r="M7" s="632"/>
+      <c r="O7" s="636"/>
       <c r="R7" s="99" t="s">
         <v>44</v>
       </c>
@@ -7388,7 +7388,7 @@
       <c r="X7" s="452" t="s">
         <v>162</v>
       </c>
-      <c r="Y7" s="649"/>
+      <c r="Y7" s="645"/>
       <c r="Z7" s="428">
         <v>1</v>
       </c>
@@ -7398,18 +7398,18 @@
       <c r="AD7" s="16"/>
       <c r="AE7" s="261"/>
       <c r="AF7" s="261"/>
-      <c r="AG7" s="622" t="s">
+      <c r="AG7" s="647" t="s">
         <v>463</v>
       </c>
       <c r="AH7" s="261"/>
-      <c r="AI7" s="621"/>
+      <c r="AI7" s="641"/>
       <c r="AJ7" s="261"/>
-      <c r="AK7" s="621"/>
+      <c r="AK7" s="641"/>
       <c r="AL7" s="80" t="s">
         <v>505</v>
       </c>
       <c r="AM7" s="449"/>
-      <c r="AN7" s="632"/>
+      <c r="AN7" s="627"/>
       <c r="AP7" s="76" t="s">
         <v>480</v>
       </c>
@@ -7426,27 +7426,27 @@
         <f>SUM(G7:N9)</f>
         <v>15</v>
       </c>
-      <c r="F8" s="611"/>
-      <c r="G8" s="666">
-        <v>0</v>
-      </c>
-      <c r="H8" s="663" t="s">
+      <c r="F8" s="632"/>
+      <c r="G8" s="617">
+        <v>0</v>
+      </c>
+      <c r="H8" s="614" t="s">
         <v>105</v>
       </c>
       <c r="I8" s="589">
         <v>0</v>
       </c>
-      <c r="J8" s="663" t="s">
+      <c r="J8" s="614" t="s">
         <v>105</v>
       </c>
-      <c r="K8" s="669"/>
-      <c r="L8" s="623"/>
-      <c r="M8" s="638"/>
-      <c r="N8" s="628">
+      <c r="K8" s="620"/>
+      <c r="L8" s="654"/>
+      <c r="M8" s="633"/>
+      <c r="N8" s="657">
         <f>N5+N11</f>
         <v>15</v>
       </c>
-      <c r="O8" s="641"/>
+      <c r="O8" s="636"/>
       <c r="T8" s="103" t="s">
         <v>44</v>
       </c>
@@ -7456,7 +7456,7 @@
       <c r="X8" s="452" t="s">
         <v>163</v>
       </c>
-      <c r="Y8" s="649"/>
+      <c r="Y8" s="645"/>
       <c r="Z8" s="430"/>
       <c r="AA8" s="312"/>
       <c r="AB8" s="213"/>
@@ -7464,14 +7464,14 @@
       <c r="AD8" s="16"/>
       <c r="AE8" s="261"/>
       <c r="AF8" s="261"/>
-      <c r="AG8" s="622"/>
+      <c r="AG8" s="647"/>
       <c r="AH8" s="261"/>
-      <c r="AI8" s="621"/>
+      <c r="AI8" s="641"/>
       <c r="AJ8" s="261"/>
       <c r="AK8" s="261"/>
       <c r="AL8" s="261"/>
       <c r="AM8" s="449"/>
-      <c r="AN8" s="632"/>
+      <c r="AN8" s="627"/>
     </row>
     <row r="9" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="236" t="s">
@@ -7486,17 +7486,17 @@
       <c r="D9" s="357" t="s">
         <v>285</v>
       </c>
-      <c r="F9" s="611"/>
-      <c r="G9" s="668"/>
-      <c r="H9" s="664"/>
+      <c r="F9" s="632"/>
+      <c r="G9" s="619"/>
+      <c r="H9" s="615"/>
       <c r="I9" s="591"/>
-      <c r="J9" s="664"/>
-      <c r="K9" s="670"/>
-      <c r="L9" s="624"/>
-      <c r="M9" s="639"/>
-      <c r="N9" s="629"/>
-      <c r="O9" s="642"/>
-      <c r="S9" s="625" t="s">
+      <c r="J9" s="615"/>
+      <c r="K9" s="621"/>
+      <c r="L9" s="655"/>
+      <c r="M9" s="634"/>
+      <c r="N9" s="658"/>
+      <c r="O9" s="637"/>
+      <c r="S9" s="648" t="s">
         <v>62</v>
       </c>
       <c r="T9" s="89"/>
@@ -7508,7 +7508,7 @@
       <c r="X9" s="452" t="s">
         <v>164</v>
       </c>
-      <c r="Y9" s="649"/>
+      <c r="Y9" s="645"/>
       <c r="Z9" s="431"/>
       <c r="AA9" s="312"/>
       <c r="AB9" s="213"/>
@@ -7518,16 +7518,16 @@
       </c>
       <c r="AE9" s="261"/>
       <c r="AF9" s="261"/>
-      <c r="AG9" s="622"/>
+      <c r="AG9" s="647"/>
       <c r="AH9" s="261"/>
-      <c r="AI9" s="621"/>
+      <c r="AI9" s="641"/>
       <c r="AJ9" s="80"/>
-      <c r="AK9" s="621" t="s">
+      <c r="AK9" s="641" t="s">
         <v>255</v>
       </c>
       <c r="AL9" s="261"/>
       <c r="AM9" s="449"/>
-      <c r="AN9" s="632"/>
+      <c r="AN9" s="627"/>
       <c r="AP9" s="2" t="s">
         <v>517</v>
       </c>
@@ -7544,20 +7544,20 @@
         <f>Boat!W8</f>
         <v>37</v>
       </c>
-      <c r="F10" s="611"/>
+      <c r="F10" s="632"/>
       <c r="N10" s="439" t="s">
         <v>403</v>
       </c>
-      <c r="O10" s="613" t="s">
+      <c r="O10" s="669" t="s">
         <v>103</v>
       </c>
-      <c r="P10" s="643" t="s">
+      <c r="P10" s="638" t="s">
         <v>407</v>
       </c>
       <c r="R10" s="74" t="s">
         <v>44</v>
       </c>
-      <c r="S10" s="626"/>
+      <c r="S10" s="656"/>
       <c r="T10" s="89"/>
       <c r="U10" s="123" t="s">
         <v>177</v>
@@ -7569,7 +7569,7 @@
       <c r="X10" s="452" t="s">
         <v>165</v>
       </c>
-      <c r="Y10" s="649"/>
+      <c r="Y10" s="645"/>
       <c r="Z10" s="430">
         <v>0</v>
       </c>
@@ -7587,16 +7587,16 @@
       <c r="AF10" s="242" t="s">
         <v>317</v>
       </c>
-      <c r="AG10" s="622"/>
+      <c r="AG10" s="647"/>
       <c r="AH10" s="80"/>
-      <c r="AI10" s="621"/>
+      <c r="AI10" s="641"/>
       <c r="AJ10" s="261"/>
-      <c r="AK10" s="621"/>
+      <c r="AK10" s="641"/>
       <c r="AL10" s="261"/>
       <c r="AM10" s="463" t="s">
         <v>324</v>
       </c>
-      <c r="AN10" s="632"/>
+      <c r="AN10" s="627"/>
       <c r="AO10" s="208" t="s">
         <v>95</v>
       </c>
@@ -7614,18 +7614,18 @@
       <c r="D11" s="174" t="s">
         <v>361</v>
       </c>
-      <c r="F11" s="611"/>
+      <c r="F11" s="632"/>
       <c r="M11" s="6"/>
       <c r="N11" s="117">
         <v>7</v>
       </c>
-      <c r="O11" s="614"/>
-      <c r="P11" s="644"/>
+      <c r="O11" s="670"/>
+      <c r="P11" s="639"/>
       <c r="Q11" s="65"/>
       <c r="R11" s="120" t="s">
         <v>222</v>
       </c>
-      <c r="S11" s="626"/>
+      <c r="S11" s="656"/>
       <c r="T11" s="102" t="s">
         <v>44</v>
       </c>
@@ -7635,7 +7635,7 @@
       <c r="X11" s="452" t="s">
         <v>166</v>
       </c>
-      <c r="Y11" s="649"/>
+      <c r="Y11" s="645"/>
       <c r="Z11" s="430"/>
       <c r="AA11" s="312">
         <v>1</v>
@@ -7649,14 +7649,14 @@
       <c r="AF11" s="261" t="s">
         <v>485</v>
       </c>
-      <c r="AG11" s="622"/>
+      <c r="AG11" s="647"/>
       <c r="AH11" s="261"/>
       <c r="AI11" s="70"/>
       <c r="AJ11" s="261"/>
       <c r="AK11" s="261"/>
       <c r="AL11" s="261"/>
       <c r="AM11" s="449"/>
-      <c r="AN11" s="632"/>
+      <c r="AN11" s="627"/>
       <c r="AP11" s="76" t="s">
         <v>493</v>
       </c>
@@ -7675,7 +7675,7 @@
       <c r="E12" s="228">
         <v>3</v>
       </c>
-      <c r="F12" s="611"/>
+      <c r="F12" s="632"/>
       <c r="G12" s="346" t="s">
         <v>407</v>
       </c>
@@ -7684,16 +7684,16 @@
       </c>
       <c r="I12" s="596"/>
       <c r="J12" s="596"/>
-      <c r="K12" s="618"/>
+      <c r="K12" s="674"/>
       <c r="L12" s="207"/>
       <c r="M12" s="207"/>
       <c r="N12" s="207"/>
-      <c r="O12" s="614"/>
-      <c r="P12" s="644"/>
+      <c r="O12" s="670"/>
+      <c r="P12" s="639"/>
       <c r="R12" s="122" t="s">
         <v>181</v>
       </c>
-      <c r="S12" s="627"/>
+      <c r="S12" s="649"/>
       <c r="T12" s="101" t="s">
         <v>44</v>
       </c>
@@ -7703,7 +7703,7 @@
       <c r="X12" s="452" t="s">
         <v>167</v>
       </c>
-      <c r="Y12" s="649"/>
+      <c r="Y12" s="645"/>
       <c r="Z12" s="428">
         <v>1</v>
       </c>
@@ -7714,16 +7714,16 @@
       <c r="AC12" s="100" t="s">
         <v>490</v>
       </c>
-      <c r="AD12" s="630" t="s">
+      <c r="AD12" s="659" t="s">
         <v>244</v>
       </c>
       <c r="AE12" s="462" t="s">
         <v>243</v>
       </c>
-      <c r="AF12" s="622" t="s">
+      <c r="AF12" s="647" t="s">
         <v>230</v>
       </c>
-      <c r="AG12" s="622"/>
+      <c r="AG12" s="647"/>
       <c r="AH12" s="242" t="s">
         <v>263</v>
       </c>
@@ -7733,10 +7733,10 @@
       <c r="AJ12" s="261"/>
       <c r="AK12" s="261"/>
       <c r="AL12" s="261"/>
-      <c r="AM12" s="646" t="s">
+      <c r="AM12" s="642" t="s">
         <v>253</v>
       </c>
-      <c r="AN12" s="632"/>
+      <c r="AN12" s="627"/>
       <c r="AO12" s="347" t="s">
         <v>97</v>
       </c>
@@ -7748,17 +7748,17 @@
       <c r="E13" s="469">
         <v>-3</v>
       </c>
-      <c r="F13" s="611"/>
+      <c r="F13" s="632"/>
       <c r="G13" s="596" t="s">
         <v>439</v>
       </c>
       <c r="H13" s="596"/>
       <c r="I13" s="596"/>
-      <c r="J13" s="618"/>
+      <c r="J13" s="674"/>
       <c r="M13" s="6"/>
       <c r="N13" s="6"/>
-      <c r="O13" s="614"/>
-      <c r="P13" s="645"/>
+      <c r="O13" s="670"/>
+      <c r="P13" s="640"/>
       <c r="T13" s="105" t="s">
         <v>44</v>
       </c>
@@ -7768,7 +7768,7 @@
       <c r="X13" s="452" t="s">
         <v>168</v>
       </c>
-      <c r="Y13" s="649"/>
+      <c r="Y13" s="645"/>
       <c r="Z13" s="428">
         <v>1</v>
       </c>
@@ -7779,8 +7779,8 @@
         <v>509</v>
       </c>
       <c r="AC13" s="16"/>
-      <c r="AD13" s="630"/>
-      <c r="AF13" s="622"/>
+      <c r="AD13" s="659"/>
+      <c r="AF13" s="647"/>
       <c r="AG13" s="80"/>
       <c r="AH13" s="242" t="s">
         <v>313</v>
@@ -7791,8 +7791,8 @@
       <c r="AJ13" s="80"/>
       <c r="AK13" s="261"/>
       <c r="AL13" s="261"/>
-      <c r="AM13" s="646"/>
-      <c r="AN13" s="632"/>
+      <c r="AM13" s="642"/>
+      <c r="AN13" s="627"/>
     </row>
     <row r="14" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="471"/>
@@ -7800,18 +7800,18 @@
       <c r="C14" s="480"/>
       <c r="D14" s="473"/>
       <c r="E14" s="474"/>
-      <c r="F14" s="611"/>
+      <c r="F14" s="632"/>
       <c r="G14" s="596" t="s">
         <v>438</v>
       </c>
       <c r="H14" s="596"/>
       <c r="I14" s="596"/>
-      <c r="J14" s="618"/>
+      <c r="J14" s="674"/>
       <c r="K14" s="2">
         <v>12</v>
       </c>
       <c r="N14" s="6"/>
-      <c r="O14" s="614"/>
+      <c r="O14" s="670"/>
       <c r="Q14" s="61" t="s">
         <v>543</v>
       </c>
@@ -7825,24 +7825,24 @@
       <c r="X14" s="452" t="s">
         <v>169</v>
       </c>
-      <c r="Y14" s="649"/>
+      <c r="Y14" s="645"/>
       <c r="Z14" s="428">
         <v>1</v>
       </c>
       <c r="AA14" s="312"/>
       <c r="AB14" s="213"/>
       <c r="AC14" s="16"/>
-      <c r="AD14" s="630"/>
+      <c r="AD14" s="659"/>
       <c r="AE14" s="261"/>
-      <c r="AF14" s="622"/>
+      <c r="AF14" s="647"/>
       <c r="AG14" s="261"/>
       <c r="AH14" s="261"/>
       <c r="AI14" s="70"/>
       <c r="AJ14" s="261"/>
       <c r="AK14" s="261"/>
       <c r="AL14" s="261"/>
-      <c r="AM14" s="646"/>
-      <c r="AN14" s="632"/>
+      <c r="AM14" s="642"/>
+      <c r="AN14" s="627"/>
     </row>
     <row r="15" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="470" t="s">
@@ -7851,8 +7851,8 @@
       <c r="C15" s="589" t="s">
         <v>379</v>
       </c>
-      <c r="F15" s="611"/>
-      <c r="O15" s="614"/>
+      <c r="F15" s="632"/>
+      <c r="O15" s="670"/>
       <c r="R15" s="99" t="s">
         <v>44</v>
       </c>
@@ -7865,7 +7865,7 @@
       <c r="X15" s="452" t="s">
         <v>170</v>
       </c>
-      <c r="Y15" s="649"/>
+      <c r="Y15" s="645"/>
       <c r="Z15" s="430">
         <v>1</v>
       </c>
@@ -7874,8 +7874,8 @@
       <c r="AC15" s="76" t="s">
         <v>488</v>
       </c>
-      <c r="AD15" s="630"/>
-      <c r="AF15" s="622"/>
+      <c r="AD15" s="659"/>
+      <c r="AF15" s="647"/>
       <c r="AG15" s="80"/>
       <c r="AH15" s="242" t="s">
         <v>457</v>
@@ -7888,8 +7888,8 @@
       </c>
       <c r="AK15" s="261"/>
       <c r="AL15" s="261"/>
-      <c r="AM15" s="646"/>
-      <c r="AN15" s="632"/>
+      <c r="AM15" s="642"/>
+      <c r="AN15" s="627"/>
       <c r="AP15" s="76" t="s">
         <v>74</v>
       </c>
@@ -7911,13 +7911,13 @@
       <c r="E16" s="228">
         <v>1</v>
       </c>
-      <c r="F16" s="611"/>
+      <c r="F16" s="632"/>
       <c r="G16" s="346" t="s">
         <v>497</v>
       </c>
       <c r="I16" s="491"/>
       <c r="J16" s="20"/>
-      <c r="O16" s="614"/>
+      <c r="O16" s="670"/>
       <c r="R16" s="456" t="s">
         <v>185</v>
       </c>
@@ -7928,7 +7928,7 @@
       <c r="X16" s="452" t="s">
         <v>171</v>
       </c>
-      <c r="Y16" s="649"/>
+      <c r="Y16" s="645"/>
       <c r="Z16" s="428">
         <v>1</v>
       </c>
@@ -7949,18 +7949,18 @@
       <c r="AM16" s="449" t="s">
         <v>323</v>
       </c>
-      <c r="AN16" s="632"/>
+      <c r="AN16" s="627"/>
       <c r="AP16" s="76" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="17" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="80"/>
-      <c r="F17" s="611"/>
+      <c r="F17" s="632"/>
       <c r="I17" s="492"/>
       <c r="J17" s="20"/>
       <c r="N17" s="6"/>
-      <c r="O17" s="614"/>
+      <c r="O17" s="670"/>
       <c r="Q17" s="21" t="s">
         <v>541</v>
       </c>
@@ -7980,7 +7980,7 @@
       <c r="X17" s="452" t="s">
         <v>172</v>
       </c>
-      <c r="Y17" s="649"/>
+      <c r="Y17" s="645"/>
       <c r="Z17" s="430"/>
       <c r="AA17" s="312"/>
       <c r="AB17" s="213"/>
@@ -8005,7 +8005,7 @@
       <c r="AK17" s="261"/>
       <c r="AL17" s="80"/>
       <c r="AM17" s="449"/>
-      <c r="AN17" s="632"/>
+      <c r="AN17" s="627"/>
       <c r="AO17" s="208" t="s">
         <v>506</v>
       </c>
@@ -8029,21 +8029,21 @@
       <c r="E18" s="99" t="s">
         <v>44</v>
       </c>
-      <c r="F18" s="611"/>
+      <c r="F18" s="632"/>
       <c r="G18" s="346" t="s">
         <v>538</v>
       </c>
       <c r="I18" s="24"/>
       <c r="J18" s="20"/>
-      <c r="O18" s="614"/>
+      <c r="O18" s="670"/>
       <c r="Q18" s="112"/>
-      <c r="R18" s="606" t="s">
+      <c r="R18" s="664" t="s">
         <v>546</v>
       </c>
       <c r="T18" s="100" t="s">
         <v>44</v>
       </c>
-      <c r="U18" s="654" t="s">
+      <c r="U18" s="603" t="s">
         <v>44</v>
       </c>
       <c r="V18" s="120"/>
@@ -8053,7 +8053,7 @@
       <c r="X18" s="452" t="s">
         <v>173</v>
       </c>
-      <c r="Y18" s="649"/>
+      <c r="Y18" s="645"/>
       <c r="Z18" s="430">
         <v>1</v>
       </c>
@@ -8064,38 +8064,38 @@
       <c r="AC18" s="16"/>
       <c r="AD18" s="16"/>
       <c r="AE18" s="261"/>
-      <c r="AF18" s="621" t="s">
+      <c r="AF18" s="641" t="s">
         <v>484</v>
       </c>
       <c r="AG18" s="261"/>
       <c r="AH18" s="70"/>
       <c r="AI18" s="70"/>
-      <c r="AJ18" s="647" t="s">
+      <c r="AJ18" s="643" t="s">
         <v>321</v>
       </c>
       <c r="AK18" s="261"/>
       <c r="AL18" s="80"/>
       <c r="AM18" s="449"/>
-      <c r="AN18" s="632"/>
+      <c r="AN18" s="627"/>
       <c r="AP18" s="76" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F19" s="611"/>
+      <c r="F19" s="632"/>
       <c r="I19" s="223"/>
-      <c r="O19" s="614"/>
-      <c r="R19" s="607"/>
+      <c r="O19" s="670"/>
+      <c r="R19" s="665"/>
       <c r="S19" s="30" t="s">
         <v>544</v>
       </c>
-      <c r="U19" s="655"/>
+      <c r="U19" s="604"/>
       <c r="V19" s="146"/>
       <c r="W19" s="146"/>
       <c r="X19" s="452" t="s">
         <v>174</v>
       </c>
-      <c r="Y19" s="649"/>
+      <c r="Y19" s="645"/>
       <c r="Z19" s="428">
         <v>1</v>
       </c>
@@ -8104,17 +8104,17 @@
       <c r="AC19" s="16"/>
       <c r="AD19" s="16"/>
       <c r="AE19" s="261"/>
-      <c r="AF19" s="621"/>
+      <c r="AF19" s="641"/>
       <c r="AG19" s="261"/>
       <c r="AH19" s="261"/>
       <c r="AI19" s="70"/>
-      <c r="AJ19" s="647"/>
+      <c r="AJ19" s="643"/>
       <c r="AK19" s="481" t="s">
         <v>255</v>
       </c>
       <c r="AL19" s="80"/>
       <c r="AM19" s="449"/>
-      <c r="AN19" s="632"/>
+      <c r="AN19" s="627"/>
       <c r="AP19" s="76" t="s">
         <v>477</v>
       </c>
@@ -8135,24 +8135,24 @@
       <c r="E20" s="458">
         <v>-1</v>
       </c>
-      <c r="F20" s="611"/>
+      <c r="F20" s="632"/>
       <c r="G20" s="346" t="s">
         <v>500</v>
       </c>
       <c r="I20" s="223"/>
-      <c r="O20" s="614"/>
-      <c r="Q20" s="616" t="s">
+      <c r="O20" s="670"/>
+      <c r="Q20" s="672" t="s">
         <v>48</v>
       </c>
       <c r="T20" s="425" t="s">
         <v>44</v>
       </c>
-      <c r="U20" s="656"/>
+      <c r="U20" s="605"/>
       <c r="W20" s="426"/>
       <c r="X20" s="453" t="s">
         <v>175</v>
       </c>
-      <c r="Y20" s="649"/>
+      <c r="Y20" s="645"/>
       <c r="Z20" s="432">
         <v>1</v>
       </c>
@@ -8177,7 +8177,7 @@
       <c r="AM20" s="397" t="s">
         <v>253</v>
       </c>
-      <c r="AN20" s="632"/>
+      <c r="AN20" s="627"/>
       <c r="AO20" s="347" t="s">
         <v>469</v>
       </c>
@@ -8198,20 +8198,20 @@
       <c r="E21" s="270">
         <v>0</v>
       </c>
-      <c r="F21" s="611"/>
+      <c r="F21" s="632"/>
       <c r="I21" s="223"/>
-      <c r="O21" s="614"/>
-      <c r="Q21" s="617"/>
+      <c r="O21" s="670"/>
+      <c r="Q21" s="673"/>
       <c r="T21" s="443"/>
       <c r="U21" s="14"/>
-      <c r="V21" s="651"/>
+      <c r="V21" s="600"/>
       <c r="W21" s="447" t="s">
         <v>176</v>
       </c>
       <c r="X21" s="450" t="s">
         <v>187</v>
       </c>
-      <c r="Y21" s="649"/>
+      <c r="Y21" s="645"/>
       <c r="Z21" s="466">
         <v>3</v>
       </c>
@@ -8242,15 +8242,15 @@
       <c r="AM21" s="449" t="s">
         <v>555</v>
       </c>
-      <c r="AN21" s="632"/>
+      <c r="AN21" s="627"/>
     </row>
     <row r="22" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F22" s="611"/>
+      <c r="F22" s="632"/>
       <c r="G22" s="346" t="s">
         <v>498</v>
       </c>
       <c r="I22" s="223"/>
-      <c r="O22" s="614"/>
+      <c r="O22" s="670"/>
       <c r="R22" s="455" t="s">
         <v>44</v>
       </c>
@@ -8258,14 +8258,14 @@
         <v>44</v>
       </c>
       <c r="U22" s="15"/>
-      <c r="V22" s="652"/>
+      <c r="V22" s="601"/>
       <c r="W22" s="447" t="s">
         <v>176</v>
       </c>
       <c r="X22" s="450" t="s">
         <v>188</v>
       </c>
-      <c r="Y22" s="649"/>
+      <c r="Y22" s="645"/>
       <c r="Z22" s="436"/>
       <c r="AA22" s="10"/>
       <c r="AB22" s="436"/>
@@ -8276,7 +8276,7 @@
       <c r="AG22" s="6"/>
       <c r="AH22" s="6"/>
       <c r="AI22" s="6"/>
-      <c r="AJ22" s="621" t="s">
+      <c r="AJ22" s="641" t="s">
         <v>481</v>
       </c>
       <c r="AK22" s="261"/>
@@ -8284,7 +8284,7 @@
         <v>487</v>
       </c>
       <c r="AM22" s="305"/>
-      <c r="AN22" s="632"/>
+      <c r="AN22" s="627"/>
     </row>
     <row r="23" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="235" t="s">
@@ -8302,22 +8302,22 @@
       <c r="E23" s="229">
         <v>1</v>
       </c>
-      <c r="F23" s="611"/>
+      <c r="F23" s="632"/>
       <c r="I23" s="223"/>
-      <c r="O23" s="614"/>
-      <c r="Q23" s="616" t="s">
+      <c r="O23" s="670"/>
+      <c r="Q23" s="672" t="s">
         <v>145</v>
       </c>
       <c r="T23" s="17"/>
       <c r="U23" s="441" t="s">
         <v>44</v>
       </c>
-      <c r="V23" s="652"/>
+      <c r="V23" s="601"/>
       <c r="W23" s="148"/>
       <c r="X23" s="450" t="s">
         <v>189</v>
       </c>
-      <c r="Y23" s="649"/>
+      <c r="Y23" s="645"/>
       <c r="Z23" s="17"/>
       <c r="AA23" s="10"/>
       <c r="AB23" s="436"/>
@@ -8328,13 +8328,13 @@
       <c r="AG23" s="6"/>
       <c r="AH23" s="6"/>
       <c r="AI23" s="6"/>
-      <c r="AJ23" s="621"/>
+      <c r="AJ23" s="641"/>
       <c r="AK23" s="261"/>
       <c r="AL23" s="80" t="s">
         <v>516</v>
       </c>
       <c r="AM23" s="305"/>
-      <c r="AN23" s="632"/>
+      <c r="AN23" s="627"/>
     </row>
     <row r="24" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="461" t="s">
@@ -8352,23 +8352,23 @@
       <c r="E24" s="457">
         <v>1</v>
       </c>
-      <c r="F24" s="611"/>
+      <c r="F24" s="632"/>
       <c r="G24" s="61" t="s">
         <v>499</v>
       </c>
       <c r="I24" s="223"/>
-      <c r="O24" s="614"/>
-      <c r="Q24" s="617"/>
+      <c r="O24" s="670"/>
+      <c r="Q24" s="673"/>
       <c r="T24" s="17"/>
       <c r="U24" s="231" t="s">
         <v>44</v>
       </c>
-      <c r="V24" s="652"/>
+      <c r="V24" s="601"/>
       <c r="W24" s="148"/>
       <c r="X24" s="450" t="s">
         <v>186</v>
       </c>
-      <c r="Y24" s="649"/>
+      <c r="Y24" s="645"/>
       <c r="Z24" s="17"/>
       <c r="AA24" s="10"/>
       <c r="AB24" s="436"/>
@@ -8387,12 +8387,12 @@
         <v>472</v>
       </c>
       <c r="AM24" s="305"/>
-      <c r="AN24" s="632"/>
+      <c r="AN24" s="627"/>
     </row>
     <row r="25" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F25" s="611"/>
+      <c r="F25" s="632"/>
       <c r="I25" s="223"/>
-      <c r="O25" s="614"/>
+      <c r="O25" s="670"/>
       <c r="P25" s="208" t="s">
         <v>284</v>
       </c>
@@ -8405,12 +8405,12 @@
       <c r="U25" s="421" t="s">
         <v>44</v>
       </c>
-      <c r="V25" s="653"/>
+      <c r="V25" s="602"/>
       <c r="W25" s="148"/>
       <c r="X25" s="450" t="s">
         <v>190</v>
       </c>
-      <c r="Y25" s="649"/>
+      <c r="Y25" s="645"/>
       <c r="Z25" s="17"/>
       <c r="AA25" s="10"/>
       <c r="AB25" s="436"/>
@@ -8427,7 +8427,7 @@
       <c r="AK25" s="142"/>
       <c r="AL25" s="6"/>
       <c r="AM25" s="305"/>
-      <c r="AN25" s="632"/>
+      <c r="AN25" s="627"/>
     </row>
     <row r="26" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="235" t="s">
@@ -8445,17 +8445,17 @@
       <c r="E26" s="395">
         <v>1</v>
       </c>
-      <c r="F26" s="611"/>
+      <c r="F26" s="632"/>
       <c r="G26" s="346" t="s">
         <v>496</v>
       </c>
       <c r="I26" s="223"/>
-      <c r="O26" s="614"/>
-      <c r="P26" s="634" t="s">
+      <c r="O26" s="670"/>
+      <c r="P26" s="629" t="s">
         <v>536</v>
       </c>
-      <c r="Q26" s="635"/>
-      <c r="R26" s="608" t="s">
+      <c r="Q26" s="630"/>
+      <c r="R26" s="666" t="s">
         <v>545</v>
       </c>
       <c r="T26" s="182"/>
@@ -8467,7 +8467,7 @@
       <c r="X26" s="450" t="s">
         <v>182</v>
       </c>
-      <c r="Y26" s="649"/>
+      <c r="Y26" s="645"/>
       <c r="Z26" s="17"/>
       <c r="AA26" s="10"/>
       <c r="AB26" s="436"/>
@@ -8494,7 +8494,7 @@
       <c r="AM26" s="463" t="s">
         <v>465</v>
       </c>
-      <c r="AN26" s="632"/>
+      <c r="AN26" s="627"/>
     </row>
     <row r="27" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="21" t="s">
@@ -8506,13 +8506,13 @@
       <c r="E27" s="270" t="s">
         <v>44</v>
       </c>
-      <c r="F27" s="612"/>
+      <c r="F27" s="668"/>
       <c r="G27" s="61" t="s">
         <v>554</v>
       </c>
       <c r="I27" s="224"/>
-      <c r="O27" s="615"/>
-      <c r="R27" s="609"/>
+      <c r="O27" s="671"/>
+      <c r="R27" s="667"/>
       <c r="S27" s="442" t="s">
         <v>54</v>
       </c>
@@ -8525,7 +8525,7 @@
       <c r="X27" s="450" t="s">
         <v>540</v>
       </c>
-      <c r="Y27" s="650"/>
+      <c r="Y27" s="646"/>
       <c r="Z27" s="163"/>
       <c r="AA27" s="13"/>
       <c r="AB27" s="437"/>
@@ -8542,10 +8542,48 @@
       <c r="AM27" s="397" t="s">
         <v>325</v>
       </c>
-      <c r="AN27" s="633"/>
+      <c r="AN27" s="628"/>
     </row>
   </sheetData>
   <mergeCells count="54">
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="R18:R19"/>
+    <mergeCell ref="R26:R27"/>
+    <mergeCell ref="F2:F27"/>
+    <mergeCell ref="O10:O27"/>
+    <mergeCell ref="Q20:Q21"/>
+    <mergeCell ref="Q23:Q24"/>
+    <mergeCell ref="G14:J14"/>
+    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="AI6:AI10"/>
+    <mergeCell ref="AF12:AF15"/>
+    <mergeCell ref="AG7:AG12"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="S9:S12"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="AD12:AD15"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="AN1:AN27"/>
+    <mergeCell ref="P26:Q26"/>
+    <mergeCell ref="Q2:Q3"/>
+    <mergeCell ref="M2:M9"/>
+    <mergeCell ref="O2:O9"/>
+    <mergeCell ref="P10:P13"/>
+    <mergeCell ref="AK6:AK7"/>
+    <mergeCell ref="AM12:AM15"/>
+    <mergeCell ref="AF18:AF19"/>
+    <mergeCell ref="AJ18:AJ19"/>
+    <mergeCell ref="Y1:Y27"/>
+    <mergeCell ref="AJ22:AJ23"/>
+    <mergeCell ref="AK9:AK10"/>
+    <mergeCell ref="AD3:AD4"/>
+    <mergeCell ref="S2:S3"/>
+    <mergeCell ref="R2:R3"/>
     <mergeCell ref="V21:V25"/>
     <mergeCell ref="U18:U20"/>
     <mergeCell ref="C2:C3"/>
@@ -8562,44 +8600,6 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="B4:B5"/>
-    <mergeCell ref="AN1:AN27"/>
-    <mergeCell ref="P26:Q26"/>
-    <mergeCell ref="Q2:Q3"/>
-    <mergeCell ref="M2:M9"/>
-    <mergeCell ref="O2:O9"/>
-    <mergeCell ref="P10:P13"/>
-    <mergeCell ref="AK6:AK7"/>
-    <mergeCell ref="AM12:AM15"/>
-    <mergeCell ref="AF18:AF19"/>
-    <mergeCell ref="AJ18:AJ19"/>
-    <mergeCell ref="Y1:Y27"/>
-    <mergeCell ref="AJ22:AJ23"/>
-    <mergeCell ref="AK9:AK10"/>
-    <mergeCell ref="AD3:AD4"/>
-    <mergeCell ref="S2:S3"/>
-    <mergeCell ref="R2:R3"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="AI6:AI10"/>
-    <mergeCell ref="AF12:AF15"/>
-    <mergeCell ref="AG7:AG12"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="S9:S12"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="AD12:AD15"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="R18:R19"/>
-    <mergeCell ref="R26:R27"/>
-    <mergeCell ref="F2:F27"/>
-    <mergeCell ref="O10:O27"/>
-    <mergeCell ref="Q20:Q21"/>
-    <mergeCell ref="Q23:Q24"/>
-    <mergeCell ref="G14:J14"/>
-    <mergeCell ref="G13:J13"/>
-    <mergeCell ref="H12:K12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8636,12 +8636,12 @@
       <c r="B1" s="594" t="s">
         <v>316</v>
       </c>
-      <c r="C1" s="618"/>
+      <c r="C1" s="674"/>
       <c r="D1" s="208"/>
       <c r="J1" s="594" t="s">
         <v>70</v>
       </c>
-      <c r="K1" s="618"/>
+      <c r="K1" s="674"/>
       <c r="L1" s="199" t="s">
         <v>336</v>
       </c>
@@ -8975,8 +8975,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB54FD83-008D-4F8B-87AC-83E7F70047CB}">
   <dimension ref="A1:AK31"/>
   <sheetViews>
-    <sheetView topLeftCell="N12" workbookViewId="0">
-      <selection activeCell="X28" sqref="X28"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="AH17" sqref="AH17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9043,7 +9043,7 @@
       <c r="P1" s="419" t="s">
         <v>404</v>
       </c>
-      <c r="Q1" s="684" t="s">
+      <c r="Q1" s="697" t="s">
         <v>181</v>
       </c>
       <c r="R1" s="100" t="s">
@@ -9067,7 +9067,7 @@
       <c r="AA1" s="546" t="s">
         <v>446</v>
       </c>
-      <c r="AB1" s="691" t="s">
+      <c r="AB1" s="704" t="s">
         <v>608</v>
       </c>
       <c r="AC1" s="99" t="s">
@@ -9088,32 +9088,32 @@
       </c>
     </row>
     <row r="2" spans="1:37" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="697">
+      <c r="A2" s="684">
         <f ca="1">TODAY()</f>
         <v>45282</v>
       </c>
-      <c r="B2" s="699" t="s">
+      <c r="B2" s="686" t="s">
         <v>386</v>
       </c>
-      <c r="C2" s="636" t="s">
+      <c r="C2" s="606" t="s">
         <v>363</v>
       </c>
-      <c r="D2" s="701" t="s">
+      <c r="D2" s="688" t="s">
         <v>103</v>
       </c>
-      <c r="E2" s="703" t="s">
+      <c r="E2" s="690" t="s">
         <v>65</v>
       </c>
       <c r="F2" s="195" t="s">
         <v>220</v>
       </c>
-      <c r="G2" s="604" t="s">
+      <c r="G2" s="650" t="s">
         <v>378</v>
       </c>
       <c r="H2" s="210" t="s">
         <v>220</v>
       </c>
-      <c r="I2" s="688" t="s">
+      <c r="I2" s="701" t="s">
         <v>103</v>
       </c>
       <c r="J2" s="417" t="s">
@@ -9137,14 +9137,14 @@
       <c r="P2" s="420">
         <v>40</v>
       </c>
-      <c r="Q2" s="685"/>
+      <c r="Q2" s="698"/>
       <c r="R2" s="21">
         <f>R7+R20</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S2" s="21">
         <f>S7+S20</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T2" s="176">
         <f>SUM(T4:T16)</f>
@@ -9162,7 +9162,7 @@
         <f>IF((Z2+T2)&gt;0,0,-1)</f>
         <v>0</v>
       </c>
-      <c r="AB2" s="692"/>
+      <c r="AB2" s="705"/>
       <c r="AC2" s="35"/>
       <c r="AH2" s="6" t="s">
         <v>617</v>
@@ -9178,14 +9178,14 @@
       </c>
     </row>
     <row r="3" spans="1:37" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="698"/>
-      <c r="B3" s="700"/>
-      <c r="C3" s="637"/>
-      <c r="D3" s="702"/>
-      <c r="E3" s="704"/>
-      <c r="G3" s="605"/>
+      <c r="A3" s="685"/>
+      <c r="B3" s="687"/>
+      <c r="C3" s="607"/>
+      <c r="D3" s="689"/>
+      <c r="E3" s="691"/>
+      <c r="G3" s="651"/>
       <c r="H3" s="6"/>
-      <c r="I3" s="689"/>
+      <c r="I3" s="702"/>
       <c r="K3" s="24">
         <v>2</v>
       </c>
@@ -9200,7 +9200,7 @@
       <c r="V3" s="492"/>
       <c r="W3" s="6"/>
       <c r="X3" s="492"/>
-      <c r="AB3" s="692"/>
+      <c r="AB3" s="705"/>
       <c r="AC3" s="35"/>
       <c r="AE3" s="100" t="s">
         <v>603</v>
@@ -9228,10 +9228,10 @@
         <v>387</v>
       </c>
       <c r="B4" s="247"/>
-      <c r="C4" s="705" t="s">
+      <c r="C4" s="692" t="s">
         <v>178</v>
       </c>
-      <c r="I4" s="689"/>
+      <c r="I4" s="702"/>
       <c r="R4" s="493" t="s">
         <v>603</v>
       </c>
@@ -9243,7 +9243,7 @@
       <c r="V4" s="492"/>
       <c r="W4" s="6"/>
       <c r="X4" s="492"/>
-      <c r="AB4" s="692"/>
+      <c r="AB4" s="705"/>
       <c r="AC4" s="35"/>
       <c r="AE4" s="20"/>
       <c r="AF4" s="100" t="s">
@@ -9273,7 +9273,7 @@
       <c r="B5" s="100" t="s">
         <v>363</v>
       </c>
-      <c r="C5" s="706"/>
+      <c r="C5" s="693"/>
       <c r="D5" s="226" t="s">
         <v>103</v>
       </c>
@@ -9289,7 +9289,7 @@
       <c r="H5" s="210" t="s">
         <v>220</v>
       </c>
-      <c r="I5" s="689"/>
+      <c r="I5" s="702"/>
       <c r="J5" s="418" t="s">
         <v>272</v>
       </c>
@@ -9316,7 +9316,7 @@
       <c r="V5" s="490"/>
       <c r="W5" s="6"/>
       <c r="X5" s="490"/>
-      <c r="AB5" s="692"/>
+      <c r="AB5" s="705"/>
       <c r="AC5" s="2" t="s">
         <v>606</v>
       </c>
@@ -9329,31 +9329,31 @@
       <c r="AK5" s="490"/>
     </row>
     <row r="6" spans="1:37" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="694" t="s">
+      <c r="A6" s="681" t="s">
         <v>289</v>
       </c>
       <c r="B6" s="105" t="s">
         <v>199</v>
       </c>
-      <c r="C6" s="619"/>
-      <c r="D6" s="620"/>
+      <c r="C6" s="652"/>
+      <c r="D6" s="653"/>
       <c r="E6" s="96">
         <v>1</v>
       </c>
       <c r="G6" s="590"/>
-      <c r="I6" s="689"/>
+      <c r="I6" s="702"/>
       <c r="P6" s="61" t="s">
         <v>606</v>
       </c>
       <c r="R6" s="64">
         <f>R7-SUM(X2:X10)+R11</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S6" s="64">
         <f>S7-S12-SUM(V2:V10)</f>
         <v>0</v>
       </c>
-      <c r="AB6" s="692"/>
+      <c r="AB6" s="705"/>
       <c r="AC6" s="35"/>
       <c r="AE6" s="64">
         <f>AE7-SUM(AI1:AI10)+AE11</f>
@@ -9361,14 +9361,14 @@
       </c>
       <c r="AF6" s="64">
         <f>AF7-SUM(AK2:AK10)+AF11</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AI6" s="112"/>
       <c r="AJ6" s="6"/>
       <c r="AK6" s="554"/>
     </row>
     <row r="7" spans="1:37" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="695"/>
+      <c r="A7" s="682"/>
       <c r="B7" s="100" t="s">
         <v>155</v>
       </c>
@@ -9379,7 +9379,7 @@
         <v>136</v>
       </c>
       <c r="G7" s="590"/>
-      <c r="I7" s="689"/>
+      <c r="I7" s="702"/>
       <c r="M7" s="16" t="s">
         <v>353</v>
       </c>
@@ -9397,21 +9397,21 @@
       </c>
       <c r="R7" s="24">
         <f>3-R11</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S7" s="24">
         <f>3-S11</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U7" s="6"/>
       <c r="V7" s="491"/>
       <c r="W7" s="6" t="s">
-        <v>518</v>
+        <v>483</v>
       </c>
       <c r="X7" s="491">
         <v>1</v>
       </c>
-      <c r="AB7" s="692"/>
+      <c r="AB7" s="705"/>
       <c r="AC7" s="99" t="s">
         <v>607</v>
       </c>
@@ -9424,7 +9424,7 @@
       </c>
       <c r="AF7" s="300">
         <f>8-AF11</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AH7" s="6" t="s">
         <v>246</v>
@@ -9436,7 +9436,7 @@
       <c r="AK7" s="491"/>
     </row>
     <row r="8" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="696"/>
+      <c r="A8" s="683"/>
       <c r="B8" s="216" t="s">
         <v>28</v>
       </c>
@@ -9445,13 +9445,21 @@
         <v>3</v>
       </c>
       <c r="G8" s="590"/>
-      <c r="I8" s="689"/>
+      <c r="I8" s="702"/>
       <c r="N8" s="80"/>
-      <c r="U8" s="6"/>
-      <c r="V8" s="24"/>
-      <c r="W8" s="6"/>
-      <c r="X8" s="489"/>
-      <c r="AB8" s="692"/>
+      <c r="U8" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="V8" s="24">
+        <v>1</v>
+      </c>
+      <c r="W8" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="X8" s="492">
+        <v>1</v>
+      </c>
+      <c r="AB8" s="705"/>
       <c r="AC8" s="544"/>
       <c r="AH8" s="6"/>
       <c r="AI8" s="578"/>
@@ -9477,7 +9485,7 @@
       </c>
       <c r="G9" s="590"/>
       <c r="H9" s="6"/>
-      <c r="I9" s="689"/>
+      <c r="I9" s="702"/>
       <c r="M9" s="19" t="s">
         <v>535</v>
       </c>
@@ -9485,7 +9493,7 @@
       <c r="U9" s="6"/>
       <c r="V9" s="24"/>
       <c r="X9" s="489"/>
-      <c r="AB9" s="692"/>
+      <c r="AB9" s="705"/>
       <c r="AC9" s="544"/>
       <c r="AE9" s="20"/>
       <c r="AF9" s="20"/>
@@ -9516,7 +9524,7 @@
         <v>37</v>
       </c>
       <c r="G10" s="590"/>
-      <c r="I10" s="689"/>
+      <c r="I10" s="702"/>
       <c r="J10" s="24" t="s">
         <v>378</v>
       </c>
@@ -9531,7 +9539,7 @@
       <c r="V10" s="492"/>
       <c r="W10" s="6"/>
       <c r="X10" s="489"/>
-      <c r="AB10" s="692"/>
+      <c r="AB10" s="705"/>
       <c r="AC10" s="544"/>
       <c r="AE10" s="20"/>
       <c r="AF10" s="20"/>
@@ -9541,12 +9549,8 @@
       <c r="AI10" s="579">
         <v>2</v>
       </c>
-      <c r="AJ10" s="6" t="s">
-        <v>253</v>
-      </c>
-      <c r="AK10" s="492">
-        <v>1</v>
-      </c>
+      <c r="AJ10" s="6"/>
+      <c r="AK10" s="492"/>
     </row>
     <row r="11" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="99" t="s">
@@ -9562,7 +9566,7 @@
         <v>269</v>
       </c>
       <c r="G11" s="590"/>
-      <c r="I11" s="689"/>
+      <c r="I11" s="702"/>
       <c r="J11" s="24" t="s">
         <v>195</v>
       </c>
@@ -9583,18 +9587,18 @@
         <v>44</v>
       </c>
       <c r="R11" s="24">
+        <v>1</v>
+      </c>
+      <c r="S11" s="24">
         <v>2</v>
       </c>
-      <c r="S11" s="24">
-        <v>3</v>
-      </c>
-      <c r="U11" s="681" t="s">
+      <c r="U11" s="694" t="s">
         <v>569</v>
       </c>
-      <c r="V11" s="682"/>
-      <c r="W11" s="682"/>
-      <c r="X11" s="683"/>
-      <c r="AB11" s="693"/>
+      <c r="V11" s="695"/>
+      <c r="W11" s="695"/>
+      <c r="X11" s="696"/>
+      <c r="AB11" s="706"/>
       <c r="AC11" s="99" t="s">
         <v>609</v>
       </c>
@@ -9605,15 +9609,15 @@
         <v>1</v>
       </c>
       <c r="AF11" s="24">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AG11" s="435"/>
-      <c r="AH11" s="681" t="s">
+      <c r="AH11" s="694" t="s">
         <v>628</v>
       </c>
-      <c r="AI11" s="682"/>
-      <c r="AJ11" s="682"/>
-      <c r="AK11" s="683"/>
+      <c r="AI11" s="695"/>
+      <c r="AJ11" s="695"/>
+      <c r="AK11" s="696"/>
     </row>
     <row r="12" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="231" t="s">
@@ -9624,7 +9628,7 @@
         <v>3</v>
       </c>
       <c r="G12" s="590"/>
-      <c r="I12" s="689"/>
+      <c r="I12" s="702"/>
       <c r="J12" s="24" t="s">
         <v>526</v>
       </c>
@@ -9657,7 +9661,7 @@
       </c>
       <c r="D13" s="20"/>
       <c r="G13" s="590"/>
-      <c r="I13" s="689"/>
+      <c r="I13" s="702"/>
       <c r="J13" s="108" t="s">
         <v>559</v>
       </c>
@@ -9701,7 +9705,7 @@
       <c r="H14" s="210" t="s">
         <v>220</v>
       </c>
-      <c r="I14" s="689"/>
+      <c r="I14" s="702"/>
       <c r="U14" s="67" t="s">
         <v>81</v>
       </c>
@@ -9728,7 +9732,7 @@
       <c r="H15" s="276">
         <v>0</v>
       </c>
-      <c r="I15" s="689"/>
+      <c r="I15" s="702"/>
       <c r="J15" s="108" t="s">
         <v>154</v>
       </c>
@@ -9759,7 +9763,7 @@
       <c r="D16" s="2" t="s">
         <v>501</v>
       </c>
-      <c r="I16" s="689"/>
+      <c r="I16" s="702"/>
       <c r="K16" s="100" t="s">
         <v>44</v>
       </c>
@@ -9803,7 +9807,7 @@
       <c r="G17" s="2" t="s">
         <v>432</v>
       </c>
-      <c r="I17" s="689"/>
+      <c r="I17" s="702"/>
       <c r="L17" s="2" t="s">
         <v>435</v>
       </c>
@@ -9821,13 +9825,13 @@
     </row>
     <row r="18" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G18" s="16"/>
-      <c r="I18" s="689"/>
+      <c r="I18" s="702"/>
       <c r="L18" s="16"/>
       <c r="M18" s="21"/>
-      <c r="O18" s="686" t="s">
+      <c r="O18" s="699" t="s">
         <v>527</v>
       </c>
-      <c r="P18" s="687"/>
+      <c r="P18" s="700"/>
       <c r="Q18" s="127" t="s">
         <v>44</v>
       </c>
@@ -9853,7 +9857,7 @@
       </c>
     </row>
     <row r="19" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I19" s="689"/>
+      <c r="I19" s="702"/>
       <c r="M19" s="21" t="s">
         <v>434</v>
       </c>
@@ -9889,7 +9893,7 @@
       <c r="G20" s="2" t="s">
         <v>432</v>
       </c>
-      <c r="I20" s="689"/>
+      <c r="I20" s="702"/>
       <c r="K20" s="19" t="s">
         <v>431</v>
       </c>
@@ -9924,7 +9928,7 @@
       </c>
     </row>
     <row r="21" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I21" s="689"/>
+      <c r="I21" s="702"/>
       <c r="M21" s="220" t="s">
         <v>418</v>
       </c>
@@ -9958,7 +9962,7 @@
       <c r="G22" s="2" t="s">
         <v>432</v>
       </c>
-      <c r="I22" s="689"/>
+      <c r="I22" s="702"/>
       <c r="P22" s="99" t="s">
         <v>605</v>
       </c>
@@ -9973,7 +9977,7 @@
       <c r="E23" s="288" t="s">
         <v>44</v>
       </c>
-      <c r="I23" s="689"/>
+      <c r="I23" s="702"/>
       <c r="Q23" s="24">
         <f>SUM(V23:V31)</f>
         <v>5</v>
@@ -9990,7 +9994,7 @@
       </c>
     </row>
     <row r="24" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I24" s="689"/>
+      <c r="I24" s="702"/>
       <c r="U24" s="35"/>
       <c r="V24" s="533">
         <v>0</v>
@@ -10018,7 +10022,7 @@
       <c r="H25" s="195" t="s">
         <v>270</v>
       </c>
-      <c r="I25" s="689"/>
+      <c r="I25" s="702"/>
       <c r="J25" s="418" t="s">
         <v>273</v>
       </c>
@@ -10063,7 +10067,7 @@
       <c r="H26" s="19" t="s">
         <v>220</v>
       </c>
-      <c r="I26" s="689"/>
+      <c r="I26" s="702"/>
       <c r="K26" s="24">
         <v>15</v>
       </c>
@@ -10098,7 +10102,7 @@
       </c>
     </row>
     <row r="27" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I27" s="689"/>
+      <c r="I27" s="702"/>
       <c r="O27" s="2" t="s">
         <v>99</v>
       </c>
@@ -10125,7 +10129,7 @@
       <c r="E28" s="219">
         <v>2</v>
       </c>
-      <c r="I28" s="689"/>
+      <c r="I28" s="702"/>
       <c r="Q28" s="6"/>
       <c r="R28" s="112"/>
       <c r="T28" s="142"/>
@@ -10147,7 +10151,7 @@
       <c r="H29" s="195" t="s">
         <v>271</v>
       </c>
-      <c r="I29" s="690"/>
+      <c r="I29" s="703"/>
       <c r="J29" s="330"/>
       <c r="L29" s="96" t="s">
         <v>277</v>
@@ -10205,6 +10209,12 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="AH11:AK11"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="U11:X11"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="I2:I29"/>
+    <mergeCell ref="AB1:AB11"/>
     <mergeCell ref="C13:C14"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="G5:G14"/>
@@ -10217,12 +10227,6 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="C2:C3"/>
-    <mergeCell ref="AH11:AK11"/>
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="U11:X11"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="I2:I29"/>
-    <mergeCell ref="AB1:AB11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10232,8 +10236,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2029A93E-B53C-4201-9F17-439C144F3CF1}">
   <dimension ref="A1:AP37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="AP11" sqref="AP11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10329,14 +10333,14 @@
         <f ca="1">TODAY()</f>
         <v>45282</v>
       </c>
-      <c r="T1" s="726"/>
+      <c r="T1" s="730"/>
       <c r="U1" s="142"/>
       <c r="V1" s="142"/>
       <c r="W1" s="6"/>
-      <c r="X1" s="710" t="s">
+      <c r="X1" s="714" t="s">
         <v>450</v>
       </c>
-      <c r="Y1" s="711"/>
+      <c r="Y1" s="715"/>
       <c r="Z1" s="311">
         <f>68-(W8+Y3+X3+U3)</f>
         <v>0</v>
@@ -10352,21 +10356,21 @@
       <c r="AD1" s="307" t="s">
         <v>44</v>
       </c>
-      <c r="AE1" s="712" t="s">
+      <c r="AE1" s="716" t="s">
         <v>191</v>
       </c>
-      <c r="AF1" s="713"/>
-      <c r="AG1" s="714"/>
-      <c r="AH1" s="715" t="s">
+      <c r="AF1" s="717"/>
+      <c r="AG1" s="718"/>
+      <c r="AH1" s="719" t="s">
         <v>297</v>
       </c>
-      <c r="AI1" s="716"/>
-      <c r="AJ1" s="717"/>
-      <c r="AK1" s="707" t="s">
+      <c r="AI1" s="720"/>
+      <c r="AJ1" s="721"/>
+      <c r="AK1" s="711" t="s">
         <v>453</v>
       </c>
-      <c r="AL1" s="708"/>
-      <c r="AM1" s="709"/>
+      <c r="AL1" s="712"/>
+      <c r="AM1" s="713"/>
       <c r="AP1" s="142"/>
     </row>
     <row r="2" spans="1:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10379,7 +10383,7 @@
       </c>
       <c r="I2" s="531">
         <f>B31-SUM(I4:I37)</f>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="K2" s="16" t="s">
         <v>235</v>
@@ -10387,19 +10391,19 @@
       <c r="L2" s="324">
         <v>-3</v>
       </c>
-      <c r="M2" s="718">
+      <c r="M2" s="722">
         <f>SUM(M5:M30)</f>
-        <v>1</v>
-      </c>
-      <c r="N2" s="720">
+        <v>2</v>
+      </c>
+      <c r="N2" s="724">
         <f>SUM(N4:N29)</f>
         <v>10</v>
       </c>
-      <c r="O2" s="722">
+      <c r="O2" s="726">
         <f>SUM(O4:O29)</f>
-        <v>9</v>
-      </c>
-      <c r="P2" s="628">
+        <v>11</v>
+      </c>
+      <c r="P2" s="657">
         <f>SUM(N30:N37)* (-1)</f>
         <v>-3</v>
       </c>
@@ -10412,14 +10416,14 @@
       <c r="S2" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="T2" s="727"/>
+      <c r="T2" s="731"/>
       <c r="U2" s="566" t="s">
         <v>266</v>
       </c>
       <c r="V2" s="505" t="s">
         <v>221</v>
       </c>
-      <c r="W2" s="724" t="s">
+      <c r="W2" s="728" t="s">
         <v>238</v>
       </c>
       <c r="X2" s="506" t="s">
@@ -10488,10 +10492,10 @@
         <f>V3+X3+Y3+U3</f>
         <v>68</v>
       </c>
-      <c r="M3" s="719"/>
-      <c r="N3" s="721"/>
-      <c r="O3" s="723"/>
-      <c r="P3" s="629"/>
+      <c r="M3" s="723"/>
+      <c r="N3" s="725"/>
+      <c r="O3" s="727"/>
+      <c r="P3" s="658"/>
       <c r="Q3" s="176">
         <f>(M2+N2)-Y3</f>
         <v>0</v>
@@ -10499,23 +10503,23 @@
       <c r="S3" s="161" t="s">
         <v>248</v>
       </c>
-      <c r="T3" s="728"/>
+      <c r="T3" s="732"/>
       <c r="U3" s="567">
         <f>SUM(U4:U29)</f>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="V3" s="507">
         <f>SUM(V4:V29)</f>
         <v>37</v>
       </c>
-      <c r="W3" s="725"/>
+      <c r="W3" s="729"/>
       <c r="X3" s="508">
         <f t="shared" ref="X3:AC3" si="0">SUM(X4:X29)</f>
         <v>8</v>
       </c>
       <c r="Y3" s="508">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="Z3" s="59">
         <f t="shared" si="0"/>
@@ -10523,15 +10527,15 @@
       </c>
       <c r="AA3" s="66">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="AB3" s="66">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="AC3" s="66">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="AD3" s="66">
         <f t="shared" ref="AD3:AM3" si="1">SUM(AD4:AD29)</f>
@@ -10539,7 +10543,7 @@
       </c>
       <c r="AE3" s="66">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="AF3" s="66">
         <f t="shared" si="1"/>
@@ -10551,7 +10555,7 @@
       </c>
       <c r="AH3" s="66">
         <f>SUM(AH4:AH29)</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="AI3" s="383">
         <f t="shared" si="1"/>
@@ -10559,19 +10563,19 @@
       </c>
       <c r="AJ3" s="100">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AK3" s="100">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="AL3" s="316">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="AM3" s="317">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="AP3" s="142"/>
     </row>
@@ -10608,7 +10612,7 @@
         <f>AC4</f>
         <v>0</v>
       </c>
-      <c r="P4" s="730" t="s">
+      <c r="P4" s="708" t="s">
         <v>200</v>
       </c>
       <c r="Q4" s="20"/>
@@ -10690,7 +10694,7 @@
         <f>AC5</f>
         <v>0</v>
       </c>
-      <c r="P5" s="731"/>
+      <c r="P5" s="709"/>
       <c r="Q5" s="20"/>
       <c r="R5" s="2" t="s">
         <v>346</v>
@@ -10766,6 +10770,9 @@
         <v>49</v>
       </c>
       <c r="G6" s="203"/>
+      <c r="I6" s="24">
+        <v>1</v>
+      </c>
       <c r="J6" s="112"/>
       <c r="L6" s="402" t="s">
         <v>311</v>
@@ -10778,9 +10785,9 @@
       </c>
       <c r="O6" s="298">
         <f>AC6</f>
-        <v>0</v>
-      </c>
-      <c r="P6" s="731"/>
+        <v>1</v>
+      </c>
+      <c r="P6" s="709"/>
       <c r="Q6" s="19" t="s">
         <v>341</v>
       </c>
@@ -10809,27 +10816,27 @@
       <c r="Z6" s="301"/>
       <c r="AA6" s="117">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB6" s="295">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC6" s="295">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD6" s="295">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AE6" s="299">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF6" s="305"/>
       <c r="AG6" s="301"/>
       <c r="AH6" s="301">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI6" s="345">
         <v>0</v>
@@ -10837,17 +10844,19 @@
       <c r="AJ6" s="158"/>
       <c r="AK6" s="313">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL6" s="314">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM6" s="315">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="AN6" s="6"/>
+        <v>1</v>
+      </c>
+      <c r="AN6" s="6" t="s">
+        <v>483</v>
+      </c>
       <c r="AO6" s="533" t="s">
         <v>571</v>
       </c>
@@ -10878,7 +10887,7 @@
         <f t="shared" ref="O7:O37" si="10">AC7</f>
         <v>0</v>
       </c>
-      <c r="P7" s="731"/>
+      <c r="P7" s="709"/>
       <c r="Q7" s="20"/>
       <c r="R7" s="2" t="s">
         <v>341</v>
@@ -10990,7 +10999,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P8" s="731"/>
+      <c r="P8" s="709"/>
       <c r="Q8" s="21" t="s">
         <v>237</v>
       </c>
@@ -11077,7 +11086,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P9" s="731"/>
+      <c r="P9" s="709"/>
       <c r="Q9" s="21" t="s">
         <v>341</v>
       </c>
@@ -11179,7 +11188,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P10" s="731"/>
+      <c r="P10" s="709"/>
       <c r="Q10" s="20"/>
       <c r="R10" s="2" t="s">
         <v>346</v>
@@ -11265,7 +11274,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P11" s="731"/>
+      <c r="P11" s="709"/>
       <c r="Q11" s="21" t="s">
         <v>341</v>
       </c>
@@ -11328,7 +11337,7 @@
       <c r="AP11" s="142"/>
     </row>
     <row r="12" spans="1:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="666" t="s">
+      <c r="A12" s="617" t="s">
         <v>55</v>
       </c>
       <c r="B12" s="30">
@@ -11337,7 +11346,7 @@
       <c r="C12" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E12" s="616" t="s">
+      <c r="E12" s="672" t="s">
         <v>57</v>
       </c>
       <c r="G12" s="266"/>
@@ -11359,7 +11368,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P12" s="731"/>
+      <c r="P12" s="709"/>
       <c r="Q12" s="21" t="s">
         <v>341</v>
       </c>
@@ -11434,14 +11443,14 @@
       </c>
     </row>
     <row r="13" spans="1:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="668"/>
+      <c r="A13" s="619"/>
       <c r="B13" s="153">
         <v>12</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E13" s="617"/>
+      <c r="E13" s="673"/>
       <c r="F13" s="176">
         <v>0</v>
       </c>
@@ -11465,7 +11474,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P13" s="731"/>
+      <c r="P13" s="709"/>
       <c r="Q13" s="21" t="s">
         <v>341</v>
       </c>
@@ -11545,7 +11554,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P14" s="731"/>
+      <c r="P14" s="709"/>
       <c r="Q14" s="20"/>
       <c r="R14" s="204" t="s">
         <v>345</v>
@@ -11644,7 +11653,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P15" s="731"/>
+      <c r="P15" s="709"/>
       <c r="Q15" s="20"/>
       <c r="R15" s="204" t="s">
         <v>345</v>
@@ -11734,7 +11743,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P16" s="731"/>
+      <c r="P16" s="709"/>
       <c r="Q16" s="21" t="s">
         <v>341</v>
       </c>
@@ -11836,7 +11845,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P17" s="731"/>
+      <c r="P17" s="709"/>
       <c r="Q17" s="20"/>
       <c r="R17" s="2" t="s">
         <v>347</v>
@@ -11935,7 +11944,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P18" s="731"/>
+      <c r="P18" s="709"/>
       <c r="Q18" s="21" t="s">
         <v>341</v>
       </c>
@@ -12022,7 +12031,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P19" s="731"/>
+      <c r="P19" s="709"/>
       <c r="Q19" s="20"/>
       <c r="R19" s="2" t="s">
         <v>340</v>
@@ -12126,11 +12135,11 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P20" s="732"/>
+      <c r="P20" s="710"/>
       <c r="Q20" s="594" t="s">
         <v>341</v>
       </c>
-      <c r="R20" s="618"/>
+      <c r="R20" s="674"/>
       <c r="S20" s="563" t="s">
         <v>86</v>
       </c>
@@ -12376,7 +12385,7 @@
     </row>
     <row r="23" spans="1:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="24"/>
-      <c r="E23" s="673" t="s">
+      <c r="E23" s="624" t="s">
         <v>293</v>
       </c>
       <c r="F23" s="184"/>
@@ -12478,29 +12487,31 @@
       <c r="C24" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="E24" s="674"/>
+      <c r="E24" s="625"/>
       <c r="F24" s="176"/>
       <c r="H24" s="42">
         <v>-1</v>
       </c>
-      <c r="I24" s="582"/>
+      <c r="I24" s="42">
+        <v>2</v>
+      </c>
       <c r="L24" s="400" t="s">
         <v>300</v>
       </c>
       <c r="M24" s="333">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N24" s="107">
         <v>0</v>
       </c>
       <c r="O24" s="298">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q24" s="594" t="s">
         <v>341</v>
       </c>
-      <c r="R24" s="618"/>
+      <c r="R24" s="674"/>
       <c r="S24" s="563" t="s">
         <v>253</v>
       </c>
@@ -12508,7 +12519,7 @@
         <v>4</v>
       </c>
       <c r="U24" s="526">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V24" s="515">
         <v>2</v>
@@ -12519,25 +12530,27 @@
       <c r="X24" s="26"/>
       <c r="Y24" s="577">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z24" s="301"/>
       <c r="AA24" s="117">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB24" s="295">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AC24" s="295">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD24" s="295">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="AE24" s="299"/>
+      <c r="AE24" s="299">
+        <v>1</v>
+      </c>
       <c r="AF24" s="107">
         <v>0</v>
       </c>
@@ -12546,21 +12559,23 @@
       </c>
       <c r="AH24" s="301">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI24" s="345"/>
-      <c r="AJ24" s="158"/>
+      <c r="AJ24" s="158">
+        <v>1</v>
+      </c>
       <c r="AK24" s="313">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL24" s="314">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM24" s="315">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN24" s="6" t="s">
         <v>518</v>
@@ -13127,10 +13142,10 @@
         <v>-1</v>
       </c>
       <c r="I32"/>
-      <c r="J32" s="669" t="s">
+      <c r="J32" s="620" t="s">
         <v>599</v>
       </c>
-      <c r="K32" s="729"/>
+      <c r="K32" s="707"/>
       <c r="L32" s="403"/>
       <c r="M32" s="537">
         <v>0</v>
@@ -13641,13 +13656,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="J32:K32"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="Q20:R20"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="Q24:R24"/>
-    <mergeCell ref="P4:P20"/>
     <mergeCell ref="AK1:AM1"/>
     <mergeCell ref="X1:Y1"/>
     <mergeCell ref="AE1:AG1"/>
@@ -13658,6 +13666,13 @@
     <mergeCell ref="P2:P3"/>
     <mergeCell ref="W2:W3"/>
     <mergeCell ref="T1:T3"/>
+    <mergeCell ref="J32:K32"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="Q20:R20"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="Q24:R24"/>
+    <mergeCell ref="P4:P20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -13725,7 +13740,7 @@
       <c r="V1" s="594" t="s">
         <v>71</v>
       </c>
-      <c r="W1" s="618"/>
+      <c r="W1" s="674"/>
       <c r="X1" s="62" t="s">
         <v>102</v>
       </c>
@@ -13744,7 +13759,7 @@
       <c r="AC1" s="116" t="s">
         <v>191</v>
       </c>
-      <c r="AD1" s="740" t="s">
+      <c r="AD1" s="747" t="s">
         <v>213</v>
       </c>
       <c r="AE1" s="116" t="s">
@@ -13761,10 +13776,10 @@
       <c r="E2" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="F2" s="739" t="s">
+      <c r="F2" s="778" t="s">
         <v>75</v>
       </c>
-      <c r="G2" s="767" t="s">
+      <c r="G2" s="735" t="s">
         <v>44</v>
       </c>
       <c r="H2" s="40" t="s">
@@ -13792,10 +13807,10 @@
       <c r="U2" s="60" t="s">
         <v>106</v>
       </c>
-      <c r="V2" s="710" t="s">
+      <c r="V2" s="714" t="s">
         <v>121</v>
       </c>
-      <c r="W2" s="711"/>
+      <c r="W2" s="715"/>
       <c r="X2" s="64" t="s">
         <v>110</v>
       </c>
@@ -13814,7 +13829,7 @@
       <c r="AC2" s="117" t="s">
         <v>99</v>
       </c>
-      <c r="AD2" s="741"/>
+      <c r="AD2" s="748"/>
       <c r="AE2" s="64" t="s">
         <v>99</v>
       </c>
@@ -13833,8 +13848,8 @@
       <c r="E3" s="39" t="s">
         <v>80</v>
       </c>
-      <c r="F3" s="670"/>
-      <c r="G3" s="768"/>
+      <c r="F3" s="621"/>
+      <c r="G3" s="736"/>
       <c r="H3" s="40" t="s">
         <v>81</v>
       </c>
@@ -13845,13 +13860,13 @@
         <v>82</v>
       </c>
       <c r="N3" s="44"/>
-      <c r="O3" s="777" t="s">
+      <c r="O3" s="745" t="s">
         <v>44</v>
       </c>
-      <c r="P3" s="759" t="s">
+      <c r="P3" s="766" t="s">
         <v>219</v>
       </c>
-      <c r="Q3" s="760"/>
+      <c r="Q3" s="767"/>
       <c r="S3" s="57" t="s">
         <v>220</v>
       </c>
@@ -13861,15 +13876,15 @@
       <c r="W3" s="59" t="s">
         <v>105</v>
       </c>
-      <c r="AD3" s="741"/>
+      <c r="AD3" s="748"/>
     </row>
     <row r="4" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G4" s="768"/>
+      <c r="G4" s="736"/>
       <c r="H4" s="6"/>
       <c r="L4" s="678" t="s">
         <v>83</v>
       </c>
-      <c r="O4" s="778"/>
+      <c r="O4" s="746"/>
       <c r="T4" s="55" t="s">
         <v>98</v>
       </c>
@@ -13883,8 +13898,8 @@
         <v>195</v>
       </c>
       <c r="Z4" s="596"/>
-      <c r="AA4" s="618"/>
-      <c r="AD4" s="741"/>
+      <c r="AA4" s="674"/>
+      <c r="AD4" s="748"/>
     </row>
     <row r="5" spans="1:31" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="52" t="s">
@@ -13899,21 +13914,21 @@
       <c r="F5" s="66" t="s">
         <v>85</v>
       </c>
-      <c r="G5" s="768"/>
+      <c r="G5" s="736"/>
       <c r="H5" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="K5" s="746" t="s">
+      <c r="K5" s="753" t="s">
         <v>217</v>
       </c>
-      <c r="L5" s="761"/>
+      <c r="L5" s="768"/>
       <c r="M5" s="2" t="s">
         <v>215</v>
       </c>
       <c r="N5" s="61" t="s">
         <v>214</v>
       </c>
-      <c r="O5" s="778"/>
+      <c r="O5" s="746"/>
       <c r="P5" s="108" t="s">
         <v>216</v>
       </c>
@@ -13929,11 +13944,11 @@
       <c r="U5" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="Y5" s="749" t="s">
+      <c r="Y5" s="756" t="s">
         <v>286</v>
       </c>
-      <c r="Z5" s="750"/>
-      <c r="AD5" s="741"/>
+      <c r="Z5" s="757"/>
+      <c r="AD5" s="748"/>
     </row>
     <row r="6" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="109"/>
@@ -13943,16 +13958,16 @@
       <c r="E6" s="45" t="s">
         <v>86</v>
       </c>
-      <c r="G6" s="768"/>
+      <c r="G6" s="736"/>
       <c r="H6" s="46" t="s">
         <v>81</v>
       </c>
       <c r="I6" s="23">
         <v>15</v>
       </c>
-      <c r="K6" s="747"/>
-      <c r="L6" s="761"/>
-      <c r="O6" s="778"/>
+      <c r="K6" s="754"/>
+      <c r="L6" s="768"/>
+      <c r="O6" s="746"/>
       <c r="T6" s="2" t="s">
         <v>101</v>
       </c>
@@ -13962,23 +13977,23 @@
       <c r="V6" s="21">
         <v>-1</v>
       </c>
-      <c r="AD6" s="741"/>
+      <c r="AD6" s="748"/>
     </row>
     <row r="7" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="110"/>
-      <c r="G7" s="768"/>
+      <c r="G7" s="736"/>
       <c r="H7" s="6"/>
-      <c r="K7" s="747"/>
-      <c r="L7" s="761"/>
+      <c r="K7" s="754"/>
+      <c r="L7" s="768"/>
       <c r="N7" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="O7" s="778"/>
+      <c r="O7" s="746"/>
       <c r="P7" s="73"/>
       <c r="U7" s="104" t="s">
         <v>20</v>
       </c>
-      <c r="AD7" s="741"/>
+      <c r="AD7" s="748"/>
     </row>
     <row r="8" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="130"/>
@@ -13991,7 +14006,7 @@
       <c r="F8" s="66" t="s">
         <v>87</v>
       </c>
-      <c r="G8" s="768"/>
+      <c r="G8" s="736"/>
       <c r="H8" s="50" t="s">
         <v>76</v>
       </c>
@@ -14001,41 +14016,41 @@
       <c r="J8" s="111">
         <v>115</v>
       </c>
-      <c r="K8" s="747"/>
-      <c r="L8" s="761"/>
-      <c r="O8" s="778"/>
+      <c r="K8" s="754"/>
+      <c r="L8" s="768"/>
+      <c r="O8" s="746"/>
       <c r="P8" s="49"/>
-      <c r="S8" s="743" t="s">
+      <c r="S8" s="750" t="s">
         <v>212</v>
       </c>
-      <c r="T8" s="744"/>
-      <c r="U8" s="744"/>
-      <c r="V8" s="744"/>
-      <c r="W8" s="744"/>
-      <c r="X8" s="744"/>
-      <c r="Y8" s="744"/>
-      <c r="Z8" s="744"/>
-      <c r="AA8" s="744"/>
-      <c r="AB8" s="744"/>
-      <c r="AC8" s="745"/>
-      <c r="AD8" s="741"/>
+      <c r="T8" s="751"/>
+      <c r="U8" s="751"/>
+      <c r="V8" s="751"/>
+      <c r="W8" s="751"/>
+      <c r="X8" s="751"/>
+      <c r="Y8" s="751"/>
+      <c r="Z8" s="751"/>
+      <c r="AA8" s="751"/>
+      <c r="AB8" s="751"/>
+      <c r="AC8" s="752"/>
+      <c r="AD8" s="748"/>
     </row>
     <row r="9" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="733"/>
-      <c r="G9" s="768"/>
+      <c r="C9" s="772"/>
+      <c r="G9" s="736"/>
       <c r="H9" s="6"/>
-      <c r="K9" s="747"/>
-      <c r="L9" s="771" t="s">
+      <c r="K9" s="754"/>
+      <c r="L9" s="739" t="s">
         <v>218</v>
       </c>
-      <c r="M9" s="772"/>
-      <c r="N9" s="773"/>
-      <c r="O9" s="778"/>
+      <c r="M9" s="740"/>
+      <c r="N9" s="741"/>
+      <c r="O9" s="746"/>
       <c r="P9" s="75"/>
-      <c r="AD9" s="741"/>
+      <c r="AD9" s="748"/>
     </row>
     <row r="10" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="734"/>
+      <c r="C10" s="773"/>
       <c r="D10" s="23"/>
       <c r="E10" s="45" t="s">
         <v>88</v>
@@ -14043,7 +14058,7 @@
       <c r="F10" s="66" t="s">
         <v>89</v>
       </c>
-      <c r="G10" s="768"/>
+      <c r="G10" s="736"/>
       <c r="H10" s="51"/>
       <c r="I10" s="21" t="s">
         <v>81</v>
@@ -14051,33 +14066,33 @@
       <c r="J10" s="3">
         <v>15</v>
       </c>
-      <c r="K10" s="747"/>
-      <c r="M10" s="736" t="s">
+      <c r="K10" s="754"/>
+      <c r="M10" s="775" t="s">
         <v>90</v>
       </c>
-      <c r="N10" s="737"/>
-      <c r="O10" s="737"/>
-      <c r="P10" s="737"/>
-      <c r="Q10" s="737"/>
-      <c r="R10" s="737"/>
-      <c r="S10" s="737"/>
-      <c r="T10" s="737"/>
-      <c r="U10" s="737"/>
-      <c r="V10" s="737"/>
-      <c r="W10" s="737"/>
-      <c r="X10" s="737"/>
-      <c r="Y10" s="737"/>
-      <c r="Z10" s="737"/>
-      <c r="AA10" s="737"/>
-      <c r="AB10" s="737"/>
-      <c r="AC10" s="738"/>
-      <c r="AD10" s="741"/>
+      <c r="N10" s="776"/>
+      <c r="O10" s="776"/>
+      <c r="P10" s="776"/>
+      <c r="Q10" s="776"/>
+      <c r="R10" s="776"/>
+      <c r="S10" s="776"/>
+      <c r="T10" s="776"/>
+      <c r="U10" s="776"/>
+      <c r="V10" s="776"/>
+      <c r="W10" s="776"/>
+      <c r="X10" s="776"/>
+      <c r="Y10" s="776"/>
+      <c r="Z10" s="776"/>
+      <c r="AA10" s="776"/>
+      <c r="AB10" s="776"/>
+      <c r="AC10" s="777"/>
+      <c r="AD10" s="748"/>
     </row>
     <row r="11" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="735"/>
-      <c r="G11" s="768"/>
+      <c r="C11" s="774"/>
+      <c r="G11" s="736"/>
       <c r="H11" s="6"/>
-      <c r="K11" s="747"/>
+      <c r="K11" s="754"/>
       <c r="R11" s="52" t="s">
         <v>44</v>
       </c>
@@ -14085,17 +14100,17 @@
       <c r="Y11" s="68" t="s">
         <v>121</v>
       </c>
-      <c r="Z11" s="757" t="s">
+      <c r="Z11" s="764" t="s">
         <v>121</v>
       </c>
-      <c r="AA11" s="758"/>
+      <c r="AA11" s="765"/>
       <c r="AB11" s="52" t="s">
         <v>44</v>
       </c>
       <c r="AC11" s="118" t="s">
         <v>121</v>
       </c>
-      <c r="AD11" s="741"/>
+      <c r="AD11" s="748"/>
     </row>
     <row r="12" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="129"/>
@@ -14108,7 +14123,7 @@
       <c r="F12" s="66" t="s">
         <v>92</v>
       </c>
-      <c r="G12" s="768"/>
+      <c r="G12" s="736"/>
       <c r="H12" s="128"/>
       <c r="I12" s="19" t="s">
         <v>81</v>
@@ -14116,8 +14131,8 @@
       <c r="J12" s="3">
         <v>15</v>
       </c>
-      <c r="K12" s="747"/>
-      <c r="L12" s="762" t="s">
+      <c r="K12" s="754"/>
+      <c r="L12" s="769" t="s">
         <v>93</v>
       </c>
       <c r="M12" s="21" t="s">
@@ -14148,25 +14163,25 @@
         <v>116</v>
       </c>
       <c r="Y12" s="6"/>
-      <c r="AA12" s="751" t="s">
+      <c r="AA12" s="758" t="s">
         <v>126</v>
       </c>
-      <c r="AB12" s="752"/>
+      <c r="AB12" s="759"/>
       <c r="AC12" s="21" t="s">
         <v>232</v>
       </c>
-      <c r="AD12" s="741"/>
+      <c r="AD12" s="748"/>
     </row>
     <row r="13" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="733"/>
-      <c r="G13" s="768"/>
-      <c r="K13" s="747"/>
-      <c r="L13" s="763"/>
+      <c r="C13" s="772"/>
+      <c r="G13" s="736"/>
+      <c r="K13" s="754"/>
+      <c r="L13" s="770"/>
       <c r="M13" s="47"/>
-      <c r="Q13" s="770" t="s">
+      <c r="Q13" s="738" t="s">
         <v>210</v>
       </c>
-      <c r="R13" s="635"/>
+      <c r="R13" s="630"/>
       <c r="S13" s="590"/>
       <c r="T13" s="6"/>
       <c r="U13" s="96" t="s">
@@ -14175,17 +14190,17 @@
       <c r="X13" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="AA13" s="753"/>
-      <c r="AB13" s="754"/>
-      <c r="AD13" s="741"/>
+      <c r="AA13" s="760"/>
+      <c r="AB13" s="761"/>
+      <c r="AD13" s="748"/>
     </row>
     <row r="14" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="C14" s="735"/>
+      <c r="C14" s="774"/>
       <c r="D14" s="23"/>
-      <c r="G14" s="768"/>
+      <c r="G14" s="736"/>
       <c r="H14" s="125"/>
       <c r="I14" s="99" t="s">
         <v>44</v>
@@ -14193,8 +14208,8 @@
       <c r="J14" s="111">
         <v>115</v>
       </c>
-      <c r="K14" s="747"/>
-      <c r="L14" s="763"/>
+      <c r="K14" s="754"/>
+      <c r="L14" s="770"/>
       <c r="M14" s="21" t="s">
         <v>111</v>
       </c>
@@ -14215,9 +14230,9 @@
       <c r="Y14" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="AA14" s="753"/>
-      <c r="AB14" s="754"/>
-      <c r="AD14" s="741"/>
+      <c r="AA14" s="760"/>
+      <c r="AB14" s="761"/>
+      <c r="AD14" s="748"/>
     </row>
     <row r="15" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="130" t="s">
@@ -14232,19 +14247,19 @@
       <c r="F15" s="66" t="s">
         <v>94</v>
       </c>
-      <c r="G15" s="768"/>
+      <c r="G15" s="736"/>
       <c r="H15" s="2" t="s">
         <v>81</v>
       </c>
       <c r="I15" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="K15" s="747"/>
-      <c r="L15" s="764"/>
-      <c r="Q15" s="770" t="s">
+      <c r="K15" s="754"/>
+      <c r="L15" s="771"/>
+      <c r="Q15" s="738" t="s">
         <v>211</v>
       </c>
-      <c r="R15" s="635"/>
+      <c r="R15" s="630"/>
       <c r="S15" s="590"/>
       <c r="T15" s="6"/>
       <c r="V15" s="68" t="s">
@@ -14253,14 +14268,14 @@
       <c r="X15" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="AA15" s="753"/>
-      <c r="AB15" s="754"/>
-      <c r="AD15" s="741"/>
+      <c r="AA15" s="760"/>
+      <c r="AB15" s="761"/>
+      <c r="AD15" s="748"/>
     </row>
     <row r="16" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C16" s="132"/>
-      <c r="G16" s="768"/>
-      <c r="K16" s="747"/>
+      <c r="G16" s="736"/>
+      <c r="K16" s="754"/>
       <c r="N16" s="47"/>
       <c r="O16" s="61" t="s">
         <v>109</v>
@@ -14279,24 +14294,24 @@
       <c r="Z16" s="76" t="s">
         <v>127</v>
       </c>
-      <c r="AA16" s="753"/>
-      <c r="AB16" s="754"/>
-      <c r="AD16" s="741"/>
+      <c r="AA16" s="760"/>
+      <c r="AB16" s="761"/>
+      <c r="AD16" s="748"/>
     </row>
     <row r="17" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C17" s="109"/>
       <c r="E17" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F17" s="765" t="s">
+      <c r="F17" s="733" t="s">
         <v>96</v>
       </c>
-      <c r="G17" s="768"/>
+      <c r="G17" s="736"/>
       <c r="H17" s="54"/>
       <c r="I17" s="133" t="s">
         <v>81</v>
       </c>
-      <c r="K17" s="747"/>
+      <c r="K17" s="754"/>
       <c r="S17" s="590"/>
       <c r="V17" s="68" t="s">
         <v>44</v>
@@ -14304,9 +14319,9 @@
       <c r="X17" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="AA17" s="753"/>
-      <c r="AB17" s="754"/>
-      <c r="AD17" s="741"/>
+      <c r="AA17" s="760"/>
+      <c r="AB17" s="761"/>
+      <c r="AD17" s="748"/>
     </row>
     <row r="18" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C18" s="130"/>
@@ -14316,15 +14331,15 @@
       <c r="E18" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="F18" s="766"/>
-      <c r="G18" s="768"/>
+      <c r="F18" s="734"/>
+      <c r="G18" s="736"/>
       <c r="H18" s="108" t="s">
         <v>76</v>
       </c>
       <c r="I18" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="K18" s="747"/>
+      <c r="K18" s="754"/>
       <c r="O18" s="64" t="s">
         <v>115</v>
       </c>
@@ -14335,42 +14350,39 @@
       <c r="X18" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="AA18" s="755"/>
-      <c r="AB18" s="756"/>
-      <c r="AD18" s="741"/>
+      <c r="AA18" s="762"/>
+      <c r="AB18" s="763"/>
+      <c r="AD18" s="748"/>
     </row>
     <row r="19" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F19" s="64" t="s">
         <v>209</v>
       </c>
-      <c r="G19" s="769"/>
-      <c r="K19" s="748"/>
+      <c r="G19" s="737"/>
+      <c r="K19" s="755"/>
       <c r="Q19" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="R19" s="774" t="s">
+      <c r="R19" s="742" t="s">
         <v>124</v>
       </c>
-      <c r="S19" s="775"/>
-      <c r="T19" s="776"/>
+      <c r="S19" s="743"/>
+      <c r="T19" s="744"/>
       <c r="V19" s="77" t="s">
         <v>115</v>
       </c>
       <c r="Y19" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="AD19" s="742"/>
+      <c r="AD19" s="749"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="G2:G19"/>
-    <mergeCell ref="Q13:R13"/>
-    <mergeCell ref="Q15:R15"/>
-    <mergeCell ref="L9:N9"/>
-    <mergeCell ref="R19:T19"/>
-    <mergeCell ref="S12:S18"/>
-    <mergeCell ref="O3:O9"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="M10:AC10"/>
+    <mergeCell ref="F2:F3"/>
     <mergeCell ref="AD1:AD19"/>
     <mergeCell ref="S8:AC8"/>
     <mergeCell ref="K5:K19"/>
@@ -14382,11 +14394,14 @@
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="L4:L8"/>
     <mergeCell ref="L12:L15"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="M10:AC10"/>
-    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G2:G19"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="Q15:R15"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="R19:T19"/>
+    <mergeCell ref="S12:S18"/>
+    <mergeCell ref="O3:O9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Boat Enabled - Bharat24
Boat Enabled - Bharat24
</commit_message>
<xml_diff>
--- a/System_2.1.8.xlsx
+++ b/System_2.1.8.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Work_For_\Work\Running AppS\System_Work_RW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED2E2440-78F0-45AE-85D2-CB6ECCB64A57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1612D891-DFB6-41A7-A7AD-FD20FB593B33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1126" uniqueCount="627">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1127" uniqueCount="628">
   <si>
     <t>Zone</t>
   </si>
@@ -1920,6 +1920,9 @@
   </si>
   <si>
     <t>AT - CT_WLFJN_X_N-10_X_Left</t>
+  </si>
+  <si>
+    <t>bharat24</t>
   </si>
 </sst>
 </file>
@@ -5060,6 +5063,186 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5072,12 +5255,6 @@
     <xf numFmtId="0" fontId="17" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5089,12 +5266,6 @@
     </xf>
     <xf numFmtId="0" fontId="38" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
@@ -5117,190 +5288,61 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="13" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5342,44 +5384,14 @@
     <xf numFmtId="0" fontId="39" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -5459,34 +5471,46 @@
     <xf numFmtId="14" fontId="5" fillId="14" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5564,46 +5588,25 @@
     <xf numFmtId="0" fontId="3" fillId="21" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -6994,7 +6997,7 @@
       <c r="H1" s="97" t="s">
         <v>344</v>
       </c>
-      <c r="I1" s="619" t="s">
+      <c r="I1" s="665" t="s">
         <v>370</v>
       </c>
       <c r="J1" s="2" t="s">
@@ -7030,7 +7033,7 @@
       <c r="X1" s="434" t="s">
         <v>155</v>
       </c>
-      <c r="Y1" s="663" t="s">
+      <c r="Y1" s="659" t="s">
         <v>530</v>
       </c>
       <c r="Z1" s="410">
@@ -7055,7 +7058,7 @@
         <v>499</v>
       </c>
       <c r="AM1" s="406"/>
-      <c r="AN1" s="646"/>
+      <c r="AN1" s="641"/>
       <c r="AO1" s="341" t="s">
         <v>470</v>
       </c>
@@ -7064,23 +7067,23 @@
       </c>
     </row>
     <row r="2" spans="1:43" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="672">
+      <c r="A2" s="623">
         <f ca="1">TODAY()</f>
-        <v>45282</v>
-      </c>
-      <c r="B2" s="674" t="s">
+        <v>45283</v>
+      </c>
+      <c r="B2" s="625" t="s">
         <v>371</v>
       </c>
-      <c r="C2" s="651" t="s">
+      <c r="C2" s="621" t="s">
         <v>358</v>
       </c>
-      <c r="D2" s="676" t="s">
+      <c r="D2" s="627" t="s">
         <v>356</v>
       </c>
-      <c r="E2" s="615" t="s">
+      <c r="E2" s="675" t="s">
         <v>64</v>
       </c>
-      <c r="F2" s="625" t="s">
+      <c r="F2" s="646" t="s">
         <v>102</v>
       </c>
       <c r="G2" s="397" t="s">
@@ -7089,31 +7092,31 @@
       <c r="H2" s="80" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="620"/>
+      <c r="I2" s="666"/>
       <c r="J2" s="81" t="s">
         <v>76</v>
       </c>
-      <c r="K2" s="617" t="s">
+      <c r="K2" s="677" t="s">
         <v>343</v>
       </c>
-      <c r="L2" s="618"/>
-      <c r="M2" s="625" t="s">
+      <c r="L2" s="678"/>
+      <c r="M2" s="646" t="s">
         <v>102</v>
       </c>
       <c r="N2" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="O2" s="655" t="s">
+      <c r="O2" s="650" t="s">
         <v>102</v>
       </c>
       <c r="P2" s="85" t="s">
         <v>147</v>
       </c>
-      <c r="Q2" s="651" t="s">
+      <c r="Q2" s="621" t="s">
         <v>143</v>
       </c>
       <c r="R2" s="604"/>
-      <c r="S2" s="640" t="s">
+      <c r="S2" s="663" t="s">
         <v>148</v>
       </c>
       <c r="T2" s="89"/>
@@ -7123,7 +7126,7 @@
       <c r="X2" s="435" t="s">
         <v>156</v>
       </c>
-      <c r="Y2" s="664"/>
+      <c r="Y2" s="660"/>
       <c r="Z2" s="411">
         <v>1</v>
       </c>
@@ -7146,15 +7149,15 @@
         <v>464</v>
       </c>
       <c r="AM2" s="432"/>
-      <c r="AN2" s="647"/>
+      <c r="AN2" s="642"/>
     </row>
     <row r="3" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="673"/>
-      <c r="B3" s="675"/>
-      <c r="C3" s="652"/>
-      <c r="D3" s="677"/>
-      <c r="E3" s="616"/>
-      <c r="F3" s="626"/>
+      <c r="A3" s="624"/>
+      <c r="B3" s="626"/>
+      <c r="C3" s="622"/>
+      <c r="D3" s="628"/>
+      <c r="E3" s="676"/>
+      <c r="F3" s="647"/>
       <c r="G3" s="398" t="s">
         <v>28</v>
       </c>
@@ -7173,17 +7176,17 @@
       <c r="L3" s="203" t="s">
         <v>107</v>
       </c>
-      <c r="M3" s="626"/>
+      <c r="M3" s="647"/>
       <c r="N3" s="69" t="s">
         <v>146</v>
       </c>
-      <c r="O3" s="656"/>
+      <c r="O3" s="651"/>
       <c r="P3" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="Q3" s="652"/>
+      <c r="Q3" s="622"/>
       <c r="R3" s="606"/>
-      <c r="S3" s="642"/>
+      <c r="S3" s="664"/>
       <c r="T3" s="89"/>
       <c r="U3" s="124"/>
       <c r="V3" s="120"/>
@@ -7191,7 +7194,7 @@
       <c r="X3" s="435" t="s">
         <v>157</v>
       </c>
-      <c r="Y3" s="664"/>
+      <c r="Y3" s="660"/>
       <c r="Z3" s="412">
         <v>1</v>
       </c>
@@ -7200,7 +7203,7 @@
       <c r="AC3" s="100" t="s">
         <v>481</v>
       </c>
-      <c r="AD3" s="637" t="s">
+      <c r="AD3" s="662" t="s">
         <v>456</v>
       </c>
       <c r="AE3" s="259"/>
@@ -7212,16 +7215,16 @@
       <c r="AK3" s="259"/>
       <c r="AL3" s="16"/>
       <c r="AM3" s="432"/>
-      <c r="AN3" s="647"/>
+      <c r="AN3" s="642"/>
     </row>
     <row r="4" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="240" t="s">
         <v>183</v>
       </c>
-      <c r="B4" s="688" t="s">
+      <c r="B4" s="639" t="s">
         <v>374</v>
       </c>
-      <c r="C4" s="651" t="s">
+      <c r="C4" s="621" t="s">
         <v>154</v>
       </c>
       <c r="D4" s="350" t="s">
@@ -7230,7 +7233,7 @@
       <c r="E4" s="381">
         <v>2</v>
       </c>
-      <c r="F4" s="626"/>
+      <c r="F4" s="647"/>
       <c r="G4" s="384" t="s">
         <v>202</v>
       </c>
@@ -7247,11 +7250,11 @@
         <v>150</v>
       </c>
       <c r="L4" s="206"/>
-      <c r="M4" s="626"/>
+      <c r="M4" s="647"/>
       <c r="N4" s="176" t="s">
         <v>69</v>
       </c>
-      <c r="O4" s="656"/>
+      <c r="O4" s="651"/>
       <c r="P4" s="2" t="s">
         <v>191</v>
       </c>
@@ -7273,12 +7276,12 @@
       <c r="X4" s="435" t="s">
         <v>158</v>
       </c>
-      <c r="Y4" s="664"/>
+      <c r="Y4" s="660"/>
       <c r="Z4" s="413"/>
       <c r="AA4" s="309"/>
       <c r="AB4" s="211"/>
       <c r="AC4" s="16"/>
-      <c r="AD4" s="637"/>
+      <c r="AD4" s="662"/>
       <c r="AE4" s="259"/>
       <c r="AF4" s="259"/>
       <c r="AG4" s="16"/>
@@ -7288,37 +7291,37 @@
       <c r="AK4" s="259"/>
       <c r="AL4" s="16"/>
       <c r="AM4" s="432"/>
-      <c r="AN4" s="647"/>
+      <c r="AN4" s="642"/>
       <c r="AO4" s="341" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="619" t="s">
+      <c r="A5" s="665" t="s">
         <v>419</v>
       </c>
-      <c r="B5" s="689"/>
-      <c r="C5" s="652"/>
+      <c r="B5" s="640"/>
+      <c r="C5" s="622"/>
       <c r="D5" s="61" t="s">
         <v>153</v>
       </c>
       <c r="E5" s="382">
         <v>1</v>
       </c>
-      <c r="F5" s="626"/>
-      <c r="G5" s="680" t="s">
+      <c r="F5" s="647"/>
+      <c r="G5" s="631" t="s">
         <v>192</v>
       </c>
-      <c r="H5" s="680"/>
-      <c r="I5" s="680"/>
-      <c r="J5" s="680"/>
-      <c r="K5" s="680"/>
-      <c r="L5" s="681"/>
-      <c r="M5" s="626"/>
+      <c r="H5" s="631"/>
+      <c r="I5" s="631"/>
+      <c r="J5" s="631"/>
+      <c r="K5" s="631"/>
+      <c r="L5" s="632"/>
+      <c r="M5" s="647"/>
       <c r="N5" s="21">
         <v>8</v>
       </c>
-      <c r="O5" s="656"/>
+      <c r="O5" s="651"/>
       <c r="T5" s="89"/>
       <c r="U5" s="124"/>
       <c r="V5" s="120"/>
@@ -7326,7 +7329,7 @@
       <c r="X5" s="435" t="s">
         <v>159</v>
       </c>
-      <c r="Y5" s="664"/>
+      <c r="Y5" s="660"/>
       <c r="Z5" s="413">
         <v>1</v>
       </c>
@@ -7349,24 +7352,24 @@
       <c r="AK5" s="259"/>
       <c r="AL5" s="80"/>
       <c r="AM5" s="432"/>
-      <c r="AN5" s="647"/>
+      <c r="AN5" s="642"/>
     </row>
     <row r="6" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="620"/>
-      <c r="B6" s="686" t="s">
+      <c r="A6" s="666"/>
+      <c r="B6" s="637" t="s">
         <v>177</v>
       </c>
-      <c r="C6" s="634"/>
-      <c r="D6" s="635"/>
-      <c r="F6" s="626"/>
-      <c r="G6" s="682"/>
-      <c r="H6" s="682"/>
-      <c r="I6" s="682"/>
-      <c r="J6" s="682"/>
-      <c r="K6" s="682"/>
-      <c r="L6" s="683"/>
-      <c r="M6" s="626"/>
-      <c r="O6" s="656"/>
+      <c r="C6" s="667"/>
+      <c r="D6" s="668"/>
+      <c r="F6" s="647"/>
+      <c r="G6" s="633"/>
+      <c r="H6" s="633"/>
+      <c r="I6" s="633"/>
+      <c r="J6" s="633"/>
+      <c r="K6" s="633"/>
+      <c r="L6" s="634"/>
+      <c r="M6" s="647"/>
+      <c r="O6" s="651"/>
       <c r="T6" s="89"/>
       <c r="U6" s="124"/>
       <c r="V6" s="98" t="s">
@@ -7376,7 +7379,7 @@
       <c r="X6" s="435" t="s">
         <v>160</v>
       </c>
-      <c r="Y6" s="664"/>
+      <c r="Y6" s="660"/>
       <c r="Z6" s="411">
         <v>1</v>
       </c>
@@ -7390,16 +7393,16 @@
       <c r="AF6" s="259"/>
       <c r="AG6" s="259"/>
       <c r="AH6" s="259"/>
-      <c r="AI6" s="636"/>
+      <c r="AI6" s="656"/>
       <c r="AJ6" s="445" t="s">
         <v>459</v>
       </c>
-      <c r="AK6" s="636" t="s">
+      <c r="AK6" s="656" t="s">
         <v>252</v>
       </c>
       <c r="AL6" s="259"/>
       <c r="AM6" s="432"/>
-      <c r="AN6" s="647"/>
+      <c r="AN6" s="642"/>
       <c r="AO6" s="341" t="s">
         <v>471</v>
       </c>
@@ -7408,7 +7411,7 @@
       <c r="A7" s="234" t="s">
         <v>574</v>
       </c>
-      <c r="B7" s="687"/>
+      <c r="B7" s="638"/>
       <c r="C7" s="204" t="s">
         <v>375</v>
       </c>
@@ -7418,7 +7421,7 @@
       <c r="E7" s="267">
         <v>3</v>
       </c>
-      <c r="F7" s="626"/>
+      <c r="F7" s="647"/>
       <c r="G7" s="399">
         <v>0</v>
       </c>
@@ -7437,8 +7440,8 @@
       <c r="L7" s="214">
         <v>0</v>
       </c>
-      <c r="M7" s="626"/>
-      <c r="O7" s="656"/>
+      <c r="M7" s="647"/>
+      <c r="O7" s="651"/>
       <c r="R7" s="99" t="s">
         <v>44</v>
       </c>
@@ -7452,7 +7455,7 @@
       <c r="X7" s="435" t="s">
         <v>161</v>
       </c>
-      <c r="Y7" s="664"/>
+      <c r="Y7" s="660"/>
       <c r="Z7" s="411">
         <v>1</v>
       </c>
@@ -7462,18 +7465,18 @@
       <c r="AD7" s="16"/>
       <c r="AE7" s="259"/>
       <c r="AF7" s="259"/>
-      <c r="AG7" s="637" t="s">
+      <c r="AG7" s="662" t="s">
         <v>455</v>
       </c>
       <c r="AH7" s="259"/>
-      <c r="AI7" s="636"/>
+      <c r="AI7" s="656"/>
       <c r="AJ7" s="259"/>
-      <c r="AK7" s="636"/>
+      <c r="AK7" s="656"/>
       <c r="AL7" s="80" t="s">
         <v>497</v>
       </c>
       <c r="AM7" s="432"/>
-      <c r="AN7" s="647"/>
+      <c r="AN7" s="642"/>
       <c r="AP7" s="76" t="s">
         <v>472</v>
       </c>
@@ -7490,27 +7493,27 @@
         <f>SUM(G7:N9)</f>
         <v>15</v>
       </c>
-      <c r="F8" s="626"/>
-      <c r="G8" s="681">
-        <v>0</v>
-      </c>
-      <c r="H8" s="678" t="s">
+      <c r="F8" s="647"/>
+      <c r="G8" s="632">
+        <v>0</v>
+      </c>
+      <c r="H8" s="629" t="s">
         <v>104</v>
       </c>
       <c r="I8" s="604">
         <v>0</v>
       </c>
-      <c r="J8" s="678" t="s">
+      <c r="J8" s="629" t="s">
         <v>104</v>
       </c>
-      <c r="K8" s="684"/>
-      <c r="L8" s="638"/>
-      <c r="M8" s="653"/>
-      <c r="N8" s="643">
+      <c r="K8" s="635"/>
+      <c r="L8" s="669"/>
+      <c r="M8" s="648"/>
+      <c r="N8" s="672">
         <f>N5+N11</f>
         <v>15</v>
       </c>
-      <c r="O8" s="656"/>
+      <c r="O8" s="651"/>
       <c r="T8" s="103" t="s">
         <v>44</v>
       </c>
@@ -7520,7 +7523,7 @@
       <c r="X8" s="435" t="s">
         <v>162</v>
       </c>
-      <c r="Y8" s="664"/>
+      <c r="Y8" s="660"/>
       <c r="Z8" s="413"/>
       <c r="AA8" s="309"/>
       <c r="AB8" s="211"/>
@@ -7528,14 +7531,14 @@
       <c r="AD8" s="16"/>
       <c r="AE8" s="259"/>
       <c r="AF8" s="259"/>
-      <c r="AG8" s="637"/>
+      <c r="AG8" s="662"/>
       <c r="AH8" s="259"/>
-      <c r="AI8" s="636"/>
+      <c r="AI8" s="656"/>
       <c r="AJ8" s="259"/>
       <c r="AK8" s="259"/>
       <c r="AL8" s="259"/>
       <c r="AM8" s="432"/>
-      <c r="AN8" s="647"/>
+      <c r="AN8" s="642"/>
     </row>
     <row r="9" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="234" t="s">
@@ -7550,17 +7553,17 @@
       <c r="D9" s="351" t="s">
         <v>282</v>
       </c>
-      <c r="F9" s="626"/>
-      <c r="G9" s="683"/>
-      <c r="H9" s="679"/>
+      <c r="F9" s="647"/>
+      <c r="G9" s="634"/>
+      <c r="H9" s="630"/>
       <c r="I9" s="606"/>
-      <c r="J9" s="679"/>
-      <c r="K9" s="685"/>
-      <c r="L9" s="639"/>
-      <c r="M9" s="654"/>
-      <c r="N9" s="644"/>
-      <c r="O9" s="657"/>
-      <c r="S9" s="640" t="s">
+      <c r="J9" s="630"/>
+      <c r="K9" s="636"/>
+      <c r="L9" s="670"/>
+      <c r="M9" s="649"/>
+      <c r="N9" s="673"/>
+      <c r="O9" s="652"/>
+      <c r="S9" s="663" t="s">
         <v>61</v>
       </c>
       <c r="T9" s="89"/>
@@ -7572,7 +7575,7 @@
       <c r="X9" s="435" t="s">
         <v>163</v>
       </c>
-      <c r="Y9" s="664"/>
+      <c r="Y9" s="660"/>
       <c r="Z9" s="414"/>
       <c r="AA9" s="309"/>
       <c r="AB9" s="211"/>
@@ -7582,16 +7585,16 @@
       </c>
       <c r="AE9" s="259"/>
       <c r="AF9" s="259"/>
-      <c r="AG9" s="637"/>
+      <c r="AG9" s="662"/>
       <c r="AH9" s="259"/>
-      <c r="AI9" s="636"/>
+      <c r="AI9" s="656"/>
       <c r="AJ9" s="80"/>
-      <c r="AK9" s="636" t="s">
+      <c r="AK9" s="656" t="s">
         <v>252</v>
       </c>
       <c r="AL9" s="259"/>
       <c r="AM9" s="432"/>
-      <c r="AN9" s="647"/>
+      <c r="AN9" s="642"/>
       <c r="AP9" s="2" t="s">
         <v>509</v>
       </c>
@@ -7606,22 +7609,22 @@
       <c r="D10" s="142"/>
       <c r="E10" s="239">
         <f>Boat!W8</f>
-        <v>37</v>
-      </c>
-      <c r="F10" s="626"/>
+        <v>36</v>
+      </c>
+      <c r="F10" s="647"/>
       <c r="N10" s="422" t="s">
         <v>397</v>
       </c>
-      <c r="O10" s="628" t="s">
+      <c r="O10" s="684" t="s">
         <v>102</v>
       </c>
-      <c r="P10" s="658" t="s">
+      <c r="P10" s="653" t="s">
         <v>401</v>
       </c>
       <c r="R10" s="74" t="s">
         <v>44</v>
       </c>
-      <c r="S10" s="641"/>
+      <c r="S10" s="671"/>
       <c r="T10" s="89"/>
       <c r="U10" s="123" t="s">
         <v>176</v>
@@ -7633,7 +7636,7 @@
       <c r="X10" s="435" t="s">
         <v>164</v>
       </c>
-      <c r="Y10" s="664"/>
+      <c r="Y10" s="660"/>
       <c r="Z10" s="413">
         <v>0</v>
       </c>
@@ -7651,16 +7654,16 @@
       <c r="AF10" s="240" t="s">
         <v>312</v>
       </c>
-      <c r="AG10" s="637"/>
+      <c r="AG10" s="662"/>
       <c r="AH10" s="80"/>
-      <c r="AI10" s="636"/>
+      <c r="AI10" s="656"/>
       <c r="AJ10" s="259"/>
-      <c r="AK10" s="636"/>
+      <c r="AK10" s="656"/>
       <c r="AL10" s="259"/>
       <c r="AM10" s="446" t="s">
         <v>319</v>
       </c>
-      <c r="AN10" s="647"/>
+      <c r="AN10" s="642"/>
       <c r="AO10" s="206" t="s">
         <v>94</v>
       </c>
@@ -7678,18 +7681,18 @@
       <c r="D11" s="172" t="s">
         <v>356</v>
       </c>
-      <c r="F11" s="626"/>
+      <c r="F11" s="647"/>
       <c r="M11" s="6"/>
       <c r="N11" s="117">
         <v>7</v>
       </c>
-      <c r="O11" s="629"/>
-      <c r="P11" s="659"/>
+      <c r="O11" s="685"/>
+      <c r="P11" s="654"/>
       <c r="Q11" s="65"/>
       <c r="R11" s="120" t="s">
         <v>221</v>
       </c>
-      <c r="S11" s="641"/>
+      <c r="S11" s="671"/>
       <c r="T11" s="102" t="s">
         <v>44</v>
       </c>
@@ -7699,7 +7702,7 @@
       <c r="X11" s="435" t="s">
         <v>165</v>
       </c>
-      <c r="Y11" s="664"/>
+      <c r="Y11" s="660"/>
       <c r="Z11" s="413"/>
       <c r="AA11" s="309">
         <v>1</v>
@@ -7713,14 +7716,14 @@
       <c r="AF11" s="259" t="s">
         <v>477</v>
       </c>
-      <c r="AG11" s="637"/>
+      <c r="AG11" s="662"/>
       <c r="AH11" s="259"/>
       <c r="AI11" s="70"/>
       <c r="AJ11" s="259"/>
       <c r="AK11" s="259"/>
       <c r="AL11" s="259"/>
       <c r="AM11" s="432"/>
-      <c r="AN11" s="647"/>
+      <c r="AN11" s="642"/>
       <c r="AP11" s="76" t="s">
         <v>485</v>
       </c>
@@ -7739,7 +7742,7 @@
       <c r="E12" s="226">
         <v>3</v>
       </c>
-      <c r="F12" s="626"/>
+      <c r="F12" s="647"/>
       <c r="G12" s="340" t="s">
         <v>401</v>
       </c>
@@ -7748,16 +7751,16 @@
       </c>
       <c r="I12" s="611"/>
       <c r="J12" s="611"/>
-      <c r="K12" s="633"/>
+      <c r="K12" s="689"/>
       <c r="L12" s="205"/>
       <c r="M12" s="205"/>
       <c r="N12" s="205"/>
-      <c r="O12" s="629"/>
-      <c r="P12" s="659"/>
+      <c r="O12" s="685"/>
+      <c r="P12" s="654"/>
       <c r="R12" s="122" t="s">
         <v>180</v>
       </c>
-      <c r="S12" s="642"/>
+      <c r="S12" s="664"/>
       <c r="T12" s="101" t="s">
         <v>44</v>
       </c>
@@ -7767,7 +7770,7 @@
       <c r="X12" s="435" t="s">
         <v>166</v>
       </c>
-      <c r="Y12" s="664"/>
+      <c r="Y12" s="660"/>
       <c r="Z12" s="411">
         <v>1</v>
       </c>
@@ -7778,16 +7781,16 @@
       <c r="AC12" s="100" t="s">
         <v>482</v>
       </c>
-      <c r="AD12" s="645" t="s">
+      <c r="AD12" s="674" t="s">
         <v>241</v>
       </c>
       <c r="AE12" s="445" t="s">
         <v>240</v>
       </c>
-      <c r="AF12" s="637" t="s">
+      <c r="AF12" s="662" t="s">
         <v>229</v>
       </c>
-      <c r="AG12" s="637"/>
+      <c r="AG12" s="662"/>
       <c r="AH12" s="240" t="s">
         <v>260</v>
       </c>
@@ -7797,10 +7800,10 @@
       <c r="AJ12" s="259"/>
       <c r="AK12" s="259"/>
       <c r="AL12" s="259"/>
-      <c r="AM12" s="661" t="s">
+      <c r="AM12" s="657" t="s">
         <v>250</v>
       </c>
-      <c r="AN12" s="647"/>
+      <c r="AN12" s="642"/>
       <c r="AO12" s="341" t="s">
         <v>96</v>
       </c>
@@ -7812,17 +7815,17 @@
       <c r="E13" s="452">
         <v>-3</v>
       </c>
-      <c r="F13" s="626"/>
+      <c r="F13" s="647"/>
       <c r="G13" s="611" t="s">
         <v>431</v>
       </c>
       <c r="H13" s="611"/>
       <c r="I13" s="611"/>
-      <c r="J13" s="633"/>
+      <c r="J13" s="689"/>
       <c r="M13" s="6"/>
       <c r="N13" s="6"/>
-      <c r="O13" s="629"/>
-      <c r="P13" s="660"/>
+      <c r="O13" s="685"/>
+      <c r="P13" s="655"/>
       <c r="T13" s="105" t="s">
         <v>44</v>
       </c>
@@ -7832,7 +7835,7 @@
       <c r="X13" s="435" t="s">
         <v>167</v>
       </c>
-      <c r="Y13" s="664"/>
+      <c r="Y13" s="660"/>
       <c r="Z13" s="411">
         <v>1</v>
       </c>
@@ -7843,8 +7846,8 @@
         <v>501</v>
       </c>
       <c r="AC13" s="16"/>
-      <c r="AD13" s="645"/>
-      <c r="AF13" s="637"/>
+      <c r="AD13" s="674"/>
+      <c r="AF13" s="662"/>
       <c r="AG13" s="80"/>
       <c r="AH13" s="240" t="s">
         <v>309</v>
@@ -7855,8 +7858,8 @@
       <c r="AJ13" s="80"/>
       <c r="AK13" s="259"/>
       <c r="AL13" s="259"/>
-      <c r="AM13" s="661"/>
-      <c r="AN13" s="647"/>
+      <c r="AM13" s="657"/>
+      <c r="AN13" s="642"/>
     </row>
     <row r="14" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="454"/>
@@ -7864,18 +7867,18 @@
       <c r="C14" s="463"/>
       <c r="D14" s="456"/>
       <c r="E14" s="457"/>
-      <c r="F14" s="626"/>
+      <c r="F14" s="647"/>
       <c r="G14" s="611" t="s">
         <v>430</v>
       </c>
       <c r="H14" s="611"/>
       <c r="I14" s="611"/>
-      <c r="J14" s="633"/>
+      <c r="J14" s="689"/>
       <c r="K14" s="2">
         <v>12</v>
       </c>
       <c r="N14" s="6"/>
-      <c r="O14" s="629"/>
+      <c r="O14" s="685"/>
       <c r="Q14" s="61" t="s">
         <v>534</v>
       </c>
@@ -7889,24 +7892,24 @@
       <c r="X14" s="435" t="s">
         <v>168</v>
       </c>
-      <c r="Y14" s="664"/>
+      <c r="Y14" s="660"/>
       <c r="Z14" s="411">
         <v>1</v>
       </c>
       <c r="AA14" s="309"/>
       <c r="AB14" s="211"/>
       <c r="AC14" s="16"/>
-      <c r="AD14" s="645"/>
+      <c r="AD14" s="674"/>
       <c r="AE14" s="259"/>
-      <c r="AF14" s="637"/>
+      <c r="AF14" s="662"/>
       <c r="AG14" s="259"/>
       <c r="AH14" s="259"/>
       <c r="AI14" s="70"/>
       <c r="AJ14" s="259"/>
       <c r="AK14" s="259"/>
       <c r="AL14" s="259"/>
-      <c r="AM14" s="661"/>
-      <c r="AN14" s="647"/>
+      <c r="AM14" s="657"/>
+      <c r="AN14" s="642"/>
     </row>
     <row r="15" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="453" t="s">
@@ -7915,8 +7918,8 @@
       <c r="C15" s="604" t="s">
         <v>374</v>
       </c>
-      <c r="F15" s="626"/>
-      <c r="O15" s="629"/>
+      <c r="F15" s="647"/>
+      <c r="O15" s="685"/>
       <c r="R15" s="99" t="s">
         <v>44</v>
       </c>
@@ -7929,7 +7932,7 @@
       <c r="X15" s="435" t="s">
         <v>169</v>
       </c>
-      <c r="Y15" s="664"/>
+      <c r="Y15" s="660"/>
       <c r="Z15" s="413">
         <v>1</v>
       </c>
@@ -7938,8 +7941,8 @@
       <c r="AC15" s="76" t="s">
         <v>480</v>
       </c>
-      <c r="AD15" s="645"/>
-      <c r="AF15" s="637"/>
+      <c r="AD15" s="674"/>
+      <c r="AF15" s="662"/>
       <c r="AG15" s="80"/>
       <c r="AH15" s="240" t="s">
         <v>449</v>
@@ -7952,8 +7955,8 @@
       </c>
       <c r="AK15" s="259"/>
       <c r="AL15" s="259"/>
-      <c r="AM15" s="661"/>
-      <c r="AN15" s="647"/>
+      <c r="AM15" s="657"/>
+      <c r="AN15" s="642"/>
       <c r="AP15" s="76" t="s">
         <v>73</v>
       </c>
@@ -7975,13 +7978,13 @@
       <c r="E16" s="226">
         <v>1</v>
       </c>
-      <c r="F16" s="626"/>
+      <c r="F16" s="647"/>
       <c r="G16" s="340" t="s">
         <v>489</v>
       </c>
       <c r="I16" s="474"/>
       <c r="J16" s="20"/>
-      <c r="O16" s="629"/>
+      <c r="O16" s="685"/>
       <c r="R16" s="439" t="s">
         <v>184</v>
       </c>
@@ -7992,7 +7995,7 @@
       <c r="X16" s="435" t="s">
         <v>170</v>
       </c>
-      <c r="Y16" s="664"/>
+      <c r="Y16" s="660"/>
       <c r="Z16" s="411">
         <v>1</v>
       </c>
@@ -8013,18 +8016,18 @@
       <c r="AM16" s="432" t="s">
         <v>318</v>
       </c>
-      <c r="AN16" s="647"/>
+      <c r="AN16" s="642"/>
       <c r="AP16" s="76" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="17" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="80"/>
-      <c r="F17" s="626"/>
+      <c r="F17" s="647"/>
       <c r="I17" s="475"/>
       <c r="J17" s="20"/>
       <c r="N17" s="6"/>
-      <c r="O17" s="629"/>
+      <c r="O17" s="685"/>
       <c r="Q17" s="21" t="s">
         <v>532</v>
       </c>
@@ -8044,7 +8047,7 @@
       <c r="X17" s="435" t="s">
         <v>171</v>
       </c>
-      <c r="Y17" s="664"/>
+      <c r="Y17" s="660"/>
       <c r="Z17" s="413"/>
       <c r="AA17" s="309"/>
       <c r="AB17" s="211"/>
@@ -8069,7 +8072,7 @@
       <c r="AK17" s="259"/>
       <c r="AL17" s="80"/>
       <c r="AM17" s="432"/>
-      <c r="AN17" s="647"/>
+      <c r="AN17" s="642"/>
       <c r="AO17" s="206" t="s">
         <v>498</v>
       </c>
@@ -8093,21 +8096,21 @@
       <c r="E18" s="99" t="s">
         <v>44</v>
       </c>
-      <c r="F18" s="626"/>
+      <c r="F18" s="647"/>
       <c r="G18" s="340" t="s">
         <v>529</v>
       </c>
       <c r="I18" s="24"/>
       <c r="J18" s="20"/>
-      <c r="O18" s="629"/>
+      <c r="O18" s="685"/>
       <c r="Q18" s="112"/>
-      <c r="R18" s="621" t="s">
+      <c r="R18" s="679" t="s">
         <v>537</v>
       </c>
       <c r="T18" s="100" t="s">
         <v>44</v>
       </c>
-      <c r="U18" s="669" t="s">
+      <c r="U18" s="618" t="s">
         <v>44</v>
       </c>
       <c r="V18" s="120"/>
@@ -8117,7 +8120,7 @@
       <c r="X18" s="435" t="s">
         <v>172</v>
       </c>
-      <c r="Y18" s="664"/>
+      <c r="Y18" s="660"/>
       <c r="Z18" s="413">
         <v>1</v>
       </c>
@@ -8128,38 +8131,38 @@
       <c r="AC18" s="16"/>
       <c r="AD18" s="16"/>
       <c r="AE18" s="259"/>
-      <c r="AF18" s="636" t="s">
+      <c r="AF18" s="656" t="s">
         <v>476</v>
       </c>
       <c r="AG18" s="259"/>
       <c r="AH18" s="70"/>
       <c r="AI18" s="70"/>
-      <c r="AJ18" s="662" t="s">
+      <c r="AJ18" s="658" t="s">
         <v>316</v>
       </c>
       <c r="AK18" s="259"/>
       <c r="AL18" s="80"/>
       <c r="AM18" s="432"/>
-      <c r="AN18" s="647"/>
+      <c r="AN18" s="642"/>
       <c r="AP18" s="76" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F19" s="626"/>
+      <c r="F19" s="647"/>
       <c r="I19" s="221"/>
-      <c r="O19" s="629"/>
-      <c r="R19" s="622"/>
+      <c r="O19" s="685"/>
+      <c r="R19" s="680"/>
       <c r="S19" s="30" t="s">
         <v>535</v>
       </c>
-      <c r="U19" s="670"/>
+      <c r="U19" s="619"/>
       <c r="V19" s="146"/>
       <c r="W19" s="146"/>
       <c r="X19" s="435" t="s">
         <v>173</v>
       </c>
-      <c r="Y19" s="664"/>
+      <c r="Y19" s="660"/>
       <c r="Z19" s="411">
         <v>1</v>
       </c>
@@ -8168,17 +8171,17 @@
       <c r="AC19" s="16"/>
       <c r="AD19" s="16"/>
       <c r="AE19" s="259"/>
-      <c r="AF19" s="636"/>
+      <c r="AF19" s="656"/>
       <c r="AG19" s="259"/>
       <c r="AH19" s="259"/>
       <c r="AI19" s="70"/>
-      <c r="AJ19" s="662"/>
+      <c r="AJ19" s="658"/>
       <c r="AK19" s="464" t="s">
         <v>252</v>
       </c>
       <c r="AL19" s="80"/>
       <c r="AM19" s="432"/>
-      <c r="AN19" s="647"/>
+      <c r="AN19" s="642"/>
       <c r="AP19" s="76" t="s">
         <v>469</v>
       </c>
@@ -8199,24 +8202,24 @@
       <c r="E20" s="441">
         <v>-1</v>
       </c>
-      <c r="F20" s="626"/>
+      <c r="F20" s="647"/>
       <c r="G20" s="340" t="s">
         <v>492</v>
       </c>
       <c r="I20" s="221"/>
-      <c r="O20" s="629"/>
-      <c r="Q20" s="631" t="s">
+      <c r="O20" s="685"/>
+      <c r="Q20" s="687" t="s">
         <v>48</v>
       </c>
       <c r="T20" s="408" t="s">
         <v>44</v>
       </c>
-      <c r="U20" s="671"/>
+      <c r="U20" s="620"/>
       <c r="W20" s="409"/>
       <c r="X20" s="436" t="s">
         <v>174</v>
       </c>
-      <c r="Y20" s="664"/>
+      <c r="Y20" s="660"/>
       <c r="Z20" s="415">
         <v>1</v>
       </c>
@@ -8241,7 +8244,7 @@
       <c r="AM20" s="384" t="s">
         <v>250</v>
       </c>
-      <c r="AN20" s="647"/>
+      <c r="AN20" s="642"/>
       <c r="AO20" s="341" t="s">
         <v>461</v>
       </c>
@@ -8262,20 +8265,20 @@
       <c r="E21" s="267">
         <v>0</v>
       </c>
-      <c r="F21" s="626"/>
+      <c r="F21" s="647"/>
       <c r="I21" s="221"/>
-      <c r="O21" s="629"/>
-      <c r="Q21" s="632"/>
+      <c r="O21" s="685"/>
+      <c r="Q21" s="688"/>
       <c r="T21" s="426"/>
       <c r="U21" s="14"/>
-      <c r="V21" s="666"/>
+      <c r="V21" s="615"/>
       <c r="W21" s="430" t="s">
         <v>175</v>
       </c>
       <c r="X21" s="433" t="s">
         <v>186</v>
       </c>
-      <c r="Y21" s="664"/>
+      <c r="Y21" s="660"/>
       <c r="Z21" s="449">
         <v>3</v>
       </c>
@@ -8306,15 +8309,15 @@
       <c r="AM21" s="432" t="s">
         <v>546</v>
       </c>
-      <c r="AN21" s="647"/>
+      <c r="AN21" s="642"/>
     </row>
     <row r="22" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F22" s="626"/>
+      <c r="F22" s="647"/>
       <c r="G22" s="340" t="s">
         <v>490</v>
       </c>
       <c r="I22" s="221"/>
-      <c r="O22" s="629"/>
+      <c r="O22" s="685"/>
       <c r="R22" s="438" t="s">
         <v>44</v>
       </c>
@@ -8322,14 +8325,14 @@
         <v>44</v>
       </c>
       <c r="U22" s="15"/>
-      <c r="V22" s="667"/>
+      <c r="V22" s="616"/>
       <c r="W22" s="430" t="s">
         <v>175</v>
       </c>
       <c r="X22" s="433" t="s">
         <v>187</v>
       </c>
-      <c r="Y22" s="664"/>
+      <c r="Y22" s="660"/>
       <c r="Z22" s="419"/>
       <c r="AA22" s="10"/>
       <c r="AB22" s="419"/>
@@ -8340,7 +8343,7 @@
       <c r="AG22" s="6"/>
       <c r="AH22" s="6"/>
       <c r="AI22" s="6"/>
-      <c r="AJ22" s="636" t="s">
+      <c r="AJ22" s="656" t="s">
         <v>473</v>
       </c>
       <c r="AK22" s="259"/>
@@ -8348,7 +8351,7 @@
         <v>479</v>
       </c>
       <c r="AM22" s="302"/>
-      <c r="AN22" s="647"/>
+      <c r="AN22" s="642"/>
     </row>
     <row r="23" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="233" t="s">
@@ -8366,22 +8369,22 @@
       <c r="E23" s="227">
         <v>1</v>
       </c>
-      <c r="F23" s="626"/>
+      <c r="F23" s="647"/>
       <c r="I23" s="221"/>
-      <c r="O23" s="629"/>
-      <c r="Q23" s="631" t="s">
+      <c r="O23" s="685"/>
+      <c r="Q23" s="687" t="s">
         <v>144</v>
       </c>
       <c r="T23" s="17"/>
       <c r="U23" s="424" t="s">
         <v>44</v>
       </c>
-      <c r="V23" s="667"/>
+      <c r="V23" s="616"/>
       <c r="W23" s="148"/>
       <c r="X23" s="433" t="s">
         <v>188</v>
       </c>
-      <c r="Y23" s="664"/>
+      <c r="Y23" s="660"/>
       <c r="Z23" s="17"/>
       <c r="AA23" s="10"/>
       <c r="AB23" s="419"/>
@@ -8392,13 +8395,13 @@
       <c r="AG23" s="6"/>
       <c r="AH23" s="6"/>
       <c r="AI23" s="6"/>
-      <c r="AJ23" s="636"/>
+      <c r="AJ23" s="656"/>
       <c r="AK23" s="259"/>
       <c r="AL23" s="80" t="s">
         <v>508</v>
       </c>
       <c r="AM23" s="302"/>
-      <c r="AN23" s="647"/>
+      <c r="AN23" s="642"/>
     </row>
     <row r="24" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="444" t="s">
@@ -8416,23 +8419,23 @@
       <c r="E24" s="440">
         <v>1</v>
       </c>
-      <c r="F24" s="626"/>
+      <c r="F24" s="647"/>
       <c r="G24" s="61" t="s">
         <v>491</v>
       </c>
       <c r="I24" s="221"/>
-      <c r="O24" s="629"/>
-      <c r="Q24" s="632"/>
+      <c r="O24" s="685"/>
+      <c r="Q24" s="688"/>
       <c r="T24" s="17"/>
       <c r="U24" s="229" t="s">
         <v>44</v>
       </c>
-      <c r="V24" s="667"/>
+      <c r="V24" s="616"/>
       <c r="W24" s="148"/>
       <c r="X24" s="433" t="s">
         <v>185</v>
       </c>
-      <c r="Y24" s="664"/>
+      <c r="Y24" s="660"/>
       <c r="Z24" s="17"/>
       <c r="AA24" s="10"/>
       <c r="AB24" s="419"/>
@@ -8451,12 +8454,12 @@
         <v>464</v>
       </c>
       <c r="AM24" s="302"/>
-      <c r="AN24" s="647"/>
+      <c r="AN24" s="642"/>
     </row>
     <row r="25" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F25" s="626"/>
+      <c r="F25" s="647"/>
       <c r="I25" s="221"/>
-      <c r="O25" s="629"/>
+      <c r="O25" s="685"/>
       <c r="P25" s="206" t="s">
         <v>281</v>
       </c>
@@ -8469,12 +8472,12 @@
       <c r="U25" s="404" t="s">
         <v>44</v>
       </c>
-      <c r="V25" s="668"/>
+      <c r="V25" s="617"/>
       <c r="W25" s="148"/>
       <c r="X25" s="433" t="s">
         <v>189</v>
       </c>
-      <c r="Y25" s="664"/>
+      <c r="Y25" s="660"/>
       <c r="Z25" s="17"/>
       <c r="AA25" s="10"/>
       <c r="AB25" s="419"/>
@@ -8491,7 +8494,7 @@
       <c r="AK25" s="142"/>
       <c r="AL25" s="6"/>
       <c r="AM25" s="302"/>
-      <c r="AN25" s="647"/>
+      <c r="AN25" s="642"/>
     </row>
     <row r="26" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="233" t="s">
@@ -8509,17 +8512,17 @@
       <c r="E26" s="383">
         <v>1</v>
       </c>
-      <c r="F26" s="626"/>
+      <c r="F26" s="647"/>
       <c r="G26" s="340" t="s">
         <v>488</v>
       </c>
       <c r="I26" s="221"/>
-      <c r="O26" s="629"/>
-      <c r="P26" s="649" t="s">
+      <c r="O26" s="685"/>
+      <c r="P26" s="644" t="s">
         <v>527</v>
       </c>
-      <c r="Q26" s="650"/>
-      <c r="R26" s="623" t="s">
+      <c r="Q26" s="645"/>
+      <c r="R26" s="681" t="s">
         <v>536</v>
       </c>
       <c r="T26" s="180"/>
@@ -8531,7 +8534,7 @@
       <c r="X26" s="433" t="s">
         <v>181</v>
       </c>
-      <c r="Y26" s="664"/>
+      <c r="Y26" s="660"/>
       <c r="Z26" s="17"/>
       <c r="AA26" s="10"/>
       <c r="AB26" s="419"/>
@@ -8558,7 +8561,7 @@
       <c r="AM26" s="446" t="s">
         <v>457</v>
       </c>
-      <c r="AN26" s="647"/>
+      <c r="AN26" s="642"/>
     </row>
     <row r="27" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="21" t="s">
@@ -8570,13 +8573,13 @@
       <c r="E27" s="267" t="s">
         <v>44</v>
       </c>
-      <c r="F27" s="627"/>
+      <c r="F27" s="683"/>
       <c r="G27" s="61" t="s">
         <v>545</v>
       </c>
       <c r="I27" s="222"/>
-      <c r="O27" s="630"/>
-      <c r="R27" s="624"/>
+      <c r="O27" s="686"/>
+      <c r="R27" s="682"/>
       <c r="S27" s="425" t="s">
         <v>54</v>
       </c>
@@ -8589,7 +8592,7 @@
       <c r="X27" s="433" t="s">
         <v>531</v>
       </c>
-      <c r="Y27" s="665"/>
+      <c r="Y27" s="661"/>
       <c r="Z27" s="161"/>
       <c r="AA27" s="13"/>
       <c r="AB27" s="420"/>
@@ -8606,10 +8609,48 @@
       <c r="AM27" s="384" t="s">
         <v>320</v>
       </c>
-      <c r="AN27" s="648"/>
+      <c r="AN27" s="643"/>
     </row>
   </sheetData>
   <mergeCells count="54">
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="R18:R19"/>
+    <mergeCell ref="R26:R27"/>
+    <mergeCell ref="F2:F27"/>
+    <mergeCell ref="O10:O27"/>
+    <mergeCell ref="Q20:Q21"/>
+    <mergeCell ref="Q23:Q24"/>
+    <mergeCell ref="G14:J14"/>
+    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="AI6:AI10"/>
+    <mergeCell ref="AF12:AF15"/>
+    <mergeCell ref="AG7:AG12"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="S9:S12"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="AD12:AD15"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="AN1:AN27"/>
+    <mergeCell ref="P26:Q26"/>
+    <mergeCell ref="Q2:Q3"/>
+    <mergeCell ref="M2:M9"/>
+    <mergeCell ref="O2:O9"/>
+    <mergeCell ref="P10:P13"/>
+    <mergeCell ref="AK6:AK7"/>
+    <mergeCell ref="AM12:AM15"/>
+    <mergeCell ref="AF18:AF19"/>
+    <mergeCell ref="AJ18:AJ19"/>
+    <mergeCell ref="Y1:Y27"/>
+    <mergeCell ref="AJ22:AJ23"/>
+    <mergeCell ref="AK9:AK10"/>
+    <mergeCell ref="AD3:AD4"/>
+    <mergeCell ref="S2:S3"/>
+    <mergeCell ref="R2:R3"/>
     <mergeCell ref="V21:V25"/>
     <mergeCell ref="U18:U20"/>
     <mergeCell ref="C2:C3"/>
@@ -8626,44 +8667,6 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="B4:B5"/>
-    <mergeCell ref="AN1:AN27"/>
-    <mergeCell ref="P26:Q26"/>
-    <mergeCell ref="Q2:Q3"/>
-    <mergeCell ref="M2:M9"/>
-    <mergeCell ref="O2:O9"/>
-    <mergeCell ref="P10:P13"/>
-    <mergeCell ref="AK6:AK7"/>
-    <mergeCell ref="AM12:AM15"/>
-    <mergeCell ref="AF18:AF19"/>
-    <mergeCell ref="AJ18:AJ19"/>
-    <mergeCell ref="Y1:Y27"/>
-    <mergeCell ref="AJ22:AJ23"/>
-    <mergeCell ref="AK9:AK10"/>
-    <mergeCell ref="AD3:AD4"/>
-    <mergeCell ref="S2:S3"/>
-    <mergeCell ref="R2:R3"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="AI6:AI10"/>
-    <mergeCell ref="AF12:AF15"/>
-    <mergeCell ref="AG7:AG12"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="S9:S12"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="AD12:AD15"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="R18:R19"/>
-    <mergeCell ref="R26:R27"/>
-    <mergeCell ref="F2:F27"/>
-    <mergeCell ref="O10:O27"/>
-    <mergeCell ref="Q20:Q21"/>
-    <mergeCell ref="Q23:Q24"/>
-    <mergeCell ref="G14:J14"/>
-    <mergeCell ref="G13:J13"/>
-    <mergeCell ref="H12:K12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8700,12 +8703,12 @@
       <c r="B1" s="609" t="s">
         <v>311</v>
       </c>
-      <c r="C1" s="633"/>
+      <c r="C1" s="689"/>
       <c r="D1" s="206"/>
       <c r="J1" s="609" t="s">
         <v>69</v>
       </c>
-      <c r="K1" s="633"/>
+      <c r="K1" s="689"/>
       <c r="L1" s="197" t="s">
         <v>331</v>
       </c>
@@ -9040,7 +9043,7 @@
   <dimension ref="A1:AL31"/>
   <sheetViews>
     <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="AI14" sqref="AI14"/>
+      <selection activeCell="AH14" sqref="AH14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9108,7 +9111,7 @@
       <c r="P1" s="402" t="s">
         <v>398</v>
       </c>
-      <c r="Q1" s="707" t="s">
+      <c r="Q1" s="720" t="s">
         <v>180</v>
       </c>
       <c r="R1" s="100" t="s">
@@ -9132,7 +9135,7 @@
       <c r="AA1" s="523" t="s">
         <v>438</v>
       </c>
-      <c r="AB1" s="701" t="s">
+      <c r="AB1" s="714" t="s">
         <v>596</v>
       </c>
       <c r="AC1" s="99" t="s">
@@ -9154,32 +9157,32 @@
       </c>
     </row>
     <row r="2" spans="1:38" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="712">
+      <c r="A2" s="699">
         <f ca="1">TODAY()</f>
-        <v>45282</v>
-      </c>
-      <c r="B2" s="714" t="s">
+        <v>45283</v>
+      </c>
+      <c r="B2" s="701" t="s">
         <v>380</v>
       </c>
-      <c r="C2" s="651" t="s">
+      <c r="C2" s="621" t="s">
         <v>358</v>
       </c>
-      <c r="D2" s="716" t="s">
+      <c r="D2" s="703" t="s">
         <v>102</v>
       </c>
-      <c r="E2" s="718" t="s">
+      <c r="E2" s="705" t="s">
         <v>64</v>
       </c>
       <c r="F2" s="193" t="s">
         <v>219</v>
       </c>
-      <c r="G2" s="619" t="s">
+      <c r="G2" s="665" t="s">
         <v>373</v>
       </c>
       <c r="H2" s="208" t="s">
         <v>219</v>
       </c>
-      <c r="I2" s="698" t="s">
+      <c r="I2" s="711" t="s">
         <v>102</v>
       </c>
       <c r="J2" s="400" t="s">
@@ -9203,7 +9206,7 @@
       <c r="P2" s="403">
         <v>40</v>
       </c>
-      <c r="Q2" s="708"/>
+      <c r="Q2" s="721"/>
       <c r="R2" s="21">
         <f>R7+R20</f>
         <v>2</v>
@@ -9228,7 +9231,7 @@
         <f>IF((Z2+T2)&gt;0,0,-1)</f>
         <v>0</v>
       </c>
-      <c r="AB2" s="702"/>
+      <c r="AB2" s="715"/>
       <c r="AC2" s="35"/>
       <c r="AH2" s="6" t="s">
         <v>453</v>
@@ -9245,14 +9248,14 @@
       </c>
     </row>
     <row r="3" spans="1:38" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="713"/>
-      <c r="B3" s="715"/>
-      <c r="C3" s="652"/>
-      <c r="D3" s="717"/>
-      <c r="E3" s="719"/>
-      <c r="G3" s="620"/>
+      <c r="A3" s="700"/>
+      <c r="B3" s="702"/>
+      <c r="C3" s="622"/>
+      <c r="D3" s="704"/>
+      <c r="E3" s="706"/>
+      <c r="G3" s="666"/>
       <c r="H3" s="6"/>
-      <c r="I3" s="699"/>
+      <c r="I3" s="712"/>
       <c r="K3" s="24">
         <v>2</v>
       </c>
@@ -9267,7 +9270,7 @@
       <c r="V3" s="475"/>
       <c r="W3" s="6"/>
       <c r="X3" s="475"/>
-      <c r="AB3" s="702"/>
+      <c r="AB3" s="715"/>
       <c r="AC3" s="35"/>
       <c r="AE3" s="100" t="s">
         <v>591</v>
@@ -9296,10 +9299,10 @@
         <v>381</v>
       </c>
       <c r="B4" s="245"/>
-      <c r="C4" s="720" t="s">
+      <c r="C4" s="707" t="s">
         <v>177</v>
       </c>
-      <c r="I4" s="699"/>
+      <c r="I4" s="712"/>
       <c r="R4" s="476" t="s">
         <v>591</v>
       </c>
@@ -9311,7 +9314,7 @@
       <c r="V4" s="475"/>
       <c r="W4" s="6"/>
       <c r="X4" s="475"/>
-      <c r="AB4" s="702"/>
+      <c r="AB4" s="715"/>
       <c r="AC4" s="35"/>
       <c r="AE4" s="20"/>
       <c r="AF4" s="100" t="s">
@@ -9342,7 +9345,7 @@
       <c r="B5" s="100" t="s">
         <v>358</v>
       </c>
-      <c r="C5" s="721"/>
+      <c r="C5" s="708"/>
       <c r="D5" s="224" t="s">
         <v>102</v>
       </c>
@@ -9358,7 +9361,7 @@
       <c r="H5" s="208" t="s">
         <v>219</v>
       </c>
-      <c r="I5" s="699"/>
+      <c r="I5" s="712"/>
       <c r="J5" s="401" t="s">
         <v>269</v>
       </c>
@@ -9385,7 +9388,7 @@
       <c r="V5" s="473"/>
       <c r="W5" s="6"/>
       <c r="X5" s="473"/>
-      <c r="AB5" s="702"/>
+      <c r="AB5" s="715"/>
       <c r="AC5" s="2" t="s">
         <v>594</v>
       </c>
@@ -9399,19 +9402,19 @@
       <c r="AL5" s="473"/>
     </row>
     <row r="6" spans="1:38" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="709" t="s">
+      <c r="A6" s="696" t="s">
         <v>286</v>
       </c>
       <c r="B6" s="105" t="s">
         <v>198</v>
       </c>
-      <c r="C6" s="634"/>
-      <c r="D6" s="635"/>
+      <c r="C6" s="667"/>
+      <c r="D6" s="668"/>
       <c r="E6" s="96">
         <v>1</v>
       </c>
       <c r="G6" s="605"/>
-      <c r="I6" s="699"/>
+      <c r="I6" s="712"/>
       <c r="P6" s="61" t="s">
         <v>594</v>
       </c>
@@ -9423,11 +9426,11 @@
         <f>S7-S12-SUM(V2:V10)</f>
         <v>0</v>
       </c>
-      <c r="AB6" s="702"/>
+      <c r="AB6" s="715"/>
       <c r="AC6" s="35"/>
       <c r="AE6" s="64">
         <f>AE7-SUM(AL2:AL10)+AE11</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF6" s="64">
         <f>AF7-SUM(AI2:AI10)+AF11</f>
@@ -9439,7 +9442,7 @@
       <c r="AL6" s="112"/>
     </row>
     <row r="7" spans="1:38" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="710"/>
+      <c r="A7" s="697"/>
       <c r="B7" s="100" t="s">
         <v>154</v>
       </c>
@@ -9450,7 +9453,7 @@
         <v>135</v>
       </c>
       <c r="G7" s="605"/>
-      <c r="I7" s="699"/>
+      <c r="I7" s="712"/>
       <c r="M7" s="16" t="s">
         <v>348</v>
       </c>
@@ -9482,7 +9485,7 @@
       <c r="X7" s="474">
         <v>1</v>
       </c>
-      <c r="AB7" s="702"/>
+      <c r="AB7" s="715"/>
       <c r="AC7" s="99" t="s">
         <v>595</v>
       </c>
@@ -9491,7 +9494,7 @@
       </c>
       <c r="AE7" s="24">
         <f>8-AE11</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AF7" s="297">
         <f>8-AF11</f>
@@ -9508,7 +9511,7 @@
       </c>
     </row>
     <row r="8" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="711"/>
+      <c r="A8" s="698"/>
       <c r="B8" s="214" t="s">
         <v>28</v>
       </c>
@@ -9517,7 +9520,7 @@
         <v>3</v>
       </c>
       <c r="G8" s="605"/>
-      <c r="I8" s="699"/>
+      <c r="I8" s="712"/>
       <c r="N8" s="80"/>
       <c r="U8" s="6" t="s">
         <v>250</v>
@@ -9531,7 +9534,7 @@
       <c r="X8" s="475">
         <v>1</v>
       </c>
-      <c r="AB8" s="702"/>
+      <c r="AB8" s="715"/>
       <c r="AC8" s="521"/>
       <c r="AH8" s="6" t="s">
         <v>600</v>
@@ -9540,8 +9543,12 @@
         <v>1</v>
       </c>
       <c r="AJ8" s="561"/>
-      <c r="AK8" s="6"/>
-      <c r="AL8" s="555"/>
+      <c r="AK8" s="6" t="s">
+        <v>627</v>
+      </c>
+      <c r="AL8" s="555">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="233" t="s">
@@ -9558,7 +9565,7 @@
       </c>
       <c r="G9" s="605"/>
       <c r="H9" s="6"/>
-      <c r="I9" s="699"/>
+      <c r="I9" s="712"/>
       <c r="M9" s="19" t="s">
         <v>526</v>
       </c>
@@ -9569,7 +9576,7 @@
         <v>510</v>
       </c>
       <c r="X9" s="472"/>
-      <c r="AB9" s="702"/>
+      <c r="AB9" s="715"/>
       <c r="AC9" s="521"/>
       <c r="AE9" s="20"/>
       <c r="AF9" s="20"/>
@@ -9598,10 +9605,10 @@
       <c r="D10" s="108"/>
       <c r="E10" s="68">
         <f>Boat!W8</f>
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G10" s="605"/>
-      <c r="I10" s="699"/>
+      <c r="I10" s="712"/>
       <c r="J10" s="24" t="s">
         <v>373</v>
       </c>
@@ -9618,7 +9625,7 @@
         <v>602</v>
       </c>
       <c r="X10" s="472"/>
-      <c r="AB10" s="702"/>
+      <c r="AB10" s="715"/>
       <c r="AC10" s="521"/>
       <c r="AE10" s="20"/>
       <c r="AF10" s="20"/>
@@ -9646,7 +9653,7 @@
         <v>266</v>
       </c>
       <c r="G11" s="605"/>
-      <c r="I11" s="699"/>
+      <c r="I11" s="712"/>
       <c r="J11" s="24" t="s">
         <v>194</v>
       </c>
@@ -9672,13 +9679,13 @@
       <c r="S11" s="24">
         <v>2</v>
       </c>
-      <c r="U11" s="704" t="s">
+      <c r="U11" s="717" t="s">
         <v>559</v>
       </c>
-      <c r="V11" s="705"/>
-      <c r="W11" s="705"/>
-      <c r="X11" s="706"/>
-      <c r="AB11" s="703"/>
+      <c r="V11" s="718"/>
+      <c r="W11" s="718"/>
+      <c r="X11" s="719"/>
+      <c r="AB11" s="716"/>
       <c r="AC11" s="99" t="s">
         <v>597</v>
       </c>
@@ -9686,19 +9693,19 @@
         <v>44</v>
       </c>
       <c r="AE11" s="24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF11" s="24">
         <v>3</v>
       </c>
       <c r="AG11" s="418"/>
-      <c r="AH11" s="704" t="s">
+      <c r="AH11" s="717" t="s">
         <v>614</v>
       </c>
-      <c r="AI11" s="705"/>
-      <c r="AJ11" s="705"/>
-      <c r="AK11" s="705"/>
-      <c r="AL11" s="706"/>
+      <c r="AI11" s="718"/>
+      <c r="AJ11" s="718"/>
+      <c r="AK11" s="718"/>
+      <c r="AL11" s="719"/>
     </row>
     <row r="12" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="229" t="s">
@@ -9709,7 +9716,7 @@
         <v>3</v>
       </c>
       <c r="G12" s="605"/>
-      <c r="I12" s="699"/>
+      <c r="I12" s="712"/>
       <c r="J12" s="24" t="s">
         <v>517</v>
       </c>
@@ -9742,7 +9749,7 @@
       </c>
       <c r="D13" s="20"/>
       <c r="G13" s="605"/>
-      <c r="I13" s="699"/>
+      <c r="I13" s="712"/>
       <c r="J13" s="108" t="s">
         <v>549</v>
       </c>
@@ -9786,7 +9793,7 @@
       <c r="H14" s="208" t="s">
         <v>219</v>
       </c>
-      <c r="I14" s="699"/>
+      <c r="I14" s="712"/>
       <c r="U14" s="67" t="s">
         <v>80</v>
       </c>
@@ -9813,7 +9820,7 @@
       <c r="H15" s="273">
         <v>0</v>
       </c>
-      <c r="I15" s="699"/>
+      <c r="I15" s="712"/>
       <c r="J15" s="108" t="s">
         <v>153</v>
       </c>
@@ -9844,7 +9851,7 @@
       <c r="D16" s="2" t="s">
         <v>493</v>
       </c>
-      <c r="I16" s="699"/>
+      <c r="I16" s="712"/>
       <c r="K16" s="100" t="s">
         <v>44</v>
       </c>
@@ -9888,7 +9895,7 @@
       <c r="G17" s="2" t="s">
         <v>424</v>
       </c>
-      <c r="I17" s="699"/>
+      <c r="I17" s="712"/>
       <c r="L17" s="2" t="s">
         <v>427</v>
       </c>
@@ -9906,13 +9913,13 @@
     </row>
     <row r="18" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G18" s="16"/>
-      <c r="I18" s="699"/>
+      <c r="I18" s="712"/>
       <c r="L18" s="16"/>
       <c r="M18" s="21"/>
-      <c r="O18" s="696" t="s">
+      <c r="O18" s="709" t="s">
         <v>518</v>
       </c>
-      <c r="P18" s="697"/>
+      <c r="P18" s="710"/>
       <c r="Q18" s="127" t="s">
         <v>44</v>
       </c>
@@ -9938,7 +9945,7 @@
       </c>
     </row>
     <row r="19" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I19" s="699"/>
+      <c r="I19" s="712"/>
       <c r="M19" s="21" t="s">
         <v>426</v>
       </c>
@@ -9974,7 +9981,7 @@
       <c r="G20" s="2" t="s">
         <v>424</v>
       </c>
-      <c r="I20" s="699"/>
+      <c r="I20" s="712"/>
       <c r="K20" s="19" t="s">
         <v>423</v>
       </c>
@@ -10009,7 +10016,7 @@
       </c>
     </row>
     <row r="21" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I21" s="699"/>
+      <c r="I21" s="712"/>
       <c r="M21" s="218" t="s">
         <v>412</v>
       </c>
@@ -10043,7 +10050,7 @@
       <c r="G22" s="2" t="s">
         <v>424</v>
       </c>
-      <c r="I22" s="699"/>
+      <c r="I22" s="712"/>
       <c r="P22" s="99" t="s">
         <v>593</v>
       </c>
@@ -10058,7 +10065,7 @@
       <c r="E23" s="285" t="s">
         <v>44</v>
       </c>
-      <c r="I23" s="699"/>
+      <c r="I23" s="712"/>
       <c r="Q23" s="24">
         <f>SUM(V23:V31)</f>
         <v>5</v>
@@ -10075,7 +10082,7 @@
       </c>
     </row>
     <row r="24" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I24" s="699"/>
+      <c r="I24" s="712"/>
       <c r="U24" s="35"/>
       <c r="V24" s="514">
         <v>0</v>
@@ -10103,7 +10110,7 @@
       <c r="H25" s="193" t="s">
         <v>267</v>
       </c>
-      <c r="I25" s="699"/>
+      <c r="I25" s="712"/>
       <c r="J25" s="401" t="s">
         <v>270</v>
       </c>
@@ -10148,7 +10155,7 @@
       <c r="H26" s="19" t="s">
         <v>219</v>
       </c>
-      <c r="I26" s="699"/>
+      <c r="I26" s="712"/>
       <c r="K26" s="24">
         <v>15</v>
       </c>
@@ -10183,7 +10190,7 @@
       </c>
     </row>
     <row r="27" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I27" s="699"/>
+      <c r="I27" s="712"/>
       <c r="O27" s="2" t="s">
         <v>98</v>
       </c>
@@ -10210,7 +10217,7 @@
       <c r="E28" s="217">
         <v>2</v>
       </c>
-      <c r="I28" s="699"/>
+      <c r="I28" s="712"/>
       <c r="Q28" s="6"/>
       <c r="R28" s="112"/>
       <c r="T28" s="142"/>
@@ -10232,7 +10239,7 @@
       <c r="H29" s="193" t="s">
         <v>268</v>
       </c>
-      <c r="I29" s="700"/>
+      <c r="I29" s="713"/>
       <c r="J29" s="326"/>
       <c r="L29" s="96" t="s">
         <v>274</v>
@@ -10290,6 +10297,13 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="I2:I29"/>
+    <mergeCell ref="AB1:AB11"/>
+    <mergeCell ref="AH11:AL11"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="U11:X11"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="G5:G14"/>
     <mergeCell ref="A2:A3"/>
@@ -10301,13 +10315,6 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="C2:C3"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="I2:I29"/>
-    <mergeCell ref="AB1:AB11"/>
-    <mergeCell ref="AH11:AL11"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="U11:X11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10318,7 +10325,7 @@
   <dimension ref="A1:AT37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10416,16 +10423,16 @@
       </c>
       <c r="S1" s="151">
         <f ca="1">TODAY()</f>
-        <v>45282</v>
-      </c>
-      <c r="T1" s="745"/>
+        <v>45283</v>
+      </c>
+      <c r="T1" s="748"/>
       <c r="U1" s="142"/>
       <c r="V1" s="6"/>
       <c r="W1" s="6"/>
-      <c r="X1" s="729" t="s">
+      <c r="X1" s="732" t="s">
         <v>442</v>
       </c>
-      <c r="Y1" s="730"/>
+      <c r="Y1" s="733"/>
       <c r="Z1" s="308">
         <f>68-(W8+Y3+X3+U3)</f>
         <v>0</v>
@@ -10441,23 +10448,23 @@
       <c r="AD1" s="304" t="s">
         <v>44</v>
       </c>
-      <c r="AE1" s="731" t="s">
+      <c r="AE1" s="734" t="s">
         <v>190</v>
       </c>
-      <c r="AF1" s="732"/>
-      <c r="AG1" s="733"/>
-      <c r="AH1" s="734" t="s">
+      <c r="AF1" s="735"/>
+      <c r="AG1" s="736"/>
+      <c r="AH1" s="737" t="s">
         <v>294</v>
       </c>
-      <c r="AI1" s="735"/>
-      <c r="AJ1" s="736"/>
+      <c r="AI1" s="738"/>
+      <c r="AJ1" s="739"/>
       <c r="AK1" s="558"/>
       <c r="AL1" s="558"/>
-      <c r="AM1" s="726" t="s">
+      <c r="AM1" s="729" t="s">
         <v>445</v>
       </c>
-      <c r="AN1" s="727"/>
-      <c r="AO1" s="728"/>
+      <c r="AN1" s="730"/>
+      <c r="AO1" s="731"/>
       <c r="AR1" s="142"/>
     </row>
     <row r="2" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10470,29 +10477,29 @@
       </c>
       <c r="J2" s="320">
         <f>K2+L2</f>
-        <v>28</v>
-      </c>
-      <c r="K2" s="724">
+        <v>30</v>
+      </c>
+      <c r="K2" s="727">
         <f>SUM(K4:K29)</f>
         <v>12</v>
       </c>
-      <c r="L2" s="722">
+      <c r="L2" s="725">
         <f>SUM(L4:L37)</f>
-        <v>16</v>
-      </c>
-      <c r="M2" s="737">
+        <v>18</v>
+      </c>
+      <c r="M2" s="740">
         <f>SUM(M5:M30)</f>
         <v>1</v>
       </c>
-      <c r="N2" s="739">
+      <c r="N2" s="742">
         <f>SUM(N4:N29)</f>
+        <v>11</v>
+      </c>
+      <c r="O2" s="744">
+        <f>SUM(O4:O29)</f>
         <v>10</v>
       </c>
-      <c r="O2" s="741">
-        <f>SUM(O4:O29)</f>
-        <v>9</v>
-      </c>
-      <c r="P2" s="643">
+      <c r="P2" s="672">
         <f>SUM(N30:N37)* (-1)</f>
         <v>-3</v>
       </c>
@@ -10505,14 +10512,14 @@
       <c r="S2" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="T2" s="746"/>
+      <c r="T2" s="749"/>
       <c r="U2" s="543" t="s">
         <v>263</v>
       </c>
       <c r="V2" s="487" t="s">
         <v>220</v>
       </c>
-      <c r="W2" s="743" t="s">
+      <c r="W2" s="746" t="s">
         <v>235</v>
       </c>
       <c r="X2" s="488" t="s">
@@ -10584,12 +10591,12 @@
         <f>V3+X3+Y3+U3</f>
         <v>68</v>
       </c>
-      <c r="K3" s="725"/>
-      <c r="L3" s="723"/>
-      <c r="M3" s="738"/>
-      <c r="N3" s="740"/>
-      <c r="O3" s="742"/>
-      <c r="P3" s="644"/>
+      <c r="K3" s="728"/>
+      <c r="L3" s="726"/>
+      <c r="M3" s="741"/>
+      <c r="N3" s="743"/>
+      <c r="O3" s="745"/>
+      <c r="P3" s="673"/>
       <c r="Q3" s="174">
         <f>(M2+N2)-Y3</f>
         <v>0</v>
@@ -10597,23 +10604,23 @@
       <c r="S3" s="159" t="s">
         <v>245</v>
       </c>
-      <c r="T3" s="747"/>
+      <c r="T3" s="750"/>
       <c r="U3" s="544">
         <f>SUM(U4:U29)</f>
         <v>11</v>
       </c>
       <c r="V3" s="489">
         <f>SUM(V4:V29)</f>
-        <v>37</v>
-      </c>
-      <c r="W3" s="744"/>
+        <v>36</v>
+      </c>
+      <c r="W3" s="747"/>
       <c r="X3" s="490">
         <f t="shared" ref="X3:AC3" si="0">SUM(X4:X29)</f>
         <v>9</v>
       </c>
       <c r="Y3" s="490">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="Z3" s="59">
         <f t="shared" si="0"/>
@@ -10621,15 +10628,15 @@
       </c>
       <c r="AA3" s="66">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AB3" s="66">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="AC3" s="66">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AD3" s="66">
         <f t="shared" ref="AD3:AO3" si="1">SUM(AD4:AD29)</f>
@@ -10637,7 +10644,7 @@
       </c>
       <c r="AE3" s="66">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AF3" s="66">
         <f t="shared" si="1"/>
@@ -10649,7 +10656,7 @@
       </c>
       <c r="AH3" s="66">
         <f>SUM(AH4:AH29)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AI3" s="377">
         <f t="shared" si="1"/>
@@ -10663,15 +10670,15 @@
       <c r="AL3" s="408"/>
       <c r="AM3" s="100">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="AN3" s="312">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AO3" s="313">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AR3" s="142"/>
     </row>
@@ -10704,7 +10711,7 @@
         <f>AC4</f>
         <v>0</v>
       </c>
-      <c r="P4" s="748" t="s">
+      <c r="P4" s="722" t="s">
         <v>199</v>
       </c>
       <c r="Q4" s="20"/>
@@ -10790,7 +10797,7 @@
         <f>AC5</f>
         <v>0</v>
       </c>
-      <c r="P5" s="749"/>
+      <c r="P5" s="723"/>
       <c r="Q5" s="20"/>
       <c r="R5" s="2" t="s">
         <v>341</v>
@@ -10888,7 +10895,7 @@
         <f>AC6</f>
         <v>1</v>
       </c>
-      <c r="P6" s="749"/>
+      <c r="P6" s="723"/>
       <c r="Q6" s="19" t="s">
         <v>336</v>
       </c>
@@ -10978,18 +10985,20 @@
       <c r="K7" s="585">
         <v>3</v>
       </c>
-      <c r="L7" s="593"/>
+      <c r="L7" s="593">
+        <v>2</v>
+      </c>
       <c r="M7" s="328">
         <v>0</v>
       </c>
       <c r="N7" s="107">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O7" s="295">
         <f t="shared" ref="O7:O37" si="10">AC7</f>
-        <v>0</v>
-      </c>
-      <c r="P7" s="749"/>
+        <v>1</v>
+      </c>
+      <c r="P7" s="723"/>
       <c r="Q7" s="20"/>
       <c r="R7" s="2" t="s">
         <v>336</v>
@@ -11004,7 +11013,7 @@
         <v>1</v>
       </c>
       <c r="V7" s="530">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W7" s="316">
         <v>-2</v>
@@ -11014,26 +11023,26 @@
       </c>
       <c r="Y7" s="185">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z7" s="298"/>
       <c r="AA7" s="117">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB7" s="292">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AC7" s="292">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD7" s="292">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AE7" s="296">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF7" s="107">
         <v>0</v>
@@ -11043,7 +11052,7 @@
       </c>
       <c r="AH7" s="298">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI7" s="378"/>
       <c r="AJ7" s="514"/>
@@ -11051,15 +11060,15 @@
       <c r="AL7" s="319"/>
       <c r="AM7" s="339">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN7" s="310">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO7" s="311">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AP7" s="6" t="s">
         <v>241</v>
@@ -11103,7 +11112,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P8" s="749"/>
+      <c r="P8" s="723"/>
       <c r="Q8" s="21" t="s">
         <v>234</v>
       </c>
@@ -11124,7 +11133,7 @@
       </c>
       <c r="W8" s="24">
         <f>V3</f>
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="X8" s="502">
         <v>0</v>
@@ -11194,7 +11203,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P9" s="749"/>
+      <c r="P9" s="723"/>
       <c r="Q9" s="21" t="s">
         <v>336</v>
       </c>
@@ -11299,7 +11308,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P10" s="749"/>
+      <c r="P10" s="723"/>
       <c r="Q10" s="20"/>
       <c r="R10" s="2" t="s">
         <v>341</v>
@@ -11389,7 +11398,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P11" s="749"/>
+      <c r="P11" s="723"/>
       <c r="Q11" s="21" t="s">
         <v>336</v>
       </c>
@@ -11454,14 +11463,14 @@
       <c r="AR11" s="513"/>
     </row>
     <row r="12" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="681" t="s">
+      <c r="A12" s="632" t="s">
         <v>55</v>
       </c>
       <c r="B12" s="30">
         <v>13</v>
       </c>
       <c r="C12" s="2"/>
-      <c r="E12" s="631" t="s">
+      <c r="E12" s="687" t="s">
         <v>56</v>
       </c>
       <c r="G12" s="264"/>
@@ -11486,7 +11495,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P12" s="749"/>
+      <c r="P12" s="723"/>
       <c r="Q12" s="21" t="s">
         <v>336</v>
       </c>
@@ -11563,14 +11572,14 @@
       </c>
     </row>
     <row r="13" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="683"/>
+      <c r="A13" s="634"/>
       <c r="B13" s="597">
         <v>12</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E13" s="632"/>
+      <c r="E13" s="688"/>
       <c r="F13" s="174">
         <v>0</v>
       </c>
@@ -11594,7 +11603,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P13" s="749"/>
+      <c r="P13" s="723"/>
       <c r="Q13" s="21" t="s">
         <v>336</v>
       </c>
@@ -11676,7 +11685,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P14" s="749"/>
+      <c r="P14" s="723"/>
       <c r="Q14" s="20"/>
       <c r="R14" s="202" t="s">
         <v>340</v>
@@ -11779,7 +11788,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P15" s="749"/>
+      <c r="P15" s="723"/>
       <c r="Q15" s="20"/>
       <c r="R15" s="202" t="s">
         <v>340</v>
@@ -11873,7 +11882,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P16" s="749"/>
+      <c r="P16" s="723"/>
       <c r="Q16" s="21" t="s">
         <v>336</v>
       </c>
@@ -11978,7 +11987,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P17" s="749"/>
+      <c r="P17" s="723"/>
       <c r="Q17" s="20"/>
       <c r="R17" s="2" t="s">
         <v>342</v>
@@ -12080,7 +12089,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P18" s="749"/>
+      <c r="P18" s="723"/>
       <c r="Q18" s="21" t="s">
         <v>336</v>
       </c>
@@ -12168,7 +12177,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P19" s="749"/>
+      <c r="P19" s="723"/>
       <c r="Q19" s="20"/>
       <c r="R19" s="2" t="s">
         <v>335</v>
@@ -12278,11 +12287,11 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P20" s="750"/>
+      <c r="P20" s="724"/>
       <c r="Q20" s="609" t="s">
         <v>336</v>
       </c>
-      <c r="R20" s="633"/>
+      <c r="R20" s="689"/>
       <c r="S20" s="540" t="s">
         <v>85</v>
       </c>
@@ -12546,7 +12555,7 @@
     </row>
     <row r="23" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="24"/>
-      <c r="E23" s="688" t="s">
+      <c r="E23" s="639" t="s">
         <v>290</v>
       </c>
       <c r="F23" s="182"/>
@@ -12649,7 +12658,7 @@
       <c r="C24" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="E24" s="689"/>
+      <c r="E24" s="640"/>
       <c r="F24" s="174"/>
       <c r="H24" s="42"/>
       <c r="J24" s="581" t="s">
@@ -12672,7 +12681,7 @@
       <c r="Q24" s="609" t="s">
         <v>336</v>
       </c>
-      <c r="R24" s="633"/>
+      <c r="R24" s="689"/>
       <c r="S24" s="540" t="s">
         <v>250</v>
       </c>
@@ -13323,8 +13332,8 @@
       <c r="AR31" s="513"/>
     </row>
     <row r="32" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="636"/>
-      <c r="B32" s="636"/>
+      <c r="A32" s="656"/>
+      <c r="B32" s="656"/>
       <c r="J32" s="582" t="s">
         <v>310</v>
       </c>
@@ -13667,7 +13676,7 @@
     </row>
     <row r="36" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="24">
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="F36" s="261" t="s">
         <v>44</v>
@@ -13858,12 +13867,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="Q24:R24"/>
-    <mergeCell ref="P4:P20"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="K2:K3"/>
     <mergeCell ref="AM1:AO1"/>
     <mergeCell ref="X1:Y1"/>
     <mergeCell ref="AE1:AG1"/>
@@ -13874,6 +13877,12 @@
     <mergeCell ref="P2:P3"/>
     <mergeCell ref="W2:W3"/>
     <mergeCell ref="T1:T3"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="Q24:R24"/>
+    <mergeCell ref="P4:P20"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="K2:K3"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="Q20:R20"/>
@@ -13939,12 +13948,12 @@
       <c r="P1" s="38"/>
       <c r="S1" s="58">
         <f ca="1">TODAY()</f>
-        <v>45282</v>
+        <v>45283</v>
       </c>
       <c r="V1" s="609" t="s">
         <v>70</v>
       </c>
-      <c r="W1" s="633"/>
+      <c r="W1" s="689"/>
       <c r="X1" s="62" t="s">
         <v>101</v>
       </c>
@@ -13963,7 +13972,7 @@
       <c r="AC1" s="116" t="s">
         <v>190</v>
       </c>
-      <c r="AD1" s="758" t="s">
+      <c r="AD1" s="765" t="s">
         <v>212</v>
       </c>
       <c r="AE1" s="116" t="s">
@@ -13980,10 +13989,10 @@
       <c r="E2" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="F2" s="757" t="s">
+      <c r="F2" s="796" t="s">
         <v>74</v>
       </c>
-      <c r="G2" s="785" t="s">
+      <c r="G2" s="753" t="s">
         <v>44</v>
       </c>
       <c r="H2" s="40" t="s">
@@ -14011,10 +14020,10 @@
       <c r="U2" s="60" t="s">
         <v>105</v>
       </c>
-      <c r="V2" s="729" t="s">
+      <c r="V2" s="732" t="s">
         <v>120</v>
       </c>
-      <c r="W2" s="730"/>
+      <c r="W2" s="733"/>
       <c r="X2" s="64" t="s">
         <v>109</v>
       </c>
@@ -14033,7 +14042,7 @@
       <c r="AC2" s="117" t="s">
         <v>98</v>
       </c>
-      <c r="AD2" s="759"/>
+      <c r="AD2" s="766"/>
       <c r="AE2" s="64" t="s">
         <v>98</v>
       </c>
@@ -14052,8 +14061,8 @@
       <c r="E3" s="39" t="s">
         <v>79</v>
       </c>
-      <c r="F3" s="685"/>
-      <c r="G3" s="786"/>
+      <c r="F3" s="636"/>
+      <c r="G3" s="754"/>
       <c r="H3" s="40" t="s">
         <v>80</v>
       </c>
@@ -14064,13 +14073,13 @@
         <v>81</v>
       </c>
       <c r="N3" s="44"/>
-      <c r="O3" s="795" t="s">
+      <c r="O3" s="763" t="s">
         <v>44</v>
       </c>
-      <c r="P3" s="777" t="s">
+      <c r="P3" s="784" t="s">
         <v>218</v>
       </c>
-      <c r="Q3" s="778"/>
+      <c r="Q3" s="785"/>
       <c r="S3" s="57" t="s">
         <v>219</v>
       </c>
@@ -14080,15 +14089,15 @@
       <c r="W3" s="59" t="s">
         <v>104</v>
       </c>
-      <c r="AD3" s="759"/>
+      <c r="AD3" s="766"/>
     </row>
     <row r="4" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G4" s="786"/>
+      <c r="G4" s="754"/>
       <c r="H4" s="6"/>
       <c r="L4" s="693" t="s">
         <v>82</v>
       </c>
-      <c r="O4" s="796"/>
+      <c r="O4" s="764"/>
       <c r="T4" s="55" t="s">
         <v>97</v>
       </c>
@@ -14102,8 +14111,8 @@
         <v>194</v>
       </c>
       <c r="Z4" s="611"/>
-      <c r="AA4" s="633"/>
-      <c r="AD4" s="759"/>
+      <c r="AA4" s="689"/>
+      <c r="AD4" s="766"/>
     </row>
     <row r="5" spans="1:31" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="52" t="s">
@@ -14118,21 +14127,21 @@
       <c r="F5" s="66" t="s">
         <v>84</v>
       </c>
-      <c r="G5" s="786"/>
+      <c r="G5" s="754"/>
       <c r="H5" s="46" t="s">
         <v>75</v>
       </c>
-      <c r="K5" s="764" t="s">
+      <c r="K5" s="771" t="s">
         <v>216</v>
       </c>
-      <c r="L5" s="779"/>
+      <c r="L5" s="786"/>
       <c r="M5" s="2" t="s">
         <v>214</v>
       </c>
       <c r="N5" s="61" t="s">
         <v>213</v>
       </c>
-      <c r="O5" s="796"/>
+      <c r="O5" s="764"/>
       <c r="P5" s="108" t="s">
         <v>215</v>
       </c>
@@ -14148,11 +14157,11 @@
       <c r="U5" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="Y5" s="767" t="s">
+      <c r="Y5" s="774" t="s">
         <v>283</v>
       </c>
-      <c r="Z5" s="768"/>
-      <c r="AD5" s="759"/>
+      <c r="Z5" s="775"/>
+      <c r="AD5" s="766"/>
     </row>
     <row r="6" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="109"/>
@@ -14162,16 +14171,16 @@
       <c r="E6" s="45" t="s">
         <v>85</v>
       </c>
-      <c r="G6" s="786"/>
+      <c r="G6" s="754"/>
       <c r="H6" s="46" t="s">
         <v>80</v>
       </c>
       <c r="I6" s="23">
         <v>15</v>
       </c>
-      <c r="K6" s="765"/>
-      <c r="L6" s="779"/>
-      <c r="O6" s="796"/>
+      <c r="K6" s="772"/>
+      <c r="L6" s="786"/>
+      <c r="O6" s="764"/>
       <c r="T6" s="2" t="s">
         <v>100</v>
       </c>
@@ -14181,23 +14190,23 @@
       <c r="V6" s="21">
         <v>-1</v>
       </c>
-      <c r="AD6" s="759"/>
+      <c r="AD6" s="766"/>
     </row>
     <row r="7" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="110"/>
-      <c r="G7" s="786"/>
+      <c r="G7" s="754"/>
       <c r="H7" s="6"/>
-      <c r="K7" s="765"/>
-      <c r="L7" s="779"/>
+      <c r="K7" s="772"/>
+      <c r="L7" s="786"/>
       <c r="N7" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="O7" s="796"/>
+      <c r="O7" s="764"/>
       <c r="P7" s="73"/>
       <c r="U7" s="104" t="s">
         <v>20</v>
       </c>
-      <c r="AD7" s="759"/>
+      <c r="AD7" s="766"/>
     </row>
     <row r="8" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="130"/>
@@ -14210,7 +14219,7 @@
       <c r="F8" s="66" t="s">
         <v>86</v>
       </c>
-      <c r="G8" s="786"/>
+      <c r="G8" s="754"/>
       <c r="H8" s="50" t="s">
         <v>75</v>
       </c>
@@ -14220,41 +14229,41 @@
       <c r="J8" s="111">
         <v>115</v>
       </c>
-      <c r="K8" s="765"/>
-      <c r="L8" s="779"/>
-      <c r="O8" s="796"/>
+      <c r="K8" s="772"/>
+      <c r="L8" s="786"/>
+      <c r="O8" s="764"/>
       <c r="P8" s="49"/>
-      <c r="S8" s="761" t="s">
+      <c r="S8" s="768" t="s">
         <v>211</v>
       </c>
-      <c r="T8" s="762"/>
-      <c r="U8" s="762"/>
-      <c r="V8" s="762"/>
-      <c r="W8" s="762"/>
-      <c r="X8" s="762"/>
-      <c r="Y8" s="762"/>
-      <c r="Z8" s="762"/>
-      <c r="AA8" s="762"/>
-      <c r="AB8" s="762"/>
-      <c r="AC8" s="763"/>
-      <c r="AD8" s="759"/>
+      <c r="T8" s="769"/>
+      <c r="U8" s="769"/>
+      <c r="V8" s="769"/>
+      <c r="W8" s="769"/>
+      <c r="X8" s="769"/>
+      <c r="Y8" s="769"/>
+      <c r="Z8" s="769"/>
+      <c r="AA8" s="769"/>
+      <c r="AB8" s="769"/>
+      <c r="AC8" s="770"/>
+      <c r="AD8" s="766"/>
     </row>
     <row r="9" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="751"/>
-      <c r="G9" s="786"/>
+      <c r="C9" s="790"/>
+      <c r="G9" s="754"/>
       <c r="H9" s="6"/>
-      <c r="K9" s="765"/>
-      <c r="L9" s="789" t="s">
+      <c r="K9" s="772"/>
+      <c r="L9" s="757" t="s">
         <v>217</v>
       </c>
-      <c r="M9" s="790"/>
-      <c r="N9" s="791"/>
-      <c r="O9" s="796"/>
+      <c r="M9" s="758"/>
+      <c r="N9" s="759"/>
+      <c r="O9" s="764"/>
       <c r="P9" s="75"/>
-      <c r="AD9" s="759"/>
+      <c r="AD9" s="766"/>
     </row>
     <row r="10" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="752"/>
+      <c r="C10" s="791"/>
       <c r="D10" s="23"/>
       <c r="E10" s="45" t="s">
         <v>87</v>
@@ -14262,7 +14271,7 @@
       <c r="F10" s="66" t="s">
         <v>88</v>
       </c>
-      <c r="G10" s="786"/>
+      <c r="G10" s="754"/>
       <c r="H10" s="51"/>
       <c r="I10" s="21" t="s">
         <v>80</v>
@@ -14270,33 +14279,33 @@
       <c r="J10" s="3">
         <v>15</v>
       </c>
-      <c r="K10" s="765"/>
-      <c r="M10" s="754" t="s">
+      <c r="K10" s="772"/>
+      <c r="M10" s="793" t="s">
         <v>89</v>
       </c>
-      <c r="N10" s="755"/>
-      <c r="O10" s="755"/>
-      <c r="P10" s="755"/>
-      <c r="Q10" s="755"/>
-      <c r="R10" s="755"/>
-      <c r="S10" s="755"/>
-      <c r="T10" s="755"/>
-      <c r="U10" s="755"/>
-      <c r="V10" s="755"/>
-      <c r="W10" s="755"/>
-      <c r="X10" s="755"/>
-      <c r="Y10" s="755"/>
-      <c r="Z10" s="755"/>
-      <c r="AA10" s="755"/>
-      <c r="AB10" s="755"/>
-      <c r="AC10" s="756"/>
-      <c r="AD10" s="759"/>
+      <c r="N10" s="794"/>
+      <c r="O10" s="794"/>
+      <c r="P10" s="794"/>
+      <c r="Q10" s="794"/>
+      <c r="R10" s="794"/>
+      <c r="S10" s="794"/>
+      <c r="T10" s="794"/>
+      <c r="U10" s="794"/>
+      <c r="V10" s="794"/>
+      <c r="W10" s="794"/>
+      <c r="X10" s="794"/>
+      <c r="Y10" s="794"/>
+      <c r="Z10" s="794"/>
+      <c r="AA10" s="794"/>
+      <c r="AB10" s="794"/>
+      <c r="AC10" s="795"/>
+      <c r="AD10" s="766"/>
     </row>
     <row r="11" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="753"/>
-      <c r="G11" s="786"/>
+      <c r="C11" s="792"/>
+      <c r="G11" s="754"/>
       <c r="H11" s="6"/>
-      <c r="K11" s="765"/>
+      <c r="K11" s="772"/>
       <c r="R11" s="52" t="s">
         <v>44</v>
       </c>
@@ -14304,17 +14313,17 @@
       <c r="Y11" s="68" t="s">
         <v>120</v>
       </c>
-      <c r="Z11" s="775" t="s">
+      <c r="Z11" s="782" t="s">
         <v>120</v>
       </c>
-      <c r="AA11" s="776"/>
+      <c r="AA11" s="783"/>
       <c r="AB11" s="52" t="s">
         <v>44</v>
       </c>
       <c r="AC11" s="118" t="s">
         <v>120</v>
       </c>
-      <c r="AD11" s="759"/>
+      <c r="AD11" s="766"/>
     </row>
     <row r="12" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="129"/>
@@ -14327,7 +14336,7 @@
       <c r="F12" s="66" t="s">
         <v>91</v>
       </c>
-      <c r="G12" s="786"/>
+      <c r="G12" s="754"/>
       <c r="H12" s="128"/>
       <c r="I12" s="19" t="s">
         <v>80</v>
@@ -14335,8 +14344,8 @@
       <c r="J12" s="3">
         <v>15</v>
       </c>
-      <c r="K12" s="765"/>
-      <c r="L12" s="780" t="s">
+      <c r="K12" s="772"/>
+      <c r="L12" s="787" t="s">
         <v>92</v>
       </c>
       <c r="M12" s="21" t="s">
@@ -14367,25 +14376,25 @@
         <v>115</v>
       </c>
       <c r="Y12" s="6"/>
-      <c r="AA12" s="769" t="s">
+      <c r="AA12" s="776" t="s">
         <v>125</v>
       </c>
-      <c r="AB12" s="770"/>
+      <c r="AB12" s="777"/>
       <c r="AC12" s="21" t="s">
         <v>231</v>
       </c>
-      <c r="AD12" s="759"/>
+      <c r="AD12" s="766"/>
     </row>
     <row r="13" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="751"/>
-      <c r="G13" s="786"/>
-      <c r="K13" s="765"/>
-      <c r="L13" s="781"/>
+      <c r="C13" s="790"/>
+      <c r="G13" s="754"/>
+      <c r="K13" s="772"/>
+      <c r="L13" s="788"/>
       <c r="M13" s="47"/>
-      <c r="Q13" s="788" t="s">
+      <c r="Q13" s="756" t="s">
         <v>209</v>
       </c>
-      <c r="R13" s="650"/>
+      <c r="R13" s="645"/>
       <c r="S13" s="605"/>
       <c r="T13" s="6"/>
       <c r="U13" s="96" t="s">
@@ -14394,17 +14403,17 @@
       <c r="X13" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="AA13" s="771"/>
-      <c r="AB13" s="772"/>
-      <c r="AD13" s="759"/>
+      <c r="AA13" s="778"/>
+      <c r="AB13" s="779"/>
+      <c r="AD13" s="766"/>
     </row>
     <row r="14" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="C14" s="753"/>
+      <c r="C14" s="792"/>
       <c r="D14" s="23"/>
-      <c r="G14" s="786"/>
+      <c r="G14" s="754"/>
       <c r="H14" s="125"/>
       <c r="I14" s="99" t="s">
         <v>44</v>
@@ -14412,8 +14421,8 @@
       <c r="J14" s="111">
         <v>115</v>
       </c>
-      <c r="K14" s="765"/>
-      <c r="L14" s="781"/>
+      <c r="K14" s="772"/>
+      <c r="L14" s="788"/>
       <c r="M14" s="21" t="s">
         <v>110</v>
       </c>
@@ -14434,9 +14443,9 @@
       <c r="Y14" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="AA14" s="771"/>
-      <c r="AB14" s="772"/>
-      <c r="AD14" s="759"/>
+      <c r="AA14" s="778"/>
+      <c r="AB14" s="779"/>
+      <c r="AD14" s="766"/>
     </row>
     <row r="15" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="130" t="s">
@@ -14451,19 +14460,19 @@
       <c r="F15" s="66" t="s">
         <v>93</v>
       </c>
-      <c r="G15" s="786"/>
+      <c r="G15" s="754"/>
       <c r="H15" s="2" t="s">
         <v>80</v>
       </c>
       <c r="I15" s="53" t="s">
         <v>80</v>
       </c>
-      <c r="K15" s="765"/>
-      <c r="L15" s="782"/>
-      <c r="Q15" s="788" t="s">
+      <c r="K15" s="772"/>
+      <c r="L15" s="789"/>
+      <c r="Q15" s="756" t="s">
         <v>210</v>
       </c>
-      <c r="R15" s="650"/>
+      <c r="R15" s="645"/>
       <c r="S15" s="605"/>
       <c r="T15" s="6"/>
       <c r="V15" s="68" t="s">
@@ -14472,14 +14481,14 @@
       <c r="X15" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="AA15" s="771"/>
-      <c r="AB15" s="772"/>
-      <c r="AD15" s="759"/>
+      <c r="AA15" s="778"/>
+      <c r="AB15" s="779"/>
+      <c r="AD15" s="766"/>
     </row>
     <row r="16" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C16" s="132"/>
-      <c r="G16" s="786"/>
-      <c r="K16" s="765"/>
+      <c r="G16" s="754"/>
+      <c r="K16" s="772"/>
       <c r="N16" s="47"/>
       <c r="O16" s="61" t="s">
         <v>108</v>
@@ -14498,24 +14507,24 @@
       <c r="Z16" s="76" t="s">
         <v>126</v>
       </c>
-      <c r="AA16" s="771"/>
-      <c r="AB16" s="772"/>
-      <c r="AD16" s="759"/>
+      <c r="AA16" s="778"/>
+      <c r="AB16" s="779"/>
+      <c r="AD16" s="766"/>
     </row>
     <row r="17" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C17" s="109"/>
       <c r="E17" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="F17" s="783" t="s">
+      <c r="F17" s="751" t="s">
         <v>95</v>
       </c>
-      <c r="G17" s="786"/>
+      <c r="G17" s="754"/>
       <c r="H17" s="54"/>
       <c r="I17" s="133" t="s">
         <v>80</v>
       </c>
-      <c r="K17" s="765"/>
+      <c r="K17" s="772"/>
       <c r="S17" s="605"/>
       <c r="V17" s="68" t="s">
         <v>44</v>
@@ -14523,9 +14532,9 @@
       <c r="X17" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="AA17" s="771"/>
-      <c r="AB17" s="772"/>
-      <c r="AD17" s="759"/>
+      <c r="AA17" s="778"/>
+      <c r="AB17" s="779"/>
+      <c r="AD17" s="766"/>
     </row>
     <row r="18" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C18" s="130"/>
@@ -14535,15 +14544,15 @@
       <c r="E18" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="F18" s="784"/>
-      <c r="G18" s="786"/>
+      <c r="F18" s="752"/>
+      <c r="G18" s="754"/>
       <c r="H18" s="108" t="s">
         <v>75</v>
       </c>
       <c r="I18" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="K18" s="765"/>
+      <c r="K18" s="772"/>
       <c r="O18" s="64" t="s">
         <v>114</v>
       </c>
@@ -14554,42 +14563,39 @@
       <c r="X18" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="AA18" s="773"/>
-      <c r="AB18" s="774"/>
-      <c r="AD18" s="759"/>
+      <c r="AA18" s="780"/>
+      <c r="AB18" s="781"/>
+      <c r="AD18" s="766"/>
     </row>
     <row r="19" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F19" s="64" t="s">
         <v>208</v>
       </c>
-      <c r="G19" s="787"/>
-      <c r="K19" s="766"/>
+      <c r="G19" s="755"/>
+      <c r="K19" s="773"/>
       <c r="Q19" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="R19" s="792" t="s">
+      <c r="R19" s="760" t="s">
         <v>123</v>
       </c>
-      <c r="S19" s="793"/>
-      <c r="T19" s="794"/>
+      <c r="S19" s="761"/>
+      <c r="T19" s="762"/>
       <c r="V19" s="77" t="s">
         <v>114</v>
       </c>
       <c r="Y19" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="AD19" s="760"/>
+      <c r="AD19" s="767"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="G2:G19"/>
-    <mergeCell ref="Q13:R13"/>
-    <mergeCell ref="Q15:R15"/>
-    <mergeCell ref="L9:N9"/>
-    <mergeCell ref="R19:T19"/>
-    <mergeCell ref="S12:S18"/>
-    <mergeCell ref="O3:O9"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="M10:AC10"/>
+    <mergeCell ref="F2:F3"/>
     <mergeCell ref="AD1:AD19"/>
     <mergeCell ref="S8:AC8"/>
     <mergeCell ref="K5:K19"/>
@@ -14601,11 +14607,14 @@
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="L4:L8"/>
     <mergeCell ref="L12:L15"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="M10:AC10"/>
-    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G2:G19"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="Q15:R15"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="R19:T19"/>
+    <mergeCell ref="S12:S18"/>
+    <mergeCell ref="O3:O9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Boat Halted - Bharat24
Boat Halted - Bharat24

In Valid Token , X-Wbt Not Applicable-X
</commit_message>
<xml_diff>
--- a/System_2.1.8.xlsx
+++ b/System_2.1.8.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Work_For_\Work\Running AppS\System_Work_RW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{468B9EDE-E9D6-407A-A553-2461EECB0696}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE475F5D-84F7-4880-9741-8E4A244AB290}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5063,6 +5063,186 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5075,12 +5255,6 @@
     <xf numFmtId="0" fontId="17" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5092,12 +5266,6 @@
     </xf>
     <xf numFmtId="0" fontId="38" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
@@ -5120,190 +5288,61 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="13" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5345,43 +5384,25 @@
     <xf numFmtId="0" fontId="39" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="43" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5450,46 +5471,46 @@
     <xf numFmtId="14" fontId="5" fillId="14" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5567,46 +5588,25 @@
     <xf numFmtId="0" fontId="3" fillId="21" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -6997,7 +6997,7 @@
       <c r="H1" s="97" t="s">
         <v>344</v>
       </c>
-      <c r="I1" s="619" t="s">
+      <c r="I1" s="665" t="s">
         <v>370</v>
       </c>
       <c r="J1" s="2" t="s">
@@ -7033,7 +7033,7 @@
       <c r="X1" s="434" t="s">
         <v>155</v>
       </c>
-      <c r="Y1" s="663" t="s">
+      <c r="Y1" s="659" t="s">
         <v>530</v>
       </c>
       <c r="Z1" s="410">
@@ -7058,7 +7058,7 @@
         <v>499</v>
       </c>
       <c r="AM1" s="406"/>
-      <c r="AN1" s="646"/>
+      <c r="AN1" s="641"/>
       <c r="AO1" s="341" t="s">
         <v>470</v>
       </c>
@@ -7067,23 +7067,23 @@
       </c>
     </row>
     <row r="2" spans="1:43" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="672">
+      <c r="A2" s="623">
         <f ca="1">TODAY()</f>
         <v>45283</v>
       </c>
-      <c r="B2" s="674" t="s">
+      <c r="B2" s="625" t="s">
         <v>371</v>
       </c>
-      <c r="C2" s="651" t="s">
+      <c r="C2" s="621" t="s">
         <v>358</v>
       </c>
-      <c r="D2" s="676" t="s">
+      <c r="D2" s="627" t="s">
         <v>356</v>
       </c>
-      <c r="E2" s="615" t="s">
+      <c r="E2" s="675" t="s">
         <v>64</v>
       </c>
-      <c r="F2" s="625" t="s">
+      <c r="F2" s="646" t="s">
         <v>102</v>
       </c>
       <c r="G2" s="397" t="s">
@@ -7092,31 +7092,31 @@
       <c r="H2" s="80" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="620"/>
+      <c r="I2" s="666"/>
       <c r="J2" s="81" t="s">
         <v>76</v>
       </c>
-      <c r="K2" s="617" t="s">
+      <c r="K2" s="677" t="s">
         <v>343</v>
       </c>
-      <c r="L2" s="618"/>
-      <c r="M2" s="625" t="s">
+      <c r="L2" s="678"/>
+      <c r="M2" s="646" t="s">
         <v>102</v>
       </c>
       <c r="N2" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="O2" s="655" t="s">
+      <c r="O2" s="650" t="s">
         <v>102</v>
       </c>
       <c r="P2" s="85" t="s">
         <v>147</v>
       </c>
-      <c r="Q2" s="651" t="s">
+      <c r="Q2" s="621" t="s">
         <v>143</v>
       </c>
       <c r="R2" s="604"/>
-      <c r="S2" s="640" t="s">
+      <c r="S2" s="663" t="s">
         <v>148</v>
       </c>
       <c r="T2" s="89"/>
@@ -7126,7 +7126,7 @@
       <c r="X2" s="435" t="s">
         <v>156</v>
       </c>
-      <c r="Y2" s="664"/>
+      <c r="Y2" s="660"/>
       <c r="Z2" s="411">
         <v>1</v>
       </c>
@@ -7149,15 +7149,15 @@
         <v>464</v>
       </c>
       <c r="AM2" s="432"/>
-      <c r="AN2" s="647"/>
+      <c r="AN2" s="642"/>
     </row>
     <row r="3" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="673"/>
-      <c r="B3" s="675"/>
-      <c r="C3" s="652"/>
-      <c r="D3" s="677"/>
-      <c r="E3" s="616"/>
-      <c r="F3" s="626"/>
+      <c r="A3" s="624"/>
+      <c r="B3" s="626"/>
+      <c r="C3" s="622"/>
+      <c r="D3" s="628"/>
+      <c r="E3" s="676"/>
+      <c r="F3" s="647"/>
       <c r="G3" s="398" t="s">
         <v>28</v>
       </c>
@@ -7176,17 +7176,17 @@
       <c r="L3" s="203" t="s">
         <v>107</v>
       </c>
-      <c r="M3" s="626"/>
+      <c r="M3" s="647"/>
       <c r="N3" s="69" t="s">
         <v>146</v>
       </c>
-      <c r="O3" s="656"/>
+      <c r="O3" s="651"/>
       <c r="P3" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="Q3" s="652"/>
+      <c r="Q3" s="622"/>
       <c r="R3" s="606"/>
-      <c r="S3" s="642"/>
+      <c r="S3" s="664"/>
       <c r="T3" s="89"/>
       <c r="U3" s="124"/>
       <c r="V3" s="120"/>
@@ -7194,7 +7194,7 @@
       <c r="X3" s="435" t="s">
         <v>157</v>
       </c>
-      <c r="Y3" s="664"/>
+      <c r="Y3" s="660"/>
       <c r="Z3" s="412">
         <v>1</v>
       </c>
@@ -7203,7 +7203,7 @@
       <c r="AC3" s="100" t="s">
         <v>481</v>
       </c>
-      <c r="AD3" s="637" t="s">
+      <c r="AD3" s="662" t="s">
         <v>456</v>
       </c>
       <c r="AE3" s="259"/>
@@ -7215,16 +7215,16 @@
       <c r="AK3" s="259"/>
       <c r="AL3" s="16"/>
       <c r="AM3" s="432"/>
-      <c r="AN3" s="647"/>
+      <c r="AN3" s="642"/>
     </row>
     <row r="4" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="240" t="s">
         <v>183</v>
       </c>
-      <c r="B4" s="688" t="s">
+      <c r="B4" s="639" t="s">
         <v>374</v>
       </c>
-      <c r="C4" s="651" t="s">
+      <c r="C4" s="621" t="s">
         <v>154</v>
       </c>
       <c r="D4" s="350" t="s">
@@ -7233,7 +7233,7 @@
       <c r="E4" s="381">
         <v>2</v>
       </c>
-      <c r="F4" s="626"/>
+      <c r="F4" s="647"/>
       <c r="G4" s="384" t="s">
         <v>202</v>
       </c>
@@ -7250,11 +7250,11 @@
         <v>150</v>
       </c>
       <c r="L4" s="206"/>
-      <c r="M4" s="626"/>
+      <c r="M4" s="647"/>
       <c r="N4" s="176" t="s">
         <v>69</v>
       </c>
-      <c r="O4" s="656"/>
+      <c r="O4" s="651"/>
       <c r="P4" s="2" t="s">
         <v>191</v>
       </c>
@@ -7276,12 +7276,12 @@
       <c r="X4" s="435" t="s">
         <v>158</v>
       </c>
-      <c r="Y4" s="664"/>
+      <c r="Y4" s="660"/>
       <c r="Z4" s="413"/>
       <c r="AA4" s="309"/>
       <c r="AB4" s="211"/>
       <c r="AC4" s="16"/>
-      <c r="AD4" s="637"/>
+      <c r="AD4" s="662"/>
       <c r="AE4" s="259"/>
       <c r="AF4" s="259"/>
       <c r="AG4" s="16"/>
@@ -7291,37 +7291,37 @@
       <c r="AK4" s="259"/>
       <c r="AL4" s="16"/>
       <c r="AM4" s="432"/>
-      <c r="AN4" s="647"/>
+      <c r="AN4" s="642"/>
       <c r="AO4" s="341" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="619" t="s">
+      <c r="A5" s="665" t="s">
         <v>419</v>
       </c>
-      <c r="B5" s="689"/>
-      <c r="C5" s="652"/>
+      <c r="B5" s="640"/>
+      <c r="C5" s="622"/>
       <c r="D5" s="61" t="s">
         <v>153</v>
       </c>
       <c r="E5" s="382">
         <v>1</v>
       </c>
-      <c r="F5" s="626"/>
-      <c r="G5" s="680" t="s">
+      <c r="F5" s="647"/>
+      <c r="G5" s="631" t="s">
         <v>192</v>
       </c>
-      <c r="H5" s="680"/>
-      <c r="I5" s="680"/>
-      <c r="J5" s="680"/>
-      <c r="K5" s="680"/>
-      <c r="L5" s="681"/>
-      <c r="M5" s="626"/>
+      <c r="H5" s="631"/>
+      <c r="I5" s="631"/>
+      <c r="J5" s="631"/>
+      <c r="K5" s="631"/>
+      <c r="L5" s="632"/>
+      <c r="M5" s="647"/>
       <c r="N5" s="21">
         <v>8</v>
       </c>
-      <c r="O5" s="656"/>
+      <c r="O5" s="651"/>
       <c r="T5" s="89"/>
       <c r="U5" s="124"/>
       <c r="V5" s="120"/>
@@ -7329,7 +7329,7 @@
       <c r="X5" s="435" t="s">
         <v>159</v>
       </c>
-      <c r="Y5" s="664"/>
+      <c r="Y5" s="660"/>
       <c r="Z5" s="413">
         <v>1</v>
       </c>
@@ -7352,24 +7352,24 @@
       <c r="AK5" s="259"/>
       <c r="AL5" s="80"/>
       <c r="AM5" s="432"/>
-      <c r="AN5" s="647"/>
+      <c r="AN5" s="642"/>
     </row>
     <row r="6" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="620"/>
-      <c r="B6" s="686" t="s">
+      <c r="A6" s="666"/>
+      <c r="B6" s="637" t="s">
         <v>177</v>
       </c>
-      <c r="C6" s="634"/>
-      <c r="D6" s="635"/>
-      <c r="F6" s="626"/>
-      <c r="G6" s="682"/>
-      <c r="H6" s="682"/>
-      <c r="I6" s="682"/>
-      <c r="J6" s="682"/>
-      <c r="K6" s="682"/>
-      <c r="L6" s="683"/>
-      <c r="M6" s="626"/>
-      <c r="O6" s="656"/>
+      <c r="C6" s="667"/>
+      <c r="D6" s="668"/>
+      <c r="F6" s="647"/>
+      <c r="G6" s="633"/>
+      <c r="H6" s="633"/>
+      <c r="I6" s="633"/>
+      <c r="J6" s="633"/>
+      <c r="K6" s="633"/>
+      <c r="L6" s="634"/>
+      <c r="M6" s="647"/>
+      <c r="O6" s="651"/>
       <c r="T6" s="89"/>
       <c r="U6" s="124"/>
       <c r="V6" s="98" t="s">
@@ -7379,7 +7379,7 @@
       <c r="X6" s="435" t="s">
         <v>160</v>
       </c>
-      <c r="Y6" s="664"/>
+      <c r="Y6" s="660"/>
       <c r="Z6" s="411">
         <v>1</v>
       </c>
@@ -7393,16 +7393,16 @@
       <c r="AF6" s="259"/>
       <c r="AG6" s="259"/>
       <c r="AH6" s="259"/>
-      <c r="AI6" s="636"/>
+      <c r="AI6" s="656"/>
       <c r="AJ6" s="445" t="s">
         <v>459</v>
       </c>
-      <c r="AK6" s="636" t="s">
+      <c r="AK6" s="656" t="s">
         <v>252</v>
       </c>
       <c r="AL6" s="259"/>
       <c r="AM6" s="432"/>
-      <c r="AN6" s="647"/>
+      <c r="AN6" s="642"/>
       <c r="AO6" s="341" t="s">
         <v>471</v>
       </c>
@@ -7411,7 +7411,7 @@
       <c r="A7" s="234" t="s">
         <v>574</v>
       </c>
-      <c r="B7" s="687"/>
+      <c r="B7" s="638"/>
       <c r="C7" s="204" t="s">
         <v>375</v>
       </c>
@@ -7421,7 +7421,7 @@
       <c r="E7" s="267">
         <v>3</v>
       </c>
-      <c r="F7" s="626"/>
+      <c r="F7" s="647"/>
       <c r="G7" s="399">
         <v>0</v>
       </c>
@@ -7440,8 +7440,8 @@
       <c r="L7" s="214">
         <v>0</v>
       </c>
-      <c r="M7" s="626"/>
-      <c r="O7" s="656"/>
+      <c r="M7" s="647"/>
+      <c r="O7" s="651"/>
       <c r="R7" s="99" t="s">
         <v>44</v>
       </c>
@@ -7455,7 +7455,7 @@
       <c r="X7" s="435" t="s">
         <v>161</v>
       </c>
-      <c r="Y7" s="664"/>
+      <c r="Y7" s="660"/>
       <c r="Z7" s="411">
         <v>1</v>
       </c>
@@ -7465,18 +7465,18 @@
       <c r="AD7" s="16"/>
       <c r="AE7" s="259"/>
       <c r="AF7" s="259"/>
-      <c r="AG7" s="637" t="s">
+      <c r="AG7" s="662" t="s">
         <v>455</v>
       </c>
       <c r="AH7" s="259"/>
-      <c r="AI7" s="636"/>
+      <c r="AI7" s="656"/>
       <c r="AJ7" s="259"/>
-      <c r="AK7" s="636"/>
+      <c r="AK7" s="656"/>
       <c r="AL7" s="80" t="s">
         <v>497</v>
       </c>
       <c r="AM7" s="432"/>
-      <c r="AN7" s="647"/>
+      <c r="AN7" s="642"/>
       <c r="AP7" s="76" t="s">
         <v>472</v>
       </c>
@@ -7493,27 +7493,27 @@
         <f>SUM(G7:N9)</f>
         <v>15</v>
       </c>
-      <c r="F8" s="626"/>
-      <c r="G8" s="681">
-        <v>0</v>
-      </c>
-      <c r="H8" s="678" t="s">
+      <c r="F8" s="647"/>
+      <c r="G8" s="632">
+        <v>0</v>
+      </c>
+      <c r="H8" s="629" t="s">
         <v>104</v>
       </c>
       <c r="I8" s="604">
         <v>0</v>
       </c>
-      <c r="J8" s="678" t="s">
+      <c r="J8" s="629" t="s">
         <v>104</v>
       </c>
-      <c r="K8" s="684"/>
-      <c r="L8" s="638"/>
-      <c r="M8" s="653"/>
-      <c r="N8" s="643">
+      <c r="K8" s="635"/>
+      <c r="L8" s="669"/>
+      <c r="M8" s="648"/>
+      <c r="N8" s="672">
         <f>N5+N11</f>
         <v>15</v>
       </c>
-      <c r="O8" s="656"/>
+      <c r="O8" s="651"/>
       <c r="T8" s="103" t="s">
         <v>44</v>
       </c>
@@ -7523,7 +7523,7 @@
       <c r="X8" s="435" t="s">
         <v>162</v>
       </c>
-      <c r="Y8" s="664"/>
+      <c r="Y8" s="660"/>
       <c r="Z8" s="413"/>
       <c r="AA8" s="309"/>
       <c r="AB8" s="211"/>
@@ -7531,14 +7531,14 @@
       <c r="AD8" s="16"/>
       <c r="AE8" s="259"/>
       <c r="AF8" s="259"/>
-      <c r="AG8" s="637"/>
+      <c r="AG8" s="662"/>
       <c r="AH8" s="259"/>
-      <c r="AI8" s="636"/>
+      <c r="AI8" s="656"/>
       <c r="AJ8" s="259"/>
       <c r="AK8" s="259"/>
       <c r="AL8" s="259"/>
       <c r="AM8" s="432"/>
-      <c r="AN8" s="647"/>
+      <c r="AN8" s="642"/>
     </row>
     <row r="9" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="234" t="s">
@@ -7553,17 +7553,17 @@
       <c r="D9" s="351" t="s">
         <v>282</v>
       </c>
-      <c r="F9" s="626"/>
-      <c r="G9" s="683"/>
-      <c r="H9" s="679"/>
+      <c r="F9" s="647"/>
+      <c r="G9" s="634"/>
+      <c r="H9" s="630"/>
       <c r="I9" s="606"/>
-      <c r="J9" s="679"/>
-      <c r="K9" s="685"/>
-      <c r="L9" s="639"/>
-      <c r="M9" s="654"/>
-      <c r="N9" s="644"/>
-      <c r="O9" s="657"/>
-      <c r="S9" s="640" t="s">
+      <c r="J9" s="630"/>
+      <c r="K9" s="636"/>
+      <c r="L9" s="670"/>
+      <c r="M9" s="649"/>
+      <c r="N9" s="673"/>
+      <c r="O9" s="652"/>
+      <c r="S9" s="663" t="s">
         <v>61</v>
       </c>
       <c r="T9" s="89"/>
@@ -7575,7 +7575,7 @@
       <c r="X9" s="435" t="s">
         <v>163</v>
       </c>
-      <c r="Y9" s="664"/>
+      <c r="Y9" s="660"/>
       <c r="Z9" s="414"/>
       <c r="AA9" s="309"/>
       <c r="AB9" s="211"/>
@@ -7585,16 +7585,16 @@
       </c>
       <c r="AE9" s="259"/>
       <c r="AF9" s="259"/>
-      <c r="AG9" s="637"/>
+      <c r="AG9" s="662"/>
       <c r="AH9" s="259"/>
-      <c r="AI9" s="636"/>
+      <c r="AI9" s="656"/>
       <c r="AJ9" s="80"/>
-      <c r="AK9" s="636" t="s">
+      <c r="AK9" s="656" t="s">
         <v>252</v>
       </c>
       <c r="AL9" s="259"/>
       <c r="AM9" s="432"/>
-      <c r="AN9" s="647"/>
+      <c r="AN9" s="642"/>
       <c r="AP9" s="2" t="s">
         <v>509</v>
       </c>
@@ -7611,20 +7611,20 @@
         <f>Boat!W8</f>
         <v>36</v>
       </c>
-      <c r="F10" s="626"/>
+      <c r="F10" s="647"/>
       <c r="N10" s="422" t="s">
         <v>397</v>
       </c>
-      <c r="O10" s="628" t="s">
+      <c r="O10" s="684" t="s">
         <v>102</v>
       </c>
-      <c r="P10" s="658" t="s">
+      <c r="P10" s="653" t="s">
         <v>401</v>
       </c>
       <c r="R10" s="74" t="s">
         <v>44</v>
       </c>
-      <c r="S10" s="641"/>
+      <c r="S10" s="671"/>
       <c r="T10" s="89"/>
       <c r="U10" s="123" t="s">
         <v>176</v>
@@ -7636,7 +7636,7 @@
       <c r="X10" s="435" t="s">
         <v>164</v>
       </c>
-      <c r="Y10" s="664"/>
+      <c r="Y10" s="660"/>
       <c r="Z10" s="413">
         <v>0</v>
       </c>
@@ -7654,16 +7654,16 @@
       <c r="AF10" s="240" t="s">
         <v>312</v>
       </c>
-      <c r="AG10" s="637"/>
+      <c r="AG10" s="662"/>
       <c r="AH10" s="80"/>
-      <c r="AI10" s="636"/>
+      <c r="AI10" s="656"/>
       <c r="AJ10" s="259"/>
-      <c r="AK10" s="636"/>
+      <c r="AK10" s="656"/>
       <c r="AL10" s="259"/>
       <c r="AM10" s="446" t="s">
         <v>319</v>
       </c>
-      <c r="AN10" s="647"/>
+      <c r="AN10" s="642"/>
       <c r="AO10" s="206" t="s">
         <v>94</v>
       </c>
@@ -7681,18 +7681,18 @@
       <c r="D11" s="172" t="s">
         <v>356</v>
       </c>
-      <c r="F11" s="626"/>
+      <c r="F11" s="647"/>
       <c r="M11" s="6"/>
       <c r="N11" s="117">
         <v>7</v>
       </c>
-      <c r="O11" s="629"/>
-      <c r="P11" s="659"/>
+      <c r="O11" s="685"/>
+      <c r="P11" s="654"/>
       <c r="Q11" s="65"/>
       <c r="R11" s="120" t="s">
         <v>221</v>
       </c>
-      <c r="S11" s="641"/>
+      <c r="S11" s="671"/>
       <c r="T11" s="102" t="s">
         <v>44</v>
       </c>
@@ -7702,7 +7702,7 @@
       <c r="X11" s="435" t="s">
         <v>165</v>
       </c>
-      <c r="Y11" s="664"/>
+      <c r="Y11" s="660"/>
       <c r="Z11" s="413"/>
       <c r="AA11" s="309">
         <v>1</v>
@@ -7716,14 +7716,14 @@
       <c r="AF11" s="259" t="s">
         <v>477</v>
       </c>
-      <c r="AG11" s="637"/>
+      <c r="AG11" s="662"/>
       <c r="AH11" s="259"/>
       <c r="AI11" s="70"/>
       <c r="AJ11" s="259"/>
       <c r="AK11" s="259"/>
       <c r="AL11" s="259"/>
       <c r="AM11" s="432"/>
-      <c r="AN11" s="647"/>
+      <c r="AN11" s="642"/>
       <c r="AP11" s="76" t="s">
         <v>485</v>
       </c>
@@ -7742,7 +7742,7 @@
       <c r="E12" s="226">
         <v>3</v>
       </c>
-      <c r="F12" s="626"/>
+      <c r="F12" s="647"/>
       <c r="G12" s="340" t="s">
         <v>401</v>
       </c>
@@ -7751,16 +7751,16 @@
       </c>
       <c r="I12" s="611"/>
       <c r="J12" s="611"/>
-      <c r="K12" s="633"/>
+      <c r="K12" s="689"/>
       <c r="L12" s="205"/>
       <c r="M12" s="205"/>
       <c r="N12" s="205"/>
-      <c r="O12" s="629"/>
-      <c r="P12" s="659"/>
+      <c r="O12" s="685"/>
+      <c r="P12" s="654"/>
       <c r="R12" s="122" t="s">
         <v>180</v>
       </c>
-      <c r="S12" s="642"/>
+      <c r="S12" s="664"/>
       <c r="T12" s="101" t="s">
         <v>44</v>
       </c>
@@ -7770,7 +7770,7 @@
       <c r="X12" s="435" t="s">
         <v>166</v>
       </c>
-      <c r="Y12" s="664"/>
+      <c r="Y12" s="660"/>
       <c r="Z12" s="411">
         <v>1</v>
       </c>
@@ -7781,16 +7781,16 @@
       <c r="AC12" s="100" t="s">
         <v>482</v>
       </c>
-      <c r="AD12" s="645" t="s">
+      <c r="AD12" s="674" t="s">
         <v>241</v>
       </c>
       <c r="AE12" s="445" t="s">
         <v>240</v>
       </c>
-      <c r="AF12" s="637" t="s">
+      <c r="AF12" s="662" t="s">
         <v>229</v>
       </c>
-      <c r="AG12" s="637"/>
+      <c r="AG12" s="662"/>
       <c r="AH12" s="240" t="s">
         <v>260</v>
       </c>
@@ -7800,10 +7800,10 @@
       <c r="AJ12" s="259"/>
       <c r="AK12" s="259"/>
       <c r="AL12" s="259"/>
-      <c r="AM12" s="661" t="s">
+      <c r="AM12" s="657" t="s">
         <v>250</v>
       </c>
-      <c r="AN12" s="647"/>
+      <c r="AN12" s="642"/>
       <c r="AO12" s="341" t="s">
         <v>96</v>
       </c>
@@ -7815,17 +7815,17 @@
       <c r="E13" s="452">
         <v>-3</v>
       </c>
-      <c r="F13" s="626"/>
+      <c r="F13" s="647"/>
       <c r="G13" s="611" t="s">
         <v>431</v>
       </c>
       <c r="H13" s="611"/>
       <c r="I13" s="611"/>
-      <c r="J13" s="633"/>
+      <c r="J13" s="689"/>
       <c r="M13" s="6"/>
       <c r="N13" s="6"/>
-      <c r="O13" s="629"/>
-      <c r="P13" s="660"/>
+      <c r="O13" s="685"/>
+      <c r="P13" s="655"/>
       <c r="T13" s="105" t="s">
         <v>44</v>
       </c>
@@ -7835,7 +7835,7 @@
       <c r="X13" s="435" t="s">
         <v>167</v>
       </c>
-      <c r="Y13" s="664"/>
+      <c r="Y13" s="660"/>
       <c r="Z13" s="411">
         <v>1</v>
       </c>
@@ -7846,8 +7846,8 @@
         <v>501</v>
       </c>
       <c r="AC13" s="16"/>
-      <c r="AD13" s="645"/>
-      <c r="AF13" s="637"/>
+      <c r="AD13" s="674"/>
+      <c r="AF13" s="662"/>
       <c r="AG13" s="80"/>
       <c r="AH13" s="240" t="s">
         <v>309</v>
@@ -7858,8 +7858,8 @@
       <c r="AJ13" s="80"/>
       <c r="AK13" s="259"/>
       <c r="AL13" s="259"/>
-      <c r="AM13" s="661"/>
-      <c r="AN13" s="647"/>
+      <c r="AM13" s="657"/>
+      <c r="AN13" s="642"/>
     </row>
     <row r="14" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="454"/>
@@ -7867,18 +7867,18 @@
       <c r="C14" s="463"/>
       <c r="D14" s="456"/>
       <c r="E14" s="457"/>
-      <c r="F14" s="626"/>
+      <c r="F14" s="647"/>
       <c r="G14" s="611" t="s">
         <v>430</v>
       </c>
       <c r="H14" s="611"/>
       <c r="I14" s="611"/>
-      <c r="J14" s="633"/>
+      <c r="J14" s="689"/>
       <c r="K14" s="2">
         <v>12</v>
       </c>
       <c r="N14" s="6"/>
-      <c r="O14" s="629"/>
+      <c r="O14" s="685"/>
       <c r="Q14" s="61" t="s">
         <v>534</v>
       </c>
@@ -7892,24 +7892,24 @@
       <c r="X14" s="435" t="s">
         <v>168</v>
       </c>
-      <c r="Y14" s="664"/>
+      <c r="Y14" s="660"/>
       <c r="Z14" s="411">
         <v>1</v>
       </c>
       <c r="AA14" s="309"/>
       <c r="AB14" s="211"/>
       <c r="AC14" s="16"/>
-      <c r="AD14" s="645"/>
+      <c r="AD14" s="674"/>
       <c r="AE14" s="259"/>
-      <c r="AF14" s="637"/>
+      <c r="AF14" s="662"/>
       <c r="AG14" s="259"/>
       <c r="AH14" s="259"/>
       <c r="AI14" s="70"/>
       <c r="AJ14" s="259"/>
       <c r="AK14" s="259"/>
       <c r="AL14" s="259"/>
-      <c r="AM14" s="661"/>
-      <c r="AN14" s="647"/>
+      <c r="AM14" s="657"/>
+      <c r="AN14" s="642"/>
     </row>
     <row r="15" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="453" t="s">
@@ -7918,8 +7918,8 @@
       <c r="C15" s="604" t="s">
         <v>374</v>
       </c>
-      <c r="F15" s="626"/>
-      <c r="O15" s="629"/>
+      <c r="F15" s="647"/>
+      <c r="O15" s="685"/>
       <c r="R15" s="99" t="s">
         <v>44</v>
       </c>
@@ -7932,7 +7932,7 @@
       <c r="X15" s="435" t="s">
         <v>169</v>
       </c>
-      <c r="Y15" s="664"/>
+      <c r="Y15" s="660"/>
       <c r="Z15" s="413">
         <v>1</v>
       </c>
@@ -7941,8 +7941,8 @@
       <c r="AC15" s="76" t="s">
         <v>480</v>
       </c>
-      <c r="AD15" s="645"/>
-      <c r="AF15" s="637"/>
+      <c r="AD15" s="674"/>
+      <c r="AF15" s="662"/>
       <c r="AG15" s="80"/>
       <c r="AH15" s="240" t="s">
         <v>449</v>
@@ -7955,8 +7955,8 @@
       </c>
       <c r="AK15" s="259"/>
       <c r="AL15" s="259"/>
-      <c r="AM15" s="661"/>
-      <c r="AN15" s="647"/>
+      <c r="AM15" s="657"/>
+      <c r="AN15" s="642"/>
       <c r="AP15" s="76" t="s">
         <v>73</v>
       </c>
@@ -7978,13 +7978,13 @@
       <c r="E16" s="226">
         <v>1</v>
       </c>
-      <c r="F16" s="626"/>
+      <c r="F16" s="647"/>
       <c r="G16" s="340" t="s">
         <v>489</v>
       </c>
       <c r="I16" s="474"/>
       <c r="J16" s="20"/>
-      <c r="O16" s="629"/>
+      <c r="O16" s="685"/>
       <c r="R16" s="439" t="s">
         <v>184</v>
       </c>
@@ -7995,7 +7995,7 @@
       <c r="X16" s="435" t="s">
         <v>170</v>
       </c>
-      <c r="Y16" s="664"/>
+      <c r="Y16" s="660"/>
       <c r="Z16" s="411">
         <v>1</v>
       </c>
@@ -8016,18 +8016,18 @@
       <c r="AM16" s="432" t="s">
         <v>318</v>
       </c>
-      <c r="AN16" s="647"/>
+      <c r="AN16" s="642"/>
       <c r="AP16" s="76" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="17" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="80"/>
-      <c r="F17" s="626"/>
+      <c r="F17" s="647"/>
       <c r="I17" s="475"/>
       <c r="J17" s="20"/>
       <c r="N17" s="6"/>
-      <c r="O17" s="629"/>
+      <c r="O17" s="685"/>
       <c r="Q17" s="21" t="s">
         <v>532</v>
       </c>
@@ -8047,7 +8047,7 @@
       <c r="X17" s="435" t="s">
         <v>171</v>
       </c>
-      <c r="Y17" s="664"/>
+      <c r="Y17" s="660"/>
       <c r="Z17" s="413"/>
       <c r="AA17" s="309"/>
       <c r="AB17" s="211"/>
@@ -8072,7 +8072,7 @@
       <c r="AK17" s="259"/>
       <c r="AL17" s="80"/>
       <c r="AM17" s="432"/>
-      <c r="AN17" s="647"/>
+      <c r="AN17" s="642"/>
       <c r="AO17" s="206" t="s">
         <v>498</v>
       </c>
@@ -8096,21 +8096,21 @@
       <c r="E18" s="99" t="s">
         <v>44</v>
       </c>
-      <c r="F18" s="626"/>
+      <c r="F18" s="647"/>
       <c r="G18" s="340" t="s">
         <v>529</v>
       </c>
       <c r="I18" s="24"/>
       <c r="J18" s="20"/>
-      <c r="O18" s="629"/>
+      <c r="O18" s="685"/>
       <c r="Q18" s="112"/>
-      <c r="R18" s="621" t="s">
+      <c r="R18" s="679" t="s">
         <v>537</v>
       </c>
       <c r="T18" s="100" t="s">
         <v>44</v>
       </c>
-      <c r="U18" s="669" t="s">
+      <c r="U18" s="618" t="s">
         <v>44</v>
       </c>
       <c r="V18" s="120"/>
@@ -8120,7 +8120,7 @@
       <c r="X18" s="435" t="s">
         <v>172</v>
       </c>
-      <c r="Y18" s="664"/>
+      <c r="Y18" s="660"/>
       <c r="Z18" s="413">
         <v>1</v>
       </c>
@@ -8131,38 +8131,38 @@
       <c r="AC18" s="16"/>
       <c r="AD18" s="16"/>
       <c r="AE18" s="259"/>
-      <c r="AF18" s="636" t="s">
+      <c r="AF18" s="656" t="s">
         <v>476</v>
       </c>
       <c r="AG18" s="259"/>
       <c r="AH18" s="70"/>
       <c r="AI18" s="70"/>
-      <c r="AJ18" s="662" t="s">
+      <c r="AJ18" s="658" t="s">
         <v>316</v>
       </c>
       <c r="AK18" s="259"/>
       <c r="AL18" s="80"/>
       <c r="AM18" s="432"/>
-      <c r="AN18" s="647"/>
+      <c r="AN18" s="642"/>
       <c r="AP18" s="76" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F19" s="626"/>
+      <c r="F19" s="647"/>
       <c r="I19" s="221"/>
-      <c r="O19" s="629"/>
-      <c r="R19" s="622"/>
+      <c r="O19" s="685"/>
+      <c r="R19" s="680"/>
       <c r="S19" s="30" t="s">
         <v>535</v>
       </c>
-      <c r="U19" s="670"/>
+      <c r="U19" s="619"/>
       <c r="V19" s="146"/>
       <c r="W19" s="146"/>
       <c r="X19" s="435" t="s">
         <v>173</v>
       </c>
-      <c r="Y19" s="664"/>
+      <c r="Y19" s="660"/>
       <c r="Z19" s="411">
         <v>1</v>
       </c>
@@ -8171,17 +8171,17 @@
       <c r="AC19" s="16"/>
       <c r="AD19" s="16"/>
       <c r="AE19" s="259"/>
-      <c r="AF19" s="636"/>
+      <c r="AF19" s="656"/>
       <c r="AG19" s="259"/>
       <c r="AH19" s="259"/>
       <c r="AI19" s="70"/>
-      <c r="AJ19" s="662"/>
+      <c r="AJ19" s="658"/>
       <c r="AK19" s="464" t="s">
         <v>252</v>
       </c>
       <c r="AL19" s="80"/>
       <c r="AM19" s="432"/>
-      <c r="AN19" s="647"/>
+      <c r="AN19" s="642"/>
       <c r="AP19" s="76" t="s">
         <v>469</v>
       </c>
@@ -8202,24 +8202,24 @@
       <c r="E20" s="441">
         <v>-1</v>
       </c>
-      <c r="F20" s="626"/>
+      <c r="F20" s="647"/>
       <c r="G20" s="340" t="s">
         <v>492</v>
       </c>
       <c r="I20" s="221"/>
-      <c r="O20" s="629"/>
-      <c r="Q20" s="631" t="s">
+      <c r="O20" s="685"/>
+      <c r="Q20" s="687" t="s">
         <v>48</v>
       </c>
       <c r="T20" s="408" t="s">
         <v>44</v>
       </c>
-      <c r="U20" s="671"/>
+      <c r="U20" s="620"/>
       <c r="W20" s="409"/>
       <c r="X20" s="436" t="s">
         <v>174</v>
       </c>
-      <c r="Y20" s="664"/>
+      <c r="Y20" s="660"/>
       <c r="Z20" s="415">
         <v>1</v>
       </c>
@@ -8244,7 +8244,7 @@
       <c r="AM20" s="384" t="s">
         <v>250</v>
       </c>
-      <c r="AN20" s="647"/>
+      <c r="AN20" s="642"/>
       <c r="AO20" s="341" t="s">
         <v>461</v>
       </c>
@@ -8265,20 +8265,20 @@
       <c r="E21" s="267">
         <v>0</v>
       </c>
-      <c r="F21" s="626"/>
+      <c r="F21" s="647"/>
       <c r="I21" s="221"/>
-      <c r="O21" s="629"/>
-      <c r="Q21" s="632"/>
+      <c r="O21" s="685"/>
+      <c r="Q21" s="688"/>
       <c r="T21" s="426"/>
       <c r="U21" s="14"/>
-      <c r="V21" s="666"/>
+      <c r="V21" s="615"/>
       <c r="W21" s="430" t="s">
         <v>175</v>
       </c>
       <c r="X21" s="433" t="s">
         <v>186</v>
       </c>
-      <c r="Y21" s="664"/>
+      <c r="Y21" s="660"/>
       <c r="Z21" s="449">
         <v>3</v>
       </c>
@@ -8309,15 +8309,15 @@
       <c r="AM21" s="432" t="s">
         <v>546</v>
       </c>
-      <c r="AN21" s="647"/>
+      <c r="AN21" s="642"/>
     </row>
     <row r="22" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F22" s="626"/>
+      <c r="F22" s="647"/>
       <c r="G22" s="340" t="s">
         <v>490</v>
       </c>
       <c r="I22" s="221"/>
-      <c r="O22" s="629"/>
+      <c r="O22" s="685"/>
       <c r="R22" s="438" t="s">
         <v>44</v>
       </c>
@@ -8325,14 +8325,14 @@
         <v>44</v>
       </c>
       <c r="U22" s="15"/>
-      <c r="V22" s="667"/>
+      <c r="V22" s="616"/>
       <c r="W22" s="430" t="s">
         <v>175</v>
       </c>
       <c r="X22" s="433" t="s">
         <v>187</v>
       </c>
-      <c r="Y22" s="664"/>
+      <c r="Y22" s="660"/>
       <c r="Z22" s="419"/>
       <c r="AA22" s="10"/>
       <c r="AB22" s="419"/>
@@ -8343,7 +8343,7 @@
       <c r="AG22" s="6"/>
       <c r="AH22" s="6"/>
       <c r="AI22" s="6"/>
-      <c r="AJ22" s="636" t="s">
+      <c r="AJ22" s="656" t="s">
         <v>473</v>
       </c>
       <c r="AK22" s="259"/>
@@ -8351,7 +8351,7 @@
         <v>479</v>
       </c>
       <c r="AM22" s="302"/>
-      <c r="AN22" s="647"/>
+      <c r="AN22" s="642"/>
     </row>
     <row r="23" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="233" t="s">
@@ -8369,22 +8369,22 @@
       <c r="E23" s="227">
         <v>1</v>
       </c>
-      <c r="F23" s="626"/>
+      <c r="F23" s="647"/>
       <c r="I23" s="221"/>
-      <c r="O23" s="629"/>
-      <c r="Q23" s="631" t="s">
+      <c r="O23" s="685"/>
+      <c r="Q23" s="687" t="s">
         <v>144</v>
       </c>
       <c r="T23" s="17"/>
       <c r="U23" s="424" t="s">
         <v>44</v>
       </c>
-      <c r="V23" s="667"/>
+      <c r="V23" s="616"/>
       <c r="W23" s="148"/>
       <c r="X23" s="433" t="s">
         <v>188</v>
       </c>
-      <c r="Y23" s="664"/>
+      <c r="Y23" s="660"/>
       <c r="Z23" s="17"/>
       <c r="AA23" s="10"/>
       <c r="AB23" s="419"/>
@@ -8395,13 +8395,13 @@
       <c r="AG23" s="6"/>
       <c r="AH23" s="6"/>
       <c r="AI23" s="6"/>
-      <c r="AJ23" s="636"/>
+      <c r="AJ23" s="656"/>
       <c r="AK23" s="259"/>
       <c r="AL23" s="80" t="s">
         <v>508</v>
       </c>
       <c r="AM23" s="302"/>
-      <c r="AN23" s="647"/>
+      <c r="AN23" s="642"/>
     </row>
     <row r="24" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="444" t="s">
@@ -8419,23 +8419,23 @@
       <c r="E24" s="440">
         <v>1</v>
       </c>
-      <c r="F24" s="626"/>
+      <c r="F24" s="647"/>
       <c r="G24" s="61" t="s">
         <v>491</v>
       </c>
       <c r="I24" s="221"/>
-      <c r="O24" s="629"/>
-      <c r="Q24" s="632"/>
+      <c r="O24" s="685"/>
+      <c r="Q24" s="688"/>
       <c r="T24" s="17"/>
       <c r="U24" s="229" t="s">
         <v>44</v>
       </c>
-      <c r="V24" s="667"/>
+      <c r="V24" s="616"/>
       <c r="W24" s="148"/>
       <c r="X24" s="433" t="s">
         <v>185</v>
       </c>
-      <c r="Y24" s="664"/>
+      <c r="Y24" s="660"/>
       <c r="Z24" s="17"/>
       <c r="AA24" s="10"/>
       <c r="AB24" s="419"/>
@@ -8454,12 +8454,12 @@
         <v>464</v>
       </c>
       <c r="AM24" s="302"/>
-      <c r="AN24" s="647"/>
+      <c r="AN24" s="642"/>
     </row>
     <row r="25" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F25" s="626"/>
+      <c r="F25" s="647"/>
       <c r="I25" s="221"/>
-      <c r="O25" s="629"/>
+      <c r="O25" s="685"/>
       <c r="P25" s="206" t="s">
         <v>281</v>
       </c>
@@ -8472,12 +8472,12 @@
       <c r="U25" s="404" t="s">
         <v>44</v>
       </c>
-      <c r="V25" s="668"/>
+      <c r="V25" s="617"/>
       <c r="W25" s="148"/>
       <c r="X25" s="433" t="s">
         <v>189</v>
       </c>
-      <c r="Y25" s="664"/>
+      <c r="Y25" s="660"/>
       <c r="Z25" s="17"/>
       <c r="AA25" s="10"/>
       <c r="AB25" s="419"/>
@@ -8494,7 +8494,7 @@
       <c r="AK25" s="142"/>
       <c r="AL25" s="6"/>
       <c r="AM25" s="302"/>
-      <c r="AN25" s="647"/>
+      <c r="AN25" s="642"/>
     </row>
     <row r="26" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="233" t="s">
@@ -8512,17 +8512,17 @@
       <c r="E26" s="383">
         <v>1</v>
       </c>
-      <c r="F26" s="626"/>
+      <c r="F26" s="647"/>
       <c r="G26" s="340" t="s">
         <v>488</v>
       </c>
       <c r="I26" s="221"/>
-      <c r="O26" s="629"/>
-      <c r="P26" s="649" t="s">
+      <c r="O26" s="685"/>
+      <c r="P26" s="644" t="s">
         <v>527</v>
       </c>
-      <c r="Q26" s="650"/>
-      <c r="R26" s="623" t="s">
+      <c r="Q26" s="645"/>
+      <c r="R26" s="681" t="s">
         <v>536</v>
       </c>
       <c r="T26" s="180"/>
@@ -8534,7 +8534,7 @@
       <c r="X26" s="433" t="s">
         <v>181</v>
       </c>
-      <c r="Y26" s="664"/>
+      <c r="Y26" s="660"/>
       <c r="Z26" s="17"/>
       <c r="AA26" s="10"/>
       <c r="AB26" s="419"/>
@@ -8561,7 +8561,7 @@
       <c r="AM26" s="446" t="s">
         <v>457</v>
       </c>
-      <c r="AN26" s="647"/>
+      <c r="AN26" s="642"/>
     </row>
     <row r="27" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="21" t="s">
@@ -8573,13 +8573,13 @@
       <c r="E27" s="267" t="s">
         <v>44</v>
       </c>
-      <c r="F27" s="627"/>
+      <c r="F27" s="683"/>
       <c r="G27" s="61" t="s">
         <v>545</v>
       </c>
       <c r="I27" s="222"/>
-      <c r="O27" s="630"/>
-      <c r="R27" s="624"/>
+      <c r="O27" s="686"/>
+      <c r="R27" s="682"/>
       <c r="S27" s="425" t="s">
         <v>54</v>
       </c>
@@ -8592,7 +8592,7 @@
       <c r="X27" s="433" t="s">
         <v>531</v>
       </c>
-      <c r="Y27" s="665"/>
+      <c r="Y27" s="661"/>
       <c r="Z27" s="161"/>
       <c r="AA27" s="13"/>
       <c r="AB27" s="420"/>
@@ -8609,10 +8609,48 @@
       <c r="AM27" s="384" t="s">
         <v>320</v>
       </c>
-      <c r="AN27" s="648"/>
+      <c r="AN27" s="643"/>
     </row>
   </sheetData>
   <mergeCells count="54">
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="R18:R19"/>
+    <mergeCell ref="R26:R27"/>
+    <mergeCell ref="F2:F27"/>
+    <mergeCell ref="O10:O27"/>
+    <mergeCell ref="Q20:Q21"/>
+    <mergeCell ref="Q23:Q24"/>
+    <mergeCell ref="G14:J14"/>
+    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="AI6:AI10"/>
+    <mergeCell ref="AF12:AF15"/>
+    <mergeCell ref="AG7:AG12"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="S9:S12"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="AD12:AD15"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="AN1:AN27"/>
+    <mergeCell ref="P26:Q26"/>
+    <mergeCell ref="Q2:Q3"/>
+    <mergeCell ref="M2:M9"/>
+    <mergeCell ref="O2:O9"/>
+    <mergeCell ref="P10:P13"/>
+    <mergeCell ref="AK6:AK7"/>
+    <mergeCell ref="AM12:AM15"/>
+    <mergeCell ref="AF18:AF19"/>
+    <mergeCell ref="AJ18:AJ19"/>
+    <mergeCell ref="Y1:Y27"/>
+    <mergeCell ref="AJ22:AJ23"/>
+    <mergeCell ref="AK9:AK10"/>
+    <mergeCell ref="AD3:AD4"/>
+    <mergeCell ref="S2:S3"/>
+    <mergeCell ref="R2:R3"/>
     <mergeCell ref="V21:V25"/>
     <mergeCell ref="U18:U20"/>
     <mergeCell ref="C2:C3"/>
@@ -8629,44 +8667,6 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="B4:B5"/>
-    <mergeCell ref="AN1:AN27"/>
-    <mergeCell ref="P26:Q26"/>
-    <mergeCell ref="Q2:Q3"/>
-    <mergeCell ref="M2:M9"/>
-    <mergeCell ref="O2:O9"/>
-    <mergeCell ref="P10:P13"/>
-    <mergeCell ref="AK6:AK7"/>
-    <mergeCell ref="AM12:AM15"/>
-    <mergeCell ref="AF18:AF19"/>
-    <mergeCell ref="AJ18:AJ19"/>
-    <mergeCell ref="Y1:Y27"/>
-    <mergeCell ref="AJ22:AJ23"/>
-    <mergeCell ref="AK9:AK10"/>
-    <mergeCell ref="AD3:AD4"/>
-    <mergeCell ref="S2:S3"/>
-    <mergeCell ref="R2:R3"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="AI6:AI10"/>
-    <mergeCell ref="AF12:AF15"/>
-    <mergeCell ref="AG7:AG12"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="S9:S12"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="AD12:AD15"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="R18:R19"/>
-    <mergeCell ref="R26:R27"/>
-    <mergeCell ref="F2:F27"/>
-    <mergeCell ref="O10:O27"/>
-    <mergeCell ref="Q20:Q21"/>
-    <mergeCell ref="Q23:Q24"/>
-    <mergeCell ref="G14:J14"/>
-    <mergeCell ref="G13:J13"/>
-    <mergeCell ref="H12:K12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8703,12 +8703,12 @@
       <c r="B1" s="609" t="s">
         <v>311</v>
       </c>
-      <c r="C1" s="633"/>
+      <c r="C1" s="689"/>
       <c r="D1" s="206"/>
       <c r="J1" s="609" t="s">
         <v>69</v>
       </c>
-      <c r="K1" s="633"/>
+      <c r="K1" s="689"/>
       <c r="L1" s="197" t="s">
         <v>331</v>
       </c>
@@ -9111,7 +9111,7 @@
       <c r="P1" s="402" t="s">
         <v>398</v>
       </c>
-      <c r="Q1" s="707" t="s">
+      <c r="Q1" s="720" t="s">
         <v>180</v>
       </c>
       <c r="R1" s="100" t="s">
@@ -9135,7 +9135,7 @@
       <c r="AA1" s="523" t="s">
         <v>438</v>
       </c>
-      <c r="AB1" s="701" t="s">
+      <c r="AB1" s="714" t="s">
         <v>596</v>
       </c>
       <c r="AC1" s="99" t="s">
@@ -9157,32 +9157,32 @@
       </c>
     </row>
     <row r="2" spans="1:38" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="712">
+      <c r="A2" s="699">
         <f ca="1">TODAY()</f>
         <v>45283</v>
       </c>
-      <c r="B2" s="714" t="s">
+      <c r="B2" s="701" t="s">
         <v>380</v>
       </c>
-      <c r="C2" s="651" t="s">
+      <c r="C2" s="621" t="s">
         <v>358</v>
       </c>
-      <c r="D2" s="716" t="s">
+      <c r="D2" s="703" t="s">
         <v>102</v>
       </c>
-      <c r="E2" s="718" t="s">
+      <c r="E2" s="705" t="s">
         <v>64</v>
       </c>
       <c r="F2" s="193" t="s">
         <v>219</v>
       </c>
-      <c r="G2" s="619" t="s">
+      <c r="G2" s="665" t="s">
         <v>373</v>
       </c>
       <c r="H2" s="208" t="s">
         <v>219</v>
       </c>
-      <c r="I2" s="698" t="s">
+      <c r="I2" s="711" t="s">
         <v>102</v>
       </c>
       <c r="J2" s="400" t="s">
@@ -9206,7 +9206,7 @@
       <c r="P2" s="403">
         <v>40</v>
       </c>
-      <c r="Q2" s="708"/>
+      <c r="Q2" s="721"/>
       <c r="R2" s="21">
         <f>R7+R20</f>
         <v>2</v>
@@ -9231,7 +9231,7 @@
         <f>IF((Z2+T2)&gt;0,0,-1)</f>
         <v>0</v>
       </c>
-      <c r="AB2" s="702"/>
+      <c r="AB2" s="715"/>
       <c r="AC2" s="35"/>
       <c r="AH2" s="6" t="s">
         <v>453</v>
@@ -9248,14 +9248,14 @@
       </c>
     </row>
     <row r="3" spans="1:38" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="713"/>
-      <c r="B3" s="715"/>
-      <c r="C3" s="652"/>
-      <c r="D3" s="717"/>
-      <c r="E3" s="719"/>
-      <c r="G3" s="620"/>
+      <c r="A3" s="700"/>
+      <c r="B3" s="702"/>
+      <c r="C3" s="622"/>
+      <c r="D3" s="704"/>
+      <c r="E3" s="706"/>
+      <c r="G3" s="666"/>
       <c r="H3" s="6"/>
-      <c r="I3" s="699"/>
+      <c r="I3" s="712"/>
       <c r="K3" s="24">
         <v>2</v>
       </c>
@@ -9270,7 +9270,7 @@
       <c r="V3" s="475"/>
       <c r="W3" s="6"/>
       <c r="X3" s="475"/>
-      <c r="AB3" s="702"/>
+      <c r="AB3" s="715"/>
       <c r="AC3" s="35"/>
       <c r="AE3" s="100" t="s">
         <v>591</v>
@@ -9299,10 +9299,10 @@
         <v>381</v>
       </c>
       <c r="B4" s="245"/>
-      <c r="C4" s="720" t="s">
+      <c r="C4" s="707" t="s">
         <v>177</v>
       </c>
-      <c r="I4" s="699"/>
+      <c r="I4" s="712"/>
       <c r="R4" s="476" t="s">
         <v>591</v>
       </c>
@@ -9314,7 +9314,7 @@
       <c r="V4" s="475"/>
       <c r="W4" s="6"/>
       <c r="X4" s="475"/>
-      <c r="AB4" s="702"/>
+      <c r="AB4" s="715"/>
       <c r="AC4" s="35"/>
       <c r="AE4" s="20"/>
       <c r="AF4" s="100" t="s">
@@ -9345,7 +9345,7 @@
       <c r="B5" s="100" t="s">
         <v>358</v>
       </c>
-      <c r="C5" s="721"/>
+      <c r="C5" s="708"/>
       <c r="D5" s="224" t="s">
         <v>102</v>
       </c>
@@ -9361,7 +9361,7 @@
       <c r="H5" s="208" t="s">
         <v>219</v>
       </c>
-      <c r="I5" s="699"/>
+      <c r="I5" s="712"/>
       <c r="J5" s="401" t="s">
         <v>269</v>
       </c>
@@ -9388,7 +9388,7 @@
       <c r="V5" s="473"/>
       <c r="W5" s="6"/>
       <c r="X5" s="473"/>
-      <c r="AB5" s="702"/>
+      <c r="AB5" s="715"/>
       <c r="AC5" s="2" t="s">
         <v>594</v>
       </c>
@@ -9402,19 +9402,19 @@
       <c r="AL5" s="473"/>
     </row>
     <row r="6" spans="1:38" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="709" t="s">
+      <c r="A6" s="696" t="s">
         <v>286</v>
       </c>
       <c r="B6" s="105" t="s">
         <v>198</v>
       </c>
-      <c r="C6" s="634"/>
-      <c r="D6" s="635"/>
+      <c r="C6" s="667"/>
+      <c r="D6" s="668"/>
       <c r="E6" s="96">
         <v>1</v>
       </c>
       <c r="G6" s="605"/>
-      <c r="I6" s="699"/>
+      <c r="I6" s="712"/>
       <c r="P6" s="61" t="s">
         <v>594</v>
       </c>
@@ -9426,7 +9426,7 @@
         <f>S7-S12-SUM(V2:V10)</f>
         <v>0</v>
       </c>
-      <c r="AB6" s="702"/>
+      <c r="AB6" s="715"/>
       <c r="AC6" s="35"/>
       <c r="AE6" s="64">
         <f>AE7-SUM(AL2:AL10)+AE11</f>
@@ -9442,7 +9442,7 @@
       <c r="AL6" s="112"/>
     </row>
     <row r="7" spans="1:38" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="710"/>
+      <c r="A7" s="697"/>
       <c r="B7" s="100" t="s">
         <v>154</v>
       </c>
@@ -9453,7 +9453,7 @@
         <v>135</v>
       </c>
       <c r="G7" s="605"/>
-      <c r="I7" s="699"/>
+      <c r="I7" s="712"/>
       <c r="M7" s="16" t="s">
         <v>348</v>
       </c>
@@ -9485,7 +9485,7 @@
       <c r="X7" s="474">
         <v>1</v>
       </c>
-      <c r="AB7" s="702"/>
+      <c r="AB7" s="715"/>
       <c r="AC7" s="99" t="s">
         <v>595</v>
       </c>
@@ -9511,7 +9511,7 @@
       </c>
     </row>
     <row r="8" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="711"/>
+      <c r="A8" s="698"/>
       <c r="B8" s="214" t="s">
         <v>28</v>
       </c>
@@ -9520,7 +9520,7 @@
         <v>3</v>
       </c>
       <c r="G8" s="605"/>
-      <c r="I8" s="699"/>
+      <c r="I8" s="712"/>
       <c r="N8" s="80"/>
       <c r="U8" s="6" t="s">
         <v>250</v>
@@ -9534,7 +9534,7 @@
       <c r="X8" s="475">
         <v>1</v>
       </c>
-      <c r="AB8" s="702"/>
+      <c r="AB8" s="715"/>
       <c r="AC8" s="521"/>
       <c r="AH8" s="6" t="s">
         <v>600</v>
@@ -9565,7 +9565,7 @@
       </c>
       <c r="G9" s="605"/>
       <c r="H9" s="6"/>
-      <c r="I9" s="699"/>
+      <c r="I9" s="712"/>
       <c r="M9" s="19" t="s">
         <v>526</v>
       </c>
@@ -9576,7 +9576,7 @@
         <v>510</v>
       </c>
       <c r="X9" s="472"/>
-      <c r="AB9" s="702"/>
+      <c r="AB9" s="715"/>
       <c r="AC9" s="521"/>
       <c r="AE9" s="20"/>
       <c r="AF9" s="20"/>
@@ -9608,7 +9608,7 @@
         <v>36</v>
       </c>
       <c r="G10" s="605"/>
-      <c r="I10" s="699"/>
+      <c r="I10" s="712"/>
       <c r="J10" s="24" t="s">
         <v>373</v>
       </c>
@@ -9625,7 +9625,7 @@
         <v>602</v>
       </c>
       <c r="X10" s="472"/>
-      <c r="AB10" s="702"/>
+      <c r="AB10" s="715"/>
       <c r="AC10" s="521"/>
       <c r="AE10" s="20"/>
       <c r="AF10" s="20"/>
@@ -9653,7 +9653,7 @@
         <v>266</v>
       </c>
       <c r="G11" s="605"/>
-      <c r="I11" s="699"/>
+      <c r="I11" s="712"/>
       <c r="J11" s="24" t="s">
         <v>194</v>
       </c>
@@ -9679,13 +9679,13 @@
       <c r="S11" s="24">
         <v>2</v>
       </c>
-      <c r="U11" s="704" t="s">
+      <c r="U11" s="717" t="s">
         <v>559</v>
       </c>
-      <c r="V11" s="705"/>
-      <c r="W11" s="705"/>
-      <c r="X11" s="706"/>
-      <c r="AB11" s="703"/>
+      <c r="V11" s="718"/>
+      <c r="W11" s="718"/>
+      <c r="X11" s="719"/>
+      <c r="AB11" s="716"/>
       <c r="AC11" s="99" t="s">
         <v>597</v>
       </c>
@@ -9699,13 +9699,13 @@
         <v>3</v>
       </c>
       <c r="AG11" s="418"/>
-      <c r="AH11" s="704" t="s">
+      <c r="AH11" s="717" t="s">
         <v>614</v>
       </c>
-      <c r="AI11" s="705"/>
-      <c r="AJ11" s="705"/>
-      <c r="AK11" s="705"/>
-      <c r="AL11" s="706"/>
+      <c r="AI11" s="718"/>
+      <c r="AJ11" s="718"/>
+      <c r="AK11" s="718"/>
+      <c r="AL11" s="719"/>
     </row>
     <row r="12" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="229" t="s">
@@ -9716,7 +9716,7 @@
         <v>3</v>
       </c>
       <c r="G12" s="605"/>
-      <c r="I12" s="699"/>
+      <c r="I12" s="712"/>
       <c r="J12" s="24" t="s">
         <v>517</v>
       </c>
@@ -9749,7 +9749,7 @@
       </c>
       <c r="D13" s="20"/>
       <c r="G13" s="605"/>
-      <c r="I13" s="699"/>
+      <c r="I13" s="712"/>
       <c r="J13" s="108" t="s">
         <v>549</v>
       </c>
@@ -9793,7 +9793,7 @@
       <c r="H14" s="208" t="s">
         <v>219</v>
       </c>
-      <c r="I14" s="699"/>
+      <c r="I14" s="712"/>
       <c r="U14" s="67" t="s">
         <v>80</v>
       </c>
@@ -9820,7 +9820,7 @@
       <c r="H15" s="273">
         <v>0</v>
       </c>
-      <c r="I15" s="699"/>
+      <c r="I15" s="712"/>
       <c r="J15" s="108" t="s">
         <v>153</v>
       </c>
@@ -9851,7 +9851,7 @@
       <c r="D16" s="2" t="s">
         <v>493</v>
       </c>
-      <c r="I16" s="699"/>
+      <c r="I16" s="712"/>
       <c r="K16" s="100" t="s">
         <v>44</v>
       </c>
@@ -9895,7 +9895,7 @@
       <c r="G17" s="2" t="s">
         <v>424</v>
       </c>
-      <c r="I17" s="699"/>
+      <c r="I17" s="712"/>
       <c r="L17" s="2" t="s">
         <v>427</v>
       </c>
@@ -9913,13 +9913,13 @@
     </row>
     <row r="18" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G18" s="16"/>
-      <c r="I18" s="699"/>
+      <c r="I18" s="712"/>
       <c r="L18" s="16"/>
       <c r="M18" s="21"/>
-      <c r="O18" s="696" t="s">
+      <c r="O18" s="709" t="s">
         <v>518</v>
       </c>
-      <c r="P18" s="697"/>
+      <c r="P18" s="710"/>
       <c r="Q18" s="127" t="s">
         <v>44</v>
       </c>
@@ -9945,7 +9945,7 @@
       </c>
     </row>
     <row r="19" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I19" s="699"/>
+      <c r="I19" s="712"/>
       <c r="M19" s="21" t="s">
         <v>426</v>
       </c>
@@ -9981,7 +9981,7 @@
       <c r="G20" s="2" t="s">
         <v>424</v>
       </c>
-      <c r="I20" s="699"/>
+      <c r="I20" s="712"/>
       <c r="K20" s="19" t="s">
         <v>423</v>
       </c>
@@ -10016,7 +10016,7 @@
       </c>
     </row>
     <row r="21" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I21" s="699"/>
+      <c r="I21" s="712"/>
       <c r="M21" s="218" t="s">
         <v>412</v>
       </c>
@@ -10050,7 +10050,7 @@
       <c r="G22" s="2" t="s">
         <v>424</v>
       </c>
-      <c r="I22" s="699"/>
+      <c r="I22" s="712"/>
       <c r="P22" s="99" t="s">
         <v>593</v>
       </c>
@@ -10065,7 +10065,7 @@
       <c r="E23" s="285" t="s">
         <v>44</v>
       </c>
-      <c r="I23" s="699"/>
+      <c r="I23" s="712"/>
       <c r="Q23" s="24">
         <f>SUM(V23:V31)</f>
         <v>5</v>
@@ -10082,7 +10082,7 @@
       </c>
     </row>
     <row r="24" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I24" s="699"/>
+      <c r="I24" s="712"/>
       <c r="U24" s="35"/>
       <c r="V24" s="514">
         <v>0</v>
@@ -10110,7 +10110,7 @@
       <c r="H25" s="193" t="s">
         <v>267</v>
       </c>
-      <c r="I25" s="699"/>
+      <c r="I25" s="712"/>
       <c r="J25" s="401" t="s">
         <v>270</v>
       </c>
@@ -10155,7 +10155,7 @@
       <c r="H26" s="19" t="s">
         <v>219</v>
       </c>
-      <c r="I26" s="699"/>
+      <c r="I26" s="712"/>
       <c r="K26" s="24">
         <v>15</v>
       </c>
@@ -10190,7 +10190,7 @@
       </c>
     </row>
     <row r="27" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I27" s="699"/>
+      <c r="I27" s="712"/>
       <c r="O27" s="2" t="s">
         <v>98</v>
       </c>
@@ -10217,7 +10217,7 @@
       <c r="E28" s="217">
         <v>2</v>
       </c>
-      <c r="I28" s="699"/>
+      <c r="I28" s="712"/>
       <c r="Q28" s="6"/>
       <c r="R28" s="112"/>
       <c r="T28" s="142"/>
@@ -10239,7 +10239,7 @@
       <c r="H29" s="193" t="s">
         <v>268</v>
       </c>
-      <c r="I29" s="700"/>
+      <c r="I29" s="713"/>
       <c r="J29" s="326"/>
       <c r="L29" s="96" t="s">
         <v>274</v>
@@ -10297,6 +10297,13 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="I2:I29"/>
+    <mergeCell ref="AB1:AB11"/>
+    <mergeCell ref="AH11:AL11"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="U11:X11"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="G5:G14"/>
     <mergeCell ref="A2:A3"/>
@@ -10308,13 +10315,6 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="C2:C3"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="I2:I29"/>
-    <mergeCell ref="AB1:AB11"/>
-    <mergeCell ref="AH11:AL11"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="U11:X11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10324,8 +10324,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2029A93E-B53C-4201-9F17-439C144F3CF1}">
   <dimension ref="A1:AT37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:L3"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="AG10" sqref="AG10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10425,21 +10425,21 @@
         <f ca="1">TODAY()</f>
         <v>45283</v>
       </c>
-      <c r="T1" s="741"/>
+      <c r="T1" s="748"/>
       <c r="U1" s="142"/>
       <c r="V1" s="6"/>
       <c r="W1" s="6"/>
-      <c r="X1" s="725" t="s">
+      <c r="X1" s="732" t="s">
         <v>442</v>
       </c>
-      <c r="Y1" s="726"/>
+      <c r="Y1" s="733"/>
       <c r="Z1" s="308">
         <f>68-(W8+Y3+X3+U3)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA1" s="102">
         <f>Z1+Z3</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB1" s="102" t="s">
         <v>441</v>
@@ -10448,23 +10448,23 @@
       <c r="AD1" s="304" t="s">
         <v>44</v>
       </c>
-      <c r="AE1" s="727" t="s">
+      <c r="AE1" s="734" t="s">
         <v>190</v>
       </c>
-      <c r="AF1" s="728"/>
-      <c r="AG1" s="729"/>
-      <c r="AH1" s="730" t="s">
+      <c r="AF1" s="735"/>
+      <c r="AG1" s="736"/>
+      <c r="AH1" s="737" t="s">
         <v>294</v>
       </c>
-      <c r="AI1" s="731"/>
-      <c r="AJ1" s="732"/>
+      <c r="AI1" s="738"/>
+      <c r="AJ1" s="739"/>
       <c r="AK1" s="558"/>
       <c r="AL1" s="558"/>
-      <c r="AM1" s="722" t="s">
+      <c r="AM1" s="729" t="s">
         <v>445</v>
       </c>
-      <c r="AN1" s="723"/>
-      <c r="AO1" s="724"/>
+      <c r="AN1" s="730"/>
+      <c r="AO1" s="731"/>
       <c r="AR1" s="142"/>
     </row>
     <row r="2" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10479,27 +10479,27 @@
         <f>K2+L2</f>
         <v>27</v>
       </c>
-      <c r="K2" s="749">
+      <c r="K2" s="727">
         <f>SUM(K4:K29)</f>
         <v>12</v>
       </c>
-      <c r="L2" s="747">
+      <c r="L2" s="725">
         <f>SUM(L4:L37)</f>
         <v>15</v>
       </c>
-      <c r="M2" s="733">
+      <c r="M2" s="740">
         <f>SUM(M5:M30)</f>
         <v>1</v>
       </c>
-      <c r="N2" s="735">
+      <c r="N2" s="742">
         <f>SUM(N4:N29)</f>
-        <v>11</v>
-      </c>
-      <c r="O2" s="737">
+        <v>10</v>
+      </c>
+      <c r="O2" s="744">
         <f>SUM(O4:O29)</f>
-        <v>10</v>
-      </c>
-      <c r="P2" s="643">
+        <v>9</v>
+      </c>
+      <c r="P2" s="672">
         <f>SUM(N30:N37)* (-1)</f>
         <v>-3</v>
       </c>
@@ -10512,14 +10512,14 @@
       <c r="S2" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="T2" s="742"/>
+      <c r="T2" s="749"/>
       <c r="U2" s="543" t="s">
         <v>263</v>
       </c>
       <c r="V2" s="487" t="s">
         <v>220</v>
       </c>
-      <c r="W2" s="739" t="s">
+      <c r="W2" s="746" t="s">
         <v>235</v>
       </c>
       <c r="X2" s="488" t="s">
@@ -10589,14 +10589,14 @@
     <row r="3" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J3" s="314">
         <f>V3+X3+Y3+U3</f>
-        <v>68</v>
-      </c>
-      <c r="K3" s="750"/>
-      <c r="L3" s="748"/>
-      <c r="M3" s="734"/>
-      <c r="N3" s="736"/>
-      <c r="O3" s="738"/>
-      <c r="P3" s="644"/>
+        <v>67</v>
+      </c>
+      <c r="K3" s="728"/>
+      <c r="L3" s="726"/>
+      <c r="M3" s="741"/>
+      <c r="N3" s="743"/>
+      <c r="O3" s="745"/>
+      <c r="P3" s="673"/>
       <c r="Q3" s="174">
         <f>(M2+N2)-Y3</f>
         <v>0</v>
@@ -10604,7 +10604,7 @@
       <c r="S3" s="159" t="s">
         <v>245</v>
       </c>
-      <c r="T3" s="743"/>
+      <c r="T3" s="750"/>
       <c r="U3" s="544">
         <f>SUM(U4:U29)</f>
         <v>11</v>
@@ -10613,14 +10613,14 @@
         <f>SUM(V4:V29)</f>
         <v>36</v>
       </c>
-      <c r="W3" s="740"/>
+      <c r="W3" s="747"/>
       <c r="X3" s="490">
         <f t="shared" ref="X3:AC3" si="0">SUM(X4:X29)</f>
         <v>9</v>
       </c>
       <c r="Y3" s="490">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Z3" s="59">
         <f t="shared" si="0"/>
@@ -10628,15 +10628,15 @@
       </c>
       <c r="AA3" s="66">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AB3" s="66">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="AC3" s="66">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AD3" s="66">
         <f t="shared" ref="AD3:AO3" si="1">SUM(AD4:AD29)</f>
@@ -10656,7 +10656,7 @@
       </c>
       <c r="AH3" s="66">
         <f>SUM(AH4:AH29)</f>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AI3" s="377">
         <f t="shared" si="1"/>
@@ -10670,15 +10670,15 @@
       <c r="AL3" s="408"/>
       <c r="AM3" s="100">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AN3" s="312">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AO3" s="313">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AR3" s="142"/>
     </row>
@@ -10711,7 +10711,7 @@
         <f>AC4</f>
         <v>0</v>
       </c>
-      <c r="P4" s="744" t="s">
+      <c r="P4" s="722" t="s">
         <v>199</v>
       </c>
       <c r="Q4" s="20"/>
@@ -10797,7 +10797,7 @@
         <f>AC5</f>
         <v>0</v>
       </c>
-      <c r="P5" s="745"/>
+      <c r="P5" s="723"/>
       <c r="Q5" s="20"/>
       <c r="R5" s="2" t="s">
         <v>341</v>
@@ -10893,7 +10893,7 @@
         <f>AC6</f>
         <v>1</v>
       </c>
-      <c r="P6" s="745"/>
+      <c r="P6" s="723"/>
       <c r="Q6" s="19" t="s">
         <v>336</v>
       </c>
@@ -10988,13 +10988,13 @@
         <v>0</v>
       </c>
       <c r="N7" s="107">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O7" s="295">
-        <f t="shared" ref="O7:O37" si="10">AC7</f>
-        <v>1</v>
-      </c>
-      <c r="P7" s="745"/>
+        <f>AC7</f>
+        <v>0</v>
+      </c>
+      <c r="P7" s="723"/>
       <c r="Q7" s="20"/>
       <c r="R7" s="2" t="s">
         <v>336</v>
@@ -11019,19 +11019,19 @@
       </c>
       <c r="Y7" s="185">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z7" s="298"/>
       <c r="AA7" s="117">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB7" s="292">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AC7" s="292">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD7" s="292">
         <f t="shared" si="4"/>
@@ -11048,7 +11048,7 @@
       </c>
       <c r="AH7" s="298">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI7" s="378"/>
       <c r="AJ7" s="514"/>
@@ -11056,15 +11056,15 @@
       <c r="AL7" s="319"/>
       <c r="AM7" s="339">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN7" s="310">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO7" s="311">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AP7" s="6" t="s">
         <v>241</v>
@@ -11105,10 +11105,10 @@
         <v>0</v>
       </c>
       <c r="O8" s="295">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="P8" s="745"/>
+        <f t="shared" ref="O7:O37" si="10">AC8</f>
+        <v>0</v>
+      </c>
+      <c r="P8" s="723"/>
       <c r="Q8" s="21" t="s">
         <v>234</v>
       </c>
@@ -11199,7 +11199,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P9" s="745"/>
+      <c r="P9" s="723"/>
       <c r="Q9" s="21" t="s">
         <v>336</v>
       </c>
@@ -11304,7 +11304,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P10" s="745"/>
+      <c r="P10" s="723"/>
       <c r="Q10" s="20"/>
       <c r="R10" s="2" t="s">
         <v>341</v>
@@ -11394,7 +11394,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P11" s="745"/>
+      <c r="P11" s="723"/>
       <c r="Q11" s="21" t="s">
         <v>336</v>
       </c>
@@ -11459,14 +11459,14 @@
       <c r="AR11" s="513"/>
     </row>
     <row r="12" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="681" t="s">
+      <c r="A12" s="632" t="s">
         <v>55</v>
       </c>
       <c r="B12" s="30">
         <v>13</v>
       </c>
       <c r="C12" s="2"/>
-      <c r="E12" s="631" t="s">
+      <c r="E12" s="687" t="s">
         <v>56</v>
       </c>
       <c r="G12" s="264"/>
@@ -11491,7 +11491,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P12" s="745"/>
+      <c r="P12" s="723"/>
       <c r="Q12" s="21" t="s">
         <v>336</v>
       </c>
@@ -11568,14 +11568,14 @@
       </c>
     </row>
     <row r="13" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="683"/>
+      <c r="A13" s="634"/>
       <c r="B13" s="597">
         <v>12</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E13" s="632"/>
+      <c r="E13" s="688"/>
       <c r="F13" s="174">
         <v>0</v>
       </c>
@@ -11599,7 +11599,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P13" s="745"/>
+      <c r="P13" s="723"/>
       <c r="Q13" s="21" t="s">
         <v>336</v>
       </c>
@@ -11681,7 +11681,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P14" s="745"/>
+      <c r="P14" s="723"/>
       <c r="Q14" s="20"/>
       <c r="R14" s="202" t="s">
         <v>340</v>
@@ -11784,7 +11784,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P15" s="745"/>
+      <c r="P15" s="723"/>
       <c r="Q15" s="20"/>
       <c r="R15" s="202" t="s">
         <v>340</v>
@@ -11878,7 +11878,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P16" s="745"/>
+      <c r="P16" s="723"/>
       <c r="Q16" s="21" t="s">
         <v>336</v>
       </c>
@@ -11983,7 +11983,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P17" s="745"/>
+      <c r="P17" s="723"/>
       <c r="Q17" s="20"/>
       <c r="R17" s="2" t="s">
         <v>342</v>
@@ -12085,7 +12085,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P18" s="745"/>
+      <c r="P18" s="723"/>
       <c r="Q18" s="21" t="s">
         <v>336</v>
       </c>
@@ -12173,7 +12173,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P19" s="745"/>
+      <c r="P19" s="723"/>
       <c r="Q19" s="20"/>
       <c r="R19" s="2" t="s">
         <v>335</v>
@@ -12283,11 +12283,11 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P20" s="746"/>
+      <c r="P20" s="724"/>
       <c r="Q20" s="609" t="s">
         <v>336</v>
       </c>
-      <c r="R20" s="633"/>
+      <c r="R20" s="689"/>
       <c r="S20" s="540" t="s">
         <v>85</v>
       </c>
@@ -12551,7 +12551,7 @@
     </row>
     <row r="23" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="24"/>
-      <c r="E23" s="688" t="s">
+      <c r="E23" s="639" t="s">
         <v>290</v>
       </c>
       <c r="F23" s="182"/>
@@ -12654,7 +12654,7 @@
       <c r="C24" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="E24" s="689"/>
+      <c r="E24" s="640"/>
       <c r="F24" s="174"/>
       <c r="H24" s="42"/>
       <c r="J24" s="581" t="s">
@@ -12677,7 +12677,7 @@
       <c r="Q24" s="609" t="s">
         <v>336</v>
       </c>
-      <c r="R24" s="633"/>
+      <c r="R24" s="689"/>
       <c r="S24" s="540" t="s">
         <v>250</v>
       </c>
@@ -13328,8 +13328,8 @@
       <c r="AR31" s="513"/>
     </row>
     <row r="32" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="636"/>
-      <c r="B32" s="636"/>
+      <c r="A32" s="656"/>
+      <c r="B32" s="656"/>
       <c r="J32" s="582" t="s">
         <v>310</v>
       </c>
@@ -13863,15 +13863,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="Q24:R24"/>
-    <mergeCell ref="P4:P20"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="Q20:R20"/>
     <mergeCell ref="AM1:AO1"/>
     <mergeCell ref="X1:Y1"/>
     <mergeCell ref="AE1:AG1"/>
@@ -13882,6 +13873,15 @@
     <mergeCell ref="P2:P3"/>
     <mergeCell ref="W2:W3"/>
     <mergeCell ref="T1:T3"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="Q24:R24"/>
+    <mergeCell ref="P4:P20"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="Q20:R20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -13949,7 +13949,7 @@
       <c r="V1" s="609" t="s">
         <v>70</v>
       </c>
-      <c r="W1" s="633"/>
+      <c r="W1" s="689"/>
       <c r="X1" s="62" t="s">
         <v>101</v>
       </c>
@@ -13968,7 +13968,7 @@
       <c r="AC1" s="116" t="s">
         <v>190</v>
       </c>
-      <c r="AD1" s="758" t="s">
+      <c r="AD1" s="765" t="s">
         <v>212</v>
       </c>
       <c r="AE1" s="116" t="s">
@@ -13985,10 +13985,10 @@
       <c r="E2" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="F2" s="757" t="s">
+      <c r="F2" s="796" t="s">
         <v>74</v>
       </c>
-      <c r="G2" s="785" t="s">
+      <c r="G2" s="753" t="s">
         <v>44</v>
       </c>
       <c r="H2" s="40" t="s">
@@ -14016,10 +14016,10 @@
       <c r="U2" s="60" t="s">
         <v>105</v>
       </c>
-      <c r="V2" s="725" t="s">
+      <c r="V2" s="732" t="s">
         <v>120</v>
       </c>
-      <c r="W2" s="726"/>
+      <c r="W2" s="733"/>
       <c r="X2" s="64" t="s">
         <v>109</v>
       </c>
@@ -14038,7 +14038,7 @@
       <c r="AC2" s="117" t="s">
         <v>98</v>
       </c>
-      <c r="AD2" s="759"/>
+      <c r="AD2" s="766"/>
       <c r="AE2" s="64" t="s">
         <v>98</v>
       </c>
@@ -14057,8 +14057,8 @@
       <c r="E3" s="39" t="s">
         <v>79</v>
       </c>
-      <c r="F3" s="685"/>
-      <c r="G3" s="786"/>
+      <c r="F3" s="636"/>
+      <c r="G3" s="754"/>
       <c r="H3" s="40" t="s">
         <v>80</v>
       </c>
@@ -14069,13 +14069,13 @@
         <v>81</v>
       </c>
       <c r="N3" s="44"/>
-      <c r="O3" s="795" t="s">
+      <c r="O3" s="763" t="s">
         <v>44</v>
       </c>
-      <c r="P3" s="777" t="s">
+      <c r="P3" s="784" t="s">
         <v>218</v>
       </c>
-      <c r="Q3" s="778"/>
+      <c r="Q3" s="785"/>
       <c r="S3" s="57" t="s">
         <v>219</v>
       </c>
@@ -14085,15 +14085,15 @@
       <c r="W3" s="59" t="s">
         <v>104</v>
       </c>
-      <c r="AD3" s="759"/>
+      <c r="AD3" s="766"/>
     </row>
     <row r="4" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G4" s="786"/>
+      <c r="G4" s="754"/>
       <c r="H4" s="6"/>
       <c r="L4" s="693" t="s">
         <v>82</v>
       </c>
-      <c r="O4" s="796"/>
+      <c r="O4" s="764"/>
       <c r="T4" s="55" t="s">
         <v>97</v>
       </c>
@@ -14107,8 +14107,8 @@
         <v>194</v>
       </c>
       <c r="Z4" s="611"/>
-      <c r="AA4" s="633"/>
-      <c r="AD4" s="759"/>
+      <c r="AA4" s="689"/>
+      <c r="AD4" s="766"/>
     </row>
     <row r="5" spans="1:31" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="52" t="s">
@@ -14123,21 +14123,21 @@
       <c r="F5" s="66" t="s">
         <v>84</v>
       </c>
-      <c r="G5" s="786"/>
+      <c r="G5" s="754"/>
       <c r="H5" s="46" t="s">
         <v>75</v>
       </c>
-      <c r="K5" s="764" t="s">
+      <c r="K5" s="771" t="s">
         <v>216</v>
       </c>
-      <c r="L5" s="779"/>
+      <c r="L5" s="786"/>
       <c r="M5" s="2" t="s">
         <v>214</v>
       </c>
       <c r="N5" s="61" t="s">
         <v>213</v>
       </c>
-      <c r="O5" s="796"/>
+      <c r="O5" s="764"/>
       <c r="P5" s="108" t="s">
         <v>215</v>
       </c>
@@ -14153,11 +14153,11 @@
       <c r="U5" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="Y5" s="767" t="s">
+      <c r="Y5" s="774" t="s">
         <v>283</v>
       </c>
-      <c r="Z5" s="768"/>
-      <c r="AD5" s="759"/>
+      <c r="Z5" s="775"/>
+      <c r="AD5" s="766"/>
     </row>
     <row r="6" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="109"/>
@@ -14167,16 +14167,16 @@
       <c r="E6" s="45" t="s">
         <v>85</v>
       </c>
-      <c r="G6" s="786"/>
+      <c r="G6" s="754"/>
       <c r="H6" s="46" t="s">
         <v>80</v>
       </c>
       <c r="I6" s="23">
         <v>15</v>
       </c>
-      <c r="K6" s="765"/>
-      <c r="L6" s="779"/>
-      <c r="O6" s="796"/>
+      <c r="K6" s="772"/>
+      <c r="L6" s="786"/>
+      <c r="O6" s="764"/>
       <c r="T6" s="2" t="s">
         <v>100</v>
       </c>
@@ -14186,23 +14186,23 @@
       <c r="V6" s="21">
         <v>-1</v>
       </c>
-      <c r="AD6" s="759"/>
+      <c r="AD6" s="766"/>
     </row>
     <row r="7" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="110"/>
-      <c r="G7" s="786"/>
+      <c r="G7" s="754"/>
       <c r="H7" s="6"/>
-      <c r="K7" s="765"/>
-      <c r="L7" s="779"/>
+      <c r="K7" s="772"/>
+      <c r="L7" s="786"/>
       <c r="N7" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="O7" s="796"/>
+      <c r="O7" s="764"/>
       <c r="P7" s="73"/>
       <c r="U7" s="104" t="s">
         <v>20</v>
       </c>
-      <c r="AD7" s="759"/>
+      <c r="AD7" s="766"/>
     </row>
     <row r="8" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="130"/>
@@ -14215,7 +14215,7 @@
       <c r="F8" s="66" t="s">
         <v>86</v>
       </c>
-      <c r="G8" s="786"/>
+      <c r="G8" s="754"/>
       <c r="H8" s="50" t="s">
         <v>75</v>
       </c>
@@ -14225,41 +14225,41 @@
       <c r="J8" s="111">
         <v>115</v>
       </c>
-      <c r="K8" s="765"/>
-      <c r="L8" s="779"/>
-      <c r="O8" s="796"/>
+      <c r="K8" s="772"/>
+      <c r="L8" s="786"/>
+      <c r="O8" s="764"/>
       <c r="P8" s="49"/>
-      <c r="S8" s="761" t="s">
+      <c r="S8" s="768" t="s">
         <v>211</v>
       </c>
-      <c r="T8" s="762"/>
-      <c r="U8" s="762"/>
-      <c r="V8" s="762"/>
-      <c r="W8" s="762"/>
-      <c r="X8" s="762"/>
-      <c r="Y8" s="762"/>
-      <c r="Z8" s="762"/>
-      <c r="AA8" s="762"/>
-      <c r="AB8" s="762"/>
-      <c r="AC8" s="763"/>
-      <c r="AD8" s="759"/>
+      <c r="T8" s="769"/>
+      <c r="U8" s="769"/>
+      <c r="V8" s="769"/>
+      <c r="W8" s="769"/>
+      <c r="X8" s="769"/>
+      <c r="Y8" s="769"/>
+      <c r="Z8" s="769"/>
+      <c r="AA8" s="769"/>
+      <c r="AB8" s="769"/>
+      <c r="AC8" s="770"/>
+      <c r="AD8" s="766"/>
     </row>
     <row r="9" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="751"/>
-      <c r="G9" s="786"/>
+      <c r="C9" s="790"/>
+      <c r="G9" s="754"/>
       <c r="H9" s="6"/>
-      <c r="K9" s="765"/>
-      <c r="L9" s="789" t="s">
+      <c r="K9" s="772"/>
+      <c r="L9" s="757" t="s">
         <v>217</v>
       </c>
-      <c r="M9" s="790"/>
-      <c r="N9" s="791"/>
-      <c r="O9" s="796"/>
+      <c r="M9" s="758"/>
+      <c r="N9" s="759"/>
+      <c r="O9" s="764"/>
       <c r="P9" s="75"/>
-      <c r="AD9" s="759"/>
+      <c r="AD9" s="766"/>
     </row>
     <row r="10" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="752"/>
+      <c r="C10" s="791"/>
       <c r="D10" s="23"/>
       <c r="E10" s="45" t="s">
         <v>87</v>
@@ -14267,7 +14267,7 @@
       <c r="F10" s="66" t="s">
         <v>88</v>
       </c>
-      <c r="G10" s="786"/>
+      <c r="G10" s="754"/>
       <c r="H10" s="51"/>
       <c r="I10" s="21" t="s">
         <v>80</v>
@@ -14275,33 +14275,33 @@
       <c r="J10" s="3">
         <v>15</v>
       </c>
-      <c r="K10" s="765"/>
-      <c r="M10" s="754" t="s">
+      <c r="K10" s="772"/>
+      <c r="M10" s="793" t="s">
         <v>89</v>
       </c>
-      <c r="N10" s="755"/>
-      <c r="O10" s="755"/>
-      <c r="P10" s="755"/>
-      <c r="Q10" s="755"/>
-      <c r="R10" s="755"/>
-      <c r="S10" s="755"/>
-      <c r="T10" s="755"/>
-      <c r="U10" s="755"/>
-      <c r="V10" s="755"/>
-      <c r="W10" s="755"/>
-      <c r="X10" s="755"/>
-      <c r="Y10" s="755"/>
-      <c r="Z10" s="755"/>
-      <c r="AA10" s="755"/>
-      <c r="AB10" s="755"/>
-      <c r="AC10" s="756"/>
-      <c r="AD10" s="759"/>
+      <c r="N10" s="794"/>
+      <c r="O10" s="794"/>
+      <c r="P10" s="794"/>
+      <c r="Q10" s="794"/>
+      <c r="R10" s="794"/>
+      <c r="S10" s="794"/>
+      <c r="T10" s="794"/>
+      <c r="U10" s="794"/>
+      <c r="V10" s="794"/>
+      <c r="W10" s="794"/>
+      <c r="X10" s="794"/>
+      <c r="Y10" s="794"/>
+      <c r="Z10" s="794"/>
+      <c r="AA10" s="794"/>
+      <c r="AB10" s="794"/>
+      <c r="AC10" s="795"/>
+      <c r="AD10" s="766"/>
     </row>
     <row r="11" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="753"/>
-      <c r="G11" s="786"/>
+      <c r="C11" s="792"/>
+      <c r="G11" s="754"/>
       <c r="H11" s="6"/>
-      <c r="K11" s="765"/>
+      <c r="K11" s="772"/>
       <c r="R11" s="52" t="s">
         <v>44</v>
       </c>
@@ -14309,17 +14309,17 @@
       <c r="Y11" s="68" t="s">
         <v>120</v>
       </c>
-      <c r="Z11" s="775" t="s">
+      <c r="Z11" s="782" t="s">
         <v>120</v>
       </c>
-      <c r="AA11" s="776"/>
+      <c r="AA11" s="783"/>
       <c r="AB11" s="52" t="s">
         <v>44</v>
       </c>
       <c r="AC11" s="118" t="s">
         <v>120</v>
       </c>
-      <c r="AD11" s="759"/>
+      <c r="AD11" s="766"/>
     </row>
     <row r="12" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="129"/>
@@ -14332,7 +14332,7 @@
       <c r="F12" s="66" t="s">
         <v>91</v>
       </c>
-      <c r="G12" s="786"/>
+      <c r="G12" s="754"/>
       <c r="H12" s="128"/>
       <c r="I12" s="19" t="s">
         <v>80</v>
@@ -14340,8 +14340,8 @@
       <c r="J12" s="3">
         <v>15</v>
       </c>
-      <c r="K12" s="765"/>
-      <c r="L12" s="780" t="s">
+      <c r="K12" s="772"/>
+      <c r="L12" s="787" t="s">
         <v>92</v>
       </c>
       <c r="M12" s="21" t="s">
@@ -14372,25 +14372,25 @@
         <v>115</v>
       </c>
       <c r="Y12" s="6"/>
-      <c r="AA12" s="769" t="s">
+      <c r="AA12" s="776" t="s">
         <v>125</v>
       </c>
-      <c r="AB12" s="770"/>
+      <c r="AB12" s="777"/>
       <c r="AC12" s="21" t="s">
         <v>231</v>
       </c>
-      <c r="AD12" s="759"/>
+      <c r="AD12" s="766"/>
     </row>
     <row r="13" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="751"/>
-      <c r="G13" s="786"/>
-      <c r="K13" s="765"/>
-      <c r="L13" s="781"/>
+      <c r="C13" s="790"/>
+      <c r="G13" s="754"/>
+      <c r="K13" s="772"/>
+      <c r="L13" s="788"/>
       <c r="M13" s="47"/>
-      <c r="Q13" s="788" t="s">
+      <c r="Q13" s="756" t="s">
         <v>209</v>
       </c>
-      <c r="R13" s="650"/>
+      <c r="R13" s="645"/>
       <c r="S13" s="605"/>
       <c r="T13" s="6"/>
       <c r="U13" s="96" t="s">
@@ -14399,17 +14399,17 @@
       <c r="X13" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="AA13" s="771"/>
-      <c r="AB13" s="772"/>
-      <c r="AD13" s="759"/>
+      <c r="AA13" s="778"/>
+      <c r="AB13" s="779"/>
+      <c r="AD13" s="766"/>
     </row>
     <row r="14" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="C14" s="753"/>
+      <c r="C14" s="792"/>
       <c r="D14" s="23"/>
-      <c r="G14" s="786"/>
+      <c r="G14" s="754"/>
       <c r="H14" s="125"/>
       <c r="I14" s="99" t="s">
         <v>44</v>
@@ -14417,8 +14417,8 @@
       <c r="J14" s="111">
         <v>115</v>
       </c>
-      <c r="K14" s="765"/>
-      <c r="L14" s="781"/>
+      <c r="K14" s="772"/>
+      <c r="L14" s="788"/>
       <c r="M14" s="21" t="s">
         <v>110</v>
       </c>
@@ -14439,9 +14439,9 @@
       <c r="Y14" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="AA14" s="771"/>
-      <c r="AB14" s="772"/>
-      <c r="AD14" s="759"/>
+      <c r="AA14" s="778"/>
+      <c r="AB14" s="779"/>
+      <c r="AD14" s="766"/>
     </row>
     <row r="15" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="130" t="s">
@@ -14456,19 +14456,19 @@
       <c r="F15" s="66" t="s">
         <v>93</v>
       </c>
-      <c r="G15" s="786"/>
+      <c r="G15" s="754"/>
       <c r="H15" s="2" t="s">
         <v>80</v>
       </c>
       <c r="I15" s="53" t="s">
         <v>80</v>
       </c>
-      <c r="K15" s="765"/>
-      <c r="L15" s="782"/>
-      <c r="Q15" s="788" t="s">
+      <c r="K15" s="772"/>
+      <c r="L15" s="789"/>
+      <c r="Q15" s="756" t="s">
         <v>210</v>
       </c>
-      <c r="R15" s="650"/>
+      <c r="R15" s="645"/>
       <c r="S15" s="605"/>
       <c r="T15" s="6"/>
       <c r="V15" s="68" t="s">
@@ -14477,14 +14477,14 @@
       <c r="X15" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="AA15" s="771"/>
-      <c r="AB15" s="772"/>
-      <c r="AD15" s="759"/>
+      <c r="AA15" s="778"/>
+      <c r="AB15" s="779"/>
+      <c r="AD15" s="766"/>
     </row>
     <row r="16" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C16" s="132"/>
-      <c r="G16" s="786"/>
-      <c r="K16" s="765"/>
+      <c r="G16" s="754"/>
+      <c r="K16" s="772"/>
       <c r="N16" s="47"/>
       <c r="O16" s="61" t="s">
         <v>108</v>
@@ -14503,24 +14503,24 @@
       <c r="Z16" s="76" t="s">
         <v>126</v>
       </c>
-      <c r="AA16" s="771"/>
-      <c r="AB16" s="772"/>
-      <c r="AD16" s="759"/>
+      <c r="AA16" s="778"/>
+      <c r="AB16" s="779"/>
+      <c r="AD16" s="766"/>
     </row>
     <row r="17" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C17" s="109"/>
       <c r="E17" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="F17" s="783" t="s">
+      <c r="F17" s="751" t="s">
         <v>95</v>
       </c>
-      <c r="G17" s="786"/>
+      <c r="G17" s="754"/>
       <c r="H17" s="54"/>
       <c r="I17" s="133" t="s">
         <v>80</v>
       </c>
-      <c r="K17" s="765"/>
+      <c r="K17" s="772"/>
       <c r="S17" s="605"/>
       <c r="V17" s="68" t="s">
         <v>44</v>
@@ -14528,9 +14528,9 @@
       <c r="X17" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="AA17" s="771"/>
-      <c r="AB17" s="772"/>
-      <c r="AD17" s="759"/>
+      <c r="AA17" s="778"/>
+      <c r="AB17" s="779"/>
+      <c r="AD17" s="766"/>
     </row>
     <row r="18" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C18" s="130"/>
@@ -14540,15 +14540,15 @@
       <c r="E18" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="F18" s="784"/>
-      <c r="G18" s="786"/>
+      <c r="F18" s="752"/>
+      <c r="G18" s="754"/>
       <c r="H18" s="108" t="s">
         <v>75</v>
       </c>
       <c r="I18" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="K18" s="765"/>
+      <c r="K18" s="772"/>
       <c r="O18" s="64" t="s">
         <v>114</v>
       </c>
@@ -14559,42 +14559,39 @@
       <c r="X18" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="AA18" s="773"/>
-      <c r="AB18" s="774"/>
-      <c r="AD18" s="759"/>
+      <c r="AA18" s="780"/>
+      <c r="AB18" s="781"/>
+      <c r="AD18" s="766"/>
     </row>
     <row r="19" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F19" s="64" t="s">
         <v>208</v>
       </c>
-      <c r="G19" s="787"/>
-      <c r="K19" s="766"/>
+      <c r="G19" s="755"/>
+      <c r="K19" s="773"/>
       <c r="Q19" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="R19" s="792" t="s">
+      <c r="R19" s="760" t="s">
         <v>123</v>
       </c>
-      <c r="S19" s="793"/>
-      <c r="T19" s="794"/>
+      <c r="S19" s="761"/>
+      <c r="T19" s="762"/>
       <c r="V19" s="77" t="s">
         <v>114</v>
       </c>
       <c r="Y19" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="AD19" s="760"/>
+      <c r="AD19" s="767"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="G2:G19"/>
-    <mergeCell ref="Q13:R13"/>
-    <mergeCell ref="Q15:R15"/>
-    <mergeCell ref="L9:N9"/>
-    <mergeCell ref="R19:T19"/>
-    <mergeCell ref="S12:S18"/>
-    <mergeCell ref="O3:O9"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="M10:AC10"/>
+    <mergeCell ref="F2:F3"/>
     <mergeCell ref="AD1:AD19"/>
     <mergeCell ref="S8:AC8"/>
     <mergeCell ref="K5:K19"/>
@@ -14606,11 +14603,14 @@
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="L4:L8"/>
     <mergeCell ref="L12:L15"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="M10:AC10"/>
-    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G2:G19"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="Q15:R15"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="R19:T19"/>
+    <mergeCell ref="S12:S18"/>
+    <mergeCell ref="O3:O9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Rw Usage Updates _8:27 PM
Rw Usage Updates _8:27 PM
Total :- 26 = 14 + 12
Boat Enabled :- BirdW - 12_X_(12 Reserved)
                          FuelW - 8
                          InCapacity :- 14
</commit_message>
<xml_diff>
--- a/System_2.1.8.xlsx
+++ b/System_2.1.8.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Work_For_\Work\Running AppS\System_Work_RW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E9604C3-3847-477D-B005-28759C025E61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A7A3DB7-5811-4E54-B904-B4CB7D28FE50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BoardRW" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1126" uniqueCount="627">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1126" uniqueCount="628">
   <si>
     <t>Zone</t>
   </si>
@@ -1859,9 +1859,6 @@
     <t>nd tv 24*7</t>
   </si>
   <si>
-    <t>3M40F</t>
-  </si>
-  <si>
     <t>IT_X_Media</t>
   </si>
   <si>
@@ -1913,13 +1910,19 @@
     <t>NodeW</t>
   </si>
   <si>
-    <t xml:space="preserve">8F Reserved </t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>AT - CT_WLFJN_X_N-10_X_Left</t>
+  </si>
+  <si>
+    <t>12F Wbt</t>
+  </si>
+  <si>
+    <t>14F Wbt</t>
+  </si>
+  <si>
+    <t>3M26F</t>
   </si>
 </sst>
 </file>
@@ -5901,8 +5904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:X28"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="X8" sqref="X8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="W17" sqref="W17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6094,7 +6097,7 @@
         <v>226</v>
       </c>
       <c r="V5" s="19">
-        <v>6540</v>
+        <v>6600</v>
       </c>
     </row>
     <row r="6" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6232,7 +6235,7 @@
         <v>1</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="R9" s="34" t="s">
         <v>44</v>
@@ -6251,7 +6254,7 @@
       </c>
       <c r="D10" s="61"/>
       <c r="F10" s="362" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>21</v>
@@ -6319,7 +6322,7 @@
         <v>225</v>
       </c>
       <c r="V11" s="64">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6384,7 +6387,7 @@
         <v>589</v>
       </c>
       <c r="V13" s="24">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6674,7 +6677,9 @@
       </c>
       <c r="P22" s="315"/>
       <c r="T22" s="613"/>
-      <c r="X22" s="19"/>
+      <c r="X22" s="19" t="s">
+        <v>625</v>
+      </c>
     </row>
     <row r="23" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="2" t="s">
@@ -6687,7 +6692,7 @@
       <c r="E23" s="61"/>
       <c r="F23" s="100"/>
       <c r="G23" s="2" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>411</v>
@@ -6725,7 +6730,7 @@
       <c r="E24" s="468"/>
       <c r="F24" s="390"/>
       <c r="G24" s="241" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="H24" s="212" t="s">
         <v>393</v>
@@ -6747,7 +6752,7 @@
       <c r="S24" s="80"/>
       <c r="T24" s="613"/>
       <c r="X24" s="19" t="s">
-        <v>624</v>
+        <v>626</v>
       </c>
     </row>
     <row r="25" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6806,10 +6811,10 @@
       <c r="E26" s="396"/>
       <c r="F26" s="362"/>
       <c r="G26" s="2" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="I26" s="61"/>
       <c r="J26" s="244"/>
@@ -6824,7 +6829,7 @@
       <c r="P26" s="315"/>
       <c r="T26" s="613"/>
       <c r="V26" s="519" t="s">
-        <v>606</v>
+        <v>627</v>
       </c>
     </row>
     <row r="27" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6838,7 +6843,7 @@
       <c r="E27" s="396"/>
       <c r="F27" s="385"/>
       <c r="G27" s="2" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="H27" s="212" t="s">
         <v>515</v>
@@ -6879,7 +6884,7 @@
       <c r="E28" s="396"/>
       <c r="F28" s="387"/>
       <c r="G28" s="2" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="H28" s="212" t="s">
         <v>580</v>
@@ -9040,7 +9045,7 @@
   <dimension ref="A1:AL31"/>
   <sheetViews>
     <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="AJ17" sqref="AJ17"/>
+      <selection activeCell="AG17" sqref="AG17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9206,7 +9211,7 @@
       <c r="Q2" s="708"/>
       <c r="R2" s="21">
         <f>R7+R20</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="S2" s="21">
         <f>S7+S20</f>
@@ -9417,7 +9422,7 @@
       </c>
       <c r="R6" s="64">
         <f>R7-SUM(X2:X10)+R11</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S6" s="64">
         <f>S7-S12-SUM(V2:V10)</f>
@@ -9468,7 +9473,7 @@
       </c>
       <c r="R7" s="24">
         <f>3-R11</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="S7" s="24">
         <f>3-S11</f>
@@ -9476,12 +9481,8 @@
       </c>
       <c r="U7" s="6"/>
       <c r="V7" s="474"/>
-      <c r="W7" s="6" t="s">
-        <v>475</v>
-      </c>
-      <c r="X7" s="474">
-        <v>1</v>
-      </c>
+      <c r="W7" s="6"/>
+      <c r="X7" s="474"/>
       <c r="AB7" s="702"/>
       <c r="AC7" s="99" t="s">
         <v>595</v>
@@ -9501,7 +9502,7 @@
       <c r="AI7" s="474"/>
       <c r="AJ7" s="561"/>
       <c r="AK7" s="6" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="AL7" s="474">
         <v>1</v>
@@ -9628,7 +9629,7 @@
       <c r="AI10" s="475"/>
       <c r="AJ10" s="562"/>
       <c r="AK10" s="6" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="AL10" s="556">
         <v>2</v>
@@ -9669,7 +9670,7 @@
         <v>44</v>
       </c>
       <c r="R11" s="24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S11" s="24">
         <v>2</v>
@@ -9695,7 +9696,7 @@
       </c>
       <c r="AG11" s="418"/>
       <c r="AH11" s="704" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="AI11" s="705"/>
       <c r="AJ11" s="705"/>
@@ -10320,8 +10321,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2029A93E-B53C-4201-9F17-439C144F3CF1}">
   <dimension ref="A1:AT37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="W9" sqref="W9"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32:B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10388,7 +10389,7 @@
         <v>0</v>
       </c>
       <c r="H1" s="80" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="I1" s="95" t="s">
         <v>41</v>
@@ -10397,7 +10398,7 @@
         <v>200</v>
       </c>
       <c r="K1" s="72" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="L1" s="591" t="s">
         <v>577</v>
@@ -10473,7 +10474,7 @@
       </c>
       <c r="J2" s="320">
         <f>K2+L2</f>
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="K2" s="749">
         <f>SUM(K4:K29)</f>
@@ -10481,7 +10482,7 @@
       </c>
       <c r="L2" s="747">
         <f>SUM(L4:L37)</f>
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="M2" s="733">
         <f>SUM(M5:M30)</f>
@@ -10493,7 +10494,7 @@
       </c>
       <c r="O2" s="737">
         <f>SUM(O4:O29)</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="P2" s="643">
         <f>SUM(N30:N37)* (-1)</f>
@@ -10558,10 +10559,10 @@
         <v>289</v>
       </c>
       <c r="AK2" s="150" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="AL2" s="150" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="AM2" s="21" t="s">
         <v>444</v>
@@ -10624,15 +10625,15 @@
       </c>
       <c r="AA3" s="66">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AB3" s="66">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="AC3" s="66">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AD3" s="66">
         <f t="shared" ref="AD3:AO3" si="1">SUM(AD4:AD29)</f>
@@ -10640,7 +10641,7 @@
       </c>
       <c r="AE3" s="66">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AF3" s="66">
         <f t="shared" si="1"/>
@@ -10652,7 +10653,7 @@
       </c>
       <c r="AH3" s="66">
         <f>SUM(AH4:AH29)</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AI3" s="377">
         <f t="shared" si="1"/>
@@ -10666,15 +10667,15 @@
       <c r="AL3" s="408"/>
       <c r="AM3" s="100">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="AN3" s="312">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AO3" s="313">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AR3" s="142"/>
     </row>
@@ -10887,7 +10888,7 @@
       </c>
       <c r="O6" s="295">
         <f>AC6</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P6" s="745"/>
       <c r="Q6" s="19" t="s">
@@ -10918,27 +10919,27 @@
       <c r="Z6" s="298"/>
       <c r="AA6" s="117">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB6" s="292">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC6" s="292">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD6" s="292">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AE6" s="296">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF6" s="302"/>
       <c r="AG6" s="298"/>
       <c r="AH6" s="298">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI6" s="378">
         <v>0</v>
@@ -10948,15 +10949,15 @@
       <c r="AL6" s="319"/>
       <c r="AM6" s="339">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN6" s="310">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO6" s="311">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AP6" s="6" t="s">
         <v>475</v>
@@ -11283,15 +11284,13 @@
         <v>0</v>
       </c>
       <c r="I10" s="111" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="J10" s="581" t="s">
         <v>357</v>
       </c>
       <c r="K10" s="585"/>
-      <c r="L10" s="593">
-        <v>2</v>
-      </c>
+      <c r="L10" s="593"/>
       <c r="M10" s="330"/>
       <c r="N10" s="107">
         <v>1</v>
@@ -11470,7 +11469,7 @@
         <v>-1</v>
       </c>
       <c r="I12" s="61" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="J12" s="581" t="s">
         <v>298</v>
@@ -11580,7 +11579,7 @@
       </c>
       <c r="H13" s="273"/>
       <c r="I13" s="111" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="J13" s="582" t="s">
         <v>303</v>
@@ -11750,7 +11749,7 @@
         <v>563</v>
       </c>
       <c r="AR14" s="513" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="15" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11769,9 +11768,7 @@
         <v>194</v>
       </c>
       <c r="K15" s="586"/>
-      <c r="L15" s="594">
-        <v>1</v>
-      </c>
+      <c r="L15" s="594"/>
       <c r="M15" s="330"/>
       <c r="N15" s="293">
         <v>1</v>
@@ -11968,9 +11965,7 @@
         <v>310</v>
       </c>
       <c r="K17" s="586"/>
-      <c r="L17" s="594">
-        <v>1</v>
-      </c>
+      <c r="L17" s="594"/>
       <c r="M17" s="330"/>
       <c r="N17" s="107">
         <v>1</v>
@@ -12160,7 +12155,9 @@
       <c r="K19" s="586">
         <v>2</v>
       </c>
-      <c r="L19" s="594"/>
+      <c r="L19" s="594">
+        <v>1</v>
+      </c>
       <c r="M19" s="118"/>
       <c r="N19" s="107">
         <v>1</v>
@@ -12269,7 +12266,7 @@
       </c>
       <c r="K20" s="586"/>
       <c r="L20" s="594">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M20" s="329"/>
       <c r="N20" s="107">
@@ -12760,9 +12757,7 @@
         <v>296</v>
       </c>
       <c r="K25" s="585"/>
-      <c r="L25" s="593">
-        <v>1</v>
-      </c>
+      <c r="L25" s="593"/>
       <c r="M25" s="334"/>
       <c r="N25" s="107">
         <v>0</v>
@@ -13252,7 +13247,7 @@
       <c r="A31" s="80"/>
       <c r="B31" s="112"/>
       <c r="C31" s="21" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>361</v>
@@ -13330,9 +13325,7 @@
         <v>310</v>
       </c>
       <c r="K32" s="590"/>
-      <c r="L32" s="593">
-        <v>2</v>
-      </c>
+      <c r="L32" s="593"/>
       <c r="M32" s="515">
         <v>0</v>
       </c>
@@ -13497,7 +13490,7 @@
       </c>
       <c r="K34" s="513"/>
       <c r="L34" s="593">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M34" s="337"/>
       <c r="N34" s="250">
@@ -13667,9 +13660,7 @@
       <c r="AR35" s="513"/>
     </row>
     <row r="36" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="24">
-        <v>-1</v>
-      </c>
+      <c r="B36" s="24"/>
       <c r="F36" s="261" t="s">
         <v>44</v>
       </c>
@@ -13756,7 +13747,7 @@
     </row>
     <row r="37" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="24">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D37" s="385">
         <v>1</v>
@@ -13769,11 +13760,11 @@
       </c>
       <c r="I37" s="2"/>
       <c r="J37" s="2" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="K37" s="559"/>
       <c r="L37" s="596">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M37" s="338"/>
       <c r="N37" s="251">

</xml_diff>